<commit_message>
Update the changelog in documenting spreadsheet.
</commit_message>
<xml_diff>
--- a/CCGX-Modbus-TCP-register-list.xlsx
+++ b/CCGX-Modbus-TCP-register-list.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2488" uniqueCount="845">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2494" uniqueCount="851">
   <si>
     <t xml:space="preserve">NOTE: Use unit-id 100 for the com.victronenergy.system data, for more information see FAQ.</t>
   </si>
@@ -2557,6 +2557,24 @@
   </si>
   <si>
     <t xml:space="preserve">Some other small textual improvements.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rev 16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Added registers for battery alarms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Changed battery relay to be writeable (only works with some batteries).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Added LowCellVoltage alarm for Lynx batteries</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Added VE.Bus temperature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Added VE.Bus reset</t>
   </si>
 </sst>
 </file>
@@ -2794,6 +2812,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2808,10 +2830,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -2899,9 +2917,9 @@
   <dimension ref="A1:N328"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="2" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A97" activeCellId="0" sqref="A97"/>
+      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2909,11 +2927,11 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="30.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="37.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="8.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="8.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="8.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="10.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="26.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="8.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="8.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="70.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="1" width="9"/>
   </cols>
@@ -5872,7 +5890,7 @@
       <c r="A97" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B97" s="0" t="s">
+      <c r="B97" s="22" t="s">
         <v>276</v>
       </c>
       <c r="C97" s="1" t="n">
@@ -12736,559 +12754,559 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="22" width="7.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="22" width="16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="22" width="23.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="22" width="8.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="23" t="s">
         <v>728</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="23" t="s">
         <v>729</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="23" t="s">
         <v>730</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="22" t="n">
         <v>246</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="22" t="n">
         <v>257</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="22" t="s">
         <v>731</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="A3" s="22" t="n">
         <v>247</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="22" t="n">
         <v>256</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="22" t="s">
         <v>732</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+      <c r="A4" s="22" t="n">
         <v>245</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="22" t="n">
         <v>258</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="24" t="s">
         <v>733</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="23" t="n">
+      <c r="A5" s="24" t="n">
         <v>243</v>
       </c>
-      <c r="B5" s="23" t="n">
+      <c r="B5" s="24" t="n">
         <v>260</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="24" t="s">
         <v>734</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="23" t="n">
+      <c r="A6" s="24" t="n">
         <v>242</v>
       </c>
-      <c r="B6" s="23" t="n">
+      <c r="B6" s="24" t="n">
         <v>261</v>
       </c>
-      <c r="C6" s="23" t="s">
+      <c r="C6" s="24" t="s">
         <v>735</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
+      <c r="A7" s="22" t="n">
         <v>100</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7" s="22" t="n">
         <v>0</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="22" t="s">
         <v>736</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B8" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C8" s="0" t="s">
+      <c r="A8" s="22" t="n">
+        <v>1</v>
+      </c>
+      <c r="B8" s="22" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" s="22" t="s">
         <v>737</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
+      <c r="A9" s="22" t="n">
         <v>2</v>
       </c>
-      <c r="B9" s="0" t="n">
+      <c r="B9" s="22" t="n">
         <v>2</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="22" t="s">
         <v>738</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
+      <c r="A10" s="22" t="n">
         <v>3</v>
       </c>
-      <c r="B10" s="0" t="n">
+      <c r="B10" s="22" t="n">
         <v>3</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" s="22" t="s">
         <v>739</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
+      <c r="A11" s="22" t="n">
         <v>4</v>
       </c>
-      <c r="B11" s="0" t="n">
+      <c r="B11" s="22" t="n">
         <v>4</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" s="22" t="s">
         <v>740</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
+      <c r="A12" s="22" t="n">
         <v>5</v>
       </c>
-      <c r="B12" s="0" t="n">
+      <c r="B12" s="22" t="n">
         <v>5</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" s="22" t="s">
         <v>741</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="n">
+      <c r="A13" s="22" t="n">
         <v>6</v>
       </c>
-      <c r="B13" s="0" t="n">
+      <c r="B13" s="22" t="n">
         <v>6</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="C13" s="22" t="s">
         <v>742</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="n">
+      <c r="A14" s="22" t="n">
         <v>7</v>
       </c>
-      <c r="B14" s="0" t="n">
+      <c r="B14" s="22" t="n">
         <v>7</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="C14" s="22" t="s">
         <v>743</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="n">
+      <c r="A15" s="22" t="n">
         <v>8</v>
       </c>
-      <c r="B15" s="0" t="n">
+      <c r="B15" s="22" t="n">
         <v>8</v>
       </c>
-      <c r="C15" s="0" t="s">
+      <c r="C15" s="22" t="s">
         <v>744</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="n">
+      <c r="A16" s="22" t="n">
         <v>9</v>
       </c>
-      <c r="B16" s="0" t="n">
+      <c r="B16" s="22" t="n">
         <v>9</v>
       </c>
-      <c r="C16" s="0" t="s">
+      <c r="C16" s="22" t="s">
         <v>745</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="n">
+      <c r="A17" s="22" t="n">
         <v>10</v>
       </c>
-      <c r="B17" s="0" t="n">
+      <c r="B17" s="22" t="n">
         <v>10</v>
       </c>
-      <c r="C17" s="0" t="s">
+      <c r="C17" s="22" t="s">
         <v>746</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="n">
+      <c r="A18" s="22" t="n">
         <v>11</v>
       </c>
-      <c r="B18" s="0" t="n">
+      <c r="B18" s="22" t="n">
         <v>11</v>
       </c>
-      <c r="C18" s="0" t="s">
+      <c r="C18" s="22" t="s">
         <v>747</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="n">
+      <c r="A19" s="22" t="n">
         <v>12</v>
       </c>
-      <c r="B19" s="0" t="n">
+      <c r="B19" s="22" t="n">
         <v>12</v>
       </c>
-      <c r="C19" s="0" t="s">
+      <c r="C19" s="22" t="s">
         <v>748</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="B20" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="C20" s="0" t="s">
+      <c r="A20" s="22" t="n">
+        <v>20</v>
+      </c>
+      <c r="B20" s="22" t="n">
+        <v>20</v>
+      </c>
+      <c r="C20" s="22" t="s">
         <v>749</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="n">
+      <c r="A21" s="22" t="n">
         <v>21</v>
       </c>
-      <c r="B21" s="0" t="n">
+      <c r="B21" s="22" t="n">
         <v>21</v>
       </c>
-      <c r="C21" s="0" t="s">
+      <c r="C21" s="22" t="s">
         <v>750</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="n">
+      <c r="A22" s="22" t="n">
         <v>22</v>
       </c>
-      <c r="B22" s="0" t="n">
+      <c r="B22" s="22" t="n">
         <v>22</v>
       </c>
-      <c r="C22" s="0" t="s">
+      <c r="C22" s="22" t="s">
         <v>751</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="n">
+      <c r="A23" s="22" t="n">
         <v>23</v>
       </c>
-      <c r="B23" s="0" t="n">
+      <c r="B23" s="22" t="n">
         <v>23</v>
       </c>
-      <c r="C23" s="0" t="s">
+      <c r="C23" s="22" t="s">
         <v>752</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="n">
+      <c r="A24" s="22" t="n">
         <v>24</v>
       </c>
-      <c r="B24" s="0" t="n">
+      <c r="B24" s="22" t="n">
         <v>24</v>
       </c>
-      <c r="C24" s="0" t="s">
+      <c r="C24" s="22" t="s">
         <v>753</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="n">
+      <c r="A25" s="22" t="n">
         <v>25</v>
       </c>
-      <c r="B25" s="0" t="n">
+      <c r="B25" s="22" t="n">
         <v>25</v>
       </c>
-      <c r="C25" s="0" t="s">
+      <c r="C25" s="22" t="s">
         <v>754</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="n">
+      <c r="A26" s="22" t="n">
         <v>26</v>
       </c>
-      <c r="B26" s="0" t="n">
+      <c r="B26" s="22" t="n">
         <v>26</v>
       </c>
-      <c r="C26" s="0" t="s">
+      <c r="C26" s="22" t="s">
         <v>755</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="n">
+      <c r="A27" s="22" t="n">
         <v>27</v>
       </c>
-      <c r="B27" s="0" t="n">
+      <c r="B27" s="22" t="n">
         <v>27</v>
       </c>
-      <c r="C27" s="0" t="s">
+      <c r="C27" s="22" t="s">
         <v>756</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="n">
+      <c r="A28" s="22" t="n">
         <v>28</v>
       </c>
-      <c r="B28" s="0" t="n">
+      <c r="B28" s="22" t="n">
         <v>28</v>
       </c>
-      <c r="C28" s="0" t="s">
+      <c r="C28" s="22" t="s">
         <v>757</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="n">
+      <c r="A29" s="22" t="n">
         <v>29</v>
       </c>
-      <c r="B29" s="0" t="n">
+      <c r="B29" s="22" t="n">
         <v>29</v>
       </c>
-      <c r="C29" s="0" t="s">
+      <c r="C29" s="22" t="s">
         <v>758</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="n">
+      <c r="A30" s="22" t="n">
         <v>30</v>
       </c>
-      <c r="B30" s="0" t="n">
+      <c r="B30" s="22" t="n">
         <v>30</v>
       </c>
-      <c r="C30" s="0" t="s">
+      <c r="C30" s="22" t="s">
         <v>759</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="n">
+      <c r="A31" s="22" t="n">
         <v>31</v>
       </c>
-      <c r="B31" s="0" t="n">
+      <c r="B31" s="22" t="n">
         <v>31</v>
       </c>
-      <c r="C31" s="0" t="s">
+      <c r="C31" s="22" t="s">
         <v>760</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="n">
+      <c r="A32" s="22" t="n">
         <v>32</v>
       </c>
-      <c r="B32" s="0" t="n">
+      <c r="B32" s="22" t="n">
         <v>32</v>
       </c>
-      <c r="C32" s="0" t="s">
+      <c r="C32" s="22" t="s">
         <v>761</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="n">
+      <c r="A33" s="22" t="n">
         <v>33</v>
       </c>
-      <c r="B33" s="0" t="n">
+      <c r="B33" s="22" t="n">
         <v>33</v>
       </c>
-      <c r="C33" s="0" t="s">
+      <c r="C33" s="22" t="s">
         <v>762</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="n">
+      <c r="A34" s="22" t="n">
         <v>34</v>
       </c>
-      <c r="B34" s="0" t="n">
+      <c r="B34" s="22" t="n">
         <v>34</v>
       </c>
-      <c r="C34" s="0" t="s">
+      <c r="C34" s="22" t="s">
         <v>763</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="n">
+      <c r="A35" s="22" t="n">
         <v>40</v>
       </c>
-      <c r="B35" s="0" t="n">
+      <c r="B35" s="22" t="n">
         <v>40</v>
       </c>
-      <c r="C35" s="0" t="s">
+      <c r="C35" s="22" t="s">
         <v>764</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="n">
+      <c r="A36" s="22" t="n">
         <v>41</v>
       </c>
-      <c r="B36" s="0" t="n">
+      <c r="B36" s="22" t="n">
         <v>41</v>
       </c>
-      <c r="C36" s="0" t="s">
+      <c r="C36" s="22" t="s">
         <v>765</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="n">
+      <c r="A37" s="22" t="n">
         <v>42</v>
       </c>
-      <c r="B37" s="0" t="n">
+      <c r="B37" s="22" t="n">
         <v>42</v>
       </c>
-      <c r="C37" s="0" t="s">
+      <c r="C37" s="22" t="s">
         <v>766</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="n">
+      <c r="A38" s="22" t="n">
         <v>43</v>
       </c>
-      <c r="B38" s="0" t="n">
+      <c r="B38" s="22" t="n">
         <v>43</v>
       </c>
-      <c r="C38" s="0" t="s">
+      <c r="C38" s="22" t="s">
         <v>767</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="n">
+      <c r="A39" s="22" t="n">
         <v>44</v>
       </c>
-      <c r="B39" s="0" t="n">
+      <c r="B39" s="22" t="n">
         <v>44</v>
       </c>
-      <c r="C39" s="0" t="s">
+      <c r="C39" s="22" t="s">
         <v>768</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="n">
+      <c r="A40" s="22" t="n">
         <v>45</v>
       </c>
-      <c r="B40" s="0" t="n">
+      <c r="B40" s="22" t="n">
         <v>45</v>
       </c>
-      <c r="C40" s="0" t="s">
+      <c r="C40" s="22" t="s">
         <v>769</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="n">
+      <c r="A41" s="22" t="n">
         <v>46</v>
       </c>
-      <c r="B41" s="0" t="n">
+      <c r="B41" s="22" t="n">
         <v>46</v>
       </c>
-      <c r="C41" s="0" t="s">
+      <c r="C41" s="22" t="s">
         <v>770</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="n">
+      <c r="A42" s="22" t="n">
         <v>239</v>
       </c>
-      <c r="B42" s="0" t="n">
+      <c r="B42" s="22" t="n">
         <v>288</v>
       </c>
-      <c r="C42" s="0" t="s">
+      <c r="C42" s="22" t="s">
         <v>771</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="n">
+      <c r="A43" s="22" t="n">
         <v>238</v>
       </c>
-      <c r="B43" s="0" t="n">
+      <c r="B43" s="22" t="n">
         <v>289</v>
       </c>
-      <c r="C43" s="0" t="s">
+      <c r="C43" s="22" t="s">
         <v>772</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="n">
+      <c r="A44" s="22" t="n">
         <v>237</v>
       </c>
-      <c r="B44" s="0" t="n">
+      <c r="B44" s="22" t="n">
         <v>290</v>
       </c>
-      <c r="C44" s="0" t="s">
+      <c r="C44" s="22" t="s">
         <v>773</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="n">
+      <c r="A45" s="22" t="n">
         <v>236</v>
       </c>
-      <c r="B45" s="0" t="n">
+      <c r="B45" s="22" t="n">
         <v>291</v>
       </c>
-      <c r="C45" s="0" t="s">
+      <c r="C45" s="22" t="s">
         <v>774</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="n">
+      <c r="A46" s="22" t="n">
         <v>235</v>
       </c>
-      <c r="B46" s="0" t="n">
+      <c r="B46" s="22" t="n">
         <v>292</v>
       </c>
-      <c r="C46" s="0" t="s">
+      <c r="C46" s="22" t="s">
         <v>775</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="n">
+      <c r="A47" s="22" t="n">
         <v>233</v>
       </c>
-      <c r="B47" s="0" t="n">
+      <c r="B47" s="22" t="n">
         <v>293</v>
       </c>
-      <c r="C47" s="0" t="s">
+      <c r="C47" s="22" t="s">
         <v>776</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="n">
+      <c r="A48" s="22" t="n">
         <v>225</v>
       </c>
-      <c r="B48" s="0" t="n">
+      <c r="B48" s="22" t="n">
         <v>512</v>
       </c>
-      <c r="C48" s="0" t="s">
+      <c r="C48" s="22" t="s">
         <v>777</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="24" t="s">
+      <c r="A50" s="25" t="s">
         <v>778</v>
       </c>
-      <c r="B50" s="24"/>
-      <c r="C50" s="24"/>
-      <c r="D50" s="24"/>
-      <c r="E50" s="24"/>
-      <c r="F50" s="24"/>
+      <c r="B50" s="25"/>
+      <c r="C50" s="25"/>
+      <c r="D50" s="25"/>
+      <c r="E50" s="25"/>
+      <c r="F50" s="25"/>
     </row>
     <row r="51" customFormat="false" ht="92.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="25" t="s">
+      <c r="A51" s="26" t="s">
         <v>779</v>
       </c>
-      <c r="B51" s="25"/>
-      <c r="C51" s="25"/>
-      <c r="D51" s="25"/>
-      <c r="E51" s="25"/>
-      <c r="F51" s="25"/>
+      <c r="B51" s="26"/>
+      <c r="C51" s="26"/>
+      <c r="D51" s="26"/>
+      <c r="E51" s="26"/>
+      <c r="F51" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -13310,240 +13328,240 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C49"/>
+  <dimension ref="A1:C54"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B49" activeCellId="0" sqref="B49"/>
+      <selection pane="topLeft" activeCell="B54" activeCellId="0" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="3.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="67.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="22" width="8.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="22" width="3.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="22" width="67.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="22" width="8.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="22" t="s">
         <v>780</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="22" t="s">
         <v>781</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="22" t="s">
         <v>782</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="22" t="s">
         <v>783</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="22" t="s">
         <v>784</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="22" t="s">
         <v>785</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="22" t="s">
         <v>786</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="22" t="s">
         <v>787</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C5" s="26" t="s">
+      <c r="C5" s="22" t="s">
         <v>788</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C6" s="26" t="s">
+      <c r="C6" s="22" t="s">
         <v>789</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C7" s="26" t="s">
+      <c r="C7" s="22" t="s">
         <v>790</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="22" t="s">
         <v>791</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="22" t="s">
         <v>792</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="22" t="s">
         <v>793</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="22" t="s">
         <v>794</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="22" t="s">
         <v>795</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="22" t="s">
         <v>796</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="22" t="s">
         <v>797</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="22" t="s">
         <v>798</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="22" t="s">
         <v>799</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="22" t="s">
         <v>800</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="0" t="s">
+      <c r="B16" s="22" t="s">
         <v>801</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="0" t="s">
+      <c r="B17" s="22" t="s">
         <v>802</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="22" t="s">
         <v>803</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" s="22" t="s">
         <v>804</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="22" t="s">
         <v>805</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="B19" s="22" t="s">
         <v>806</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="0" t="s">
+      <c r="B20" s="22" t="s">
         <v>807</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="0" t="s">
+      <c r="B21" s="22" t="s">
         <v>808</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+      <c r="A22" s="22" t="s">
         <v>809</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="B22" s="22" t="s">
         <v>810</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="0" t="s">
+      <c r="B23" s="22" t="s">
         <v>811</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="0" t="s">
+      <c r="B24" s="22" t="s">
         <v>812</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="0" t="s">
+      <c r="B25" s="22" t="s">
         <v>813</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="0" t="s">
+      <c r="B26" s="22" t="s">
         <v>814</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="0" t="s">
+      <c r="B27" s="22" t="s">
         <v>815</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="0" t="s">
+      <c r="B28" s="22" t="s">
         <v>816</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="0" t="s">
+      <c r="B29" s="22" t="s">
         <v>817</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
+      <c r="A30" s="22" t="s">
         <v>818</v>
       </c>
-      <c r="B30" s="0" t="s">
+      <c r="B30" s="22" t="s">
         <v>819</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="0" t="s">
+      <c r="B31" s="22" t="s">
         <v>820</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="0" t="s">
+      <c r="B32" s="22" t="s">
         <v>821</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
+      <c r="A33" s="22" t="s">
         <v>822</v>
       </c>
-      <c r="B33" s="0" t="s">
+      <c r="B33" s="22" t="s">
         <v>823</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="0" t="s">
+      <c r="B34" s="22" t="s">
         <v>824</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="0" t="s">
+      <c r="B35" s="22" t="s">
         <v>825</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="0" t="s">
+      <c r="B36" s="22" t="s">
         <v>826</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="0" t="s">
+      <c r="B37" s="22" t="s">
         <v>827</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="0" t="s">
+      <c r="B38" s="22" t="s">
         <v>828</v>
       </c>
     </row>
@@ -13553,68 +13571,96 @@
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
+      <c r="A40" s="22" t="s">
         <v>830</v>
       </c>
-      <c r="B40" s="0" t="s">
+      <c r="B40" s="22" t="s">
         <v>831</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
+      <c r="A41" s="22" t="s">
         <v>832</v>
       </c>
-      <c r="B41" s="0" t="s">
+      <c r="B41" s="22" t="s">
         <v>833</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="0" t="s">
+      <c r="B42" s="22" t="s">
         <v>834</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="0" t="s">
+      <c r="B43" s="22" t="s">
         <v>835</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
+      <c r="A44" s="22" t="s">
         <v>836</v>
       </c>
-      <c r="B44" s="0" t="s">
+      <c r="B44" s="22" t="s">
         <v>837</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="0" t="s">
+      <c r="B45" s="22" t="s">
         <v>838</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="0" t="s">
+      <c r="B46" s="22" t="s">
         <v>839</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="s">
+      <c r="A47" s="22" t="s">
         <v>840</v>
       </c>
-      <c r="B47" s="0" t="s">
+      <c r="B47" s="22" t="s">
         <v>841</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="s">
+      <c r="A48" s="22" t="s">
         <v>842</v>
       </c>
-      <c r="B48" s="0" t="s">
+      <c r="B48" s="22" t="s">
         <v>843</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B49" s="0" t="s">
+      <c r="B49" s="22" t="s">
         <v>844</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="22" t="s">
+        <v>845</v>
+      </c>
+      <c r="B50" s="22" t="s">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B51" s="22" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B52" s="22" t="s">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B53" s="22" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B54" s="22" t="s">
+        <v>850</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add registers for generator start/stop.
 - Add writable register to manually start the generator
 - Add register with generator runtime
 - Add RunByConditionCode register that shows the reason why the generator is running.

https://github.com/victronenergy/venus/issues/161
</commit_message>
<xml_diff>
--- a/CCGX-Modbus-TCP-register-list.xlsx
+++ b/CCGX-Modbus-TCP-register-list.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Field list" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2494" uniqueCount="851">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2517" uniqueCount="861">
   <si>
     <t xml:space="preserve">NOTE: Use unit-id 100 for the com.victronenergy.system data, for more information see FAQ.</t>
   </si>
@@ -2208,6 +2208,30 @@
     <t xml:space="preserve">2=Door;3=Bilge pump;4=Bilge alarm;5=Burglar alarm;6=Smoke alarm;7=Fire alarm;8=CO2 alarm</t>
   </si>
   <si>
+    <t xml:space="preserve">com.victronenergy.generator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manual Start</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Generator0/Runtime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0=Stop generator; 1=Start generator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Condition that started the generator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Generator0/RunningByConditionCode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0=Stopped;1=Manual;2=TestRun;3=LossOfComms;4=Soc;5=AcLoad;6=BatteryCurrent;7=BatteryVoltage;8=InverterTemperatur;9=InverterOverload;10=StopOnAc1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Runtime in seconds</t>
+  </si>
+  <si>
     <t xml:space="preserve">Unit ID</t>
   </si>
   <si>
@@ -2575,6 +2599,12 @@
   </si>
   <si>
     <t xml:space="preserve">Added VE.Bus reset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rev 17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Added registers for generator start/stop</t>
   </si>
 </sst>
 </file>
@@ -2914,12 +2944,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N328"/>
+  <dimension ref="A1:N331"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="2" topLeftCell="A316" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A331" activeCellId="0" sqref="A331"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12725,6 +12755,93 @@
       </c>
       <c r="I328" s="1" t="s">
         <v>727</v>
+      </c>
+    </row>
+    <row r="329" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A329" s="1" t="s">
+        <v>728</v>
+      </c>
+      <c r="B329" s="1" t="s">
+        <v>729</v>
+      </c>
+      <c r="C329" s="1" t="n">
+        <v>3500</v>
+      </c>
+      <c r="D329" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E329" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F329" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G329" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="H329" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I329" s="1" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="330" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A330" s="1" t="s">
+        <v>728</v>
+      </c>
+      <c r="B330" s="1" t="s">
+        <v>732</v>
+      </c>
+      <c r="C330" s="1" t="n">
+        <v>3501</v>
+      </c>
+      <c r="D330" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E330" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F330" s="3" t="s">
+        <v>725</v>
+      </c>
+      <c r="G330" s="1" t="s">
+        <v>733</v>
+      </c>
+      <c r="H330" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I330" s="1" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="331" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A331" s="1" t="s">
+        <v>728</v>
+      </c>
+      <c r="B331" s="1" t="s">
+        <v>735</v>
+      </c>
+      <c r="C331" s="1" t="n">
+        <v>3502</v>
+      </c>
+      <c r="D331" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E331" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F331" s="3" t="s">
+        <v>725</v>
+      </c>
+      <c r="G331" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="H331" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I331" s="1" t="s">
+        <v>340</v>
       </c>
     </row>
   </sheetData>
@@ -12762,13 +12879,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="23" t="s">
-        <v>728</v>
+        <v>736</v>
       </c>
       <c r="B1" s="23" t="s">
-        <v>729</v>
+        <v>737</v>
       </c>
       <c r="C1" s="23" t="s">
-        <v>730</v>
+        <v>738</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12779,7 +12896,7 @@
         <v>257</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>731</v>
+        <v>739</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12790,7 +12907,7 @@
         <v>256</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>732</v>
+        <v>740</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12801,7 +12918,7 @@
         <v>258</v>
       </c>
       <c r="C4" s="24" t="s">
-        <v>733</v>
+        <v>741</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12812,7 +12929,7 @@
         <v>260</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>734</v>
+        <v>742</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12823,7 +12940,7 @@
         <v>261</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>735</v>
+        <v>743</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12834,7 +12951,7 @@
         <v>0</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>736</v>
+        <v>744</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12845,7 +12962,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>737</v>
+        <v>745</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12856,7 +12973,7 @@
         <v>2</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>738</v>
+        <v>746</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12867,7 +12984,7 @@
         <v>3</v>
       </c>
       <c r="C10" s="22" t="s">
-        <v>739</v>
+        <v>747</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12878,7 +12995,7 @@
         <v>4</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>740</v>
+        <v>748</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12889,7 +13006,7 @@
         <v>5</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>741</v>
+        <v>749</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12900,7 +13017,7 @@
         <v>6</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>742</v>
+        <v>750</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12911,7 +13028,7 @@
         <v>7</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>743</v>
+        <v>751</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12922,7 +13039,7 @@
         <v>8</v>
       </c>
       <c r="C15" s="22" t="s">
-        <v>744</v>
+        <v>752</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12933,7 +13050,7 @@
         <v>9</v>
       </c>
       <c r="C16" s="22" t="s">
-        <v>745</v>
+        <v>753</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12944,7 +13061,7 @@
         <v>10</v>
       </c>
       <c r="C17" s="22" t="s">
-        <v>746</v>
+        <v>754</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12955,7 +13072,7 @@
         <v>11</v>
       </c>
       <c r="C18" s="22" t="s">
-        <v>747</v>
+        <v>755</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12966,7 +13083,7 @@
         <v>12</v>
       </c>
       <c r="C19" s="22" t="s">
-        <v>748</v>
+        <v>756</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12977,7 +13094,7 @@
         <v>20</v>
       </c>
       <c r="C20" s="22" t="s">
-        <v>749</v>
+        <v>757</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12988,7 +13105,7 @@
         <v>21</v>
       </c>
       <c r="C21" s="22" t="s">
-        <v>750</v>
+        <v>758</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12999,7 +13116,7 @@
         <v>22</v>
       </c>
       <c r="C22" s="22" t="s">
-        <v>751</v>
+        <v>759</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13010,7 +13127,7 @@
         <v>23</v>
       </c>
       <c r="C23" s="22" t="s">
-        <v>752</v>
+        <v>760</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13021,7 +13138,7 @@
         <v>24</v>
       </c>
       <c r="C24" s="22" t="s">
-        <v>753</v>
+        <v>761</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13032,7 +13149,7 @@
         <v>25</v>
       </c>
       <c r="C25" s="22" t="s">
-        <v>754</v>
+        <v>762</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13043,7 +13160,7 @@
         <v>26</v>
       </c>
       <c r="C26" s="22" t="s">
-        <v>755</v>
+        <v>763</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13054,7 +13171,7 @@
         <v>27</v>
       </c>
       <c r="C27" s="22" t="s">
-        <v>756</v>
+        <v>764</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13065,7 +13182,7 @@
         <v>28</v>
       </c>
       <c r="C28" s="22" t="s">
-        <v>757</v>
+        <v>765</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13076,7 +13193,7 @@
         <v>29</v>
       </c>
       <c r="C29" s="22" t="s">
-        <v>758</v>
+        <v>766</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13087,7 +13204,7 @@
         <v>30</v>
       </c>
       <c r="C30" s="22" t="s">
-        <v>759</v>
+        <v>767</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13098,7 +13215,7 @@
         <v>31</v>
       </c>
       <c r="C31" s="22" t="s">
-        <v>760</v>
+        <v>768</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13109,7 +13226,7 @@
         <v>32</v>
       </c>
       <c r="C32" s="22" t="s">
-        <v>761</v>
+        <v>769</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13120,7 +13237,7 @@
         <v>33</v>
       </c>
       <c r="C33" s="22" t="s">
-        <v>762</v>
+        <v>770</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13131,7 +13248,7 @@
         <v>34</v>
       </c>
       <c r="C34" s="22" t="s">
-        <v>763</v>
+        <v>771</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13142,7 +13259,7 @@
         <v>40</v>
       </c>
       <c r="C35" s="22" t="s">
-        <v>764</v>
+        <v>772</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13153,7 +13270,7 @@
         <v>41</v>
       </c>
       <c r="C36" s="22" t="s">
-        <v>765</v>
+        <v>773</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13164,7 +13281,7 @@
         <v>42</v>
       </c>
       <c r="C37" s="22" t="s">
-        <v>766</v>
+        <v>774</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13175,7 +13292,7 @@
         <v>43</v>
       </c>
       <c r="C38" s="22" t="s">
-        <v>767</v>
+        <v>775</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13186,7 +13303,7 @@
         <v>44</v>
       </c>
       <c r="C39" s="22" t="s">
-        <v>768</v>
+        <v>776</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13197,7 +13314,7 @@
         <v>45</v>
       </c>
       <c r="C40" s="22" t="s">
-        <v>769</v>
+        <v>777</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13208,7 +13325,7 @@
         <v>46</v>
       </c>
       <c r="C41" s="22" t="s">
-        <v>770</v>
+        <v>778</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13219,7 +13336,7 @@
         <v>288</v>
       </c>
       <c r="C42" s="22" t="s">
-        <v>771</v>
+        <v>779</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13230,7 +13347,7 @@
         <v>289</v>
       </c>
       <c r="C43" s="22" t="s">
-        <v>772</v>
+        <v>780</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13241,7 +13358,7 @@
         <v>290</v>
       </c>
       <c r="C44" s="22" t="s">
-        <v>773</v>
+        <v>781</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13252,7 +13369,7 @@
         <v>291</v>
       </c>
       <c r="C45" s="22" t="s">
-        <v>774</v>
+        <v>782</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13263,7 +13380,7 @@
         <v>292</v>
       </c>
       <c r="C46" s="22" t="s">
-        <v>775</v>
+        <v>783</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13274,7 +13391,7 @@
         <v>293</v>
       </c>
       <c r="C47" s="22" t="s">
-        <v>776</v>
+        <v>784</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13285,12 +13402,12 @@
         <v>512</v>
       </c>
       <c r="C48" s="22" t="s">
-        <v>777</v>
+        <v>785</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="25" t="s">
-        <v>778</v>
+        <v>786</v>
       </c>
       <c r="B50" s="25"/>
       <c r="C50" s="25"/>
@@ -13300,7 +13417,7 @@
     </row>
     <row r="51" customFormat="false" ht="92.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="26" t="s">
-        <v>779</v>
+        <v>787</v>
       </c>
       <c r="B51" s="26"/>
       <c r="C51" s="26"/>
@@ -13328,10 +13445,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C54"/>
+  <dimension ref="A1:C55"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B54" activeCellId="0" sqref="B54"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C55" activeCellId="0" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13344,323 +13461,331 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="22" t="s">
-        <v>780</v>
+        <v>788</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>781</v>
+        <v>789</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="22" t="s">
-        <v>782</v>
+        <v>790</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>783</v>
+        <v>791</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="22" t="s">
-        <v>784</v>
+        <v>792</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>785</v>
+        <v>793</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="22" t="s">
-        <v>786</v>
+        <v>794</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>787</v>
+        <v>795</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="22" t="s">
-        <v>788</v>
+        <v>796</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="22" t="s">
-        <v>789</v>
+        <v>797</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="22" t="s">
-        <v>790</v>
+        <v>798</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="22" t="s">
-        <v>791</v>
+        <v>799</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="22" t="s">
-        <v>792</v>
+        <v>800</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>793</v>
+        <v>801</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="22" t="s">
-        <v>794</v>
+        <v>802</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="22" t="s">
-        <v>795</v>
+        <v>803</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="22" t="s">
-        <v>796</v>
+        <v>804</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>797</v>
+        <v>805</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="22" t="s">
-        <v>798</v>
+        <v>806</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="22" t="s">
-        <v>799</v>
+        <v>807</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="22" t="s">
-        <v>800</v>
+        <v>808</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="22" t="s">
-        <v>801</v>
+        <v>809</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="22" t="s">
-        <v>802</v>
+        <v>810</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="22" t="s">
-        <v>803</v>
+        <v>811</v>
       </c>
       <c r="B18" s="22" t="s">
-        <v>804</v>
+        <v>812</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="22" t="s">
-        <v>805</v>
+        <v>813</v>
       </c>
       <c r="B19" s="22" t="s">
-        <v>806</v>
+        <v>814</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="22" t="s">
-        <v>807</v>
+        <v>815</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="22" t="s">
-        <v>808</v>
+        <v>816</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="22" t="s">
-        <v>809</v>
+        <v>817</v>
       </c>
       <c r="B22" s="22" t="s">
-        <v>810</v>
+        <v>818</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="22" t="s">
-        <v>811</v>
+        <v>819</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="22" t="s">
-        <v>812</v>
+        <v>820</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="22" t="s">
-        <v>813</v>
+        <v>821</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="22" t="s">
-        <v>814</v>
+        <v>822</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="22" t="s">
-        <v>815</v>
+        <v>823</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="22" t="s">
-        <v>816</v>
+        <v>824</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="22" t="s">
-        <v>817</v>
+        <v>825</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="22" t="s">
-        <v>818</v>
+        <v>826</v>
       </c>
       <c r="B30" s="22" t="s">
-        <v>819</v>
+        <v>827</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="22" t="s">
-        <v>820</v>
+        <v>828</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="22" t="s">
-        <v>821</v>
+        <v>829</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="22" t="s">
-        <v>822</v>
+        <v>830</v>
       </c>
       <c r="B33" s="22" t="s">
-        <v>823</v>
+        <v>831</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="22" t="s">
-        <v>824</v>
+        <v>832</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="22" t="s">
-        <v>825</v>
+        <v>833</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="22" t="s">
-        <v>826</v>
+        <v>834</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="22" t="s">
-        <v>827</v>
+        <v>835</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="22" t="s">
-        <v>828</v>
+        <v>836</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C39" s="27" t="s">
-        <v>829</v>
+        <v>837</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="22" t="s">
-        <v>830</v>
+        <v>838</v>
       </c>
       <c r="B40" s="22" t="s">
-        <v>831</v>
+        <v>839</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="22" t="s">
-        <v>832</v>
+        <v>840</v>
       </c>
       <c r="B41" s="22" t="s">
-        <v>833</v>
+        <v>841</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="22" t="s">
-        <v>834</v>
+        <v>842</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="22" t="s">
-        <v>835</v>
+        <v>843</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="22" t="s">
-        <v>836</v>
+        <v>844</v>
       </c>
       <c r="B44" s="22" t="s">
-        <v>837</v>
+        <v>845</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="22" t="s">
-        <v>838</v>
+        <v>846</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="22" t="s">
-        <v>839</v>
+        <v>847</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="22" t="s">
-        <v>840</v>
+        <v>848</v>
       </c>
       <c r="B47" s="22" t="s">
-        <v>841</v>
+        <v>849</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="22" t="s">
-        <v>842</v>
+        <v>850</v>
       </c>
       <c r="B48" s="22" t="s">
-        <v>843</v>
+        <v>851</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="22" t="s">
-        <v>844</v>
+        <v>852</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="22" t="s">
-        <v>845</v>
+        <v>853</v>
       </c>
       <c r="B50" s="22" t="s">
-        <v>846</v>
+        <v>854</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="22" t="s">
-        <v>847</v>
+        <v>855</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="22" t="s">
-        <v>848</v>
+        <v>856</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="22" t="s">
-        <v>849</v>
+        <v>857</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="22" t="s">
-        <v>850</v>
+        <v>858</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="22" t="s">
+        <v>859</v>
+      </c>
+      <c r="B55" s="22" t="s">
+        <v>860</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated solarcharger mode ESS->External Control.
</commit_message>
<xml_diff>
--- a/CCGX-Modbus-TCP-register-list.xlsx
+++ b/CCGX-Modbus-TCP-register-list.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Field list" sheetId="1" state="visible" r:id="rId2"/>
@@ -1278,7 +1278,7 @@
     <t xml:space="preserve">Charge state</t>
   </si>
   <si>
-    <t xml:space="preserve">0=Off;2=Fault;3=Bulk;4=Absorption;5=Float;6=Storage;7=Equalize;11=Other (Hub-1);252=Hub-1</t>
+    <t xml:space="preserve">0=Off;2=Fault;3=Bulk;4=Absorption;5=Float;6=Storage;7=Equalize;11=Other (Hub-1);252=External control</t>
   </si>
   <si>
     <t xml:space="preserve">PV voltage</t>
@@ -2946,10 +2946,10 @@
   </sheetPr>
   <dimension ref="A1:N331"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="2" topLeftCell="A316" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A331" activeCellId="0" sqref="A331"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="2" topLeftCell="A246" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="B260" activeCellId="0" sqref="B260"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13447,7 +13447,7 @@
   </sheetPr>
   <dimension ref="A1:C55"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C55" activeCellId="0" sqref="C55"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added register for ESS mode.
</commit_message>
<xml_diff>
--- a/CCGX-Modbus-TCP-register-list.xlsx
+++ b/CCGX-Modbus-TCP-register-list.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2517" uniqueCount="861">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2527" uniqueCount="867">
   <si>
     <t xml:space="preserve">NOTE: Use unit-id 100 for the com.victronenergy.system data, for more information see FAQ.</t>
   </si>
@@ -1875,7 +1875,7 @@
     <t xml:space="preserve">/Settings/CGwacs/BatteryLife/State</t>
   </si>
   <si>
-    <t xml:space="preserve">0=External control or BL disabled;1=Restarting;2=Self-consumption;3=Self-consumption;4=Self-consumption;5=Discharge disabled;6=Force charge;7=Sustain;9=Keep batteries charged;10=BL Disabled;11=BL Disabled (Low SoC)</t>
+    <t xml:space="preserve">0=Unused, BL disabled;1=Restarting;2=Self-consumption;3=Self-consumption;4=Self-consumption;5=Discharge disabled;6=Force charge;7=Sustain;9=Keep batteries charged;10=BL Disabled;11=BL Disabled (Low SoC)</t>
   </si>
   <si>
     <t xml:space="preserve">Use value 0 (disable) and 1(enable) for writing only</t>
@@ -1890,6 +1890,15 @@
     <t xml:space="preserve">Same as the setting in the GUI</t>
   </si>
   <si>
+    <t xml:space="preserve">ESS Mode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Settings/Cgwacs/Hub4Mode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1=ESS with Phase Compensation;2=ESS without phase compensation;3=Disabled/External Control</t>
+  </si>
+  <si>
     <t xml:space="preserve">com.victronenergy.tank</t>
   </si>
   <si>
@@ -1899,6 +1908,9 @@
     <t xml:space="preserve">/ProductId</t>
   </si>
   <si>
+    <t xml:space="preserve"/>
+  </si>
+  <si>
     <t xml:space="preserve">Tank capacity</t>
   </si>
   <si>
@@ -2605,6 +2617,12 @@
   </si>
   <si>
     <t xml:space="preserve">Added registers for generator start/stop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rev 18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Added register for ESS mode</t>
   </si>
 </sst>
 </file>
@@ -2614,7 +2632,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2651,6 +2669,18 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="6.4"/>
+      <color rgb="FF4C4C4C"/>
+      <name val="Ubuntu"/>
+      <family val="0"/>
     </font>
   </fonts>
   <fills count="3">
@@ -2753,7 +2783,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2846,6 +2876,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2933,7 +2971,7 @@
       <rgbColor rgb="FF993300"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="FF4C4C4C"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -2944,12 +2982,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N331"/>
+  <dimension ref="A1:N332"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A246" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="B260" activeCellId="0" sqref="B260"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A272" activeCellId="0" sqref="A272"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11131,15 +11169,15 @@
         <v>621</v>
       </c>
     </row>
-    <row r="272" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A272" s="1" t="s">
+    <row r="272" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A272" s="23" t="s">
+        <v>614</v>
+      </c>
+      <c r="B272" s="1" t="s">
         <v>622</v>
       </c>
-      <c r="B272" s="1" t="s">
-        <v>623</v>
-      </c>
       <c r="C272" s="1" t="n">
-        <v>3000</v>
+        <v>2902</v>
       </c>
       <c r="D272" s="2" t="s">
         <v>20</v>
@@ -11151,282 +11189,286 @@
         <v>29</v>
       </c>
       <c r="G272" s="1" t="s">
+        <v>623</v>
+      </c>
+      <c r="H272" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I272" s="0" t="s">
         <v>624</v>
       </c>
-      <c r="H272" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="273" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J272" s="21"/>
+    </row>
+    <row r="273" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A273" s="1" t="s">
-        <v>622</v>
+        <v>625</v>
       </c>
       <c r="B273" s="1" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="C273" s="1" t="n">
-        <v>3001</v>
+        <v>3000</v>
       </c>
       <c r="D273" s="2" t="s">
-        <v>581</v>
+        <v>20</v>
       </c>
       <c r="E273" s="1" t="n">
-        <v>10000</v>
+        <v>1</v>
       </c>
       <c r="F273" s="3" t="s">
-        <v>626</v>
+        <v>29</v>
       </c>
       <c r="G273" s="1" t="s">
-        <v>383</v>
+        <v>627</v>
       </c>
       <c r="H273" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I273" s="1" t="s">
-        <v>627</v>
+      <c r="I273" s="24" t="s">
+        <v>628</v>
       </c>
     </row>
     <row r="274" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A274" s="1" t="s">
-        <v>622</v>
+        <v>625</v>
       </c>
       <c r="B274" s="1" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="C274" s="1" t="n">
-        <v>3003</v>
+        <v>3001</v>
       </c>
       <c r="D274" s="2" t="s">
-        <v>20</v>
+        <v>581</v>
       </c>
       <c r="E274" s="1" t="n">
-        <v>1</v>
+        <v>10000</v>
       </c>
       <c r="F274" s="3" t="s">
-        <v>29</v>
+        <v>630</v>
       </c>
       <c r="G274" s="1" t="s">
-        <v>629</v>
+        <v>383</v>
       </c>
       <c r="H274" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I274" s="1" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
     </row>
     <row r="275" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A275" s="1" t="s">
-        <v>622</v>
+        <v>625</v>
       </c>
       <c r="B275" s="1" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="C275" s="1" t="n">
-        <v>3004</v>
+        <v>3003</v>
       </c>
       <c r="D275" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E275" s="1" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F275" s="3" t="s">
-        <v>79</v>
+        <v>29</v>
       </c>
       <c r="G275" s="1" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="H275" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I275" s="1" t="s">
-        <v>93</v>
+        <v>634</v>
       </c>
     </row>
     <row r="276" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A276" s="1" t="s">
-        <v>622</v>
+        <v>625</v>
       </c>
       <c r="B276" s="1" t="s">
-        <v>633</v>
+        <v>635</v>
       </c>
       <c r="C276" s="1" t="n">
-        <v>3005</v>
+        <v>3004</v>
       </c>
       <c r="D276" s="2" t="s">
-        <v>581</v>
+        <v>20</v>
       </c>
       <c r="E276" s="1" t="n">
-        <v>10000</v>
+        <v>10</v>
       </c>
       <c r="F276" s="3" t="s">
-        <v>626</v>
+        <v>79</v>
       </c>
       <c r="G276" s="1" t="s">
-        <v>634</v>
+        <v>636</v>
       </c>
       <c r="H276" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I276" s="1" t="s">
-        <v>627</v>
+        <v>93</v>
       </c>
     </row>
     <row r="277" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A277" s="1" t="s">
-        <v>622</v>
+        <v>625</v>
       </c>
       <c r="B277" s="1" t="s">
-        <v>635</v>
+        <v>637</v>
       </c>
       <c r="C277" s="1" t="n">
-        <v>3007</v>
+        <v>3005</v>
       </c>
       <c r="D277" s="2" t="s">
-        <v>20</v>
+        <v>581</v>
       </c>
       <c r="E277" s="1" t="n">
-        <v>1</v>
+        <v>10000</v>
       </c>
       <c r="F277" s="3" t="s">
-        <v>29</v>
+        <v>630</v>
       </c>
       <c r="G277" s="1" t="s">
-        <v>636</v>
+        <v>638</v>
       </c>
       <c r="H277" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I277" s="1" t="s">
-        <v>637</v>
+        <v>631</v>
       </c>
     </row>
     <row r="278" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A278" s="1" t="s">
-        <v>638</v>
+        <v>625</v>
       </c>
       <c r="B278" s="1" t="s">
         <v>639</v>
       </c>
       <c r="C278" s="1" t="n">
-        <v>3100</v>
+        <v>3007</v>
       </c>
       <c r="D278" s="2" t="s">
-        <v>59</v>
+        <v>20</v>
       </c>
       <c r="E278" s="1" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F278" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G278" s="1" t="s">
         <v>640</v>
       </c>
-      <c r="G278" s="1" t="s">
-        <v>165</v>
-      </c>
       <c r="H278" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I278" s="1" t="s">
-        <v>134</v>
+        <v>641</v>
       </c>
     </row>
     <row r="279" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A279" s="1" t="s">
-        <v>638</v>
+        <v>642</v>
       </c>
       <c r="B279" s="1" t="s">
-        <v>641</v>
+        <v>643</v>
       </c>
       <c r="C279" s="1" t="n">
-        <v>3101</v>
+        <v>3100</v>
       </c>
       <c r="D279" s="2" t="s">
-        <v>20</v>
+        <v>59</v>
       </c>
       <c r="E279" s="1" t="n">
         <v>10</v>
       </c>
       <c r="F279" s="3" t="s">
-        <v>642</v>
+        <v>644</v>
       </c>
       <c r="G279" s="1" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="H279" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I279" s="1" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
     </row>
     <row r="280" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A280" s="1" t="s">
-        <v>638</v>
+        <v>642</v>
       </c>
       <c r="B280" s="1" t="s">
-        <v>184</v>
+        <v>645</v>
       </c>
       <c r="C280" s="1" t="n">
-        <v>3105</v>
+        <v>3101</v>
       </c>
       <c r="D280" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E280" s="1" t="n">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="F280" s="3" t="s">
-        <v>643</v>
+        <v>646</v>
       </c>
       <c r="G280" s="1" t="s">
-        <v>186</v>
+        <v>159</v>
       </c>
       <c r="H280" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I280" s="1" t="s">
-        <v>81</v>
+        <v>127</v>
       </c>
     </row>
     <row r="281" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A281" s="1" t="s">
-        <v>638</v>
+        <v>642</v>
       </c>
       <c r="B281" s="1" t="s">
-        <v>308</v>
+        <v>184</v>
       </c>
       <c r="C281" s="1" t="n">
-        <v>3110</v>
+        <v>3105</v>
       </c>
       <c r="D281" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E281" s="1" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="F281" s="3" t="s">
-        <v>644</v>
+        <v>647</v>
       </c>
       <c r="G281" s="1" t="s">
-        <v>208</v>
+        <v>186</v>
       </c>
       <c r="H281" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I281" s="1" t="s">
-        <v>645</v>
+        <v>81</v>
       </c>
     </row>
     <row r="282" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A282" s="1" t="s">
-        <v>638</v>
+        <v>642</v>
       </c>
       <c r="B282" s="1" t="s">
-        <v>646</v>
+        <v>308</v>
       </c>
       <c r="C282" s="1" t="n">
-        <v>3111</v>
+        <v>3110</v>
       </c>
       <c r="D282" s="2" t="s">
         <v>20</v>
@@ -11435,27 +11477,27 @@
         <v>1</v>
       </c>
       <c r="F282" s="3" t="s">
-        <v>644</v>
+        <v>648</v>
       </c>
       <c r="G282" s="1" t="s">
-        <v>299</v>
+        <v>208</v>
       </c>
       <c r="H282" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I282" s="1" t="s">
-        <v>645</v>
+        <v>649</v>
       </c>
     </row>
     <row r="283" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A283" s="1" t="s">
-        <v>638</v>
+        <v>642</v>
       </c>
       <c r="B283" s="1" t="s">
-        <v>647</v>
+        <v>650</v>
       </c>
       <c r="C283" s="1" t="n">
-        <v>3112</v>
+        <v>3111</v>
       </c>
       <c r="D283" s="2" t="s">
         <v>20</v>
@@ -11464,27 +11506,27 @@
         <v>1</v>
       </c>
       <c r="F283" s="3" t="s">
-        <v>644</v>
+        <v>648</v>
       </c>
       <c r="G283" s="1" t="s">
-        <v>648</v>
+        <v>299</v>
       </c>
       <c r="H283" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I283" s="1" t="s">
-        <v>645</v>
+        <v>649</v>
       </c>
     </row>
     <row r="284" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A284" s="1" t="s">
-        <v>638</v>
+        <v>642</v>
       </c>
       <c r="B284" s="1" t="s">
-        <v>306</v>
+        <v>651</v>
       </c>
       <c r="C284" s="1" t="n">
-        <v>3113</v>
+        <v>3112</v>
       </c>
       <c r="D284" s="2" t="s">
         <v>20</v>
@@ -11493,56 +11535,56 @@
         <v>1</v>
       </c>
       <c r="F284" s="3" t="s">
-        <v>644</v>
+        <v>648</v>
       </c>
       <c r="G284" s="1" t="s">
-        <v>307</v>
+        <v>652</v>
       </c>
       <c r="H284" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I284" s="1" t="s">
-        <v>645</v>
+        <v>649</v>
       </c>
     </row>
     <row r="285" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A285" s="1" t="s">
-        <v>638</v>
+        <v>642</v>
       </c>
       <c r="B285" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="C285" s="1" t="n">
+        <v>3113</v>
+      </c>
+      <c r="D285" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E285" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F285" s="3" t="s">
+        <v>648</v>
+      </c>
+      <c r="G285" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="H285" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I285" s="1" t="s">
         <v>649</v>
-      </c>
-      <c r="C285" s="1" t="n">
-        <v>3114</v>
-      </c>
-      <c r="D285" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E285" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="F285" s="3" t="s">
-        <v>644</v>
-      </c>
-      <c r="G285" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="H285" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I285" s="1" t="s">
-        <v>645</v>
       </c>
     </row>
     <row r="286" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A286" s="1" t="s">
-        <v>638</v>
+        <v>642</v>
       </c>
       <c r="B286" s="1" t="s">
-        <v>650</v>
+        <v>653</v>
       </c>
       <c r="C286" s="1" t="n">
-        <v>3115</v>
+        <v>3114</v>
       </c>
       <c r="D286" s="2" t="s">
         <v>20</v>
@@ -11551,27 +11593,27 @@
         <v>1</v>
       </c>
       <c r="F286" s="3" t="s">
-        <v>644</v>
+        <v>648</v>
       </c>
       <c r="G286" s="1" t="s">
-        <v>651</v>
+        <v>297</v>
       </c>
       <c r="H286" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I286" s="1" t="s">
-        <v>645</v>
+        <v>649</v>
       </c>
     </row>
     <row r="287" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A287" s="1" t="s">
-        <v>638</v>
+        <v>642</v>
       </c>
       <c r="B287" s="1" t="s">
-        <v>212</v>
+        <v>654</v>
       </c>
       <c r="C287" s="1" t="n">
-        <v>3116</v>
+        <v>3115</v>
       </c>
       <c r="D287" s="2" t="s">
         <v>20</v>
@@ -11580,27 +11622,27 @@
         <v>1</v>
       </c>
       <c r="F287" s="3" t="s">
-        <v>644</v>
+        <v>648</v>
       </c>
       <c r="G287" s="1" t="s">
-        <v>213</v>
+        <v>655</v>
       </c>
       <c r="H287" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I287" s="1" t="s">
-        <v>645</v>
+        <v>649</v>
       </c>
     </row>
     <row r="288" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A288" s="1" t="s">
-        <v>638</v>
+        <v>642</v>
       </c>
       <c r="B288" s="1" t="s">
-        <v>652</v>
+        <v>212</v>
       </c>
       <c r="C288" s="1" t="n">
-        <v>3117</v>
+        <v>3116</v>
       </c>
       <c r="D288" s="2" t="s">
         <v>20</v>
@@ -11609,27 +11651,27 @@
         <v>1</v>
       </c>
       <c r="F288" s="3" t="s">
-        <v>644</v>
+        <v>648</v>
       </c>
       <c r="G288" s="1" t="s">
-        <v>653</v>
+        <v>213</v>
       </c>
       <c r="H288" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I288" s="1" t="s">
-        <v>645</v>
+        <v>649</v>
       </c>
     </row>
     <row r="289" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A289" s="1" t="s">
-        <v>638</v>
+        <v>642</v>
       </c>
       <c r="B289" s="1" t="s">
-        <v>654</v>
+        <v>656</v>
       </c>
       <c r="C289" s="1" t="n">
-        <v>3125</v>
+        <v>3117</v>
       </c>
       <c r="D289" s="2" t="s">
         <v>20</v>
@@ -11638,24 +11680,27 @@
         <v>1</v>
       </c>
       <c r="F289" s="3" t="s">
-        <v>644</v>
+        <v>648</v>
       </c>
       <c r="G289" s="1" t="s">
-        <v>655</v>
+        <v>657</v>
       </c>
       <c r="H289" s="1" t="s">
         <v>17</v>
+      </c>
+      <c r="I289" s="1" t="s">
+        <v>649</v>
       </c>
     </row>
     <row r="290" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A290" s="1" t="s">
-        <v>638</v>
+        <v>642</v>
       </c>
       <c r="B290" s="1" t="s">
-        <v>656</v>
+        <v>658</v>
       </c>
       <c r="C290" s="1" t="n">
-        <v>3126</v>
+        <v>3125</v>
       </c>
       <c r="D290" s="2" t="s">
         <v>20</v>
@@ -11664,27 +11709,24 @@
         <v>1</v>
       </c>
       <c r="F290" s="3" t="s">
-        <v>644</v>
+        <v>648</v>
       </c>
       <c r="G290" s="1" t="s">
-        <v>205</v>
+        <v>659</v>
       </c>
       <c r="H290" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I290" s="1" t="s">
-        <v>657</v>
+        <v>17</v>
       </c>
     </row>
     <row r="291" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A291" s="1" t="s">
-        <v>638</v>
+        <v>642</v>
       </c>
       <c r="B291" s="1" t="s">
-        <v>658</v>
+        <v>660</v>
       </c>
       <c r="C291" s="1" t="n">
-        <v>3127</v>
+        <v>3126</v>
       </c>
       <c r="D291" s="2" t="s">
         <v>20</v>
@@ -11693,24 +11735,27 @@
         <v>1</v>
       </c>
       <c r="F291" s="3" t="s">
-        <v>644</v>
+        <v>648</v>
       </c>
       <c r="G291" s="1" t="s">
-        <v>624</v>
+        <v>205</v>
       </c>
       <c r="H291" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
+      </c>
+      <c r="I291" s="1" t="s">
+        <v>661</v>
       </c>
     </row>
     <row r="292" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A292" s="1" t="s">
-        <v>638</v>
+        <v>642</v>
       </c>
       <c r="B292" s="1" t="s">
-        <v>659</v>
+        <v>662</v>
       </c>
       <c r="C292" s="1" t="n">
-        <v>3128</v>
+        <v>3127</v>
       </c>
       <c r="D292" s="2" t="s">
         <v>20</v>
@@ -11719,56 +11764,53 @@
         <v>1</v>
       </c>
       <c r="F292" s="3" t="s">
-        <v>644</v>
+        <v>648</v>
       </c>
       <c r="G292" s="1" t="s">
-        <v>199</v>
+        <v>627</v>
       </c>
       <c r="H292" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="I292" s="1" t="s">
-        <v>660</v>
       </c>
     </row>
     <row r="293" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A293" s="1" t="s">
-        <v>661</v>
+        <v>642</v>
       </c>
       <c r="B293" s="1" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="C293" s="1" t="n">
-        <v>3200</v>
+        <v>3128</v>
       </c>
       <c r="D293" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E293" s="1" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F293" s="3" t="s">
-        <v>642</v>
+        <v>648</v>
       </c>
       <c r="G293" s="1" t="s">
-        <v>458</v>
+        <v>199</v>
       </c>
       <c r="H293" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I293" s="1" t="s">
-        <v>127</v>
+        <v>664</v>
       </c>
     </row>
     <row r="294" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A294" s="1" t="s">
-        <v>661</v>
+        <v>665</v>
       </c>
       <c r="B294" s="1" t="s">
-        <v>663</v>
+        <v>666</v>
       </c>
       <c r="C294" s="1" t="n">
-        <v>3201</v>
+        <v>3200</v>
       </c>
       <c r="D294" s="2" t="s">
         <v>20</v>
@@ -11777,10 +11819,10 @@
         <v>10</v>
       </c>
       <c r="F294" s="3" t="s">
-        <v>642</v>
+        <v>646</v>
       </c>
       <c r="G294" s="1" t="s">
-        <v>466</v>
+        <v>458</v>
       </c>
       <c r="H294" s="1" t="s">
         <v>17</v>
@@ -11791,13 +11833,13 @@
     </row>
     <row r="295" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A295" s="1" t="s">
-        <v>661</v>
+        <v>665</v>
       </c>
       <c r="B295" s="1" t="s">
-        <v>664</v>
+        <v>667</v>
       </c>
       <c r="C295" s="1" t="n">
-        <v>3202</v>
+        <v>3201</v>
       </c>
       <c r="D295" s="2" t="s">
         <v>20</v>
@@ -11806,10 +11848,10 @@
         <v>10</v>
       </c>
       <c r="F295" s="3" t="s">
-        <v>642</v>
+        <v>646</v>
       </c>
       <c r="G295" s="1" t="s">
-        <v>474</v>
+        <v>466</v>
       </c>
       <c r="H295" s="1" t="s">
         <v>17</v>
@@ -11820,42 +11862,42 @@
     </row>
     <row r="296" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A296" s="1" t="s">
-        <v>661</v>
+        <v>665</v>
       </c>
       <c r="B296" s="1" t="s">
-        <v>665</v>
+        <v>668</v>
       </c>
       <c r="C296" s="1" t="n">
-        <v>3203</v>
+        <v>3202</v>
       </c>
       <c r="D296" s="2" t="s">
-        <v>59</v>
+        <v>20</v>
       </c>
       <c r="E296" s="1" t="n">
         <v>10</v>
       </c>
       <c r="F296" s="3" t="s">
-        <v>640</v>
+        <v>646</v>
       </c>
       <c r="G296" s="1" t="s">
-        <v>460</v>
+        <v>474</v>
       </c>
       <c r="H296" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I296" s="1" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
     </row>
     <row r="297" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A297" s="1" t="s">
-        <v>661</v>
+        <v>665</v>
       </c>
       <c r="B297" s="1" t="s">
-        <v>666</v>
+        <v>669</v>
       </c>
       <c r="C297" s="1" t="n">
-        <v>3204</v>
+        <v>3203</v>
       </c>
       <c r="D297" s="2" t="s">
         <v>59</v>
@@ -11864,10 +11906,10 @@
         <v>10</v>
       </c>
       <c r="F297" s="3" t="s">
-        <v>640</v>
+        <v>644</v>
       </c>
       <c r="G297" s="1" t="s">
-        <v>468</v>
+        <v>460</v>
       </c>
       <c r="H297" s="1" t="s">
         <v>17</v>
@@ -11878,13 +11920,13 @@
     </row>
     <row r="298" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A298" s="1" t="s">
-        <v>661</v>
+        <v>665</v>
       </c>
       <c r="B298" s="1" t="s">
-        <v>667</v>
+        <v>670</v>
       </c>
       <c r="C298" s="1" t="n">
-        <v>3205</v>
+        <v>3204</v>
       </c>
       <c r="D298" s="2" t="s">
         <v>59</v>
@@ -11893,10 +11935,10 @@
         <v>10</v>
       </c>
       <c r="F298" s="3" t="s">
-        <v>640</v>
+        <v>644</v>
       </c>
       <c r="G298" s="1" t="s">
-        <v>476</v>
+        <v>468</v>
       </c>
       <c r="H298" s="1" t="s">
         <v>17</v>
@@ -11907,42 +11949,42 @@
     </row>
     <row r="299" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A299" s="1" t="s">
-        <v>661</v>
+        <v>665</v>
       </c>
       <c r="B299" s="1" t="s">
-        <v>668</v>
+        <v>671</v>
       </c>
       <c r="C299" s="1" t="n">
-        <v>3206</v>
+        <v>3205</v>
       </c>
       <c r="D299" s="2" t="s">
         <v>59</v>
       </c>
       <c r="E299" s="1" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F299" s="3" t="s">
-        <v>669</v>
+        <v>644</v>
       </c>
       <c r="G299" s="1" t="s">
-        <v>462</v>
+        <v>476</v>
       </c>
       <c r="H299" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I299" s="1" t="s">
-        <v>31</v>
+        <v>134</v>
       </c>
     </row>
     <row r="300" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A300" s="1" t="s">
-        <v>661</v>
+        <v>665</v>
       </c>
       <c r="B300" s="1" t="s">
-        <v>670</v>
+        <v>672</v>
       </c>
       <c r="C300" s="1" t="n">
-        <v>3207</v>
+        <v>3206</v>
       </c>
       <c r="D300" s="2" t="s">
         <v>59</v>
@@ -11951,10 +11993,10 @@
         <v>1</v>
       </c>
       <c r="F300" s="3" t="s">
-        <v>669</v>
+        <v>673</v>
       </c>
       <c r="G300" s="1" t="s">
-        <v>470</v>
+        <v>462</v>
       </c>
       <c r="H300" s="1" t="s">
         <v>17</v>
@@ -11965,13 +12007,13 @@
     </row>
     <row r="301" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A301" s="1" t="s">
-        <v>661</v>
+        <v>665</v>
       </c>
       <c r="B301" s="1" t="s">
-        <v>671</v>
+        <v>674</v>
       </c>
       <c r="C301" s="1" t="n">
-        <v>3208</v>
+        <v>3207</v>
       </c>
       <c r="D301" s="2" t="s">
         <v>59</v>
@@ -11980,10 +12022,10 @@
         <v>1</v>
       </c>
       <c r="F301" s="3" t="s">
-        <v>669</v>
+        <v>673</v>
       </c>
       <c r="G301" s="1" t="s">
-        <v>478</v>
+        <v>470</v>
       </c>
       <c r="H301" s="1" t="s">
         <v>17</v>
@@ -11994,42 +12036,42 @@
     </row>
     <row r="302" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A302" s="1" t="s">
-        <v>661</v>
+        <v>665</v>
       </c>
       <c r="B302" s="1" t="s">
-        <v>672</v>
+        <v>675</v>
       </c>
       <c r="C302" s="1" t="n">
-        <v>3209</v>
+        <v>3208</v>
       </c>
       <c r="D302" s="2" t="s">
-        <v>20</v>
+        <v>59</v>
       </c>
       <c r="E302" s="1" t="n">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="F302" s="3" t="s">
-        <v>643</v>
+        <v>673</v>
       </c>
       <c r="G302" s="1" t="s">
-        <v>673</v>
+        <v>478</v>
       </c>
       <c r="H302" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I302" s="1" t="s">
-        <v>143</v>
+        <v>31</v>
       </c>
     </row>
     <row r="303" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A303" s="1" t="s">
-        <v>661</v>
+        <v>665</v>
       </c>
       <c r="B303" s="1" t="s">
-        <v>674</v>
+        <v>676</v>
       </c>
       <c r="C303" s="1" t="n">
-        <v>3210</v>
+        <v>3209</v>
       </c>
       <c r="D303" s="2" t="s">
         <v>20</v>
@@ -12038,10 +12080,10 @@
         <v>100</v>
       </c>
       <c r="F303" s="3" t="s">
-        <v>643</v>
+        <v>647</v>
       </c>
       <c r="G303" s="1" t="s">
-        <v>675</v>
+        <v>677</v>
       </c>
       <c r="H303" s="1" t="s">
         <v>17</v>
@@ -12052,13 +12094,13 @@
     </row>
     <row r="304" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A304" s="1" t="s">
-        <v>661</v>
+        <v>665</v>
       </c>
       <c r="B304" s="1" t="s">
-        <v>676</v>
+        <v>678</v>
       </c>
       <c r="C304" s="1" t="n">
-        <v>3211</v>
+        <v>3210</v>
       </c>
       <c r="D304" s="2" t="s">
         <v>20</v>
@@ -12067,10 +12109,10 @@
         <v>100</v>
       </c>
       <c r="F304" s="3" t="s">
-        <v>643</v>
+        <v>647</v>
       </c>
       <c r="G304" s="1" t="s">
-        <v>677</v>
+        <v>679</v>
       </c>
       <c r="H304" s="1" t="s">
         <v>17</v>
@@ -12081,39 +12123,42 @@
     </row>
     <row r="305" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A305" s="1" t="s">
-        <v>661</v>
+        <v>665</v>
       </c>
       <c r="B305" s="1" t="s">
-        <v>678</v>
+        <v>680</v>
       </c>
       <c r="C305" s="1" t="n">
-        <v>3212</v>
+        <v>3211</v>
       </c>
       <c r="D305" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E305" s="1" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="F305" s="3" t="s">
-        <v>644</v>
+        <v>647</v>
       </c>
       <c r="G305" s="1" t="s">
-        <v>624</v>
+        <v>681</v>
       </c>
       <c r="H305" s="1" t="s">
         <v>17</v>
+      </c>
+      <c r="I305" s="1" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="306" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A306" s="1" t="s">
-        <v>661</v>
+        <v>665</v>
       </c>
       <c r="B306" s="1" t="s">
-        <v>679</v>
+        <v>682</v>
       </c>
       <c r="C306" s="1" t="n">
-        <v>3213</v>
+        <v>3212</v>
       </c>
       <c r="D306" s="2" t="s">
         <v>20</v>
@@ -12122,27 +12167,24 @@
         <v>1</v>
       </c>
       <c r="F306" s="3" t="s">
-        <v>644</v>
+        <v>648</v>
       </c>
       <c r="G306" s="1" t="s">
-        <v>680</v>
+        <v>627</v>
       </c>
       <c r="H306" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="I306" s="1" t="s">
-        <v>681</v>
       </c>
     </row>
     <row r="307" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A307" s="1" t="s">
-        <v>661</v>
+        <v>665</v>
       </c>
       <c r="B307" s="1" t="s">
-        <v>487</v>
+        <v>683</v>
       </c>
       <c r="C307" s="1" t="n">
-        <v>3214</v>
+        <v>3213</v>
       </c>
       <c r="D307" s="2" t="s">
         <v>20</v>
@@ -12151,27 +12193,27 @@
         <v>1</v>
       </c>
       <c r="F307" s="3" t="s">
-        <v>644</v>
+        <v>648</v>
       </c>
       <c r="G307" s="1" t="s">
-        <v>446</v>
+        <v>684</v>
       </c>
       <c r="H307" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I307" s="1" t="s">
-        <v>682</v>
+        <v>685</v>
       </c>
     </row>
     <row r="308" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A308" s="1" t="s">
-        <v>661</v>
+        <v>665</v>
       </c>
       <c r="B308" s="1" t="s">
-        <v>683</v>
+        <v>487</v>
       </c>
       <c r="C308" s="1" t="n">
-        <v>3215</v>
+        <v>3214</v>
       </c>
       <c r="D308" s="2" t="s">
         <v>20</v>
@@ -12180,27 +12222,27 @@
         <v>1</v>
       </c>
       <c r="F308" s="3" t="s">
-        <v>644</v>
+        <v>648</v>
       </c>
       <c r="G308" s="1" t="s">
-        <v>684</v>
+        <v>446</v>
       </c>
       <c r="H308" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I308" s="1" t="s">
-        <v>491</v>
+        <v>686</v>
       </c>
     </row>
     <row r="309" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A309" s="1" t="s">
-        <v>661</v>
+        <v>665</v>
       </c>
       <c r="B309" s="1" t="s">
-        <v>685</v>
+        <v>687</v>
       </c>
       <c r="C309" s="1" t="n">
-        <v>3216</v>
+        <v>3215</v>
       </c>
       <c r="D309" s="2" t="s">
         <v>20</v>
@@ -12209,27 +12251,27 @@
         <v>1</v>
       </c>
       <c r="F309" s="3" t="s">
-        <v>644</v>
+        <v>648</v>
       </c>
       <c r="G309" s="1" t="s">
-        <v>686</v>
+        <v>688</v>
       </c>
       <c r="H309" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I309" s="1" t="s">
-        <v>93</v>
+        <v>491</v>
       </c>
     </row>
     <row r="310" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A310" s="1" t="s">
-        <v>661</v>
+        <v>665</v>
       </c>
       <c r="B310" s="1" t="s">
-        <v>687</v>
+        <v>689</v>
       </c>
       <c r="C310" s="1" t="n">
-        <v>3217</v>
+        <v>3216</v>
       </c>
       <c r="D310" s="2" t="s">
         <v>20</v>
@@ -12238,85 +12280,85 @@
         <v>1</v>
       </c>
       <c r="F310" s="3" t="s">
-        <v>644</v>
+        <v>648</v>
       </c>
       <c r="G310" s="1" t="s">
-        <v>688</v>
+        <v>690</v>
       </c>
       <c r="H310" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I310" s="1" t="s">
-        <v>530</v>
+        <v>93</v>
       </c>
     </row>
     <row r="311" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A311" s="1" t="s">
-        <v>661</v>
+        <v>665</v>
       </c>
       <c r="B311" s="1" t="s">
-        <v>689</v>
+        <v>691</v>
       </c>
       <c r="C311" s="1" t="n">
-        <v>3218</v>
+        <v>3217</v>
       </c>
       <c r="D311" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E311" s="1" t="n">
-        <v>0.01</v>
+        <v>1</v>
       </c>
       <c r="F311" s="3" t="s">
-        <v>690</v>
+        <v>648</v>
       </c>
       <c r="G311" s="1" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
       <c r="H311" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I311" s="1" t="s">
-        <v>105</v>
+        <v>530</v>
       </c>
     </row>
     <row r="312" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A312" s="1" t="s">
-        <v>661</v>
+        <v>665</v>
       </c>
       <c r="B312" s="1" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
       <c r="C312" s="1" t="n">
-        <v>3219</v>
+        <v>3218</v>
       </c>
       <c r="D312" s="2" t="s">
-        <v>59</v>
+        <v>20</v>
       </c>
       <c r="E312" s="1" t="n">
-        <v>10</v>
+        <v>0.01</v>
       </c>
       <c r="F312" s="3" t="s">
-        <v>640</v>
+        <v>694</v>
       </c>
       <c r="G312" s="1" t="s">
-        <v>693</v>
+        <v>695</v>
       </c>
       <c r="H312" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I312" s="1" t="s">
-        <v>275</v>
+        <v>105</v>
       </c>
     </row>
     <row r="313" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A313" s="1" t="s">
-        <v>661</v>
+        <v>665</v>
       </c>
       <c r="B313" s="1" t="s">
-        <v>694</v>
+        <v>696</v>
       </c>
       <c r="C313" s="1" t="n">
-        <v>3220</v>
+        <v>3219</v>
       </c>
       <c r="D313" s="2" t="s">
         <v>59</v>
@@ -12325,10 +12367,10 @@
         <v>10</v>
       </c>
       <c r="F313" s="3" t="s">
-        <v>640</v>
+        <v>644</v>
       </c>
       <c r="G313" s="1" t="s">
-        <v>695</v>
+        <v>697</v>
       </c>
       <c r="H313" s="1" t="s">
         <v>17</v>
@@ -12339,13 +12381,13 @@
     </row>
     <row r="314" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A314" s="1" t="s">
-        <v>661</v>
+        <v>665</v>
       </c>
       <c r="B314" s="1" t="s">
-        <v>696</v>
+        <v>698</v>
       </c>
       <c r="C314" s="1" t="n">
-        <v>3221</v>
+        <v>3220</v>
       </c>
       <c r="D314" s="2" t="s">
         <v>59</v>
@@ -12354,10 +12396,10 @@
         <v>10</v>
       </c>
       <c r="F314" s="3" t="s">
-        <v>640</v>
+        <v>644</v>
       </c>
       <c r="G314" s="1" t="s">
-        <v>697</v>
+        <v>699</v>
       </c>
       <c r="H314" s="1" t="s">
         <v>17</v>
@@ -12368,71 +12410,71 @@
     </row>
     <row r="315" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A315" s="1" t="s">
-        <v>661</v>
+        <v>665</v>
       </c>
       <c r="B315" s="1" t="s">
-        <v>698</v>
+        <v>700</v>
       </c>
       <c r="C315" s="1" t="n">
-        <v>3222</v>
+        <v>3221</v>
       </c>
       <c r="D315" s="2" t="s">
-        <v>20</v>
+        <v>59</v>
       </c>
       <c r="E315" s="1" t="n">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="F315" s="3" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="G315" s="1" t="s">
-        <v>699</v>
+        <v>701</v>
       </c>
       <c r="H315" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I315" s="1" t="s">
-        <v>81</v>
+        <v>275</v>
       </c>
     </row>
     <row r="316" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A316" s="1" t="s">
-        <v>661</v>
+        <v>665</v>
       </c>
       <c r="B316" s="1" t="s">
-        <v>700</v>
+        <v>702</v>
       </c>
       <c r="C316" s="1" t="n">
-        <v>3223</v>
+        <v>3222</v>
       </c>
       <c r="D316" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E316" s="1" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="F316" s="3" t="s">
-        <v>644</v>
+        <v>647</v>
       </c>
       <c r="G316" s="1" t="s">
-        <v>701</v>
+        <v>703</v>
       </c>
       <c r="H316" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="I316" s="1" t="s">
-        <v>702</v>
+        <v>81</v>
       </c>
     </row>
     <row r="317" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A317" s="1" t="s">
-        <v>703</v>
+        <v>665</v>
       </c>
       <c r="B317" s="1" t="s">
-        <v>623</v>
+        <v>704</v>
       </c>
       <c r="C317" s="1" t="n">
-        <v>3300</v>
+        <v>3223</v>
       </c>
       <c r="D317" s="2" t="s">
         <v>20</v>
@@ -12441,36 +12483,39 @@
         <v>1</v>
       </c>
       <c r="F317" s="3" t="s">
-        <v>29</v>
+        <v>648</v>
       </c>
       <c r="G317" s="1" t="s">
-        <v>624</v>
+        <v>705</v>
       </c>
       <c r="H317" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
+      </c>
+      <c r="I317" s="1" t="s">
+        <v>706</v>
       </c>
     </row>
     <row r="318" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A318" s="1" t="s">
-        <v>703</v>
+        <v>707</v>
       </c>
       <c r="B318" s="1" t="s">
-        <v>704</v>
+        <v>626</v>
       </c>
       <c r="C318" s="1" t="n">
-        <v>3301</v>
+        <v>3300</v>
       </c>
       <c r="D318" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E318" s="1" t="n">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="F318" s="3" t="s">
-        <v>185</v>
+        <v>29</v>
       </c>
       <c r="G318" s="1" t="s">
-        <v>705</v>
+        <v>627</v>
       </c>
       <c r="H318" s="1" t="s">
         <v>17</v>
@@ -12478,25 +12523,25 @@
     </row>
     <row r="319" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A319" s="1" t="s">
-        <v>703</v>
+        <v>707</v>
       </c>
       <c r="B319" s="1" t="s">
-        <v>706</v>
+        <v>708</v>
       </c>
       <c r="C319" s="1" t="n">
-        <v>3302</v>
+        <v>3301</v>
       </c>
       <c r="D319" s="2" t="s">
-        <v>59</v>
+        <v>20</v>
       </c>
       <c r="E319" s="1" t="n">
         <v>100</v>
       </c>
       <c r="F319" s="3" t="s">
-        <v>141</v>
+        <v>185</v>
       </c>
       <c r="G319" s="1" t="s">
-        <v>707</v>
+        <v>709</v>
       </c>
       <c r="H319" s="1" t="s">
         <v>17</v>
@@ -12504,129 +12549,126 @@
     </row>
     <row r="320" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A320" s="1" t="s">
-        <v>703</v>
+        <v>707</v>
       </c>
       <c r="B320" s="1" t="s">
-        <v>708</v>
+        <v>710</v>
       </c>
       <c r="C320" s="1" t="n">
-        <v>3303</v>
+        <v>3302</v>
       </c>
       <c r="D320" s="2" t="s">
-        <v>20</v>
+        <v>59</v>
       </c>
       <c r="E320" s="1" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="F320" s="3" t="s">
-        <v>29</v>
+        <v>141</v>
       </c>
       <c r="G320" s="1" t="s">
-        <v>709</v>
+        <v>711</v>
       </c>
       <c r="H320" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="I320" s="1" t="s">
-        <v>710</v>
       </c>
     </row>
     <row r="321" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A321" s="1" t="s">
-        <v>703</v>
+        <v>707</v>
       </c>
       <c r="B321" s="1" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
       <c r="C321" s="1" t="n">
-        <v>3304</v>
+        <v>3303</v>
       </c>
       <c r="D321" s="2" t="s">
-        <v>59</v>
+        <v>20</v>
       </c>
       <c r="E321" s="1" t="n">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="F321" s="3" t="s">
-        <v>141</v>
+        <v>29</v>
       </c>
       <c r="G321" s="1" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="H321" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I321" s="1" t="s">
-        <v>275</v>
+        <v>714</v>
       </c>
     </row>
     <row r="322" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A322" s="1" t="s">
-        <v>703</v>
+        <v>707</v>
       </c>
       <c r="B322" s="1" t="s">
-        <v>713</v>
+        <v>715</v>
       </c>
       <c r="C322" s="1" t="n">
-        <v>3305</v>
+        <v>3304</v>
       </c>
       <c r="D322" s="2" t="s">
-        <v>20</v>
+        <v>59</v>
       </c>
       <c r="E322" s="1" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="F322" s="3" t="s">
-        <v>29</v>
+        <v>141</v>
       </c>
       <c r="G322" s="1" t="s">
-        <v>636</v>
+        <v>716</v>
       </c>
       <c r="H322" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I322" s="1" t="s">
-        <v>637</v>
+        <v>275</v>
       </c>
     </row>
     <row r="323" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A323" s="1" t="s">
-        <v>714</v>
+        <v>707</v>
       </c>
       <c r="B323" s="1" t="s">
-        <v>715</v>
+        <v>717</v>
       </c>
       <c r="C323" s="1" t="n">
-        <v>3400</v>
+        <v>3305</v>
       </c>
       <c r="D323" s="2" t="s">
-        <v>581</v>
+        <v>20</v>
       </c>
       <c r="E323" s="1" t="n">
         <v>1</v>
       </c>
       <c r="F323" s="3" t="s">
-        <v>716</v>
+        <v>29</v>
       </c>
       <c r="G323" s="1" t="s">
-        <v>717</v>
+        <v>640</v>
       </c>
       <c r="H323" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I323" s="1" t="s">
-        <v>627</v>
+        <v>641</v>
       </c>
     </row>
     <row r="324" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A324" s="1" t="s">
-        <v>714</v>
+        <v>718</v>
       </c>
       <c r="B324" s="1" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="C324" s="1" t="n">
-        <v>3402</v>
+        <v>3400</v>
       </c>
       <c r="D324" s="2" t="s">
         <v>581</v>
@@ -12635,24 +12677,27 @@
         <v>1</v>
       </c>
       <c r="F324" s="3" t="s">
-        <v>716</v>
+        <v>720</v>
       </c>
       <c r="G324" s="1" t="s">
-        <v>719</v>
+        <v>721</v>
       </c>
       <c r="H324" s="1" t="s">
         <v>17</v>
+      </c>
+      <c r="I324" s="1" t="s">
+        <v>631</v>
       </c>
     </row>
     <row r="325" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A325" s="1" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="B325" s="1" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
       <c r="C325" s="1" t="n">
-        <v>3420</v>
+        <v>3402</v>
       </c>
       <c r="D325" s="2" t="s">
         <v>581</v>
@@ -12661,10 +12706,10 @@
         <v>1</v>
       </c>
       <c r="F325" s="3" t="s">
-        <v>716</v>
+        <v>720</v>
       </c>
       <c r="G325" s="1" t="s">
-        <v>719</v>
+        <v>723</v>
       </c>
       <c r="H325" s="1" t="s">
         <v>17</v>
@@ -12672,42 +12717,39 @@
     </row>
     <row r="326" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A326" s="1" t="s">
+        <v>724</v>
+      </c>
+      <c r="B326" s="1" t="s">
+        <v>725</v>
+      </c>
+      <c r="C326" s="1" t="n">
+        <v>3420</v>
+      </c>
+      <c r="D326" s="2" t="s">
+        <v>581</v>
+      </c>
+      <c r="E326" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F326" s="3" t="s">
         <v>720</v>
       </c>
-      <c r="B326" s="1" t="s">
-        <v>485</v>
-      </c>
-      <c r="C326" s="1" t="n">
-        <v>3422</v>
-      </c>
-      <c r="D326" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E326" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="F326" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="G326" s="1" t="s">
-        <v>199</v>
+        <v>723</v>
       </c>
       <c r="H326" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="I326" s="1" t="s">
-        <v>722</v>
       </c>
     </row>
     <row r="327" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A327" s="1" t="s">
-        <v>720</v>
+        <v>724</v>
       </c>
       <c r="B327" s="1" t="s">
-        <v>292</v>
+        <v>485</v>
       </c>
       <c r="C327" s="1" t="n">
-        <v>3423</v>
+        <v>3422</v>
       </c>
       <c r="D327" s="2" t="s">
         <v>20</v>
@@ -12716,71 +12758,71 @@
         <v>1</v>
       </c>
       <c r="F327" s="3" t="s">
-        <v>723</v>
+        <v>21</v>
       </c>
       <c r="G327" s="1" t="s">
-        <v>724</v>
+        <v>199</v>
       </c>
       <c r="H327" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I327" s="1" t="s">
-        <v>294</v>
+        <v>726</v>
       </c>
     </row>
     <row r="328" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A328" s="1" t="s">
-        <v>720</v>
+        <v>724</v>
       </c>
       <c r="B328" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="C328" s="1" t="n">
+        <v>3423</v>
+      </c>
+      <c r="D328" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E328" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F328" s="3" t="s">
+        <v>727</v>
+      </c>
+      <c r="G328" s="1" t="s">
+        <v>728</v>
+      </c>
+      <c r="H328" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I328" s="1" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="329" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A329" s="1" t="s">
+        <v>724</v>
+      </c>
+      <c r="B329" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C328" s="1" t="n">
+      <c r="C329" s="1" t="n">
         <v>3424</v>
       </c>
-      <c r="D328" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E328" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="F328" s="3" t="s">
-        <v>725</v>
-      </c>
-      <c r="G328" s="1" t="s">
-        <v>726</v>
-      </c>
-      <c r="H328" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I328" s="1" t="s">
-        <v>727</v>
-      </c>
-    </row>
-    <row r="329" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A329" s="1" t="s">
-        <v>728</v>
-      </c>
-      <c r="B329" s="1" t="s">
+      <c r="D329" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E329" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F329" s="3" t="s">
         <v>729</v>
-      </c>
-      <c r="C329" s="1" t="n">
-        <v>3500</v>
-      </c>
-      <c r="D329" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E329" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="F329" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="G329" s="1" t="s">
         <v>730</v>
       </c>
       <c r="H329" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="I329" s="1" t="s">
         <v>731</v>
@@ -12788,13 +12830,13 @@
     </row>
     <row r="330" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A330" s="1" t="s">
-        <v>728</v>
+        <v>732</v>
       </c>
       <c r="B330" s="1" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c r="C330" s="1" t="n">
-        <v>3501</v>
+        <v>3500</v>
       </c>
       <c r="D330" s="2" t="s">
         <v>20</v>
@@ -12803,44 +12845,73 @@
         <v>1</v>
       </c>
       <c r="F330" s="3" t="s">
-        <v>725</v>
+        <v>21</v>
       </c>
       <c r="G330" s="1" t="s">
-        <v>733</v>
+        <v>734</v>
       </c>
       <c r="H330" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="I330" s="1" t="s">
-        <v>734</v>
+        <v>735</v>
       </c>
     </row>
     <row r="331" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A331" s="1" t="s">
-        <v>728</v>
+        <v>732</v>
       </c>
       <c r="B331" s="1" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
       <c r="C331" s="1" t="n">
+        <v>3501</v>
+      </c>
+      <c r="D331" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E331" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F331" s="3" t="s">
+        <v>729</v>
+      </c>
+      <c r="G331" s="1" t="s">
+        <v>737</v>
+      </c>
+      <c r="H331" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I331" s="1" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="332" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A332" s="1" t="s">
+        <v>732</v>
+      </c>
+      <c r="B332" s="1" t="s">
+        <v>739</v>
+      </c>
+      <c r="C332" s="1" t="n">
         <v>3502</v>
       </c>
-      <c r="D331" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E331" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="F331" s="3" t="s">
-        <v>725</v>
-      </c>
-      <c r="G331" s="1" t="s">
-        <v>730</v>
-      </c>
-      <c r="H331" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I331" s="1" t="s">
+      <c r="D332" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E332" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F332" s="3" t="s">
+        <v>729</v>
+      </c>
+      <c r="G332" s="1" t="s">
+        <v>734</v>
+      </c>
+      <c r="H332" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I332" s="1" t="s">
         <v>340</v>
       </c>
     </row>
@@ -12878,14 +12949,14 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="23" t="s">
-        <v>736</v>
-      </c>
-      <c r="B1" s="23" t="s">
-        <v>737</v>
-      </c>
-      <c r="C1" s="23" t="s">
-        <v>738</v>
+      <c r="A1" s="25" t="s">
+        <v>740</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>741</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>742</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12896,7 +12967,7 @@
         <v>257</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>739</v>
+        <v>743</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12907,7 +12978,7 @@
         <v>256</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>740</v>
+        <v>744</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12917,30 +12988,30 @@
       <c r="B4" s="22" t="n">
         <v>258</v>
       </c>
-      <c r="C4" s="24" t="s">
-        <v>741</v>
+      <c r="C4" s="26" t="s">
+        <v>745</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="24" t="n">
+      <c r="A5" s="26" t="n">
         <v>243</v>
       </c>
-      <c r="B5" s="24" t="n">
+      <c r="B5" s="26" t="n">
         <v>260</v>
       </c>
-      <c r="C5" s="24" t="s">
-        <v>742</v>
+      <c r="C5" s="26" t="s">
+        <v>746</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="24" t="n">
+      <c r="A6" s="26" t="n">
         <v>242</v>
       </c>
-      <c r="B6" s="24" t="n">
+      <c r="B6" s="26" t="n">
         <v>261</v>
       </c>
-      <c r="C6" s="24" t="s">
-        <v>743</v>
+      <c r="C6" s="26" t="s">
+        <v>747</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12951,7 +13022,7 @@
         <v>0</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>744</v>
+        <v>748</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12962,7 +13033,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>745</v>
+        <v>749</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12973,7 +13044,7 @@
         <v>2</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>746</v>
+        <v>750</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12984,7 +13055,7 @@
         <v>3</v>
       </c>
       <c r="C10" s="22" t="s">
-        <v>747</v>
+        <v>751</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12995,7 +13066,7 @@
         <v>4</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>748</v>
+        <v>752</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13006,7 +13077,7 @@
         <v>5</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>749</v>
+        <v>753</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13017,7 +13088,7 @@
         <v>6</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>750</v>
+        <v>754</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13028,7 +13099,7 @@
         <v>7</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>751</v>
+        <v>755</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13039,7 +13110,7 @@
         <v>8</v>
       </c>
       <c r="C15" s="22" t="s">
-        <v>752</v>
+        <v>756</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13050,7 +13121,7 @@
         <v>9</v>
       </c>
       <c r="C16" s="22" t="s">
-        <v>753</v>
+        <v>757</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13061,7 +13132,7 @@
         <v>10</v>
       </c>
       <c r="C17" s="22" t="s">
-        <v>754</v>
+        <v>758</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13072,7 +13143,7 @@
         <v>11</v>
       </c>
       <c r="C18" s="22" t="s">
-        <v>755</v>
+        <v>759</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13083,7 +13154,7 @@
         <v>12</v>
       </c>
       <c r="C19" s="22" t="s">
-        <v>756</v>
+        <v>760</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13094,7 +13165,7 @@
         <v>20</v>
       </c>
       <c r="C20" s="22" t="s">
-        <v>757</v>
+        <v>761</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13105,7 +13176,7 @@
         <v>21</v>
       </c>
       <c r="C21" s="22" t="s">
-        <v>758</v>
+        <v>762</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13116,7 +13187,7 @@
         <v>22</v>
       </c>
       <c r="C22" s="22" t="s">
-        <v>759</v>
+        <v>763</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13127,7 +13198,7 @@
         <v>23</v>
       </c>
       <c r="C23" s="22" t="s">
-        <v>760</v>
+        <v>764</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13138,7 +13209,7 @@
         <v>24</v>
       </c>
       <c r="C24" s="22" t="s">
-        <v>761</v>
+        <v>765</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13149,7 +13220,7 @@
         <v>25</v>
       </c>
       <c r="C25" s="22" t="s">
-        <v>762</v>
+        <v>766</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13160,7 +13231,7 @@
         <v>26</v>
       </c>
       <c r="C26" s="22" t="s">
-        <v>763</v>
+        <v>767</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13171,7 +13242,7 @@
         <v>27</v>
       </c>
       <c r="C27" s="22" t="s">
-        <v>764</v>
+        <v>768</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13182,7 +13253,7 @@
         <v>28</v>
       </c>
       <c r="C28" s="22" t="s">
-        <v>765</v>
+        <v>769</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13193,7 +13264,7 @@
         <v>29</v>
       </c>
       <c r="C29" s="22" t="s">
-        <v>766</v>
+        <v>770</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13204,7 +13275,7 @@
         <v>30</v>
       </c>
       <c r="C30" s="22" t="s">
-        <v>767</v>
+        <v>771</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13215,7 +13286,7 @@
         <v>31</v>
       </c>
       <c r="C31" s="22" t="s">
-        <v>768</v>
+        <v>772</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13226,7 +13297,7 @@
         <v>32</v>
       </c>
       <c r="C32" s="22" t="s">
-        <v>769</v>
+        <v>773</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13237,7 +13308,7 @@
         <v>33</v>
       </c>
       <c r="C33" s="22" t="s">
-        <v>770</v>
+        <v>774</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13248,7 +13319,7 @@
         <v>34</v>
       </c>
       <c r="C34" s="22" t="s">
-        <v>771</v>
+        <v>775</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13259,7 +13330,7 @@
         <v>40</v>
       </c>
       <c r="C35" s="22" t="s">
-        <v>772</v>
+        <v>776</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13270,7 +13341,7 @@
         <v>41</v>
       </c>
       <c r="C36" s="22" t="s">
-        <v>773</v>
+        <v>777</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13281,7 +13352,7 @@
         <v>42</v>
       </c>
       <c r="C37" s="22" t="s">
-        <v>774</v>
+        <v>778</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13292,7 +13363,7 @@
         <v>43</v>
       </c>
       <c r="C38" s="22" t="s">
-        <v>775</v>
+        <v>779</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13303,7 +13374,7 @@
         <v>44</v>
       </c>
       <c r="C39" s="22" t="s">
-        <v>776</v>
+        <v>780</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13314,7 +13385,7 @@
         <v>45</v>
       </c>
       <c r="C40" s="22" t="s">
-        <v>777</v>
+        <v>781</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13325,7 +13396,7 @@
         <v>46</v>
       </c>
       <c r="C41" s="22" t="s">
-        <v>778</v>
+        <v>782</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13336,7 +13407,7 @@
         <v>288</v>
       </c>
       <c r="C42" s="22" t="s">
-        <v>779</v>
+        <v>783</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13347,7 +13418,7 @@
         <v>289</v>
       </c>
       <c r="C43" s="22" t="s">
-        <v>780</v>
+        <v>784</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13358,7 +13429,7 @@
         <v>290</v>
       </c>
       <c r="C44" s="22" t="s">
-        <v>781</v>
+        <v>785</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13369,7 +13440,7 @@
         <v>291</v>
       </c>
       <c r="C45" s="22" t="s">
-        <v>782</v>
+        <v>786</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13380,7 +13451,7 @@
         <v>292</v>
       </c>
       <c r="C46" s="22" t="s">
-        <v>783</v>
+        <v>787</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13391,7 +13462,7 @@
         <v>293</v>
       </c>
       <c r="C47" s="22" t="s">
-        <v>784</v>
+        <v>788</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13402,28 +13473,28 @@
         <v>512</v>
       </c>
       <c r="C48" s="22" t="s">
-        <v>785</v>
+        <v>789</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="25" t="s">
-        <v>786</v>
-      </c>
-      <c r="B50" s="25"/>
-      <c r="C50" s="25"/>
-      <c r="D50" s="25"/>
-      <c r="E50" s="25"/>
-      <c r="F50" s="25"/>
+      <c r="A50" s="27" t="s">
+        <v>790</v>
+      </c>
+      <c r="B50" s="27"/>
+      <c r="C50" s="27"/>
+      <c r="D50" s="27"/>
+      <c r="E50" s="27"/>
+      <c r="F50" s="27"/>
     </row>
     <row r="51" customFormat="false" ht="92.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="26" t="s">
-        <v>787</v>
-      </c>
-      <c r="B51" s="26"/>
-      <c r="C51" s="26"/>
-      <c r="D51" s="26"/>
-      <c r="E51" s="26"/>
-      <c r="F51" s="26"/>
+      <c r="A51" s="28" t="s">
+        <v>791</v>
+      </c>
+      <c r="B51" s="28"/>
+      <c r="C51" s="28"/>
+      <c r="D51" s="28"/>
+      <c r="E51" s="28"/>
+      <c r="F51" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -13445,10 +13516,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C55"/>
+  <dimension ref="A1:C56"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C55" activeCellId="0" sqref="C55"/>
+      <selection pane="topLeft" activeCell="A57" activeCellId="0" sqref="A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13461,331 +13532,339 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="22" t="s">
-        <v>788</v>
+        <v>792</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>789</v>
+        <v>793</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="22" t="s">
-        <v>790</v>
+        <v>794</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>791</v>
+        <v>795</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="22" t="s">
-        <v>792</v>
+        <v>796</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>793</v>
+        <v>797</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="22" t="s">
-        <v>794</v>
+        <v>798</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>795</v>
+        <v>799</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="22" t="s">
-        <v>796</v>
+        <v>800</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="22" t="s">
-        <v>797</v>
+        <v>801</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="22" t="s">
-        <v>798</v>
+        <v>802</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="22" t="s">
-        <v>799</v>
+        <v>803</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="22" t="s">
-        <v>800</v>
+        <v>804</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>801</v>
+        <v>805</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="22" t="s">
-        <v>802</v>
+        <v>806</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="22" t="s">
-        <v>803</v>
+        <v>807</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="22" t="s">
-        <v>804</v>
+        <v>808</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>805</v>
+        <v>809</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="22" t="s">
-        <v>806</v>
+        <v>810</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="22" t="s">
-        <v>807</v>
+        <v>811</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="22" t="s">
-        <v>808</v>
+        <v>812</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="22" t="s">
-        <v>809</v>
+        <v>813</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="22" t="s">
-        <v>810</v>
+        <v>814</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="22" t="s">
-        <v>811</v>
+        <v>815</v>
       </c>
       <c r="B18" s="22" t="s">
-        <v>812</v>
+        <v>816</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="22" t="s">
-        <v>813</v>
+        <v>817</v>
       </c>
       <c r="B19" s="22" t="s">
-        <v>814</v>
+        <v>818</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="22" t="s">
-        <v>815</v>
+        <v>819</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="22" t="s">
-        <v>816</v>
+        <v>820</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="22" t="s">
-        <v>817</v>
+        <v>821</v>
       </c>
       <c r="B22" s="22" t="s">
-        <v>818</v>
+        <v>822</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="22" t="s">
-        <v>819</v>
+        <v>823</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="22" t="s">
-        <v>820</v>
+        <v>824</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="22" t="s">
-        <v>821</v>
+        <v>825</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="22" t="s">
-        <v>822</v>
+        <v>826</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="22" t="s">
-        <v>823</v>
+        <v>827</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="22" t="s">
-        <v>824</v>
+        <v>828</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="22" t="s">
-        <v>825</v>
+        <v>829</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="22" t="s">
-        <v>826</v>
+        <v>830</v>
       </c>
       <c r="B30" s="22" t="s">
-        <v>827</v>
+        <v>831</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="22" t="s">
-        <v>828</v>
+        <v>832</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="22" t="s">
-        <v>829</v>
+        <v>833</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="22" t="s">
-        <v>830</v>
+        <v>834</v>
       </c>
       <c r="B33" s="22" t="s">
-        <v>831</v>
+        <v>835</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="22" t="s">
-        <v>832</v>
+        <v>836</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="22" t="s">
-        <v>833</v>
+        <v>837</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="22" t="s">
-        <v>834</v>
+        <v>838</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="22" t="s">
-        <v>835</v>
+        <v>839</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="22" t="s">
-        <v>836</v>
+        <v>840</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C39" s="27" t="s">
-        <v>837</v>
+      <c r="C39" s="29" t="s">
+        <v>841</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="22" t="s">
-        <v>838</v>
+        <v>842</v>
       </c>
       <c r="B40" s="22" t="s">
-        <v>839</v>
+        <v>843</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="22" t="s">
-        <v>840</v>
+        <v>844</v>
       </c>
       <c r="B41" s="22" t="s">
-        <v>841</v>
+        <v>845</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="22" t="s">
-        <v>842</v>
+        <v>846</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="22" t="s">
-        <v>843</v>
+        <v>847</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="22" t="s">
-        <v>844</v>
+        <v>848</v>
       </c>
       <c r="B44" s="22" t="s">
-        <v>845</v>
+        <v>849</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="22" t="s">
-        <v>846</v>
+        <v>850</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="22" t="s">
-        <v>847</v>
+        <v>851</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="22" t="s">
-        <v>848</v>
+        <v>852</v>
       </c>
       <c r="B47" s="22" t="s">
-        <v>849</v>
+        <v>853</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="22" t="s">
-        <v>850</v>
+        <v>854</v>
       </c>
       <c r="B48" s="22" t="s">
-        <v>851</v>
+        <v>855</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="22" t="s">
-        <v>852</v>
+        <v>856</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="22" t="s">
-        <v>853</v>
+        <v>857</v>
       </c>
       <c r="B50" s="22" t="s">
-        <v>854</v>
+        <v>858</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="22" t="s">
-        <v>855</v>
+        <v>859</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="22" t="s">
-        <v>856</v>
+        <v>860</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="22" t="s">
-        <v>857</v>
+        <v>861</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="22" t="s">
-        <v>858</v>
+        <v>862</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="22" t="s">
-        <v>859</v>
+        <v>863</v>
       </c>
       <c r="B55" s="22" t="s">
-        <v>860</v>
+        <v>864</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="22" t="s">
+        <v>865</v>
+      </c>
+      <c r="B56" s="22" t="s">
+        <v>866</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add registers for maximum discharge power and max system charge current.
https://github.com/victronenergy/venus/issues/302
</commit_message>
<xml_diff>
--- a/CCGX-Modbus-TCP-register-list.xlsx
+++ b/CCGX-Modbus-TCP-register-list.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2542" uniqueCount="874">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2562" uniqueCount="884">
   <si>
     <t xml:space="preserve">NOTE: Use unit-id 100 for the com.victronenergy.system data, for more information see FAQ.</t>
   </si>
@@ -1791,13 +1791,13 @@
     <t xml:space="preserve">0 to 42949672.96</t>
   </si>
   <si>
-    <t xml:space="preserve">com.victronenergy.hub4</t>
+    <t xml:space="preserve">com.victronenergy.settings</t>
   </si>
   <si>
     <t xml:space="preserve">ESS control loop setpoint</t>
   </si>
   <si>
-    <t xml:space="preserve">/AcPowerSetpoint</t>
+    <t xml:space="preserve">/Settings/Cgwacs/AcPowerSetPoint</t>
   </si>
   <si>
     <t xml:space="preserve">ESS Mode 2 - Setpoint for the ESS control-loop in the CCGX. The control-loop will increase/decrease the Multi charge/discharge power to get the grid L1 reading at J224this setpoint</t>
@@ -1806,24 +1806,48 @@
     <t xml:space="preserve">ESS max charge current (fractional)</t>
   </si>
   <si>
-    <t xml:space="preserve">/MaxChargePercentage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ESS Mode 2 - Max charge current for ESS control-loop. The control-loop will use this value to limit the multi power setpoint.</t>
+    <t xml:space="preserve">/Settings/Cgwacs/MaxChargePercentage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ESS Mode 2 - Max charge current for ESS control-loop. The control-loop will use this value to limit the multi power setpoint. For DVCC, use 2705 instead.</t>
   </si>
   <si>
     <t xml:space="preserve">ESS max discharge current (fractional)</t>
   </si>
   <si>
-    <t xml:space="preserve">/MaxDischargePercentage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ESS Mode 2 - Max discharge current for ESS control-loop. The control-loop will use this value to limit the multi power setpoint. Currently a value &lt; 50% will disable discharge completely. &gt;=50% allows maximum discharge</t>
+    <t xml:space="preserve">/Settings/Cgwacs/MaxDischargePercentage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ESS Mode 2 - Max discharge current for ESS control-loop. The control-loop will use this value to limit the multi power setpoint. Currently a value &lt; 50% will disable discharge completely. &gt;=50% allows. Consider using 2704 instead.</t>
   </si>
   <si>
     <t xml:space="preserve">-3266800 to 3266800</t>
   </si>
   <si>
+    <t xml:space="preserve">ESS Mode 2 – Same as 2700, but with a different scale factor. Meant for values larger than 65kW.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ESS max discharge current</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 to 655360</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Settings/Cgwacs/MaxDischargePower</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ESS Mode 2 – similar to 2702, but as an absolute value instead of a percentage.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DVCC system max charge current</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Settings/SystemSetup/MaxChargeCurrent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ESS Mode 2 with DVCC – Maximum system charge current. -1 Disables.</t>
+  </si>
+  <si>
     <t xml:space="preserve">com.victronenergy.gps</t>
   </si>
   <si>
@@ -1884,9 +1908,6 @@
     <t xml:space="preserve">/NrOfSatellites</t>
   </si>
   <si>
-    <t xml:space="preserve">com.victronenergy.settings</t>
-  </si>
-  <si>
     <t xml:space="preserve">ESS BatteryLife state</t>
   </si>
   <si>
@@ -2644,6 +2665,15 @@
   </si>
   <si>
     <t xml:space="preserve">Added register for solar charger’s MPP operation mode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rev 19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Added register for ESS mode 2 maximum discharge current</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Added register for DVCC maximum system charge current</t>
   </si>
 </sst>
 </file>
@@ -2994,10 +3024,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N334"/>
+  <dimension ref="A1:N336"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="2" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
@@ -10883,7 +10913,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="262" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="262" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A262" s="1" t="s">
         <v>589</v>
       </c>
@@ -10915,7 +10945,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="263" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="263" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A263" s="1" t="s">
         <v>589</v>
       </c>
@@ -10947,7 +10977,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="264" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="264" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A264" s="1" t="s">
         <v>589</v>
       </c>
@@ -10979,7 +11009,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="265" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="265" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A265" s="1" t="s">
         <v>589</v>
       </c>
@@ -11007,22 +11037,25 @@
       <c r="I265" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="266" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J265" s="1" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="266" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A266" s="1" t="s">
-        <v>600</v>
+        <v>589</v>
       </c>
       <c r="B266" s="1" t="s">
         <v>601</v>
       </c>
       <c r="C266" s="1" t="n">
-        <v>2800</v>
+        <v>2704</v>
       </c>
       <c r="D266" s="2" t="s">
-        <v>388</v>
+        <v>20</v>
       </c>
       <c r="E266" s="1" t="n">
-        <v>10000000</v>
+        <v>0.1</v>
       </c>
       <c r="F266" s="3" t="s">
         <v>602</v>
@@ -11031,123 +11064,123 @@
         <v>603</v>
       </c>
       <c r="H266" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="I266" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J266" s="1" t="s">
         <v>604</v>
       </c>
     </row>
-    <row r="267" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="267" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A267" s="1" t="s">
-        <v>600</v>
+        <v>589</v>
       </c>
       <c r="B267" s="1" t="s">
         <v>605</v>
       </c>
       <c r="C267" s="1" t="n">
-        <v>2802</v>
+        <v>2705</v>
       </c>
       <c r="D267" s="2" t="s">
-        <v>388</v>
+        <v>59</v>
       </c>
       <c r="E267" s="1" t="n">
-        <v>10000000</v>
+        <v>1</v>
       </c>
       <c r="F267" s="3" t="s">
-        <v>602</v>
+        <v>60</v>
       </c>
       <c r="G267" s="1" t="s">
         <v>606</v>
       </c>
       <c r="H267" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="I267" s="1" t="s">
-        <v>604</v>
+        <v>86</v>
+      </c>
+      <c r="J267" s="1" t="s">
+        <v>607</v>
       </c>
     </row>
     <row r="268" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A268" s="1" t="s">
-        <v>600</v>
+        <v>608</v>
       </c>
       <c r="B268" s="1" t="s">
-        <v>607</v>
+        <v>609</v>
       </c>
       <c r="C268" s="1" t="n">
-        <v>2804</v>
+        <v>2800</v>
       </c>
       <c r="D268" s="2" t="s">
-        <v>20</v>
+        <v>388</v>
       </c>
       <c r="E268" s="1" t="n">
-        <v>100</v>
+        <v>10000000</v>
       </c>
       <c r="F268" s="3" t="s">
-        <v>185</v>
+        <v>610</v>
       </c>
       <c r="G268" s="1" t="s">
-        <v>608</v>
+        <v>611</v>
       </c>
       <c r="H268" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I268" s="1" t="s">
-        <v>609</v>
-      </c>
-      <c r="J268" s="1" t="s">
-        <v>610</v>
+        <v>612</v>
       </c>
     </row>
     <row r="269" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A269" s="1" t="s">
-        <v>600</v>
+        <v>608</v>
       </c>
       <c r="B269" s="1" t="s">
-        <v>611</v>
+        <v>613</v>
       </c>
       <c r="C269" s="1" t="n">
-        <v>2805</v>
+        <v>2802</v>
       </c>
       <c r="D269" s="2" t="s">
-        <v>20</v>
+        <v>388</v>
       </c>
       <c r="E269" s="1" t="n">
-        <v>100</v>
+        <v>10000000</v>
       </c>
       <c r="F269" s="3" t="s">
-        <v>185</v>
+        <v>610</v>
       </c>
       <c r="G269" s="1" t="s">
+        <v>614</v>
+      </c>
+      <c r="H269" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I269" s="1" t="s">
         <v>612</v>
-      </c>
-      <c r="H269" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I269" s="1" t="s">
-        <v>613</v>
-      </c>
-      <c r="J269" s="1" t="s">
-        <v>614</v>
       </c>
     </row>
     <row r="270" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A270" s="1" t="s">
-        <v>600</v>
+        <v>608</v>
       </c>
       <c r="B270" s="1" t="s">
         <v>615</v>
       </c>
       <c r="C270" s="1" t="n">
-        <v>2806</v>
+        <v>2804</v>
       </c>
       <c r="D270" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E270" s="1" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="F270" s="3" t="s">
-        <v>29</v>
+        <v>185</v>
       </c>
       <c r="G270" s="1" t="s">
         <v>616</v>
@@ -11155,45 +11188,54 @@
       <c r="H270" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="I270" s="1" t="s">
+        <v>617</v>
+      </c>
       <c r="J270" s="1" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
     </row>
     <row r="271" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A271" s="1" t="s">
-        <v>600</v>
+        <v>608</v>
       </c>
       <c r="B271" s="1" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="C271" s="1" t="n">
-        <v>2807</v>
+        <v>2805</v>
       </c>
       <c r="D271" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E271" s="1" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="F271" s="3" t="s">
-        <v>29</v>
+        <v>185</v>
       </c>
       <c r="G271" s="1" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="H271" s="1" t="s">
         <v>17</v>
+      </c>
+      <c r="I271" s="1" t="s">
+        <v>621</v>
+      </c>
+      <c r="J271" s="1" t="s">
+        <v>622</v>
       </c>
     </row>
     <row r="272" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A272" s="1" t="s">
-        <v>620</v>
+        <v>608</v>
       </c>
       <c r="B272" s="1" t="s">
-        <v>621</v>
+        <v>623</v>
       </c>
       <c r="C272" s="1" t="n">
-        <v>2900</v>
+        <v>2806</v>
       </c>
       <c r="D272" s="2" t="s">
         <v>20</v>
@@ -11201,66 +11243,60 @@
       <c r="E272" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="F272" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="G272" s="1" t="s">
-        <v>622</v>
+        <v>624</v>
       </c>
       <c r="H272" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I272" s="1" t="s">
-        <v>623</v>
+        <v>17</v>
       </c>
       <c r="J272" s="1" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
     </row>
     <row r="273" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A273" s="1" t="s">
-        <v>620</v>
+        <v>608</v>
       </c>
       <c r="B273" s="1" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="C273" s="1" t="n">
-        <v>2901</v>
+        <v>2807</v>
       </c>
       <c r="D273" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E273" s="1" t="n">
-        <v>10</v>
+        <v>1</v>
+      </c>
+      <c r="F273" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="G273" s="1" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="H273" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I273" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="J273" s="21" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="274" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A274" s="21" t="s">
-        <v>620</v>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="274" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A274" s="1" t="s">
+        <v>589</v>
       </c>
       <c r="B274" s="1" t="s">
         <v>628</v>
       </c>
       <c r="C274" s="1" t="n">
-        <v>2902</v>
+        <v>2900</v>
       </c>
       <c r="D274" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E274" s="1" t="n">
         <v>1</v>
-      </c>
-      <c r="F274" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="G274" s="1" t="s">
         <v>629</v>
@@ -11268,76 +11304,81 @@
       <c r="H274" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="I274" s="22" t="s">
+      <c r="I274" s="1" t="s">
         <v>630</v>
       </c>
-      <c r="J274" s="21"/>
-    </row>
-    <row r="275" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J274" s="1" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="275" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A275" s="1" t="s">
-        <v>631</v>
+        <v>589</v>
       </c>
       <c r="B275" s="1" t="s">
         <v>632</v>
       </c>
       <c r="C275" s="1" t="n">
-        <v>3000</v>
+        <v>2901</v>
       </c>
       <c r="D275" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E275" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="F275" s="3" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="G275" s="1" t="s">
         <v>633</v>
       </c>
       <c r="H275" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I275" s="23"/>
-    </row>
-    <row r="276" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A276" s="1" t="s">
-        <v>631</v>
+        <v>23</v>
+      </c>
+      <c r="I275" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="J275" s="21" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="276" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A276" s="21" t="s">
+        <v>589</v>
       </c>
       <c r="B276" s="1" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="C276" s="1" t="n">
-        <v>3001</v>
+        <v>2902</v>
       </c>
       <c r="D276" s="2" t="s">
-        <v>587</v>
+        <v>20</v>
       </c>
       <c r="E276" s="1" t="n">
-        <v>10000</v>
+        <v>1</v>
       </c>
       <c r="F276" s="3" t="s">
-        <v>635</v>
+        <v>29</v>
       </c>
       <c r="G276" s="1" t="s">
-        <v>386</v>
+        <v>636</v>
       </c>
       <c r="H276" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I276" s="1" t="s">
-        <v>636</v>
-      </c>
-    </row>
-    <row r="277" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+      <c r="I276" s="22" t="s">
+        <v>637</v>
+      </c>
+      <c r="J276" s="21"/>
+    </row>
+    <row r="277" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A277" s="1" t="s">
-        <v>631</v>
+        <v>638</v>
       </c>
       <c r="B277" s="1" t="s">
-        <v>637</v>
+        <v>639</v>
       </c>
       <c r="C277" s="1" t="n">
-        <v>3003</v>
+        <v>3000</v>
       </c>
       <c r="D277" s="2" t="s">
         <v>20</v>
@@ -11349,256 +11390,254 @@
         <v>29</v>
       </c>
       <c r="G277" s="1" t="s">
-        <v>638</v>
+        <v>640</v>
       </c>
       <c r="H277" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I277" s="1" t="s">
-        <v>639</v>
-      </c>
+      <c r="I277" s="23"/>
     </row>
     <row r="278" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A278" s="1" t="s">
-        <v>631</v>
+        <v>638</v>
       </c>
       <c r="B278" s="1" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="C278" s="1" t="n">
-        <v>3004</v>
+        <v>3001</v>
       </c>
       <c r="D278" s="2" t="s">
-        <v>20</v>
+        <v>587</v>
       </c>
       <c r="E278" s="1" t="n">
-        <v>10</v>
+        <v>10000</v>
       </c>
       <c r="F278" s="3" t="s">
-        <v>79</v>
+        <v>642</v>
       </c>
       <c r="G278" s="1" t="s">
-        <v>641</v>
+        <v>386</v>
       </c>
       <c r="H278" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I278" s="1" t="s">
-        <v>93</v>
+        <v>643</v>
       </c>
     </row>
     <row r="279" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A279" s="1" t="s">
-        <v>631</v>
+        <v>638</v>
       </c>
       <c r="B279" s="1" t="s">
-        <v>642</v>
+        <v>644</v>
       </c>
       <c r="C279" s="1" t="n">
-        <v>3005</v>
+        <v>3003</v>
       </c>
       <c r="D279" s="2" t="s">
-        <v>587</v>
+        <v>20</v>
       </c>
       <c r="E279" s="1" t="n">
-        <v>10000</v>
+        <v>1</v>
       </c>
       <c r="F279" s="3" t="s">
-        <v>635</v>
+        <v>29</v>
       </c>
       <c r="G279" s="1" t="s">
-        <v>643</v>
+        <v>645</v>
       </c>
       <c r="H279" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I279" s="1" t="s">
-        <v>636</v>
+        <v>646</v>
       </c>
     </row>
     <row r="280" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A280" s="1" t="s">
-        <v>631</v>
+        <v>638</v>
       </c>
       <c r="B280" s="1" t="s">
-        <v>644</v>
+        <v>647</v>
       </c>
       <c r="C280" s="1" t="n">
-        <v>3007</v>
+        <v>3004</v>
       </c>
       <c r="D280" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E280" s="1" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F280" s="3" t="s">
-        <v>29</v>
+        <v>79</v>
       </c>
       <c r="G280" s="1" t="s">
-        <v>645</v>
+        <v>648</v>
       </c>
       <c r="H280" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I280" s="1" t="s">
-        <v>646</v>
+        <v>93</v>
       </c>
     </row>
     <row r="281" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A281" s="1" t="s">
-        <v>647</v>
+        <v>638</v>
       </c>
       <c r="B281" s="1" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="C281" s="1" t="n">
-        <v>3100</v>
+        <v>3005</v>
       </c>
       <c r="D281" s="2" t="s">
-        <v>59</v>
+        <v>587</v>
       </c>
       <c r="E281" s="1" t="n">
-        <v>10</v>
+        <v>10000</v>
       </c>
       <c r="F281" s="3" t="s">
-        <v>649</v>
+        <v>642</v>
       </c>
       <c r="G281" s="1" t="s">
-        <v>165</v>
+        <v>650</v>
       </c>
       <c r="H281" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I281" s="1" t="s">
-        <v>134</v>
+        <v>643</v>
       </c>
     </row>
     <row r="282" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A282" s="1" t="s">
-        <v>647</v>
+        <v>638</v>
       </c>
       <c r="B282" s="1" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="C282" s="1" t="n">
-        <v>3101</v>
+        <v>3007</v>
       </c>
       <c r="D282" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E282" s="1" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F282" s="3" t="s">
-        <v>651</v>
+        <v>29</v>
       </c>
       <c r="G282" s="1" t="s">
-        <v>159</v>
+        <v>652</v>
       </c>
       <c r="H282" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I282" s="1" t="s">
-        <v>127</v>
+        <v>653</v>
       </c>
     </row>
     <row r="283" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A283" s="1" t="s">
-        <v>647</v>
+        <v>654</v>
       </c>
       <c r="B283" s="1" t="s">
-        <v>184</v>
+        <v>655</v>
       </c>
       <c r="C283" s="1" t="n">
-        <v>3105</v>
+        <v>3100</v>
       </c>
       <c r="D283" s="2" t="s">
-        <v>20</v>
+        <v>59</v>
       </c>
       <c r="E283" s="1" t="n">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="F283" s="3" t="s">
-        <v>652</v>
+        <v>656</v>
       </c>
       <c r="G283" s="1" t="s">
-        <v>186</v>
+        <v>165</v>
       </c>
       <c r="H283" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I283" s="1" t="s">
-        <v>81</v>
+        <v>134</v>
       </c>
     </row>
     <row r="284" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A284" s="1" t="s">
-        <v>647</v>
+        <v>654</v>
       </c>
       <c r="B284" s="1" t="s">
-        <v>311</v>
+        <v>657</v>
       </c>
       <c r="C284" s="1" t="n">
-        <v>3110</v>
+        <v>3101</v>
       </c>
       <c r="D284" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E284" s="1" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F284" s="3" t="s">
-        <v>653</v>
+        <v>658</v>
       </c>
       <c r="G284" s="1" t="s">
-        <v>208</v>
+        <v>159</v>
       </c>
       <c r="H284" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I284" s="1" t="s">
-        <v>654</v>
+        <v>127</v>
       </c>
     </row>
     <row r="285" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A285" s="1" t="s">
-        <v>647</v>
+        <v>654</v>
       </c>
       <c r="B285" s="1" t="s">
-        <v>655</v>
+        <v>184</v>
       </c>
       <c r="C285" s="1" t="n">
-        <v>3111</v>
+        <v>3105</v>
       </c>
       <c r="D285" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E285" s="1" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="F285" s="3" t="s">
-        <v>653</v>
+        <v>659</v>
       </c>
       <c r="G285" s="1" t="s">
-        <v>302</v>
+        <v>186</v>
       </c>
       <c r="H285" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I285" s="1" t="s">
-        <v>654</v>
+        <v>81</v>
       </c>
     </row>
     <row r="286" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A286" s="1" t="s">
-        <v>647</v>
+        <v>654</v>
       </c>
       <c r="B286" s="1" t="s">
-        <v>656</v>
+        <v>311</v>
       </c>
       <c r="C286" s="1" t="n">
-        <v>3112</v>
+        <v>3110</v>
       </c>
       <c r="D286" s="2" t="s">
         <v>20</v>
@@ -11607,27 +11646,27 @@
         <v>1</v>
       </c>
       <c r="F286" s="3" t="s">
-        <v>653</v>
+        <v>660</v>
       </c>
       <c r="G286" s="1" t="s">
-        <v>657</v>
+        <v>208</v>
       </c>
       <c r="H286" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I286" s="1" t="s">
-        <v>654</v>
+        <v>661</v>
       </c>
     </row>
     <row r="287" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A287" s="1" t="s">
-        <v>647</v>
+        <v>654</v>
       </c>
       <c r="B287" s="1" t="s">
-        <v>309</v>
+        <v>662</v>
       </c>
       <c r="C287" s="1" t="n">
-        <v>3113</v>
+        <v>3111</v>
       </c>
       <c r="D287" s="2" t="s">
         <v>20</v>
@@ -11636,27 +11675,27 @@
         <v>1</v>
       </c>
       <c r="F287" s="3" t="s">
-        <v>653</v>
+        <v>660</v>
       </c>
       <c r="G287" s="1" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="H287" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I287" s="1" t="s">
-        <v>654</v>
+        <v>661</v>
       </c>
     </row>
     <row r="288" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A288" s="1" t="s">
-        <v>647</v>
+        <v>654</v>
       </c>
       <c r="B288" s="1" t="s">
-        <v>658</v>
+        <v>663</v>
       </c>
       <c r="C288" s="1" t="n">
-        <v>3114</v>
+        <v>3112</v>
       </c>
       <c r="D288" s="2" t="s">
         <v>20</v>
@@ -11665,27 +11704,27 @@
         <v>1</v>
       </c>
       <c r="F288" s="3" t="s">
-        <v>653</v>
+        <v>660</v>
       </c>
       <c r="G288" s="1" t="s">
-        <v>300</v>
+        <v>664</v>
       </c>
       <c r="H288" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I288" s="1" t="s">
-        <v>654</v>
+        <v>661</v>
       </c>
     </row>
     <row r="289" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A289" s="1" t="s">
-        <v>647</v>
+        <v>654</v>
       </c>
       <c r="B289" s="1" t="s">
-        <v>659</v>
+        <v>309</v>
       </c>
       <c r="C289" s="1" t="n">
-        <v>3115</v>
+        <v>3113</v>
       </c>
       <c r="D289" s="2" t="s">
         <v>20</v>
@@ -11694,27 +11733,27 @@
         <v>1</v>
       </c>
       <c r="F289" s="3" t="s">
-        <v>653</v>
+        <v>660</v>
       </c>
       <c r="G289" s="1" t="s">
-        <v>660</v>
+        <v>310</v>
       </c>
       <c r="H289" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I289" s="1" t="s">
-        <v>654</v>
+        <v>661</v>
       </c>
     </row>
     <row r="290" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A290" s="1" t="s">
-        <v>647</v>
+        <v>654</v>
       </c>
       <c r="B290" s="1" t="s">
-        <v>212</v>
+        <v>665</v>
       </c>
       <c r="C290" s="1" t="n">
-        <v>3116</v>
+        <v>3114</v>
       </c>
       <c r="D290" s="2" t="s">
         <v>20</v>
@@ -11723,56 +11762,56 @@
         <v>1</v>
       </c>
       <c r="F290" s="3" t="s">
-        <v>653</v>
+        <v>660</v>
       </c>
       <c r="G290" s="1" t="s">
-        <v>213</v>
+        <v>300</v>
       </c>
       <c r="H290" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I290" s="1" t="s">
-        <v>654</v>
+        <v>661</v>
       </c>
     </row>
     <row r="291" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A291" s="1" t="s">
-        <v>647</v>
+        <v>654</v>
       </c>
       <c r="B291" s="1" t="s">
+        <v>666</v>
+      </c>
+      <c r="C291" s="1" t="n">
+        <v>3115</v>
+      </c>
+      <c r="D291" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E291" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F291" s="3" t="s">
+        <v>660</v>
+      </c>
+      <c r="G291" s="1" t="s">
+        <v>667</v>
+      </c>
+      <c r="H291" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I291" s="1" t="s">
         <v>661</v>
-      </c>
-      <c r="C291" s="1" t="n">
-        <v>3117</v>
-      </c>
-      <c r="D291" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E291" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="F291" s="3" t="s">
-        <v>653</v>
-      </c>
-      <c r="G291" s="1" t="s">
-        <v>662</v>
-      </c>
-      <c r="H291" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I291" s="1" t="s">
-        <v>654</v>
       </c>
     </row>
     <row r="292" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A292" s="1" t="s">
-        <v>647</v>
+        <v>654</v>
       </c>
       <c r="B292" s="1" t="s">
-        <v>663</v>
+        <v>212</v>
       </c>
       <c r="C292" s="1" t="n">
-        <v>3125</v>
+        <v>3116</v>
       </c>
       <c r="D292" s="2" t="s">
         <v>20</v>
@@ -11781,24 +11820,27 @@
         <v>1</v>
       </c>
       <c r="F292" s="3" t="s">
-        <v>653</v>
+        <v>660</v>
       </c>
       <c r="G292" s="1" t="s">
-        <v>664</v>
+        <v>213</v>
       </c>
       <c r="H292" s="1" t="s">
         <v>17</v>
+      </c>
+      <c r="I292" s="1" t="s">
+        <v>661</v>
       </c>
     </row>
     <row r="293" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A293" s="1" t="s">
-        <v>647</v>
+        <v>654</v>
       </c>
       <c r="B293" s="1" t="s">
-        <v>665</v>
+        <v>668</v>
       </c>
       <c r="C293" s="1" t="n">
-        <v>3126</v>
+        <v>3117</v>
       </c>
       <c r="D293" s="2" t="s">
         <v>20</v>
@@ -11807,27 +11849,27 @@
         <v>1</v>
       </c>
       <c r="F293" s="3" t="s">
-        <v>653</v>
+        <v>660</v>
       </c>
       <c r="G293" s="1" t="s">
-        <v>205</v>
+        <v>669</v>
       </c>
       <c r="H293" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="I293" s="1" t="s">
-        <v>666</v>
+        <v>661</v>
       </c>
     </row>
     <row r="294" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A294" s="1" t="s">
-        <v>647</v>
+        <v>654</v>
       </c>
       <c r="B294" s="1" t="s">
-        <v>667</v>
+        <v>670</v>
       </c>
       <c r="C294" s="1" t="n">
-        <v>3127</v>
+        <v>3125</v>
       </c>
       <c r="D294" s="2" t="s">
         <v>20</v>
@@ -11836,10 +11878,10 @@
         <v>1</v>
       </c>
       <c r="F294" s="3" t="s">
-        <v>653</v>
+        <v>660</v>
       </c>
       <c r="G294" s="1" t="s">
-        <v>633</v>
+        <v>671</v>
       </c>
       <c r="H294" s="1" t="s">
         <v>17</v>
@@ -11847,13 +11889,13 @@
     </row>
     <row r="295" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A295" s="1" t="s">
-        <v>647</v>
+        <v>654</v>
       </c>
       <c r="B295" s="1" t="s">
-        <v>668</v>
+        <v>672</v>
       </c>
       <c r="C295" s="1" t="n">
-        <v>3128</v>
+        <v>3126</v>
       </c>
       <c r="D295" s="2" t="s">
         <v>20</v>
@@ -11862,85 +11904,82 @@
         <v>1</v>
       </c>
       <c r="F295" s="3" t="s">
-        <v>653</v>
+        <v>660</v>
       </c>
       <c r="G295" s="1" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="H295" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="I295" s="1" t="s">
-        <v>669</v>
+        <v>673</v>
       </c>
     </row>
     <row r="296" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A296" s="1" t="s">
-        <v>670</v>
+        <v>654</v>
       </c>
       <c r="B296" s="1" t="s">
-        <v>671</v>
+        <v>674</v>
       </c>
       <c r="C296" s="1" t="n">
-        <v>3200</v>
+        <v>3127</v>
       </c>
       <c r="D296" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E296" s="1" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F296" s="3" t="s">
-        <v>651</v>
+        <v>660</v>
       </c>
       <c r="G296" s="1" t="s">
-        <v>464</v>
+        <v>640</v>
       </c>
       <c r="H296" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="I296" s="1" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="297" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A297" s="1" t="s">
-        <v>670</v>
+        <v>654</v>
       </c>
       <c r="B297" s="1" t="s">
-        <v>672</v>
+        <v>675</v>
       </c>
       <c r="C297" s="1" t="n">
-        <v>3201</v>
+        <v>3128</v>
       </c>
       <c r="D297" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E297" s="1" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F297" s="3" t="s">
-        <v>651</v>
+        <v>660</v>
       </c>
       <c r="G297" s="1" t="s">
-        <v>472</v>
+        <v>199</v>
       </c>
       <c r="H297" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I297" s="1" t="s">
-        <v>127</v>
+        <v>676</v>
       </c>
     </row>
     <row r="298" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A298" s="1" t="s">
-        <v>670</v>
+        <v>677</v>
       </c>
       <c r="B298" s="1" t="s">
-        <v>673</v>
+        <v>678</v>
       </c>
       <c r="C298" s="1" t="n">
-        <v>3202</v>
+        <v>3200</v>
       </c>
       <c r="D298" s="2" t="s">
         <v>20</v>
@@ -11949,10 +11988,10 @@
         <v>10</v>
       </c>
       <c r="F298" s="3" t="s">
-        <v>651</v>
+        <v>658</v>
       </c>
       <c r="G298" s="1" t="s">
-        <v>480</v>
+        <v>464</v>
       </c>
       <c r="H298" s="1" t="s">
         <v>17</v>
@@ -11963,71 +12002,71 @@
     </row>
     <row r="299" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A299" s="1" t="s">
-        <v>670</v>
+        <v>677</v>
       </c>
       <c r="B299" s="1" t="s">
-        <v>674</v>
+        <v>679</v>
       </c>
       <c r="C299" s="1" t="n">
-        <v>3203</v>
+        <v>3201</v>
       </c>
       <c r="D299" s="2" t="s">
-        <v>59</v>
+        <v>20</v>
       </c>
       <c r="E299" s="1" t="n">
         <v>10</v>
       </c>
       <c r="F299" s="3" t="s">
-        <v>649</v>
+        <v>658</v>
       </c>
       <c r="G299" s="1" t="s">
-        <v>466</v>
+        <v>472</v>
       </c>
       <c r="H299" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I299" s="1" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
     </row>
     <row r="300" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A300" s="1" t="s">
-        <v>670</v>
+        <v>677</v>
       </c>
       <c r="B300" s="1" t="s">
-        <v>675</v>
+        <v>680</v>
       </c>
       <c r="C300" s="1" t="n">
-        <v>3204</v>
+        <v>3202</v>
       </c>
       <c r="D300" s="2" t="s">
-        <v>59</v>
+        <v>20</v>
       </c>
       <c r="E300" s="1" t="n">
         <v>10</v>
       </c>
       <c r="F300" s="3" t="s">
-        <v>649</v>
+        <v>658</v>
       </c>
       <c r="G300" s="1" t="s">
-        <v>474</v>
+        <v>480</v>
       </c>
       <c r="H300" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I300" s="1" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
     </row>
     <row r="301" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A301" s="1" t="s">
-        <v>670</v>
+        <v>677</v>
       </c>
       <c r="B301" s="1" t="s">
-        <v>676</v>
+        <v>681</v>
       </c>
       <c r="C301" s="1" t="n">
-        <v>3205</v>
+        <v>3203</v>
       </c>
       <c r="D301" s="2" t="s">
         <v>59</v>
@@ -12036,10 +12075,10 @@
         <v>10</v>
       </c>
       <c r="F301" s="3" t="s">
-        <v>649</v>
+        <v>656</v>
       </c>
       <c r="G301" s="1" t="s">
-        <v>482</v>
+        <v>466</v>
       </c>
       <c r="H301" s="1" t="s">
         <v>17</v>
@@ -12050,71 +12089,71 @@
     </row>
     <row r="302" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A302" s="1" t="s">
-        <v>670</v>
+        <v>677</v>
       </c>
       <c r="B302" s="1" t="s">
-        <v>677</v>
+        <v>682</v>
       </c>
       <c r="C302" s="1" t="n">
-        <v>3206</v>
+        <v>3204</v>
       </c>
       <c r="D302" s="2" t="s">
         <v>59</v>
       </c>
       <c r="E302" s="1" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F302" s="3" t="s">
-        <v>678</v>
+        <v>656</v>
       </c>
       <c r="G302" s="1" t="s">
-        <v>468</v>
+        <v>474</v>
       </c>
       <c r="H302" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I302" s="1" t="s">
-        <v>31</v>
+        <v>134</v>
       </c>
     </row>
     <row r="303" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A303" s="1" t="s">
-        <v>670</v>
+        <v>677</v>
       </c>
       <c r="B303" s="1" t="s">
-        <v>679</v>
+        <v>683</v>
       </c>
       <c r="C303" s="1" t="n">
-        <v>3207</v>
+        <v>3205</v>
       </c>
       <c r="D303" s="2" t="s">
         <v>59</v>
       </c>
       <c r="E303" s="1" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F303" s="3" t="s">
-        <v>678</v>
+        <v>656</v>
       </c>
       <c r="G303" s="1" t="s">
-        <v>476</v>
+        <v>482</v>
       </c>
       <c r="H303" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I303" s="1" t="s">
-        <v>31</v>
+        <v>134</v>
       </c>
     </row>
     <row r="304" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A304" s="1" t="s">
-        <v>670</v>
+        <v>677</v>
       </c>
       <c r="B304" s="1" t="s">
-        <v>680</v>
+        <v>684</v>
       </c>
       <c r="C304" s="1" t="n">
-        <v>3208</v>
+        <v>3206</v>
       </c>
       <c r="D304" s="2" t="s">
         <v>59</v>
@@ -12123,10 +12162,10 @@
         <v>1</v>
       </c>
       <c r="F304" s="3" t="s">
-        <v>678</v>
+        <v>685</v>
       </c>
       <c r="G304" s="1" t="s">
-        <v>484</v>
+        <v>468</v>
       </c>
       <c r="H304" s="1" t="s">
         <v>17</v>
@@ -12137,71 +12176,71 @@
     </row>
     <row r="305" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A305" s="1" t="s">
-        <v>670</v>
+        <v>677</v>
       </c>
       <c r="B305" s="1" t="s">
-        <v>681</v>
+        <v>686</v>
       </c>
       <c r="C305" s="1" t="n">
-        <v>3209</v>
+        <v>3207</v>
       </c>
       <c r="D305" s="2" t="s">
-        <v>20</v>
+        <v>59</v>
       </c>
       <c r="E305" s="1" t="n">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="F305" s="3" t="s">
-        <v>652</v>
+        <v>685</v>
       </c>
       <c r="G305" s="1" t="s">
-        <v>682</v>
+        <v>476</v>
       </c>
       <c r="H305" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I305" s="1" t="s">
-        <v>143</v>
+        <v>31</v>
       </c>
     </row>
     <row r="306" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A306" s="1" t="s">
-        <v>670</v>
+        <v>677</v>
       </c>
       <c r="B306" s="1" t="s">
-        <v>683</v>
+        <v>687</v>
       </c>
       <c r="C306" s="1" t="n">
-        <v>3210</v>
+        <v>3208</v>
       </c>
       <c r="D306" s="2" t="s">
-        <v>20</v>
+        <v>59</v>
       </c>
       <c r="E306" s="1" t="n">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="F306" s="3" t="s">
-        <v>652</v>
+        <v>685</v>
       </c>
       <c r="G306" s="1" t="s">
-        <v>684</v>
+        <v>484</v>
       </c>
       <c r="H306" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I306" s="1" t="s">
-        <v>143</v>
+        <v>31</v>
       </c>
     </row>
     <row r="307" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A307" s="1" t="s">
-        <v>670</v>
+        <v>677</v>
       </c>
       <c r="B307" s="1" t="s">
-        <v>685</v>
+        <v>688</v>
       </c>
       <c r="C307" s="1" t="n">
-        <v>3211</v>
+        <v>3209</v>
       </c>
       <c r="D307" s="2" t="s">
         <v>20</v>
@@ -12210,10 +12249,10 @@
         <v>100</v>
       </c>
       <c r="F307" s="3" t="s">
-        <v>652</v>
+        <v>659</v>
       </c>
       <c r="G307" s="1" t="s">
-        <v>686</v>
+        <v>689</v>
       </c>
       <c r="H307" s="1" t="s">
         <v>17</v>
@@ -12224,68 +12263,71 @@
     </row>
     <row r="308" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A308" s="1" t="s">
-        <v>670</v>
+        <v>677</v>
       </c>
       <c r="B308" s="1" t="s">
-        <v>687</v>
+        <v>690</v>
       </c>
       <c r="C308" s="1" t="n">
-        <v>3212</v>
+        <v>3210</v>
       </c>
       <c r="D308" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E308" s="1" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="F308" s="3" t="s">
-        <v>653</v>
+        <v>659</v>
       </c>
       <c r="G308" s="1" t="s">
-        <v>633</v>
+        <v>691</v>
       </c>
       <c r="H308" s="1" t="s">
         <v>17</v>
+      </c>
+      <c r="I308" s="1" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="309" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A309" s="1" t="s">
-        <v>670</v>
+        <v>677</v>
       </c>
       <c r="B309" s="1" t="s">
-        <v>688</v>
+        <v>692</v>
       </c>
       <c r="C309" s="1" t="n">
-        <v>3213</v>
+        <v>3211</v>
       </c>
       <c r="D309" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E309" s="1" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="F309" s="3" t="s">
-        <v>653</v>
+        <v>659</v>
       </c>
       <c r="G309" s="1" t="s">
-        <v>689</v>
+        <v>693</v>
       </c>
       <c r="H309" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I309" s="1" t="s">
-        <v>690</v>
+        <v>143</v>
       </c>
     </row>
     <row r="310" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A310" s="1" t="s">
-        <v>670</v>
+        <v>677</v>
       </c>
       <c r="B310" s="1" t="s">
-        <v>493</v>
+        <v>694</v>
       </c>
       <c r="C310" s="1" t="n">
-        <v>3214</v>
+        <v>3212</v>
       </c>
       <c r="D310" s="2" t="s">
         <v>20</v>
@@ -12294,27 +12336,24 @@
         <v>1</v>
       </c>
       <c r="F310" s="3" t="s">
-        <v>653</v>
+        <v>660</v>
       </c>
       <c r="G310" s="1" t="s">
-        <v>449</v>
+        <v>640</v>
       </c>
       <c r="H310" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="I310" s="1" t="s">
-        <v>691</v>
       </c>
     </row>
     <row r="311" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A311" s="1" t="s">
-        <v>670</v>
+        <v>677</v>
       </c>
       <c r="B311" s="1" t="s">
-        <v>692</v>
+        <v>695</v>
       </c>
       <c r="C311" s="1" t="n">
-        <v>3215</v>
+        <v>3213</v>
       </c>
       <c r="D311" s="2" t="s">
         <v>20</v>
@@ -12323,27 +12362,27 @@
         <v>1</v>
       </c>
       <c r="F311" s="3" t="s">
-        <v>653</v>
+        <v>660</v>
       </c>
       <c r="G311" s="1" t="s">
-        <v>693</v>
+        <v>696</v>
       </c>
       <c r="H311" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I311" s="1" t="s">
-        <v>497</v>
+        <v>697</v>
       </c>
     </row>
     <row r="312" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A312" s="1" t="s">
-        <v>670</v>
+        <v>677</v>
       </c>
       <c r="B312" s="1" t="s">
-        <v>694</v>
+        <v>493</v>
       </c>
       <c r="C312" s="1" t="n">
-        <v>3216</v>
+        <v>3214</v>
       </c>
       <c r="D312" s="2" t="s">
         <v>20</v>
@@ -12352,27 +12391,27 @@
         <v>1</v>
       </c>
       <c r="F312" s="3" t="s">
-        <v>653</v>
+        <v>660</v>
       </c>
       <c r="G312" s="1" t="s">
-        <v>695</v>
+        <v>449</v>
       </c>
       <c r="H312" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I312" s="1" t="s">
-        <v>93</v>
+        <v>698</v>
       </c>
     </row>
     <row r="313" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A313" s="1" t="s">
-        <v>670</v>
+        <v>677</v>
       </c>
       <c r="B313" s="1" t="s">
-        <v>696</v>
+        <v>699</v>
       </c>
       <c r="C313" s="1" t="n">
-        <v>3217</v>
+        <v>3215</v>
       </c>
       <c r="D313" s="2" t="s">
         <v>20</v>
@@ -12381,114 +12420,114 @@
         <v>1</v>
       </c>
       <c r="F313" s="3" t="s">
-        <v>653</v>
+        <v>660</v>
       </c>
       <c r="G313" s="1" t="s">
-        <v>697</v>
+        <v>700</v>
       </c>
       <c r="H313" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I313" s="1" t="s">
-        <v>536</v>
+        <v>497</v>
       </c>
     </row>
     <row r="314" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A314" s="1" t="s">
-        <v>670</v>
+        <v>677</v>
       </c>
       <c r="B314" s="1" t="s">
-        <v>698</v>
+        <v>701</v>
       </c>
       <c r="C314" s="1" t="n">
-        <v>3218</v>
+        <v>3216</v>
       </c>
       <c r="D314" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E314" s="1" t="n">
-        <v>0.01</v>
+        <v>1</v>
       </c>
       <c r="F314" s="3" t="s">
-        <v>699</v>
+        <v>660</v>
       </c>
       <c r="G314" s="1" t="s">
-        <v>700</v>
+        <v>702</v>
       </c>
       <c r="H314" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I314" s="1" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
     </row>
     <row r="315" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A315" s="1" t="s">
-        <v>670</v>
+        <v>677</v>
       </c>
       <c r="B315" s="1" t="s">
-        <v>701</v>
+        <v>703</v>
       </c>
       <c r="C315" s="1" t="n">
-        <v>3219</v>
+        <v>3217</v>
       </c>
       <c r="D315" s="2" t="s">
-        <v>59</v>
+        <v>20</v>
       </c>
       <c r="E315" s="1" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F315" s="3" t="s">
-        <v>649</v>
+        <v>660</v>
       </c>
       <c r="G315" s="1" t="s">
-        <v>702</v>
+        <v>704</v>
       </c>
       <c r="H315" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I315" s="1" t="s">
-        <v>275</v>
+        <v>536</v>
       </c>
     </row>
     <row r="316" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A316" s="1" t="s">
-        <v>670</v>
+        <v>677</v>
       </c>
       <c r="B316" s="1" t="s">
-        <v>703</v>
+        <v>705</v>
       </c>
       <c r="C316" s="1" t="n">
-        <v>3220</v>
+        <v>3218</v>
       </c>
       <c r="D316" s="2" t="s">
-        <v>59</v>
+        <v>20</v>
       </c>
       <c r="E316" s="1" t="n">
-        <v>10</v>
+        <v>0.01</v>
       </c>
       <c r="F316" s="3" t="s">
-        <v>649</v>
+        <v>706</v>
       </c>
       <c r="G316" s="1" t="s">
-        <v>704</v>
+        <v>707</v>
       </c>
       <c r="H316" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I316" s="1" t="s">
-        <v>275</v>
+        <v>105</v>
       </c>
     </row>
     <row r="317" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A317" s="1" t="s">
-        <v>670</v>
+        <v>677</v>
       </c>
       <c r="B317" s="1" t="s">
-        <v>705</v>
+        <v>708</v>
       </c>
       <c r="C317" s="1" t="n">
-        <v>3221</v>
+        <v>3219</v>
       </c>
       <c r="D317" s="2" t="s">
         <v>59</v>
@@ -12497,10 +12536,10 @@
         <v>10</v>
       </c>
       <c r="F317" s="3" t="s">
-        <v>649</v>
+        <v>656</v>
       </c>
       <c r="G317" s="1" t="s">
-        <v>706</v>
+        <v>709</v>
       </c>
       <c r="H317" s="1" t="s">
         <v>17</v>
@@ -12511,135 +12550,141 @@
     </row>
     <row r="318" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A318" s="1" t="s">
-        <v>670</v>
+        <v>677</v>
       </c>
       <c r="B318" s="1" t="s">
-        <v>707</v>
+        <v>710</v>
       </c>
       <c r="C318" s="1" t="n">
-        <v>3222</v>
+        <v>3220</v>
       </c>
       <c r="D318" s="2" t="s">
-        <v>20</v>
+        <v>59</v>
       </c>
       <c r="E318" s="1" t="n">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="F318" s="3" t="s">
-        <v>652</v>
+        <v>656</v>
       </c>
       <c r="G318" s="1" t="s">
-        <v>708</v>
+        <v>711</v>
       </c>
       <c r="H318" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I318" s="1" t="s">
-        <v>81</v>
+        <v>275</v>
       </c>
     </row>
     <row r="319" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A319" s="1" t="s">
-        <v>670</v>
+        <v>677</v>
       </c>
       <c r="B319" s="1" t="s">
-        <v>709</v>
+        <v>712</v>
       </c>
       <c r="C319" s="1" t="n">
-        <v>3223</v>
+        <v>3221</v>
       </c>
       <c r="D319" s="2" t="s">
-        <v>20</v>
+        <v>59</v>
       </c>
       <c r="E319" s="1" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F319" s="3" t="s">
-        <v>653</v>
+        <v>656</v>
       </c>
       <c r="G319" s="1" t="s">
-        <v>710</v>
+        <v>713</v>
       </c>
       <c r="H319" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="I319" s="1" t="s">
-        <v>711</v>
+        <v>275</v>
       </c>
     </row>
     <row r="320" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A320" s="1" t="s">
-        <v>712</v>
+        <v>677</v>
       </c>
       <c r="B320" s="1" t="s">
-        <v>632</v>
+        <v>714</v>
       </c>
       <c r="C320" s="1" t="n">
-        <v>3300</v>
+        <v>3222</v>
       </c>
       <c r="D320" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E320" s="1" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="F320" s="3" t="s">
-        <v>29</v>
+        <v>659</v>
       </c>
       <c r="G320" s="1" t="s">
-        <v>633</v>
+        <v>715</v>
       </c>
       <c r="H320" s="1" t="s">
         <v>17</v>
+      </c>
+      <c r="I320" s="1" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="321" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A321" s="1" t="s">
-        <v>712</v>
+        <v>677</v>
       </c>
       <c r="B321" s="1" t="s">
-        <v>713</v>
+        <v>716</v>
       </c>
       <c r="C321" s="1" t="n">
-        <v>3301</v>
+        <v>3223</v>
       </c>
       <c r="D321" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E321" s="1" t="n">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="F321" s="3" t="s">
-        <v>185</v>
+        <v>660</v>
       </c>
       <c r="G321" s="1" t="s">
-        <v>714</v>
+        <v>717</v>
       </c>
       <c r="H321" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
+      </c>
+      <c r="I321" s="1" t="s">
+        <v>718</v>
       </c>
     </row>
     <row r="322" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A322" s="1" t="s">
-        <v>712</v>
+        <v>719</v>
       </c>
       <c r="B322" s="1" t="s">
-        <v>715</v>
+        <v>639</v>
       </c>
       <c r="C322" s="1" t="n">
-        <v>3302</v>
+        <v>3300</v>
       </c>
       <c r="D322" s="2" t="s">
-        <v>59</v>
+        <v>20</v>
       </c>
       <c r="E322" s="1" t="n">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="F322" s="3" t="s">
-        <v>141</v>
+        <v>29</v>
       </c>
       <c r="G322" s="1" t="s">
-        <v>716</v>
+        <v>640</v>
       </c>
       <c r="H322" s="1" t="s">
         <v>17</v>
@@ -12647,42 +12692,39 @@
     </row>
     <row r="323" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A323" s="1" t="s">
-        <v>712</v>
+        <v>719</v>
       </c>
       <c r="B323" s="1" t="s">
-        <v>717</v>
+        <v>720</v>
       </c>
       <c r="C323" s="1" t="n">
-        <v>3303</v>
+        <v>3301</v>
       </c>
       <c r="D323" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E323" s="1" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="F323" s="3" t="s">
-        <v>29</v>
+        <v>185</v>
       </c>
       <c r="G323" s="1" t="s">
-        <v>718</v>
+        <v>721</v>
       </c>
       <c r="H323" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="I323" s="1" t="s">
-        <v>719</v>
       </c>
     </row>
     <row r="324" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A324" s="1" t="s">
-        <v>712</v>
+        <v>719</v>
       </c>
       <c r="B324" s="1" t="s">
-        <v>720</v>
+        <v>722</v>
       </c>
       <c r="C324" s="1" t="n">
-        <v>3304</v>
+        <v>3302</v>
       </c>
       <c r="D324" s="2" t="s">
         <v>59</v>
@@ -12694,24 +12736,21 @@
         <v>141</v>
       </c>
       <c r="G324" s="1" t="s">
-        <v>721</v>
+        <v>723</v>
       </c>
       <c r="H324" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="I324" s="1" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="325" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A325" s="1" t="s">
-        <v>712</v>
+        <v>719</v>
       </c>
       <c r="B325" s="1" t="s">
-        <v>722</v>
+        <v>724</v>
       </c>
       <c r="C325" s="1" t="n">
-        <v>3305</v>
+        <v>3303</v>
       </c>
       <c r="D325" s="2" t="s">
         <v>20</v>
@@ -12723,79 +12762,82 @@
         <v>29</v>
       </c>
       <c r="G325" s="1" t="s">
-        <v>645</v>
+        <v>725</v>
       </c>
       <c r="H325" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I325" s="1" t="s">
-        <v>646</v>
+        <v>726</v>
       </c>
     </row>
     <row r="326" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A326" s="1" t="s">
-        <v>723</v>
+        <v>719</v>
       </c>
       <c r="B326" s="1" t="s">
-        <v>724</v>
+        <v>727</v>
       </c>
       <c r="C326" s="1" t="n">
-        <v>3400</v>
+        <v>3304</v>
       </c>
       <c r="D326" s="2" t="s">
-        <v>587</v>
+        <v>59</v>
       </c>
       <c r="E326" s="1" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="F326" s="3" t="s">
-        <v>725</v>
+        <v>141</v>
       </c>
       <c r="G326" s="1" t="s">
-        <v>726</v>
+        <v>728</v>
       </c>
       <c r="H326" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I326" s="1" t="s">
-        <v>636</v>
+        <v>275</v>
       </c>
     </row>
     <row r="327" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A327" s="1" t="s">
-        <v>723</v>
+        <v>719</v>
       </c>
       <c r="B327" s="1" t="s">
-        <v>727</v>
+        <v>729</v>
       </c>
       <c r="C327" s="1" t="n">
-        <v>3402</v>
+        <v>3305</v>
       </c>
       <c r="D327" s="2" t="s">
-        <v>587</v>
+        <v>20</v>
       </c>
       <c r="E327" s="1" t="n">
         <v>1</v>
       </c>
       <c r="F327" s="3" t="s">
-        <v>725</v>
+        <v>29</v>
       </c>
       <c r="G327" s="1" t="s">
-        <v>728</v>
+        <v>652</v>
       </c>
       <c r="H327" s="1" t="s">
         <v>17</v>
+      </c>
+      <c r="I327" s="1" t="s">
+        <v>653</v>
       </c>
     </row>
     <row r="328" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A328" s="1" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="B328" s="1" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="C328" s="1" t="n">
-        <v>3420</v>
+        <v>3400</v>
       </c>
       <c r="D328" s="2" t="s">
         <v>587</v>
@@ -12804,56 +12846,56 @@
         <v>1</v>
       </c>
       <c r="F328" s="3" t="s">
-        <v>725</v>
+        <v>732</v>
       </c>
       <c r="G328" s="1" t="s">
-        <v>728</v>
+        <v>733</v>
       </c>
       <c r="H328" s="1" t="s">
         <v>17</v>
+      </c>
+      <c r="I328" s="1" t="s">
+        <v>643</v>
       </c>
     </row>
     <row r="329" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A329" s="1" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="B329" s="1" t="s">
-        <v>491</v>
+        <v>734</v>
       </c>
       <c r="C329" s="1" t="n">
-        <v>3422</v>
+        <v>3402</v>
       </c>
       <c r="D329" s="2" t="s">
-        <v>20</v>
+        <v>587</v>
       </c>
       <c r="E329" s="1" t="n">
         <v>1</v>
       </c>
       <c r="F329" s="3" t="s">
-        <v>21</v>
+        <v>732</v>
       </c>
       <c r="G329" s="1" t="s">
-        <v>199</v>
+        <v>735</v>
       </c>
       <c r="H329" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="I329" s="1" t="s">
-        <v>731</v>
       </c>
     </row>
     <row r="330" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A330" s="1" t="s">
-        <v>729</v>
+        <v>736</v>
       </c>
       <c r="B330" s="1" t="s">
-        <v>295</v>
+        <v>737</v>
       </c>
       <c r="C330" s="1" t="n">
-        <v>3423</v>
+        <v>3420</v>
       </c>
       <c r="D330" s="2" t="s">
-        <v>20</v>
+        <v>587</v>
       </c>
       <c r="E330" s="1" t="n">
         <v>1</v>
@@ -12862,91 +12904,88 @@
         <v>732</v>
       </c>
       <c r="G330" s="1" t="s">
-        <v>733</v>
+        <v>735</v>
       </c>
       <c r="H330" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="I330" s="1" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="331" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A331" s="1" t="s">
-        <v>729</v>
+        <v>736</v>
       </c>
       <c r="B331" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="C331" s="1" t="n">
+        <v>3422</v>
+      </c>
+      <c r="D331" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E331" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F331" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G331" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="H331" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I331" s="1" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="332" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A332" s="1" t="s">
+        <v>736</v>
+      </c>
+      <c r="B332" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="C332" s="1" t="n">
+        <v>3423</v>
+      </c>
+      <c r="D332" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E332" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F332" s="3" t="s">
+        <v>739</v>
+      </c>
+      <c r="G332" s="1" t="s">
+        <v>740</v>
+      </c>
+      <c r="H332" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I332" s="1" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="333" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A333" s="1" t="s">
+        <v>736</v>
+      </c>
+      <c r="B333" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C331" s="1" t="n">
+      <c r="C333" s="1" t="n">
         <v>3424</v>
       </c>
-      <c r="D331" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E331" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="F331" s="3" t="s">
-        <v>734</v>
-      </c>
-      <c r="G331" s="1" t="s">
-        <v>735</v>
-      </c>
-      <c r="H331" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I331" s="1" t="s">
-        <v>736</v>
-      </c>
-    </row>
-    <row r="332" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A332" s="1" t="s">
-        <v>737</v>
-      </c>
-      <c r="B332" s="1" t="s">
-        <v>738</v>
-      </c>
-      <c r="C332" s="1" t="n">
-        <v>3500</v>
-      </c>
-      <c r="D332" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E332" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="F332" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G332" s="1" t="s">
-        <v>739</v>
-      </c>
-      <c r="H332" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I332" s="1" t="s">
-        <v>740</v>
-      </c>
-    </row>
-    <row r="333" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A333" s="1" t="s">
-        <v>737</v>
-      </c>
-      <c r="B333" s="1" t="s">
+      <c r="D333" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E333" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F333" s="3" t="s">
         <v>741</v>
-      </c>
-      <c r="C333" s="1" t="n">
-        <v>3501</v>
-      </c>
-      <c r="D333" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E333" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="F333" s="3" t="s">
-        <v>734</v>
       </c>
       <c r="G333" s="1" t="s">
         <v>742</v>
@@ -12960,30 +12999,88 @@
     </row>
     <row r="334" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A334" s="1" t="s">
-        <v>737</v>
+        <v>744</v>
       </c>
       <c r="B334" s="1" t="s">
+        <v>745</v>
+      </c>
+      <c r="C334" s="1" t="n">
+        <v>3500</v>
+      </c>
+      <c r="D334" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E334" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F334" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G334" s="1" t="s">
+        <v>746</v>
+      </c>
+      <c r="H334" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I334" s="1" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="335" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A335" s="1" t="s">
         <v>744</v>
       </c>
-      <c r="C334" s="1" t="n">
+      <c r="B335" s="1" t="s">
+        <v>748</v>
+      </c>
+      <c r="C335" s="1" t="n">
+        <v>3501</v>
+      </c>
+      <c r="D335" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E335" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F335" s="3" t="s">
+        <v>741</v>
+      </c>
+      <c r="G335" s="1" t="s">
+        <v>749</v>
+      </c>
+      <c r="H335" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I335" s="1" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="336" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A336" s="1" t="s">
+        <v>744</v>
+      </c>
+      <c r="B336" s="1" t="s">
+        <v>751</v>
+      </c>
+      <c r="C336" s="1" t="n">
         <v>3502</v>
       </c>
-      <c r="D334" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E334" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="F334" s="3" t="s">
-        <v>734</v>
-      </c>
-      <c r="G334" s="1" t="s">
-        <v>739</v>
-      </c>
-      <c r="H334" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I334" s="1" t="s">
+      <c r="D336" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E336" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F336" s="3" t="s">
+        <v>741</v>
+      </c>
+      <c r="G336" s="1" t="s">
+        <v>746</v>
+      </c>
+      <c r="H336" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I336" s="1" t="s">
         <v>343</v>
       </c>
     </row>
@@ -13008,8 +13105,8 @@
   </sheetPr>
   <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B43" activeCellId="0" sqref="B43"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13022,13 +13119,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="24" t="s">
-        <v>745</v>
+        <v>752</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>746</v>
+        <v>753</v>
       </c>
       <c r="C1" s="24" t="s">
-        <v>747</v>
+        <v>754</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13039,7 +13136,7 @@
         <v>257</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>748</v>
+        <v>755</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13050,7 +13147,7 @@
         <v>256</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>749</v>
+        <v>756</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13061,7 +13158,7 @@
         <v>258</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>750</v>
+        <v>757</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13072,7 +13169,7 @@
         <v>260</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>751</v>
+        <v>758</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13083,7 +13180,7 @@
         <v>261</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>752</v>
+        <v>759</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13094,7 +13191,7 @@
         <v>0</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>753</v>
+        <v>760</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13105,7 +13202,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>754</v>
+        <v>761</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13116,7 +13213,7 @@
         <v>2</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>755</v>
+        <v>762</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13127,7 +13224,7 @@
         <v>3</v>
       </c>
       <c r="C10" s="22" t="s">
-        <v>756</v>
+        <v>763</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13138,7 +13235,7 @@
         <v>4</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>757</v>
+        <v>764</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13149,7 +13246,7 @@
         <v>5</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>758</v>
+        <v>765</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13160,7 +13257,7 @@
         <v>6</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>759</v>
+        <v>766</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13171,7 +13268,7 @@
         <v>7</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>760</v>
+        <v>767</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13182,7 +13279,7 @@
         <v>8</v>
       </c>
       <c r="C15" s="22" t="s">
-        <v>761</v>
+        <v>768</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13193,7 +13290,7 @@
         <v>9</v>
       </c>
       <c r="C16" s="22" t="s">
-        <v>762</v>
+        <v>769</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13204,7 +13301,7 @@
         <v>10</v>
       </c>
       <c r="C17" s="22" t="s">
-        <v>763</v>
+        <v>770</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13215,7 +13312,7 @@
         <v>11</v>
       </c>
       <c r="C18" s="22" t="s">
-        <v>764</v>
+        <v>771</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13226,7 +13323,7 @@
         <v>12</v>
       </c>
       <c r="C19" s="22" t="s">
-        <v>765</v>
+        <v>772</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13237,7 +13334,7 @@
         <v>20</v>
       </c>
       <c r="C20" s="22" t="s">
-        <v>766</v>
+        <v>773</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13248,7 +13345,7 @@
         <v>21</v>
       </c>
       <c r="C21" s="22" t="s">
-        <v>767</v>
+        <v>774</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13259,7 +13356,7 @@
         <v>22</v>
       </c>
       <c r="C22" s="22" t="s">
-        <v>768</v>
+        <v>775</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13270,7 +13367,7 @@
         <v>23</v>
       </c>
       <c r="C23" s="22" t="s">
-        <v>769</v>
+        <v>776</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13281,7 +13378,7 @@
         <v>24</v>
       </c>
       <c r="C24" s="22" t="s">
-        <v>770</v>
+        <v>777</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13292,7 +13389,7 @@
         <v>25</v>
       </c>
       <c r="C25" s="22" t="s">
-        <v>771</v>
+        <v>778</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13303,7 +13400,7 @@
         <v>26</v>
       </c>
       <c r="C26" s="22" t="s">
-        <v>772</v>
+        <v>779</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13314,7 +13411,7 @@
         <v>27</v>
       </c>
       <c r="C27" s="22" t="s">
-        <v>773</v>
+        <v>780</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13325,7 +13422,7 @@
         <v>28</v>
       </c>
       <c r="C28" s="22" t="s">
-        <v>774</v>
+        <v>781</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13336,7 +13433,7 @@
         <v>29</v>
       </c>
       <c r="C29" s="22" t="s">
-        <v>775</v>
+        <v>782</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13347,7 +13444,7 @@
         <v>30</v>
       </c>
       <c r="C30" s="22" t="s">
-        <v>776</v>
+        <v>783</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13358,7 +13455,7 @@
         <v>31</v>
       </c>
       <c r="C31" s="22" t="s">
-        <v>777</v>
+        <v>784</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13369,7 +13466,7 @@
         <v>32</v>
       </c>
       <c r="C32" s="22" t="s">
-        <v>778</v>
+        <v>785</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13380,7 +13477,7 @@
         <v>33</v>
       </c>
       <c r="C33" s="22" t="s">
-        <v>779</v>
+        <v>786</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13391,7 +13488,7 @@
         <v>34</v>
       </c>
       <c r="C34" s="22" t="s">
-        <v>780</v>
+        <v>787</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13402,7 +13499,7 @@
         <v>40</v>
       </c>
       <c r="C35" s="22" t="s">
-        <v>781</v>
+        <v>788</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13413,7 +13510,7 @@
         <v>41</v>
       </c>
       <c r="C36" s="22" t="s">
-        <v>782</v>
+        <v>789</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13424,7 +13521,7 @@
         <v>42</v>
       </c>
       <c r="C37" s="22" t="s">
-        <v>783</v>
+        <v>790</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13435,7 +13532,7 @@
         <v>43</v>
       </c>
       <c r="C38" s="22" t="s">
-        <v>784</v>
+        <v>791</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13446,7 +13543,7 @@
         <v>44</v>
       </c>
       <c r="C39" s="22" t="s">
-        <v>785</v>
+        <v>792</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13457,7 +13554,7 @@
         <v>45</v>
       </c>
       <c r="C40" s="22" t="s">
-        <v>786</v>
+        <v>793</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13468,7 +13565,7 @@
         <v>46</v>
       </c>
       <c r="C41" s="22" t="s">
-        <v>787</v>
+        <v>794</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13479,7 +13576,7 @@
         <v>288</v>
       </c>
       <c r="C42" s="22" t="s">
-        <v>788</v>
+        <v>795</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13490,7 +13587,7 @@
         <v>289</v>
       </c>
       <c r="C43" s="22" t="s">
-        <v>789</v>
+        <v>796</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13501,7 +13598,7 @@
         <v>290</v>
       </c>
       <c r="C44" s="22" t="s">
-        <v>790</v>
+        <v>797</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13512,7 +13609,7 @@
         <v>291</v>
       </c>
       <c r="C45" s="22" t="s">
-        <v>791</v>
+        <v>798</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13523,7 +13620,7 @@
         <v>292</v>
       </c>
       <c r="C46" s="22" t="s">
-        <v>792</v>
+        <v>799</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13534,7 +13631,7 @@
         <v>293</v>
       </c>
       <c r="C47" s="22" t="s">
-        <v>793</v>
+        <v>800</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13545,12 +13642,12 @@
         <v>512</v>
       </c>
       <c r="C48" s="22" t="s">
-        <v>794</v>
+        <v>801</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="26" t="s">
-        <v>795</v>
+        <v>802</v>
       </c>
       <c r="B50" s="26"/>
       <c r="C50" s="26"/>
@@ -13560,7 +13657,7 @@
     </row>
     <row r="51" customFormat="false" ht="92.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="27" t="s">
-        <v>796</v>
+        <v>803</v>
       </c>
       <c r="B51" s="27"/>
       <c r="C51" s="27"/>
@@ -13588,10 +13685,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C58"/>
+  <dimension ref="A1:C60"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B57" activeCellId="0" sqref="B57"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13604,349 +13701,362 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="22" t="s">
-        <v>797</v>
+        <v>804</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>798</v>
+        <v>805</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="22" t="s">
-        <v>799</v>
+        <v>806</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>800</v>
+        <v>807</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="22" t="s">
-        <v>801</v>
+        <v>808</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>802</v>
+        <v>809</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="22" t="s">
-        <v>803</v>
+        <v>810</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>804</v>
+        <v>811</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="22" t="s">
-        <v>805</v>
+        <v>812</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="22" t="s">
-        <v>806</v>
+        <v>813</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="22" t="s">
-        <v>807</v>
+        <v>814</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="22" t="s">
-        <v>808</v>
+        <v>815</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="22" t="s">
-        <v>809</v>
+        <v>816</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>810</v>
+        <v>817</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="22" t="s">
-        <v>811</v>
+        <v>818</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="22" t="s">
-        <v>812</v>
+        <v>819</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="22" t="s">
-        <v>813</v>
+        <v>820</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>814</v>
+        <v>821</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="22" t="s">
-        <v>815</v>
+        <v>822</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="22" t="s">
-        <v>816</v>
+        <v>823</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="22" t="s">
-        <v>817</v>
+        <v>824</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="22" t="s">
-        <v>818</v>
+        <v>825</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="22" t="s">
-        <v>819</v>
+        <v>826</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="22" t="s">
-        <v>820</v>
+        <v>827</v>
       </c>
       <c r="B18" s="22" t="s">
-        <v>821</v>
+        <v>828</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="22" t="s">
-        <v>822</v>
+        <v>829</v>
       </c>
       <c r="B19" s="22" t="s">
-        <v>823</v>
+        <v>830</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="22" t="s">
-        <v>824</v>
+        <v>831</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="22" t="s">
-        <v>825</v>
+        <v>832</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="22" t="s">
-        <v>826</v>
+        <v>833</v>
       </c>
       <c r="B22" s="22" t="s">
-        <v>827</v>
+        <v>834</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="22" t="s">
-        <v>828</v>
+        <v>835</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="22" t="s">
-        <v>829</v>
+        <v>836</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="22" t="s">
-        <v>830</v>
+        <v>837</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="22" t="s">
-        <v>831</v>
+        <v>838</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="22" t="s">
-        <v>832</v>
+        <v>839</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="22" t="s">
-        <v>833</v>
+        <v>840</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="22" t="s">
-        <v>834</v>
+        <v>841</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="22" t="s">
-        <v>835</v>
+        <v>842</v>
       </c>
       <c r="B30" s="22" t="s">
-        <v>836</v>
+        <v>843</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="22" t="s">
-        <v>837</v>
+        <v>844</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="22" t="s">
-        <v>838</v>
+        <v>845</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="22" t="s">
-        <v>839</v>
+        <v>846</v>
       </c>
       <c r="B33" s="22" t="s">
-        <v>840</v>
+        <v>847</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="22" t="s">
-        <v>841</v>
+        <v>848</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="22" t="s">
-        <v>842</v>
+        <v>849</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="22" t="s">
-        <v>843</v>
+        <v>850</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="22" t="s">
-        <v>844</v>
+        <v>851</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="22" t="s">
-        <v>845</v>
+        <v>852</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C39" s="28" t="s">
-        <v>846</v>
+        <v>853</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="22" t="s">
-        <v>847</v>
+        <v>854</v>
       </c>
       <c r="B40" s="22" t="s">
-        <v>848</v>
+        <v>855</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="22" t="s">
-        <v>849</v>
+        <v>856</v>
       </c>
       <c r="B41" s="22" t="s">
-        <v>850</v>
+        <v>857</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="22" t="s">
-        <v>851</v>
+        <v>858</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="22" t="s">
-        <v>852</v>
+        <v>859</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="22" t="s">
-        <v>853</v>
+        <v>860</v>
       </c>
       <c r="B44" s="22" t="s">
-        <v>854</v>
+        <v>861</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="22" t="s">
-        <v>855</v>
+        <v>862</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="22" t="s">
-        <v>856</v>
+        <v>863</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="22" t="s">
-        <v>857</v>
+        <v>864</v>
       </c>
       <c r="B47" s="22" t="s">
-        <v>858</v>
+        <v>865</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="22" t="s">
-        <v>859</v>
+        <v>866</v>
       </c>
       <c r="B48" s="22" t="s">
-        <v>860</v>
+        <v>867</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="22" t="s">
-        <v>861</v>
+        <v>868</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="22" t="s">
-        <v>862</v>
+        <v>869</v>
       </c>
       <c r="B50" s="22" t="s">
-        <v>863</v>
+        <v>870</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="22" t="s">
-        <v>864</v>
+        <v>871</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="22" t="s">
-        <v>865</v>
+        <v>872</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="22" t="s">
-        <v>866</v>
+        <v>873</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="22" t="s">
-        <v>867</v>
+        <v>874</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="22" t="s">
-        <v>868</v>
+        <v>875</v>
       </c>
       <c r="B55" s="22" t="s">
-        <v>869</v>
+        <v>876</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="22" t="s">
-        <v>870</v>
+        <v>877</v>
       </c>
       <c r="B56" s="22" t="s">
-        <v>871</v>
+        <v>878</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="22" t="s">
-        <v>872</v>
+        <v>879</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="22" t="s">
-        <v>873</v>
+        <v>880</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="22" t="s">
+        <v>881</v>
+      </c>
+      <c r="B59" s="22" t="s">
+        <v>882</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B60" s="22" t="s">
+        <v>883</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated document revision of modbus spreadsheet
</commit_message>
<xml_diff>
--- a/CCGX-Modbus-TCP-register-list.xlsx
+++ b/CCGX-Modbus-TCP-register-list.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2586" uniqueCount="887">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2588" uniqueCount="889">
   <si>
     <t xml:space="preserve">NOTE: Use unit-id 100 for the com.victronenergy.system data, for more information see FAQ.</t>
   </si>
@@ -2683,6 +2683,12 @@
   </si>
   <si>
     <t xml:space="preserve">Added register for DVCC maximum system charge current</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rev 20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Added 32-bit registers for PV-inverters</t>
   </si>
 </sst>
 </file>
@@ -3035,10 +3041,10 @@
   </sheetPr>
   <dimension ref="A1:N339"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="2" topLeftCell="A169" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="F200" activeCellId="0" sqref="F200"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13790,7 +13796,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C60"/>
+  <dimension ref="A1:C61"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -14164,6 +14170,14 @@
         <v>886</v>
       </c>
     </row>
+    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="22" t="s">
+        <v>887</v>
+      </c>
+      <c r="B61" s="22" t="s">
+        <v>888</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Add registers for IMT solar irradiation sensor.
</commit_message>
<xml_diff>
--- a/CCGX-Modbus-TCP-register-list.xlsx
+++ b/CCGX-Modbus-TCP-register-list.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Field list" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2588" uniqueCount="889">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2614" uniqueCount="903">
   <si>
     <t xml:space="preserve">NOTE: Use unit-id 100 for the com.victronenergy.system data, for more information see FAQ.</t>
   </si>
@@ -2289,6 +2289,42 @@
     <t xml:space="preserve">Runtime in seconds</t>
   </si>
   <si>
+    <t xml:space="preserve">com.victronenergy.meteo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Solar irradiance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 to 6553.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Irradiance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">W/m^2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wind speed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/WindSpeed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cell temperature of sensor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-3276.8 to 3276.7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/CellTemperature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">External temperature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/ExternalTemperature</t>
+  </si>
+  <si>
     <t xml:space="preserve">Unit ID</t>
   </si>
   <si>
@@ -2689,6 +2725,12 @@
   </si>
   <si>
     <t xml:space="preserve">Added 32-bit registers for PV-inverters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rev 21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Added registers for IMT solar irradiation sensors</t>
   </si>
 </sst>
 </file>
@@ -3039,12 +3081,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N339"/>
+  <dimension ref="A1:N343"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="2" topLeftCell="A324" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A343" activeCellId="0" sqref="A343"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13193,6 +13235,110 @@
       </c>
       <c r="I339" s="1" t="s">
         <v>343</v>
+      </c>
+    </row>
+    <row r="340" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A340" s="1" t="s">
+        <v>755</v>
+      </c>
+      <c r="B340" s="0" t="s">
+        <v>756</v>
+      </c>
+      <c r="C340" s="1" t="n">
+        <v>3600</v>
+      </c>
+      <c r="D340" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E340" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="F340" s="3" t="s">
+        <v>757</v>
+      </c>
+      <c r="G340" s="1" t="s">
+        <v>758</v>
+      </c>
+      <c r="I340" s="1" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="341" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A341" s="1" t="s">
+        <v>755</v>
+      </c>
+      <c r="B341" s="0" t="s">
+        <v>760</v>
+      </c>
+      <c r="C341" s="1" t="n">
+        <v>3601</v>
+      </c>
+      <c r="D341" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E341" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="F341" s="3" t="s">
+        <v>757</v>
+      </c>
+      <c r="G341" s="1" t="s">
+        <v>761</v>
+      </c>
+      <c r="I341" s="1" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="342" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A342" s="1" t="s">
+        <v>755</v>
+      </c>
+      <c r="B342" s="0" t="s">
+        <v>762</v>
+      </c>
+      <c r="C342" s="1" t="n">
+        <v>3602</v>
+      </c>
+      <c r="D342" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E342" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="F342" s="3" t="s">
+        <v>763</v>
+      </c>
+      <c r="G342" s="1" t="s">
+        <v>764</v>
+      </c>
+      <c r="I342" s="1" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="343" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A343" s="1" t="s">
+        <v>755</v>
+      </c>
+      <c r="B343" s="0" t="s">
+        <v>765</v>
+      </c>
+      <c r="C343" s="1" t="n">
+        <v>3603</v>
+      </c>
+      <c r="D343" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E343" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="F343" s="3" t="s">
+        <v>763</v>
+      </c>
+      <c r="G343" s="1" t="s">
+        <v>766</v>
+      </c>
+      <c r="I343" s="1" t="s">
+        <v>275</v>
       </c>
     </row>
   </sheetData>
@@ -13230,13 +13376,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="24" t="s">
-        <v>755</v>
+        <v>767</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>756</v>
+        <v>768</v>
       </c>
       <c r="C1" s="24" t="s">
-        <v>757</v>
+        <v>769</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13247,7 +13393,7 @@
         <v>257</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>758</v>
+        <v>770</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13258,7 +13404,7 @@
         <v>256</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>759</v>
+        <v>771</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13269,7 +13415,7 @@
         <v>258</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>760</v>
+        <v>772</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13280,7 +13426,7 @@
         <v>260</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>761</v>
+        <v>773</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13291,7 +13437,7 @@
         <v>261</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>762</v>
+        <v>774</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13302,7 +13448,7 @@
         <v>0</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>763</v>
+        <v>775</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13313,7 +13459,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>764</v>
+        <v>776</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13324,7 +13470,7 @@
         <v>2</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>765</v>
+        <v>777</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13335,7 +13481,7 @@
         <v>3</v>
       </c>
       <c r="C10" s="22" t="s">
-        <v>766</v>
+        <v>778</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13346,7 +13492,7 @@
         <v>4</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>767</v>
+        <v>779</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13357,7 +13503,7 @@
         <v>5</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>768</v>
+        <v>780</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13368,7 +13514,7 @@
         <v>6</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>769</v>
+        <v>781</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13379,7 +13525,7 @@
         <v>7</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>770</v>
+        <v>782</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13390,7 +13536,7 @@
         <v>8</v>
       </c>
       <c r="C15" s="22" t="s">
-        <v>771</v>
+        <v>783</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13401,7 +13547,7 @@
         <v>9</v>
       </c>
       <c r="C16" s="22" t="s">
-        <v>772</v>
+        <v>784</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13412,7 +13558,7 @@
         <v>10</v>
       </c>
       <c r="C17" s="22" t="s">
-        <v>773</v>
+        <v>785</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13423,7 +13569,7 @@
         <v>11</v>
       </c>
       <c r="C18" s="22" t="s">
-        <v>774</v>
+        <v>786</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13434,7 +13580,7 @@
         <v>12</v>
       </c>
       <c r="C19" s="22" t="s">
-        <v>775</v>
+        <v>787</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13445,7 +13591,7 @@
         <v>20</v>
       </c>
       <c r="C20" s="22" t="s">
-        <v>776</v>
+        <v>788</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13456,7 +13602,7 @@
         <v>21</v>
       </c>
       <c r="C21" s="22" t="s">
-        <v>777</v>
+        <v>789</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13467,7 +13613,7 @@
         <v>22</v>
       </c>
       <c r="C22" s="22" t="s">
-        <v>778</v>
+        <v>790</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13478,7 +13624,7 @@
         <v>23</v>
       </c>
       <c r="C23" s="22" t="s">
-        <v>779</v>
+        <v>791</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13489,7 +13635,7 @@
         <v>24</v>
       </c>
       <c r="C24" s="22" t="s">
-        <v>780</v>
+        <v>792</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13500,7 +13646,7 @@
         <v>25</v>
       </c>
       <c r="C25" s="22" t="s">
-        <v>781</v>
+        <v>793</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13511,7 +13657,7 @@
         <v>26</v>
       </c>
       <c r="C26" s="22" t="s">
-        <v>782</v>
+        <v>794</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13522,7 +13668,7 @@
         <v>27</v>
       </c>
       <c r="C27" s="22" t="s">
-        <v>783</v>
+        <v>795</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13533,7 +13679,7 @@
         <v>28</v>
       </c>
       <c r="C28" s="22" t="s">
-        <v>784</v>
+        <v>796</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13544,7 +13690,7 @@
         <v>29</v>
       </c>
       <c r="C29" s="22" t="s">
-        <v>785</v>
+        <v>797</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13555,7 +13701,7 @@
         <v>30</v>
       </c>
       <c r="C30" s="22" t="s">
-        <v>786</v>
+        <v>798</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13566,7 +13712,7 @@
         <v>31</v>
       </c>
       <c r="C31" s="22" t="s">
-        <v>787</v>
+        <v>799</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13577,7 +13723,7 @@
         <v>32</v>
       </c>
       <c r="C32" s="22" t="s">
-        <v>788</v>
+        <v>800</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13588,7 +13734,7 @@
         <v>33</v>
       </c>
       <c r="C33" s="22" t="s">
-        <v>789</v>
+        <v>801</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13599,7 +13745,7 @@
         <v>34</v>
       </c>
       <c r="C34" s="22" t="s">
-        <v>790</v>
+        <v>802</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13610,7 +13756,7 @@
         <v>40</v>
       </c>
       <c r="C35" s="22" t="s">
-        <v>791</v>
+        <v>803</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13621,7 +13767,7 @@
         <v>41</v>
       </c>
       <c r="C36" s="22" t="s">
-        <v>792</v>
+        <v>804</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13632,7 +13778,7 @@
         <v>42</v>
       </c>
       <c r="C37" s="22" t="s">
-        <v>793</v>
+        <v>805</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13643,7 +13789,7 @@
         <v>43</v>
       </c>
       <c r="C38" s="22" t="s">
-        <v>794</v>
+        <v>806</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13654,7 +13800,7 @@
         <v>44</v>
       </c>
       <c r="C39" s="22" t="s">
-        <v>795</v>
+        <v>807</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13665,7 +13811,7 @@
         <v>45</v>
       </c>
       <c r="C40" s="22" t="s">
-        <v>796</v>
+        <v>808</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13676,7 +13822,7 @@
         <v>46</v>
       </c>
       <c r="C41" s="22" t="s">
-        <v>797</v>
+        <v>809</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13687,7 +13833,7 @@
         <v>288</v>
       </c>
       <c r="C42" s="22" t="s">
-        <v>798</v>
+        <v>810</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13698,7 +13844,7 @@
         <v>289</v>
       </c>
       <c r="C43" s="22" t="s">
-        <v>799</v>
+        <v>811</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13709,7 +13855,7 @@
         <v>290</v>
       </c>
       <c r="C44" s="22" t="s">
-        <v>800</v>
+        <v>812</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13720,7 +13866,7 @@
         <v>291</v>
       </c>
       <c r="C45" s="22" t="s">
-        <v>801</v>
+        <v>813</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13731,7 +13877,7 @@
         <v>292</v>
       </c>
       <c r="C46" s="22" t="s">
-        <v>802</v>
+        <v>814</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13742,7 +13888,7 @@
         <v>293</v>
       </c>
       <c r="C47" s="22" t="s">
-        <v>803</v>
+        <v>815</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13753,12 +13899,12 @@
         <v>512</v>
       </c>
       <c r="C48" s="22" t="s">
-        <v>804</v>
+        <v>816</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="26" t="s">
-        <v>805</v>
+        <v>817</v>
       </c>
       <c r="B50" s="26"/>
       <c r="C50" s="26"/>
@@ -13768,7 +13914,7 @@
     </row>
     <row r="51" customFormat="false" ht="92.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="27" t="s">
-        <v>806</v>
+        <v>818</v>
       </c>
       <c r="B51" s="27"/>
       <c r="C51" s="27"/>
@@ -13796,9 +13942,9 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C61"/>
+  <dimension ref="A1:C62"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -13812,370 +13958,378 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="22" t="s">
-        <v>807</v>
+        <v>819</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>808</v>
+        <v>820</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="22" t="s">
-        <v>809</v>
+        <v>821</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>810</v>
+        <v>822</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="22" t="s">
-        <v>811</v>
+        <v>823</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>812</v>
+        <v>824</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="22" t="s">
-        <v>813</v>
+        <v>825</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>814</v>
+        <v>826</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="22" t="s">
-        <v>815</v>
+        <v>827</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="22" t="s">
-        <v>816</v>
+        <v>828</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="22" t="s">
-        <v>817</v>
+        <v>829</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="22" t="s">
-        <v>818</v>
+        <v>830</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="22" t="s">
-        <v>819</v>
+        <v>831</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>820</v>
+        <v>832</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="22" t="s">
-        <v>821</v>
+        <v>833</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="22" t="s">
-        <v>822</v>
+        <v>834</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="22" t="s">
-        <v>823</v>
+        <v>835</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>824</v>
+        <v>836</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="22" t="s">
-        <v>825</v>
+        <v>837</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="22" t="s">
-        <v>826</v>
+        <v>838</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="22" t="s">
-        <v>827</v>
+        <v>839</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="22" t="s">
-        <v>828</v>
+        <v>840</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="22" t="s">
-        <v>829</v>
+        <v>841</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="22" t="s">
-        <v>830</v>
+        <v>842</v>
       </c>
       <c r="B18" s="22" t="s">
-        <v>831</v>
+        <v>843</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="22" t="s">
-        <v>832</v>
+        <v>844</v>
       </c>
       <c r="B19" s="22" t="s">
-        <v>833</v>
+        <v>845</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="22" t="s">
-        <v>834</v>
+        <v>846</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="22" t="s">
-        <v>835</v>
+        <v>847</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="22" t="s">
-        <v>836</v>
+        <v>848</v>
       </c>
       <c r="B22" s="22" t="s">
-        <v>837</v>
+        <v>849</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="22" t="s">
-        <v>838</v>
+        <v>850</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="22" t="s">
-        <v>839</v>
+        <v>851</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="22" t="s">
-        <v>840</v>
+        <v>852</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="22" t="s">
-        <v>841</v>
+        <v>853</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="22" t="s">
-        <v>842</v>
+        <v>854</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="22" t="s">
-        <v>843</v>
+        <v>855</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="22" t="s">
-        <v>844</v>
+        <v>856</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="22" t="s">
-        <v>845</v>
+        <v>857</v>
       </c>
       <c r="B30" s="22" t="s">
-        <v>846</v>
+        <v>858</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="22" t="s">
-        <v>847</v>
+        <v>859</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="22" t="s">
-        <v>848</v>
+        <v>860</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="22" t="s">
-        <v>849</v>
+        <v>861</v>
       </c>
       <c r="B33" s="22" t="s">
-        <v>850</v>
+        <v>862</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="22" t="s">
-        <v>851</v>
+        <v>863</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="22" t="s">
-        <v>852</v>
+        <v>864</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="22" t="s">
-        <v>853</v>
+        <v>865</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="22" t="s">
-        <v>854</v>
+        <v>866</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="22" t="s">
-        <v>855</v>
+        <v>867</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C39" s="28" t="s">
-        <v>856</v>
+        <v>868</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="22" t="s">
-        <v>857</v>
+        <v>869</v>
       </c>
       <c r="B40" s="22" t="s">
-        <v>858</v>
+        <v>870</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="22" t="s">
-        <v>859</v>
+        <v>871</v>
       </c>
       <c r="B41" s="22" t="s">
-        <v>860</v>
+        <v>872</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="22" t="s">
-        <v>861</v>
+        <v>873</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="22" t="s">
-        <v>862</v>
+        <v>874</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="22" t="s">
-        <v>863</v>
+        <v>875</v>
       </c>
       <c r="B44" s="22" t="s">
-        <v>864</v>
+        <v>876</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="22" t="s">
-        <v>865</v>
+        <v>877</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="22" t="s">
-        <v>866</v>
+        <v>878</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="22" t="s">
-        <v>867</v>
+        <v>879</v>
       </c>
       <c r="B47" s="22" t="s">
-        <v>868</v>
+        <v>880</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="22" t="s">
-        <v>869</v>
+        <v>881</v>
       </c>
       <c r="B48" s="22" t="s">
-        <v>870</v>
+        <v>882</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="22" t="s">
-        <v>871</v>
+        <v>883</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="22" t="s">
-        <v>872</v>
+        <v>884</v>
       </c>
       <c r="B50" s="22" t="s">
-        <v>873</v>
+        <v>885</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="22" t="s">
-        <v>874</v>
+        <v>886</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="22" t="s">
-        <v>875</v>
+        <v>887</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="22" t="s">
-        <v>876</v>
+        <v>888</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="22" t="s">
-        <v>877</v>
+        <v>889</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="22" t="s">
-        <v>878</v>
+        <v>890</v>
       </c>
       <c r="B55" s="22" t="s">
-        <v>879</v>
+        <v>891</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="22" t="s">
-        <v>880</v>
+        <v>892</v>
       </c>
       <c r="B56" s="22" t="s">
-        <v>881</v>
+        <v>893</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="22" t="s">
-        <v>882</v>
+        <v>894</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="22" t="s">
-        <v>883</v>
+        <v>895</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="22" t="s">
-        <v>884</v>
+        <v>896</v>
       </c>
       <c r="B59" s="22" t="s">
-        <v>885</v>
+        <v>897</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="22" t="s">
-        <v>886</v>
+        <v>898</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="22" t="s">
-        <v>887</v>
+        <v>899</v>
       </c>
       <c r="B61" s="22" t="s">
-        <v>888</v>
+        <v>900</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="22" t="s">
+        <v>901</v>
+      </c>
+      <c r="B62" s="22" t="s">
+        <v>902</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Move the 32-bit energy registers for PV-inverters
This was needed because it overlapped with the serial number.
</commit_message>
<xml_diff>
--- a/CCGX-Modbus-TCP-register-list.xlsx
+++ b/CCGX-Modbus-TCP-register-list.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2614" uniqueCount="903">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2616" uniqueCount="905">
   <si>
     <t xml:space="preserve">NOTE: Use unit-id 100 for the com.victronenergy.system data, for more information see FAQ.</t>
   </si>
@@ -1437,7 +1437,7 @@
     <t xml:space="preserve">/Ac/L1/Energy/Forward</t>
   </si>
   <si>
-    <t xml:space="preserve">Deprecated. Use 1040 instead.</t>
+    <t xml:space="preserve">Deprecated. Use 1046 instead.</t>
   </si>
   <si>
     <t xml:space="preserve">L2 Voltage</t>
@@ -1464,7 +1464,7 @@
     <t xml:space="preserve">/Ac/L2/Energy/Forward</t>
   </si>
   <si>
-    <t xml:space="preserve">Deprecated. Use 1042 instead.</t>
+    <t xml:space="preserve">Deprecated. Use 1048 instead.</t>
   </si>
   <si>
     <t xml:space="preserve">L3 Voltage</t>
@@ -1491,7 +1491,7 @@
     <t xml:space="preserve">/Ac/L3/Energy/Forward</t>
   </si>
   <si>
-    <t xml:space="preserve">Deprecated. Use 1044 instead.</t>
+    <t xml:space="preserve">Deprecated. Use 1050 instead.</t>
   </si>
   <si>
     <t xml:space="preserve">Serial</t>
@@ -2724,13 +2724,19 @@
     <t xml:space="preserve">Rev 20</t>
   </si>
   <si>
-    <t xml:space="preserve">Added 32-bit registers for PV-inverters</t>
+    <t xml:space="preserve">Added 32-bit energy registers for PV-inverters</t>
   </si>
   <si>
     <t xml:space="preserve">Rev 21</t>
   </si>
   <si>
     <t xml:space="preserve">Added registers for IMT solar irradiation sensors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rev 22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moved 32-bit energy registers added in Rev-20 because they overlapped with the serial number</t>
   </si>
 </sst>
 </file>
@@ -3084,9 +3090,9 @@
   <dimension ref="A1:N343"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="2" topLeftCell="A324" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="2" topLeftCell="A173" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A343" activeCellId="0" sqref="A343"/>
+      <selection pane="bottomLeft" activeCell="C200" activeCellId="0" sqref="C200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9131,7 +9137,7 @@
         <v>469</v>
       </c>
       <c r="C198" s="1" t="n">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="D198" s="2" t="s">
         <v>494</v>
@@ -9160,7 +9166,7 @@
         <v>478</v>
       </c>
       <c r="C199" s="1" t="n">
-        <v>1042</v>
+        <v>1048</v>
       </c>
       <c r="D199" s="2" t="s">
         <v>494</v>
@@ -9189,7 +9195,7 @@
         <v>487</v>
       </c>
       <c r="C200" s="1" t="n">
-        <v>1044</v>
+        <v>1050</v>
       </c>
       <c r="D200" s="2" t="s">
         <v>494</v>
@@ -13241,7 +13247,7 @@
       <c r="A340" s="1" t="s">
         <v>755</v>
       </c>
-      <c r="B340" s="0" t="s">
+      <c r="B340" s="22" t="s">
         <v>756</v>
       </c>
       <c r="C340" s="1" t="n">
@@ -13267,7 +13273,7 @@
       <c r="A341" s="1" t="s">
         <v>755</v>
       </c>
-      <c r="B341" s="0" t="s">
+      <c r="B341" s="22" t="s">
         <v>760</v>
       </c>
       <c r="C341" s="1" t="n">
@@ -13293,7 +13299,7 @@
       <c r="A342" s="1" t="s">
         <v>755</v>
       </c>
-      <c r="B342" s="0" t="s">
+      <c r="B342" s="22" t="s">
         <v>762</v>
       </c>
       <c r="C342" s="1" t="n">
@@ -13319,7 +13325,7 @@
       <c r="A343" s="1" t="s">
         <v>755</v>
       </c>
-      <c r="B343" s="0" t="s">
+      <c r="B343" s="22" t="s">
         <v>765</v>
       </c>
       <c r="C343" s="1" t="n">
@@ -13942,7 +13948,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C62"/>
+  <dimension ref="A1:C63"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -14332,6 +14338,14 @@
         <v>902</v>
       </c>
     </row>
+    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="22" t="s">
+        <v>903</v>
+      </c>
+      <c r="B63" s="22" t="s">
+        <v>904</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Map unitid 228 to 275, the nanopi VE.Bus port.
This is for EasySolar-II-GX and Multiplus-II-GX models.
</commit_message>
<xml_diff>
--- a/CCGX-Modbus-TCP-register-list.xlsx
+++ b/CCGX-Modbus-TCP-register-list.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Field list" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2625" uniqueCount="910">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2628" uniqueCount="913">
   <si>
     <t xml:space="preserve">NOTE: Use unit-id 100 for the com.victronenergy.system data, for more information see FAQ.</t>
   </si>
@@ -2358,6 +2358,9 @@
     <t xml:space="preserve">Venus GX VE.Bus port (ttyO5)</t>
   </si>
   <si>
+    <t xml:space="preserve">EasySolar-II/Multiplus-II GX VE.Bus port (ttyS3)</t>
+  </si>
+  <si>
     <t xml:space="preserve">VE.Can device instance 0 and all registers listed as com.victronenergy.system</t>
   </si>
   <si>
@@ -2752,6 +2755,12 @@
   </si>
   <si>
     <t xml:space="preserve">Added register for GridLost alarm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rev 24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Added mapping for EasySolar-II/Multiplus-II GX VE.Bus port</t>
   </si>
 </sst>
 </file>
@@ -3104,10 +3113,10 @@
   </sheetPr>
   <dimension ref="A1:N344"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="2" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A38" activeCellId="0" sqref="A38"/>
+      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13410,10 +13419,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F51"/>
+  <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A33" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C49" activeCellId="0" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13490,23 +13499,23 @@
         <v>777</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="22" t="n">
-        <v>100</v>
-      </c>
-      <c r="B7" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="C7" s="22" t="s">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="25" t="n">
+        <v>228</v>
+      </c>
+      <c r="B7" s="25" t="n">
+        <v>275</v>
+      </c>
+      <c r="C7" s="25" t="s">
         <v>778</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="22" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="B8" s="22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8" s="22" t="s">
         <v>779</v>
@@ -13514,10 +13523,10 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="22" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B9" s="22" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C9" s="22" t="s">
         <v>780</v>
@@ -13525,10 +13534,10 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="22" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B10" s="22" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C10" s="22" t="s">
         <v>781</v>
@@ -13536,10 +13545,10 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="22" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B11" s="22" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C11" s="22" t="s">
         <v>782</v>
@@ -13547,10 +13556,10 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="22" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B12" s="22" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C12" s="22" t="s">
         <v>783</v>
@@ -13558,10 +13567,10 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="22" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B13" s="22" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C13" s="22" t="s">
         <v>784</v>
@@ -13569,10 +13578,10 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="22" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B14" s="22" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C14" s="22" t="s">
         <v>785</v>
@@ -13580,10 +13589,10 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="22" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B15" s="22" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C15" s="22" t="s">
         <v>786</v>
@@ -13591,10 +13600,10 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="22" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B16" s="22" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C16" s="22" t="s">
         <v>787</v>
@@ -13602,10 +13611,10 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="22" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B17" s="22" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C17" s="22" t="s">
         <v>788</v>
@@ -13613,10 +13622,10 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="22" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B18" s="22" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C18" s="22" t="s">
         <v>789</v>
@@ -13624,10 +13633,10 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="22" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B19" s="22" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C19" s="22" t="s">
         <v>790</v>
@@ -13635,10 +13644,10 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="22" t="n">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B20" s="22" t="n">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C20" s="22" t="s">
         <v>791</v>
@@ -13646,10 +13655,10 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="22" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B21" s="22" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C21" s="22" t="s">
         <v>792</v>
@@ -13657,10 +13666,10 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="22" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B22" s="22" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C22" s="22" t="s">
         <v>793</v>
@@ -13668,10 +13677,10 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="22" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B23" s="22" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C23" s="22" t="s">
         <v>794</v>
@@ -13679,10 +13688,10 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="22" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B24" s="22" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C24" s="22" t="s">
         <v>795</v>
@@ -13690,10 +13699,10 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="22" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B25" s="22" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C25" s="22" t="s">
         <v>796</v>
@@ -13701,10 +13710,10 @@
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="22" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B26" s="22" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C26" s="22" t="s">
         <v>797</v>
@@ -13712,10 +13721,10 @@
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="22" t="n">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B27" s="22" t="n">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C27" s="22" t="s">
         <v>798</v>
@@ -13723,10 +13732,10 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="22" t="n">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B28" s="22" t="n">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C28" s="22" t="s">
         <v>799</v>
@@ -13734,10 +13743,10 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="22" t="n">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B29" s="22" t="n">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C29" s="22" t="s">
         <v>800</v>
@@ -13745,10 +13754,10 @@
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="22" t="n">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B30" s="22" t="n">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C30" s="22" t="s">
         <v>801</v>
@@ -13756,10 +13765,10 @@
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="22" t="n">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B31" s="22" t="n">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C31" s="22" t="s">
         <v>802</v>
@@ -13767,10 +13776,10 @@
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="22" t="n">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B32" s="22" t="n">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C32" s="22" t="s">
         <v>803</v>
@@ -13778,10 +13787,10 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="22" t="n">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B33" s="22" t="n">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C33" s="22" t="s">
         <v>804</v>
@@ -13789,10 +13798,10 @@
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="22" t="n">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B34" s="22" t="n">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C34" s="22" t="s">
         <v>805</v>
@@ -13800,10 +13809,10 @@
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="22" t="n">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B35" s="22" t="n">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C35" s="22" t="s">
         <v>806</v>
@@ -13811,10 +13820,10 @@
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="22" t="n">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B36" s="22" t="n">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C36" s="22" t="s">
         <v>807</v>
@@ -13822,10 +13831,10 @@
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="22" t="n">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B37" s="22" t="n">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C37" s="22" t="s">
         <v>808</v>
@@ -13833,10 +13842,10 @@
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="22" t="n">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B38" s="22" t="n">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C38" s="22" t="s">
         <v>809</v>
@@ -13844,10 +13853,10 @@
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="22" t="n">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B39" s="22" t="n">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C39" s="22" t="s">
         <v>810</v>
@@ -13855,10 +13864,10 @@
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="22" t="n">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B40" s="22" t="n">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C40" s="22" t="s">
         <v>811</v>
@@ -13866,10 +13875,10 @@
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="22" t="n">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B41" s="22" t="n">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C41" s="22" t="s">
         <v>812</v>
@@ -13877,10 +13886,10 @@
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="22" t="n">
-        <v>239</v>
+        <v>46</v>
       </c>
       <c r="B42" s="22" t="n">
-        <v>288</v>
+        <v>46</v>
       </c>
       <c r="C42" s="22" t="s">
         <v>813</v>
@@ -13888,10 +13897,10 @@
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="22" t="n">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B43" s="22" t="n">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C43" s="22" t="s">
         <v>814</v>
@@ -13899,10 +13908,10 @@
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="22" t="n">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B44" s="22" t="n">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C44" s="22" t="s">
         <v>815</v>
@@ -13910,10 +13919,10 @@
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="22" t="n">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B45" s="22" t="n">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C45" s="22" t="s">
         <v>816</v>
@@ -13921,10 +13930,10 @@
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="22" t="n">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B46" s="22" t="n">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C46" s="22" t="s">
         <v>817</v>
@@ -13932,10 +13941,10 @@
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="22" t="n">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="B47" s="22" t="n">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C47" s="22" t="s">
         <v>818</v>
@@ -13943,39 +13952,50 @@
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="22" t="n">
-        <v>225</v>
+        <v>233</v>
       </c>
       <c r="B48" s="22" t="n">
-        <v>512</v>
+        <v>293</v>
       </c>
       <c r="C48" s="22" t="s">
         <v>819</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="26" t="s">
+    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="22" t="n">
+        <v>225</v>
+      </c>
+      <c r="B49" s="22" t="n">
+        <v>512</v>
+      </c>
+      <c r="C49" s="22" t="s">
         <v>820</v>
       </c>
-      <c r="B50" s="26"/>
-      <c r="C50" s="26"/>
-      <c r="D50" s="26"/>
-      <c r="E50" s="26"/>
-      <c r="F50" s="26"/>
-    </row>
-    <row r="51" customFormat="false" ht="92.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="27" t="s">
+    </row>
+    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="26" t="s">
         <v>821</v>
       </c>
-      <c r="B51" s="27"/>
-      <c r="C51" s="27"/>
-      <c r="D51" s="27"/>
-      <c r="E51" s="27"/>
-      <c r="F51" s="27"/>
+      <c r="B51" s="26"/>
+      <c r="C51" s="26"/>
+      <c r="D51" s="26"/>
+      <c r="E51" s="26"/>
+      <c r="F51" s="26"/>
+    </row>
+    <row r="52" customFormat="false" ht="92.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A52" s="27" t="s">
+        <v>822</v>
+      </c>
+      <c r="B52" s="27"/>
+      <c r="C52" s="27"/>
+      <c r="D52" s="27"/>
+      <c r="E52" s="27"/>
+      <c r="F52" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A50:F50"/>
     <mergeCell ref="A51:F51"/>
+    <mergeCell ref="A52:F52"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -13992,10 +14012,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C64"/>
+  <dimension ref="A1:C65"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B65" activeCellId="0" sqref="B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14008,394 +14028,402 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="22" t="s">
-        <v>822</v>
+        <v>823</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>823</v>
+        <v>824</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="22" t="s">
-        <v>824</v>
+        <v>825</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>825</v>
+        <v>826</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="22" t="s">
-        <v>826</v>
+        <v>827</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>827</v>
+        <v>828</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="22" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="22" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="22" t="s">
-        <v>831</v>
+        <v>832</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="22" t="s">
-        <v>832</v>
+        <v>833</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="22" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="22" t="s">
-        <v>834</v>
+        <v>835</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>835</v>
+        <v>836</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="22" t="s">
-        <v>836</v>
+        <v>837</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="22" t="s">
-        <v>837</v>
+        <v>838</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="22" t="s">
-        <v>838</v>
+        <v>839</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>839</v>
+        <v>840</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="22" t="s">
-        <v>840</v>
+        <v>841</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="22" t="s">
-        <v>841</v>
+        <v>842</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="22" t="s">
-        <v>842</v>
+        <v>843</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="22" t="s">
-        <v>843</v>
+        <v>844</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="22" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="22" t="s">
-        <v>845</v>
+        <v>846</v>
       </c>
       <c r="B18" s="22" t="s">
-        <v>846</v>
+        <v>847</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="22" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="B19" s="22" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="22" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="22" t="s">
-        <v>850</v>
+        <v>851</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="22" t="s">
-        <v>851</v>
+        <v>852</v>
       </c>
       <c r="B22" s="22" t="s">
-        <v>852</v>
+        <v>853</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="22" t="s">
-        <v>853</v>
+        <v>854</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="22" t="s">
-        <v>854</v>
+        <v>855</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="22" t="s">
-        <v>855</v>
+        <v>856</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="22" t="s">
-        <v>856</v>
+        <v>857</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="22" t="s">
-        <v>857</v>
+        <v>858</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="22" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="22" t="s">
-        <v>859</v>
+        <v>860</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="22" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
       <c r="B30" s="22" t="s">
-        <v>861</v>
+        <v>862</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="22" t="s">
-        <v>862</v>
+        <v>863</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="22" t="s">
-        <v>863</v>
+        <v>864</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="22" t="s">
-        <v>864</v>
+        <v>865</v>
       </c>
       <c r="B33" s="22" t="s">
-        <v>865</v>
+        <v>866</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="22" t="s">
-        <v>866</v>
+        <v>867</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="22" t="s">
-        <v>867</v>
+        <v>868</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="22" t="s">
-        <v>868</v>
+        <v>869</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="22" t="s">
-        <v>869</v>
+        <v>870</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="22" t="s">
-        <v>870</v>
+        <v>871</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C39" s="28" t="s">
-        <v>871</v>
+        <v>872</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="22" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="B40" s="22" t="s">
-        <v>873</v>
+        <v>874</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="22" t="s">
-        <v>874</v>
+        <v>875</v>
       </c>
       <c r="B41" s="22" t="s">
-        <v>875</v>
+        <v>876</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="22" t="s">
-        <v>876</v>
+        <v>877</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="22" t="s">
-        <v>877</v>
+        <v>878</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="22" t="s">
-        <v>878</v>
+        <v>879</v>
       </c>
       <c r="B44" s="22" t="s">
-        <v>879</v>
+        <v>880</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="22" t="s">
-        <v>880</v>
+        <v>881</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="22" t="s">
-        <v>881</v>
+        <v>882</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="22" t="s">
-        <v>882</v>
+        <v>883</v>
       </c>
       <c r="B47" s="22" t="s">
-        <v>883</v>
+        <v>884</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="22" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="B48" s="22" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="22" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="22" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="B50" s="22" t="s">
-        <v>888</v>
+        <v>889</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="22" t="s">
-        <v>889</v>
+        <v>890</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="22" t="s">
-        <v>890</v>
+        <v>891</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="22" t="s">
-        <v>891</v>
+        <v>892</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="22" t="s">
-        <v>892</v>
+        <v>893</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="22" t="s">
-        <v>893</v>
+        <v>894</v>
       </c>
       <c r="B55" s="22" t="s">
-        <v>894</v>
+        <v>895</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="22" t="s">
-        <v>895</v>
+        <v>896</v>
       </c>
       <c r="B56" s="22" t="s">
-        <v>896</v>
+        <v>897</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="22" t="s">
-        <v>897</v>
+        <v>898</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="22" t="s">
-        <v>898</v>
+        <v>899</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="22" t="s">
-        <v>899</v>
+        <v>900</v>
       </c>
       <c r="B59" s="22" t="s">
-        <v>900</v>
+        <v>901</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="22" t="s">
-        <v>901</v>
+        <v>902</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="22" t="s">
-        <v>902</v>
+        <v>903</v>
       </c>
       <c r="B61" s="22" t="s">
-        <v>903</v>
+        <v>904</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="22" t="s">
-        <v>904</v>
+        <v>905</v>
       </c>
       <c r="B62" s="22" t="s">
-        <v>905</v>
+        <v>906</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="22" t="s">
-        <v>906</v>
+        <v>907</v>
       </c>
       <c r="B63" s="22" t="s">
-        <v>907</v>
+        <v>908</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="22" t="s">
-        <v>908</v>
+        <v>909</v>
       </c>
       <c r="B64" s="22" t="s">
-        <v>909</v>
+        <v>910</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="22" t="s">
+        <v>911</v>
+      </c>
+      <c r="B65" s="22" t="s">
+        <v>912</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add register for gps altitude
</commit_message>
<xml_diff>
--- a/CCGX-Modbus-TCP-register-list.xlsx
+++ b/CCGX-Modbus-TCP-register-list.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Field list" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2628" uniqueCount="913">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2637" uniqueCount="918">
   <si>
     <t xml:space="preserve">NOTE: Use unit-id 100 for the com.victronenergy.system data, for more information see FAQ.</t>
   </si>
@@ -1926,6 +1926,15 @@
     <t xml:space="preserve">/NrOfSatellites</t>
   </si>
   <si>
+    <t xml:space="preserve">Altitude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-214748364.8 to 214748364.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Altitude</t>
+  </si>
+  <si>
     <t xml:space="preserve">ESS BatteryLife state</t>
   </si>
   <si>
@@ -2761,6 +2770,12 @@
   </si>
   <si>
     <t xml:space="preserve">Added mapping for EasySolar-II/Multiplus-II GX VE.Bus port</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rev 25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Added GPS Altitude</t>
   </si>
 </sst>
 </file>
@@ -3111,9 +3126,9 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N344"/>
+  <dimension ref="A1:N345"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
@@ -11494,33 +11509,33 @@
         <v>17</v>
       </c>
     </row>
-    <row r="278" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="278" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A278" s="1" t="s">
-        <v>595</v>
+        <v>614</v>
       </c>
       <c r="B278" s="1" t="s">
         <v>634</v>
       </c>
       <c r="C278" s="1" t="n">
-        <v>2900</v>
+        <v>2808</v>
       </c>
       <c r="D278" s="2" t="s">
-        <v>20</v>
+        <v>391</v>
       </c>
       <c r="E278" s="1" t="n">
-        <v>1</v>
+        <v>10</v>
+      </c>
+      <c r="F278" s="3" t="s">
+        <v>635</v>
       </c>
       <c r="G278" s="1" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="H278" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="I278" s="1" t="s">
-        <v>636</v>
-      </c>
-      <c r="J278" s="1" t="s">
-        <v>637</v>
+        <v>627</v>
       </c>
     </row>
     <row r="279" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11528,48 +11543,45 @@
         <v>595</v>
       </c>
       <c r="B279" s="1" t="s">
+        <v>637</v>
+      </c>
+      <c r="C279" s="1" t="n">
+        <v>2900</v>
+      </c>
+      <c r="D279" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E279" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G279" s="1" t="s">
         <v>638</v>
-      </c>
-      <c r="C279" s="1" t="n">
-        <v>2901</v>
-      </c>
-      <c r="D279" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E279" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="G279" s="1" t="s">
-        <v>639</v>
       </c>
       <c r="H279" s="1" t="s">
         <v>23</v>
       </c>
       <c r="I279" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="J279" s="21" t="s">
+        <v>639</v>
+      </c>
+      <c r="J279" s="1" t="s">
         <v>640</v>
       </c>
     </row>
-    <row r="280" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A280" s="21" t="s">
+    <row r="280" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A280" s="1" t="s">
         <v>595</v>
       </c>
       <c r="B280" s="1" t="s">
         <v>641</v>
       </c>
       <c r="C280" s="1" t="n">
-        <v>2902</v>
+        <v>2901</v>
       </c>
       <c r="D280" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E280" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="F280" s="3" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="G280" s="1" t="s">
         <v>642</v>
@@ -11577,20 +11589,22 @@
       <c r="H280" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="I280" s="22" t="s">
+      <c r="I280" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="J280" s="21" t="s">
         <v>643</v>
       </c>
-      <c r="J280" s="21"/>
     </row>
     <row r="281" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A281" s="1" t="s">
+      <c r="A281" s="21" t="s">
+        <v>595</v>
+      </c>
+      <c r="B281" s="1" t="s">
         <v>644</v>
       </c>
-      <c r="B281" s="1" t="s">
-        <v>645</v>
-      </c>
       <c r="C281" s="1" t="n">
-        <v>3000</v>
+        <v>2902</v>
       </c>
       <c r="D281" s="2" t="s">
         <v>20</v>
@@ -11602,63 +11616,64 @@
         <v>29</v>
       </c>
       <c r="G281" s="1" t="s">
+        <v>645</v>
+      </c>
+      <c r="H281" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I281" s="22" t="s">
         <v>646</v>
       </c>
-      <c r="H281" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I281" s="23"/>
-    </row>
-    <row r="282" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J281" s="21"/>
+    </row>
+    <row r="282" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A282" s="1" t="s">
-        <v>644</v>
+        <v>647</v>
       </c>
       <c r="B282" s="1" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="C282" s="1" t="n">
-        <v>3001</v>
+        <v>3000</v>
       </c>
       <c r="D282" s="2" t="s">
-        <v>497</v>
+        <v>20</v>
       </c>
       <c r="E282" s="1" t="n">
-        <v>10000</v>
+        <v>1</v>
       </c>
       <c r="F282" s="3" t="s">
-        <v>648</v>
+        <v>29</v>
       </c>
       <c r="G282" s="1" t="s">
-        <v>389</v>
+        <v>649</v>
       </c>
       <c r="H282" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I282" s="1" t="s">
-        <v>649</v>
-      </c>
+      <c r="I282" s="23"/>
     </row>
     <row r="283" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A283" s="1" t="s">
-        <v>644</v>
+        <v>647</v>
       </c>
       <c r="B283" s="1" t="s">
         <v>650</v>
       </c>
       <c r="C283" s="1" t="n">
-        <v>3003</v>
+        <v>3001</v>
       </c>
       <c r="D283" s="2" t="s">
-        <v>20</v>
+        <v>497</v>
       </c>
       <c r="E283" s="1" t="n">
-        <v>1</v>
+        <v>10000</v>
       </c>
       <c r="F283" s="3" t="s">
-        <v>29</v>
+        <v>651</v>
       </c>
       <c r="G283" s="1" t="s">
-        <v>651</v>
+        <v>389</v>
       </c>
       <c r="H283" s="1" t="s">
         <v>17</v>
@@ -11669,22 +11684,22 @@
     </row>
     <row r="284" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A284" s="1" t="s">
-        <v>644</v>
+        <v>647</v>
       </c>
       <c r="B284" s="1" t="s">
         <v>653</v>
       </c>
       <c r="C284" s="1" t="n">
-        <v>3004</v>
+        <v>3003</v>
       </c>
       <c r="D284" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E284" s="1" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F284" s="3" t="s">
-        <v>79</v>
+        <v>29</v>
       </c>
       <c r="G284" s="1" t="s">
         <v>654</v>
@@ -11693,192 +11708,192 @@
         <v>17</v>
       </c>
       <c r="I284" s="1" t="s">
-        <v>93</v>
+        <v>655</v>
       </c>
     </row>
     <row r="285" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A285" s="1" t="s">
-        <v>644</v>
+        <v>647</v>
       </c>
       <c r="B285" s="1" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="C285" s="1" t="n">
-        <v>3005</v>
+        <v>3004</v>
       </c>
       <c r="D285" s="2" t="s">
-        <v>497</v>
+        <v>20</v>
       </c>
       <c r="E285" s="1" t="n">
-        <v>10000</v>
+        <v>10</v>
       </c>
       <c r="F285" s="3" t="s">
-        <v>648</v>
+        <v>79</v>
       </c>
       <c r="G285" s="1" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="H285" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I285" s="1" t="s">
-        <v>649</v>
+        <v>93</v>
       </c>
     </row>
     <row r="286" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A286" s="1" t="s">
-        <v>644</v>
+        <v>647</v>
       </c>
       <c r="B286" s="1" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="C286" s="1" t="n">
-        <v>3007</v>
+        <v>3005</v>
       </c>
       <c r="D286" s="2" t="s">
-        <v>20</v>
+        <v>497</v>
       </c>
       <c r="E286" s="1" t="n">
-        <v>1</v>
+        <v>10000</v>
       </c>
       <c r="F286" s="3" t="s">
-        <v>29</v>
+        <v>651</v>
       </c>
       <c r="G286" s="1" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="H286" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I286" s="1" t="s">
-        <v>659</v>
+        <v>652</v>
       </c>
     </row>
     <row r="287" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A287" s="1" t="s">
+        <v>647</v>
+      </c>
+      <c r="B287" s="1" t="s">
         <v>660</v>
       </c>
-      <c r="B287" s="1" t="s">
+      <c r="C287" s="1" t="n">
+        <v>3007</v>
+      </c>
+      <c r="D287" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E287" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F287" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G287" s="1" t="s">
         <v>661</v>
       </c>
-      <c r="C287" s="1" t="n">
-        <v>3100</v>
-      </c>
-      <c r="D287" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E287" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="F287" s="3" t="s">
+      <c r="H287" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I287" s="1" t="s">
         <v>662</v>
-      </c>
-      <c r="G287" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="H287" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I287" s="1" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="288" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A288" s="1" t="s">
-        <v>660</v>
+        <v>663</v>
       </c>
       <c r="B288" s="1" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
       <c r="C288" s="1" t="n">
-        <v>3101</v>
+        <v>3100</v>
       </c>
       <c r="D288" s="2" t="s">
-        <v>20</v>
+        <v>59</v>
       </c>
       <c r="E288" s="1" t="n">
         <v>10</v>
       </c>
       <c r="F288" s="3" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="G288" s="1" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="H288" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I288" s="1" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
     </row>
     <row r="289" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A289" s="1" t="s">
-        <v>660</v>
+        <v>663</v>
       </c>
       <c r="B289" s="1" t="s">
-        <v>187</v>
+        <v>666</v>
       </c>
       <c r="C289" s="1" t="n">
-        <v>3105</v>
+        <v>3101</v>
       </c>
       <c r="D289" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E289" s="1" t="n">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="F289" s="3" t="s">
-        <v>665</v>
+        <v>667</v>
       </c>
       <c r="G289" s="1" t="s">
-        <v>189</v>
+        <v>162</v>
       </c>
       <c r="H289" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I289" s="1" t="s">
-        <v>81</v>
+        <v>130</v>
       </c>
     </row>
     <row r="290" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A290" s="1" t="s">
-        <v>660</v>
+        <v>663</v>
       </c>
       <c r="B290" s="1" t="s">
-        <v>314</v>
+        <v>187</v>
       </c>
       <c r="C290" s="1" t="n">
-        <v>3110</v>
+        <v>3105</v>
       </c>
       <c r="D290" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E290" s="1" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="F290" s="3" t="s">
-        <v>666</v>
+        <v>668</v>
       </c>
       <c r="G290" s="1" t="s">
-        <v>211</v>
+        <v>189</v>
       </c>
       <c r="H290" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I290" s="1" t="s">
-        <v>667</v>
+        <v>81</v>
       </c>
     </row>
     <row r="291" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A291" s="1" t="s">
-        <v>660</v>
+        <v>663</v>
       </c>
       <c r="B291" s="1" t="s">
-        <v>668</v>
+        <v>314</v>
       </c>
       <c r="C291" s="1" t="n">
-        <v>3111</v>
+        <v>3110</v>
       </c>
       <c r="D291" s="2" t="s">
         <v>20</v>
@@ -11887,56 +11902,56 @@
         <v>1</v>
       </c>
       <c r="F291" s="3" t="s">
-        <v>666</v>
+        <v>669</v>
       </c>
       <c r="G291" s="1" t="s">
-        <v>305</v>
+        <v>211</v>
       </c>
       <c r="H291" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I291" s="1" t="s">
-        <v>667</v>
+        <v>670</v>
       </c>
     </row>
     <row r="292" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A292" s="1" t="s">
-        <v>660</v>
+        <v>663</v>
       </c>
       <c r="B292" s="1" t="s">
+        <v>671</v>
+      </c>
+      <c r="C292" s="1" t="n">
+        <v>3111</v>
+      </c>
+      <c r="D292" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E292" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F292" s="3" t="s">
         <v>669</v>
       </c>
-      <c r="C292" s="1" t="n">
-        <v>3112</v>
-      </c>
-      <c r="D292" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E292" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="F292" s="3" t="s">
-        <v>666</v>
-      </c>
       <c r="G292" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="H292" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I292" s="1" t="s">
         <v>670</v>
-      </c>
-      <c r="H292" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I292" s="1" t="s">
-        <v>667</v>
       </c>
     </row>
     <row r="293" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A293" s="1" t="s">
-        <v>660</v>
+        <v>663</v>
       </c>
       <c r="B293" s="1" t="s">
-        <v>312</v>
+        <v>672</v>
       </c>
       <c r="C293" s="1" t="n">
-        <v>3113</v>
+        <v>3112</v>
       </c>
       <c r="D293" s="2" t="s">
         <v>20</v>
@@ -11945,27 +11960,27 @@
         <v>1</v>
       </c>
       <c r="F293" s="3" t="s">
-        <v>666</v>
+        <v>669</v>
       </c>
       <c r="G293" s="1" t="s">
-        <v>313</v>
+        <v>673</v>
       </c>
       <c r="H293" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I293" s="1" t="s">
-        <v>667</v>
+        <v>670</v>
       </c>
     </row>
     <row r="294" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A294" s="1" t="s">
-        <v>660</v>
+        <v>663</v>
       </c>
       <c r="B294" s="1" t="s">
-        <v>671</v>
+        <v>312</v>
       </c>
       <c r="C294" s="1" t="n">
-        <v>3114</v>
+        <v>3113</v>
       </c>
       <c r="D294" s="2" t="s">
         <v>20</v>
@@ -11974,27 +11989,27 @@
         <v>1</v>
       </c>
       <c r="F294" s="3" t="s">
-        <v>666</v>
+        <v>669</v>
       </c>
       <c r="G294" s="1" t="s">
-        <v>303</v>
+        <v>313</v>
       </c>
       <c r="H294" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I294" s="1" t="s">
-        <v>667</v>
+        <v>670</v>
       </c>
     </row>
     <row r="295" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A295" s="1" t="s">
-        <v>660</v>
+        <v>663</v>
       </c>
       <c r="B295" s="1" t="s">
-        <v>672</v>
+        <v>674</v>
       </c>
       <c r="C295" s="1" t="n">
-        <v>3115</v>
+        <v>3114</v>
       </c>
       <c r="D295" s="2" t="s">
         <v>20</v>
@@ -12003,27 +12018,27 @@
         <v>1</v>
       </c>
       <c r="F295" s="3" t="s">
-        <v>666</v>
+        <v>669</v>
       </c>
       <c r="G295" s="1" t="s">
-        <v>673</v>
+        <v>303</v>
       </c>
       <c r="H295" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I295" s="1" t="s">
-        <v>667</v>
+        <v>670</v>
       </c>
     </row>
     <row r="296" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A296" s="1" t="s">
-        <v>660</v>
+        <v>663</v>
       </c>
       <c r="B296" s="1" t="s">
-        <v>215</v>
+        <v>675</v>
       </c>
       <c r="C296" s="1" t="n">
-        <v>3116</v>
+        <v>3115</v>
       </c>
       <c r="D296" s="2" t="s">
         <v>20</v>
@@ -12032,27 +12047,27 @@
         <v>1</v>
       </c>
       <c r="F296" s="3" t="s">
-        <v>666</v>
+        <v>669</v>
       </c>
       <c r="G296" s="1" t="s">
-        <v>216</v>
+        <v>676</v>
       </c>
       <c r="H296" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I296" s="1" t="s">
-        <v>667</v>
+        <v>670</v>
       </c>
     </row>
     <row r="297" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A297" s="1" t="s">
-        <v>660</v>
+        <v>663</v>
       </c>
       <c r="B297" s="1" t="s">
-        <v>674</v>
+        <v>215</v>
       </c>
       <c r="C297" s="1" t="n">
-        <v>3117</v>
+        <v>3116</v>
       </c>
       <c r="D297" s="2" t="s">
         <v>20</v>
@@ -12061,27 +12076,27 @@
         <v>1</v>
       </c>
       <c r="F297" s="3" t="s">
-        <v>666</v>
+        <v>669</v>
       </c>
       <c r="G297" s="1" t="s">
-        <v>675</v>
+        <v>216</v>
       </c>
       <c r="H297" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I297" s="1" t="s">
-        <v>667</v>
+        <v>670</v>
       </c>
     </row>
     <row r="298" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A298" s="1" t="s">
-        <v>660</v>
+        <v>663</v>
       </c>
       <c r="B298" s="1" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
       <c r="C298" s="1" t="n">
-        <v>3125</v>
+        <v>3117</v>
       </c>
       <c r="D298" s="2" t="s">
         <v>20</v>
@@ -12090,24 +12105,27 @@
         <v>1</v>
       </c>
       <c r="F298" s="3" t="s">
-        <v>666</v>
+        <v>669</v>
       </c>
       <c r="G298" s="1" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="H298" s="1" t="s">
         <v>17</v>
+      </c>
+      <c r="I298" s="1" t="s">
+        <v>670</v>
       </c>
     </row>
     <row r="299" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A299" s="1" t="s">
-        <v>660</v>
+        <v>663</v>
       </c>
       <c r="B299" s="1" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c r="C299" s="1" t="n">
-        <v>3126</v>
+        <v>3125</v>
       </c>
       <c r="D299" s="2" t="s">
         <v>20</v>
@@ -12116,27 +12134,24 @@
         <v>1</v>
       </c>
       <c r="F299" s="3" t="s">
-        <v>666</v>
+        <v>669</v>
       </c>
       <c r="G299" s="1" t="s">
-        <v>208</v>
+        <v>680</v>
       </c>
       <c r="H299" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I299" s="1" t="s">
-        <v>679</v>
+        <v>17</v>
       </c>
     </row>
     <row r="300" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A300" s="1" t="s">
-        <v>660</v>
+        <v>663</v>
       </c>
       <c r="B300" s="1" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="C300" s="1" t="n">
-        <v>3127</v>
+        <v>3126</v>
       </c>
       <c r="D300" s="2" t="s">
         <v>20</v>
@@ -12145,24 +12160,27 @@
         <v>1</v>
       </c>
       <c r="F300" s="3" t="s">
-        <v>666</v>
+        <v>669</v>
       </c>
       <c r="G300" s="1" t="s">
-        <v>646</v>
+        <v>208</v>
       </c>
       <c r="H300" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
+      </c>
+      <c r="I300" s="1" t="s">
+        <v>682</v>
       </c>
     </row>
     <row r="301" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A301" s="1" t="s">
-        <v>660</v>
+        <v>663</v>
       </c>
       <c r="B301" s="1" t="s">
-        <v>681</v>
+        <v>683</v>
       </c>
       <c r="C301" s="1" t="n">
-        <v>3128</v>
+        <v>3127</v>
       </c>
       <c r="D301" s="2" t="s">
         <v>20</v>
@@ -12171,56 +12189,53 @@
         <v>1</v>
       </c>
       <c r="F301" s="3" t="s">
-        <v>666</v>
+        <v>669</v>
       </c>
       <c r="G301" s="1" t="s">
-        <v>202</v>
+        <v>649</v>
       </c>
       <c r="H301" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="I301" s="1" t="s">
-        <v>682</v>
       </c>
     </row>
     <row r="302" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A302" s="1" t="s">
-        <v>683</v>
+        <v>663</v>
       </c>
       <c r="B302" s="1" t="s">
         <v>684</v>
       </c>
       <c r="C302" s="1" t="n">
-        <v>3200</v>
+        <v>3128</v>
       </c>
       <c r="D302" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E302" s="1" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F302" s="3" t="s">
-        <v>664</v>
+        <v>669</v>
       </c>
       <c r="G302" s="1" t="s">
-        <v>467</v>
+        <v>202</v>
       </c>
       <c r="H302" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I302" s="1" t="s">
-        <v>130</v>
+        <v>685</v>
       </c>
     </row>
     <row r="303" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A303" s="1" t="s">
-        <v>683</v>
+        <v>686</v>
       </c>
       <c r="B303" s="1" t="s">
-        <v>685</v>
+        <v>687</v>
       </c>
       <c r="C303" s="1" t="n">
-        <v>3201</v>
+        <v>3200</v>
       </c>
       <c r="D303" s="2" t="s">
         <v>20</v>
@@ -12229,10 +12244,10 @@
         <v>10</v>
       </c>
       <c r="F303" s="3" t="s">
-        <v>664</v>
+        <v>667</v>
       </c>
       <c r="G303" s="1" t="s">
-        <v>476</v>
+        <v>467</v>
       </c>
       <c r="H303" s="1" t="s">
         <v>17</v>
@@ -12243,13 +12258,13 @@
     </row>
     <row r="304" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A304" s="1" t="s">
-        <v>683</v>
+        <v>686</v>
       </c>
       <c r="B304" s="1" t="s">
-        <v>686</v>
+        <v>688</v>
       </c>
       <c r="C304" s="1" t="n">
-        <v>3202</v>
+        <v>3201</v>
       </c>
       <c r="D304" s="2" t="s">
         <v>20</v>
@@ -12258,10 +12273,10 @@
         <v>10</v>
       </c>
       <c r="F304" s="3" t="s">
-        <v>664</v>
+        <v>667</v>
       </c>
       <c r="G304" s="1" t="s">
-        <v>485</v>
+        <v>476</v>
       </c>
       <c r="H304" s="1" t="s">
         <v>17</v>
@@ -12272,42 +12287,42 @@
     </row>
     <row r="305" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A305" s="1" t="s">
-        <v>683</v>
+        <v>686</v>
       </c>
       <c r="B305" s="1" t="s">
-        <v>687</v>
+        <v>689</v>
       </c>
       <c r="C305" s="1" t="n">
-        <v>3203</v>
+        <v>3202</v>
       </c>
       <c r="D305" s="2" t="s">
-        <v>59</v>
+        <v>20</v>
       </c>
       <c r="E305" s="1" t="n">
         <v>10</v>
       </c>
       <c r="F305" s="3" t="s">
-        <v>662</v>
+        <v>667</v>
       </c>
       <c r="G305" s="1" t="s">
-        <v>469</v>
+        <v>485</v>
       </c>
       <c r="H305" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I305" s="1" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
     </row>
     <row r="306" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A306" s="1" t="s">
-        <v>683</v>
+        <v>686</v>
       </c>
       <c r="B306" s="1" t="s">
-        <v>688</v>
+        <v>690</v>
       </c>
       <c r="C306" s="1" t="n">
-        <v>3204</v>
+        <v>3203</v>
       </c>
       <c r="D306" s="2" t="s">
         <v>59</v>
@@ -12316,10 +12331,10 @@
         <v>10</v>
       </c>
       <c r="F306" s="3" t="s">
-        <v>662</v>
+        <v>665</v>
       </c>
       <c r="G306" s="1" t="s">
-        <v>478</v>
+        <v>469</v>
       </c>
       <c r="H306" s="1" t="s">
         <v>17</v>
@@ -12330,13 +12345,13 @@
     </row>
     <row r="307" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A307" s="1" t="s">
-        <v>683</v>
+        <v>686</v>
       </c>
       <c r="B307" s="1" t="s">
-        <v>689</v>
+        <v>691</v>
       </c>
       <c r="C307" s="1" t="n">
-        <v>3205</v>
+        <v>3204</v>
       </c>
       <c r="D307" s="2" t="s">
         <v>59</v>
@@ -12345,10 +12360,10 @@
         <v>10</v>
       </c>
       <c r="F307" s="3" t="s">
-        <v>662</v>
+        <v>665</v>
       </c>
       <c r="G307" s="1" t="s">
-        <v>487</v>
+        <v>478</v>
       </c>
       <c r="H307" s="1" t="s">
         <v>17</v>
@@ -12359,42 +12374,42 @@
     </row>
     <row r="308" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A308" s="1" t="s">
-        <v>683</v>
+        <v>686</v>
       </c>
       <c r="B308" s="1" t="s">
-        <v>690</v>
+        <v>692</v>
       </c>
       <c r="C308" s="1" t="n">
-        <v>3206</v>
+        <v>3205</v>
       </c>
       <c r="D308" s="2" t="s">
         <v>59</v>
       </c>
       <c r="E308" s="1" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F308" s="3" t="s">
-        <v>691</v>
+        <v>665</v>
       </c>
       <c r="G308" s="1" t="s">
-        <v>471</v>
+        <v>487</v>
       </c>
       <c r="H308" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I308" s="1" t="s">
-        <v>31</v>
+        <v>137</v>
       </c>
     </row>
     <row r="309" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A309" s="1" t="s">
-        <v>683</v>
+        <v>686</v>
       </c>
       <c r="B309" s="1" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
       <c r="C309" s="1" t="n">
-        <v>3207</v>
+        <v>3206</v>
       </c>
       <c r="D309" s="2" t="s">
         <v>59</v>
@@ -12403,10 +12418,10 @@
         <v>1</v>
       </c>
       <c r="F309" s="3" t="s">
-        <v>691</v>
+        <v>694</v>
       </c>
       <c r="G309" s="1" t="s">
-        <v>480</v>
+        <v>471</v>
       </c>
       <c r="H309" s="1" t="s">
         <v>17</v>
@@ -12417,13 +12432,13 @@
     </row>
     <row r="310" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A310" s="1" t="s">
-        <v>683</v>
+        <v>686</v>
       </c>
       <c r="B310" s="1" t="s">
-        <v>693</v>
+        <v>695</v>
       </c>
       <c r="C310" s="1" t="n">
-        <v>3208</v>
+        <v>3207</v>
       </c>
       <c r="D310" s="2" t="s">
         <v>59</v>
@@ -12432,10 +12447,10 @@
         <v>1</v>
       </c>
       <c r="F310" s="3" t="s">
-        <v>691</v>
+        <v>694</v>
       </c>
       <c r="G310" s="1" t="s">
-        <v>489</v>
+        <v>480</v>
       </c>
       <c r="H310" s="1" t="s">
         <v>17</v>
@@ -12446,42 +12461,42 @@
     </row>
     <row r="311" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A311" s="1" t="s">
-        <v>683</v>
+        <v>686</v>
       </c>
       <c r="B311" s="1" t="s">
+        <v>696</v>
+      </c>
+      <c r="C311" s="1" t="n">
+        <v>3208</v>
+      </c>
+      <c r="D311" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E311" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F311" s="3" t="s">
         <v>694</v>
       </c>
-      <c r="C311" s="1" t="n">
-        <v>3209</v>
-      </c>
-      <c r="D311" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E311" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="F311" s="3" t="s">
-        <v>665</v>
-      </c>
       <c r="G311" s="1" t="s">
-        <v>695</v>
+        <v>489</v>
       </c>
       <c r="H311" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I311" s="1" t="s">
-        <v>146</v>
+        <v>31</v>
       </c>
     </row>
     <row r="312" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A312" s="1" t="s">
-        <v>683</v>
+        <v>686</v>
       </c>
       <c r="B312" s="1" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
       <c r="C312" s="1" t="n">
-        <v>3210</v>
+        <v>3209</v>
       </c>
       <c r="D312" s="2" t="s">
         <v>20</v>
@@ -12490,10 +12505,10 @@
         <v>100</v>
       </c>
       <c r="F312" s="3" t="s">
-        <v>665</v>
+        <v>668</v>
       </c>
       <c r="G312" s="1" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
       <c r="H312" s="1" t="s">
         <v>17</v>
@@ -12504,13 +12519,13 @@
     </row>
     <row r="313" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A313" s="1" t="s">
-        <v>683</v>
+        <v>686</v>
       </c>
       <c r="B313" s="1" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
       <c r="C313" s="1" t="n">
-        <v>3211</v>
+        <v>3210</v>
       </c>
       <c r="D313" s="2" t="s">
         <v>20</v>
@@ -12519,10 +12534,10 @@
         <v>100</v>
       </c>
       <c r="F313" s="3" t="s">
-        <v>665</v>
+        <v>668</v>
       </c>
       <c r="G313" s="1" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
       <c r="H313" s="1" t="s">
         <v>17</v>
@@ -12533,39 +12548,42 @@
     </row>
     <row r="314" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A314" s="1" t="s">
-        <v>683</v>
+        <v>686</v>
       </c>
       <c r="B314" s="1" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
       <c r="C314" s="1" t="n">
-        <v>3212</v>
+        <v>3211</v>
       </c>
       <c r="D314" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E314" s="1" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="F314" s="3" t="s">
-        <v>666</v>
+        <v>668</v>
       </c>
       <c r="G314" s="1" t="s">
-        <v>646</v>
+        <v>702</v>
       </c>
       <c r="H314" s="1" t="s">
         <v>17</v>
+      </c>
+      <c r="I314" s="1" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="315" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A315" s="1" t="s">
-        <v>683</v>
+        <v>686</v>
       </c>
       <c r="B315" s="1" t="s">
-        <v>701</v>
+        <v>703</v>
       </c>
       <c r="C315" s="1" t="n">
-        <v>3213</v>
+        <v>3212</v>
       </c>
       <c r="D315" s="2" t="s">
         <v>20</v>
@@ -12574,27 +12592,24 @@
         <v>1</v>
       </c>
       <c r="F315" s="3" t="s">
-        <v>666</v>
+        <v>669</v>
       </c>
       <c r="G315" s="1" t="s">
-        <v>702</v>
+        <v>649</v>
       </c>
       <c r="H315" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="I315" s="1" t="s">
-        <v>703</v>
       </c>
     </row>
     <row r="316" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A316" s="1" t="s">
-        <v>683</v>
+        <v>686</v>
       </c>
       <c r="B316" s="1" t="s">
-        <v>501</v>
+        <v>704</v>
       </c>
       <c r="C316" s="1" t="n">
-        <v>3214</v>
+        <v>3213</v>
       </c>
       <c r="D316" s="2" t="s">
         <v>20</v>
@@ -12603,27 +12618,27 @@
         <v>1</v>
       </c>
       <c r="F316" s="3" t="s">
-        <v>666</v>
+        <v>669</v>
       </c>
       <c r="G316" s="1" t="s">
-        <v>452</v>
+        <v>705</v>
       </c>
       <c r="H316" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I316" s="1" t="s">
-        <v>704</v>
+        <v>706</v>
       </c>
     </row>
     <row r="317" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A317" s="1" t="s">
-        <v>683</v>
+        <v>686</v>
       </c>
       <c r="B317" s="1" t="s">
-        <v>705</v>
+        <v>501</v>
       </c>
       <c r="C317" s="1" t="n">
-        <v>3215</v>
+        <v>3214</v>
       </c>
       <c r="D317" s="2" t="s">
         <v>20</v>
@@ -12632,27 +12647,27 @@
         <v>1</v>
       </c>
       <c r="F317" s="3" t="s">
-        <v>666</v>
+        <v>669</v>
       </c>
       <c r="G317" s="1" t="s">
-        <v>706</v>
+        <v>452</v>
       </c>
       <c r="H317" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I317" s="1" t="s">
-        <v>505</v>
+        <v>707</v>
       </c>
     </row>
     <row r="318" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A318" s="1" t="s">
-        <v>683</v>
+        <v>686</v>
       </c>
       <c r="B318" s="1" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="C318" s="1" t="n">
-        <v>3216</v>
+        <v>3215</v>
       </c>
       <c r="D318" s="2" t="s">
         <v>20</v>
@@ -12661,27 +12676,27 @@
         <v>1</v>
       </c>
       <c r="F318" s="3" t="s">
-        <v>666</v>
+        <v>669</v>
       </c>
       <c r="G318" s="1" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="H318" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I318" s="1" t="s">
-        <v>93</v>
+        <v>505</v>
       </c>
     </row>
     <row r="319" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A319" s="1" t="s">
-        <v>683</v>
+        <v>686</v>
       </c>
       <c r="B319" s="1" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
       <c r="C319" s="1" t="n">
-        <v>3217</v>
+        <v>3216</v>
       </c>
       <c r="D319" s="2" t="s">
         <v>20</v>
@@ -12690,36 +12705,36 @@
         <v>1</v>
       </c>
       <c r="F319" s="3" t="s">
-        <v>666</v>
+        <v>669</v>
       </c>
       <c r="G319" s="1" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
       <c r="H319" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I319" s="1" t="s">
-        <v>544</v>
+        <v>93</v>
       </c>
     </row>
     <row r="320" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A320" s="1" t="s">
-        <v>683</v>
+        <v>686</v>
       </c>
       <c r="B320" s="1" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
       <c r="C320" s="1" t="n">
-        <v>3218</v>
+        <v>3217</v>
       </c>
       <c r="D320" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E320" s="1" t="n">
-        <v>0.01</v>
+        <v>1</v>
       </c>
       <c r="F320" s="3" t="s">
-        <v>712</v>
+        <v>669</v>
       </c>
       <c r="G320" s="1" t="s">
         <v>713</v>
@@ -12728,47 +12743,47 @@
         <v>17</v>
       </c>
       <c r="I320" s="1" t="s">
-        <v>105</v>
+        <v>544</v>
       </c>
     </row>
     <row r="321" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A321" s="1" t="s">
-        <v>683</v>
+        <v>686</v>
       </c>
       <c r="B321" s="1" t="s">
         <v>714</v>
       </c>
       <c r="C321" s="1" t="n">
-        <v>3219</v>
+        <v>3218</v>
       </c>
       <c r="D321" s="2" t="s">
-        <v>59</v>
+        <v>20</v>
       </c>
       <c r="E321" s="1" t="n">
-        <v>10</v>
+        <v>0.01</v>
       </c>
       <c r="F321" s="3" t="s">
-        <v>662</v>
+        <v>715</v>
       </c>
       <c r="G321" s="1" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="H321" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I321" s="1" t="s">
-        <v>278</v>
+        <v>105</v>
       </c>
     </row>
     <row r="322" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A322" s="1" t="s">
-        <v>683</v>
+        <v>686</v>
       </c>
       <c r="B322" s="1" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
       <c r="C322" s="1" t="n">
-        <v>3220</v>
+        <v>3219</v>
       </c>
       <c r="D322" s="2" t="s">
         <v>59</v>
@@ -12777,10 +12792,10 @@
         <v>10</v>
       </c>
       <c r="F322" s="3" t="s">
-        <v>662</v>
+        <v>665</v>
       </c>
       <c r="G322" s="1" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="H322" s="1" t="s">
         <v>17</v>
@@ -12791,13 +12806,13 @@
     </row>
     <row r="323" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A323" s="1" t="s">
-        <v>683</v>
+        <v>686</v>
       </c>
       <c r="B323" s="1" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="C323" s="1" t="n">
-        <v>3221</v>
+        <v>3220</v>
       </c>
       <c r="D323" s="2" t="s">
         <v>59</v>
@@ -12806,10 +12821,10 @@
         <v>10</v>
       </c>
       <c r="F323" s="3" t="s">
-        <v>662</v>
+        <v>665</v>
       </c>
       <c r="G323" s="1" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="H323" s="1" t="s">
         <v>17</v>
@@ -12820,71 +12835,71 @@
     </row>
     <row r="324" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A324" s="1" t="s">
-        <v>683</v>
+        <v>686</v>
       </c>
       <c r="B324" s="1" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c r="C324" s="1" t="n">
-        <v>3222</v>
+        <v>3221</v>
       </c>
       <c r="D324" s="2" t="s">
-        <v>20</v>
+        <v>59</v>
       </c>
       <c r="E324" s="1" t="n">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="F324" s="3" t="s">
         <v>665</v>
       </c>
       <c r="G324" s="1" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
       <c r="H324" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I324" s="1" t="s">
-        <v>81</v>
+        <v>278</v>
       </c>
     </row>
     <row r="325" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A325" s="1" t="s">
-        <v>683</v>
+        <v>686</v>
       </c>
       <c r="B325" s="1" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="C325" s="1" t="n">
-        <v>3223</v>
+        <v>3222</v>
       </c>
       <c r="D325" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E325" s="1" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="F325" s="3" t="s">
-        <v>666</v>
+        <v>668</v>
       </c>
       <c r="G325" s="1" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="H325" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="I325" s="1" t="s">
-        <v>724</v>
+        <v>81</v>
       </c>
     </row>
     <row r="326" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A326" s="1" t="s">
+        <v>686</v>
+      </c>
+      <c r="B326" s="1" t="s">
         <v>725</v>
       </c>
-      <c r="B326" s="1" t="s">
-        <v>645</v>
-      </c>
       <c r="C326" s="1" t="n">
-        <v>3300</v>
+        <v>3223</v>
       </c>
       <c r="D326" s="2" t="s">
         <v>20</v>
@@ -12893,36 +12908,39 @@
         <v>1</v>
       </c>
       <c r="F326" s="3" t="s">
-        <v>29</v>
+        <v>669</v>
       </c>
       <c r="G326" s="1" t="s">
-        <v>646</v>
+        <v>726</v>
       </c>
       <c r="H326" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
+      </c>
+      <c r="I326" s="1" t="s">
+        <v>727</v>
       </c>
     </row>
     <row r="327" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A327" s="1" t="s">
-        <v>725</v>
+        <v>728</v>
       </c>
       <c r="B327" s="1" t="s">
-        <v>726</v>
+        <v>648</v>
       </c>
       <c r="C327" s="1" t="n">
-        <v>3301</v>
+        <v>3300</v>
       </c>
       <c r="D327" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E327" s="1" t="n">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="F327" s="3" t="s">
-        <v>188</v>
+        <v>29</v>
       </c>
       <c r="G327" s="1" t="s">
-        <v>727</v>
+        <v>649</v>
       </c>
       <c r="H327" s="1" t="s">
         <v>17</v>
@@ -12930,25 +12948,25 @@
     </row>
     <row r="328" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A328" s="1" t="s">
-        <v>725</v>
+        <v>728</v>
       </c>
       <c r="B328" s="1" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="C328" s="1" t="n">
-        <v>3302</v>
+        <v>3301</v>
       </c>
       <c r="D328" s="2" t="s">
-        <v>59</v>
+        <v>20</v>
       </c>
       <c r="E328" s="1" t="n">
         <v>100</v>
       </c>
       <c r="F328" s="3" t="s">
-        <v>144</v>
+        <v>188</v>
       </c>
       <c r="G328" s="1" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="H328" s="1" t="s">
         <v>17</v>
@@ -12956,51 +12974,48 @@
     </row>
     <row r="329" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A329" s="1" t="s">
-        <v>725</v>
+        <v>728</v>
       </c>
       <c r="B329" s="1" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="C329" s="1" t="n">
-        <v>3303</v>
+        <v>3302</v>
       </c>
       <c r="D329" s="2" t="s">
-        <v>20</v>
+        <v>59</v>
       </c>
       <c r="E329" s="1" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="F329" s="3" t="s">
-        <v>29</v>
+        <v>144</v>
       </c>
       <c r="G329" s="1" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="H329" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="I329" s="1" t="s">
-        <v>732</v>
       </c>
     </row>
     <row r="330" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A330" s="1" t="s">
-        <v>725</v>
+        <v>728</v>
       </c>
       <c r="B330" s="1" t="s">
         <v>733</v>
       </c>
       <c r="C330" s="1" t="n">
-        <v>3304</v>
+        <v>3303</v>
       </c>
       <c r="D330" s="2" t="s">
-        <v>59</v>
+        <v>20</v>
       </c>
       <c r="E330" s="1" t="n">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="F330" s="3" t="s">
-        <v>144</v>
+        <v>29</v>
       </c>
       <c r="G330" s="1" t="s">
         <v>734</v>
@@ -13009,76 +13024,76 @@
         <v>17</v>
       </c>
       <c r="I330" s="1" t="s">
-        <v>278</v>
+        <v>735</v>
       </c>
     </row>
     <row r="331" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A331" s="1" t="s">
-        <v>725</v>
+        <v>728</v>
       </c>
       <c r="B331" s="1" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
       <c r="C331" s="1" t="n">
-        <v>3305</v>
+        <v>3304</v>
       </c>
       <c r="D331" s="2" t="s">
-        <v>20</v>
+        <v>59</v>
       </c>
       <c r="E331" s="1" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="F331" s="3" t="s">
-        <v>29</v>
+        <v>144</v>
       </c>
       <c r="G331" s="1" t="s">
-        <v>658</v>
+        <v>737</v>
       </c>
       <c r="H331" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I331" s="1" t="s">
-        <v>659</v>
+        <v>278</v>
       </c>
     </row>
     <row r="332" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A332" s="1" t="s">
-        <v>736</v>
+        <v>728</v>
       </c>
       <c r="B332" s="1" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
       <c r="C332" s="1" t="n">
-        <v>3400</v>
+        <v>3305</v>
       </c>
       <c r="D332" s="2" t="s">
-        <v>497</v>
+        <v>20</v>
       </c>
       <c r="E332" s="1" t="n">
         <v>1</v>
       </c>
       <c r="F332" s="3" t="s">
-        <v>738</v>
+        <v>29</v>
       </c>
       <c r="G332" s="1" t="s">
-        <v>739</v>
+        <v>661</v>
       </c>
       <c r="H332" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I332" s="1" t="s">
-        <v>649</v>
+        <v>662</v>
       </c>
     </row>
     <row r="333" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A333" s="1" t="s">
-        <v>736</v>
+        <v>739</v>
       </c>
       <c r="B333" s="1" t="s">
         <v>740</v>
       </c>
       <c r="C333" s="1" t="n">
-        <v>3402</v>
+        <v>3400</v>
       </c>
       <c r="D333" s="2" t="s">
         <v>497</v>
@@ -13087,24 +13102,27 @@
         <v>1</v>
       </c>
       <c r="F333" s="3" t="s">
-        <v>738</v>
+        <v>741</v>
       </c>
       <c r="G333" s="1" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
       <c r="H333" s="1" t="s">
         <v>17</v>
+      </c>
+      <c r="I333" s="1" t="s">
+        <v>652</v>
       </c>
     </row>
     <row r="334" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A334" s="1" t="s">
-        <v>742</v>
+        <v>739</v>
       </c>
       <c r="B334" s="1" t="s">
         <v>743</v>
       </c>
       <c r="C334" s="1" t="n">
-        <v>3420</v>
+        <v>3402</v>
       </c>
       <c r="D334" s="2" t="s">
         <v>497</v>
@@ -13113,10 +13131,10 @@
         <v>1</v>
       </c>
       <c r="F334" s="3" t="s">
-        <v>738</v>
+        <v>741</v>
       </c>
       <c r="G334" s="1" t="s">
-        <v>741</v>
+        <v>744</v>
       </c>
       <c r="H334" s="1" t="s">
         <v>17</v>
@@ -13124,42 +13142,39 @@
     </row>
     <row r="335" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A335" s="1" t="s">
-        <v>742</v>
+        <v>745</v>
       </c>
       <c r="B335" s="1" t="s">
-        <v>499</v>
+        <v>746</v>
       </c>
       <c r="C335" s="1" t="n">
-        <v>3422</v>
+        <v>3420</v>
       </c>
       <c r="D335" s="2" t="s">
-        <v>20</v>
+        <v>497</v>
       </c>
       <c r="E335" s="1" t="n">
         <v>1</v>
       </c>
       <c r="F335" s="3" t="s">
-        <v>21</v>
+        <v>741</v>
       </c>
       <c r="G335" s="1" t="s">
-        <v>202</v>
+        <v>744</v>
       </c>
       <c r="H335" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="I335" s="1" t="s">
-        <v>744</v>
       </c>
     </row>
     <row r="336" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A336" s="1" t="s">
-        <v>742</v>
+        <v>745</v>
       </c>
       <c r="B336" s="1" t="s">
-        <v>298</v>
+        <v>499</v>
       </c>
       <c r="C336" s="1" t="n">
-        <v>3423</v>
+        <v>3422</v>
       </c>
       <c r="D336" s="2" t="s">
         <v>20</v>
@@ -13168,85 +13183,85 @@
         <v>1</v>
       </c>
       <c r="F336" s="3" t="s">
-        <v>745</v>
+        <v>21</v>
       </c>
       <c r="G336" s="1" t="s">
-        <v>746</v>
+        <v>202</v>
       </c>
       <c r="H336" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I336" s="1" t="s">
-        <v>300</v>
+        <v>747</v>
       </c>
     </row>
     <row r="337" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A337" s="1" t="s">
-        <v>742</v>
+        <v>745</v>
       </c>
       <c r="B337" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="C337" s="1" t="n">
+        <v>3423</v>
+      </c>
+      <c r="D337" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E337" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F337" s="3" t="s">
+        <v>748</v>
+      </c>
+      <c r="G337" s="1" t="s">
+        <v>749</v>
+      </c>
+      <c r="H337" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I337" s="1" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="338" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A338" s="1" t="s">
+        <v>745</v>
+      </c>
+      <c r="B338" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C337" s="1" t="n">
+      <c r="C338" s="1" t="n">
         <v>3424</v>
       </c>
-      <c r="D337" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E337" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="F337" s="3" t="s">
-        <v>747</v>
-      </c>
-      <c r="G337" s="1" t="s">
-        <v>748</v>
-      </c>
-      <c r="H337" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I337" s="1" t="s">
-        <v>749</v>
-      </c>
-    </row>
-    <row r="338" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A338" s="1" t="s">
+      <c r="D338" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E338" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F338" s="3" t="s">
         <v>750</v>
       </c>
-      <c r="B338" s="1" t="s">
+      <c r="G338" s="1" t="s">
         <v>751</v>
       </c>
-      <c r="C338" s="1" t="n">
-        <v>3500</v>
-      </c>
-      <c r="D338" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E338" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="F338" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G338" s="1" t="s">
+      <c r="H338" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I338" s="1" t="s">
         <v>752</v>
-      </c>
-      <c r="H338" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I338" s="1" t="s">
-        <v>753</v>
       </c>
     </row>
     <row r="339" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A339" s="1" t="s">
-        <v>750</v>
+        <v>753</v>
       </c>
       <c r="B339" s="1" t="s">
         <v>754</v>
       </c>
       <c r="C339" s="1" t="n">
-        <v>3501</v>
+        <v>3500</v>
       </c>
       <c r="D339" s="2" t="s">
         <v>20</v>
@@ -13255,13 +13270,13 @@
         <v>1</v>
       </c>
       <c r="F339" s="3" t="s">
-        <v>747</v>
+        <v>21</v>
       </c>
       <c r="G339" s="1" t="s">
         <v>755</v>
       </c>
       <c r="H339" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="I339" s="1" t="s">
         <v>756</v>
@@ -13269,13 +13284,13 @@
     </row>
     <row r="340" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A340" s="1" t="s">
-        <v>750</v>
+        <v>753</v>
       </c>
       <c r="B340" s="1" t="s">
         <v>757</v>
       </c>
       <c r="C340" s="1" t="n">
-        <v>3502</v>
+        <v>3501</v>
       </c>
       <c r="D340" s="2" t="s">
         <v>20</v>
@@ -13284,53 +13299,56 @@
         <v>1</v>
       </c>
       <c r="F340" s="3" t="s">
-        <v>747</v>
+        <v>750</v>
       </c>
       <c r="G340" s="1" t="s">
-        <v>752</v>
+        <v>758</v>
       </c>
       <c r="H340" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I340" s="1" t="s">
-        <v>346</v>
+        <v>759</v>
       </c>
     </row>
     <row r="341" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A341" s="1" t="s">
-        <v>758</v>
-      </c>
-      <c r="B341" s="22" t="s">
-        <v>759</v>
+        <v>753</v>
+      </c>
+      <c r="B341" s="1" t="s">
+        <v>760</v>
       </c>
       <c r="C341" s="1" t="n">
-        <v>3600</v>
+        <v>3502</v>
       </c>
       <c r="D341" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E341" s="1" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F341" s="3" t="s">
-        <v>760</v>
+        <v>750</v>
       </c>
       <c r="G341" s="1" t="s">
-        <v>761</v>
+        <v>755</v>
+      </c>
+      <c r="H341" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="I341" s="1" t="s">
-        <v>762</v>
+        <v>346</v>
       </c>
     </row>
     <row r="342" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A342" s="1" t="s">
-        <v>758</v>
+        <v>761</v>
       </c>
       <c r="B342" s="22" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="C342" s="1" t="n">
-        <v>3601</v>
+        <v>3600</v>
       </c>
       <c r="D342" s="2" t="s">
         <v>20</v>
@@ -13339,50 +13357,50 @@
         <v>10</v>
       </c>
       <c r="F342" s="3" t="s">
-        <v>760</v>
+        <v>763</v>
       </c>
       <c r="G342" s="1" t="s">
         <v>764</v>
       </c>
       <c r="I342" s="1" t="s">
-        <v>627</v>
+        <v>765</v>
       </c>
     </row>
     <row r="343" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A343" s="1" t="s">
-        <v>758</v>
+        <v>761</v>
       </c>
       <c r="B343" s="22" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="C343" s="1" t="n">
-        <v>3602</v>
+        <v>3601</v>
       </c>
       <c r="D343" s="2" t="s">
-        <v>59</v>
+        <v>20</v>
       </c>
       <c r="E343" s="1" t="n">
         <v>10</v>
       </c>
       <c r="F343" s="3" t="s">
-        <v>766</v>
+        <v>763</v>
       </c>
       <c r="G343" s="1" t="s">
         <v>767</v>
       </c>
       <c r="I343" s="1" t="s">
-        <v>278</v>
+        <v>627</v>
       </c>
     </row>
     <row r="344" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A344" s="1" t="s">
-        <v>758</v>
+        <v>761</v>
       </c>
       <c r="B344" s="22" t="s">
         <v>768</v>
       </c>
       <c r="C344" s="1" t="n">
-        <v>3603</v>
+        <v>3602</v>
       </c>
       <c r="D344" s="2" t="s">
         <v>59</v>
@@ -13391,12 +13409,38 @@
         <v>10</v>
       </c>
       <c r="F344" s="3" t="s">
-        <v>766</v>
+        <v>769</v>
       </c>
       <c r="G344" s="1" t="s">
+        <v>770</v>
+      </c>
+      <c r="I344" s="1" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="345" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A345" s="1" t="s">
+        <v>761</v>
+      </c>
+      <c r="B345" s="22" t="s">
+        <v>771</v>
+      </c>
+      <c r="C345" s="1" t="n">
+        <v>3603</v>
+      </c>
+      <c r="D345" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E345" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="F345" s="3" t="s">
         <v>769</v>
       </c>
-      <c r="I344" s="1" t="s">
+      <c r="G345" s="1" t="s">
+        <v>772</v>
+      </c>
+      <c r="I345" s="1" t="s">
         <v>278</v>
       </c>
     </row>
@@ -13435,13 +13479,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="24" t="s">
-        <v>770</v>
+        <v>773</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>771</v>
+        <v>774</v>
       </c>
       <c r="C1" s="24" t="s">
-        <v>772</v>
+        <v>775</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13452,7 +13496,7 @@
         <v>257</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>773</v>
+        <v>776</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13463,7 +13507,7 @@
         <v>256</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>774</v>
+        <v>777</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13474,7 +13518,7 @@
         <v>258</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>775</v>
+        <v>778</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13485,7 +13529,7 @@
         <v>260</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>776</v>
+        <v>779</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13496,7 +13540,7 @@
         <v>261</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>777</v>
+        <v>780</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13507,7 +13551,7 @@
         <v>275</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>778</v>
+        <v>781</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13518,7 +13562,7 @@
         <v>0</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>779</v>
+        <v>782</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13529,7 +13573,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>780</v>
+        <v>783</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13540,7 +13584,7 @@
         <v>2</v>
       </c>
       <c r="C10" s="22" t="s">
-        <v>781</v>
+        <v>784</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13551,7 +13595,7 @@
         <v>3</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>782</v>
+        <v>785</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13562,7 +13606,7 @@
         <v>4</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>783</v>
+        <v>786</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13573,7 +13617,7 @@
         <v>5</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>784</v>
+        <v>787</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13584,7 +13628,7 @@
         <v>6</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>785</v>
+        <v>788</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13595,7 +13639,7 @@
         <v>7</v>
       </c>
       <c r="C15" s="22" t="s">
-        <v>786</v>
+        <v>789</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13606,7 +13650,7 @@
         <v>8</v>
       </c>
       <c r="C16" s="22" t="s">
-        <v>787</v>
+        <v>790</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13617,7 +13661,7 @@
         <v>9</v>
       </c>
       <c r="C17" s="22" t="s">
-        <v>788</v>
+        <v>791</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13628,7 +13672,7 @@
         <v>10</v>
       </c>
       <c r="C18" s="22" t="s">
-        <v>789</v>
+        <v>792</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13639,7 +13683,7 @@
         <v>11</v>
       </c>
       <c r="C19" s="22" t="s">
-        <v>790</v>
+        <v>793</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13650,7 +13694,7 @@
         <v>12</v>
       </c>
       <c r="C20" s="22" t="s">
-        <v>791</v>
+        <v>794</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13661,7 +13705,7 @@
         <v>20</v>
       </c>
       <c r="C21" s="22" t="s">
-        <v>792</v>
+        <v>795</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13672,7 +13716,7 @@
         <v>21</v>
       </c>
       <c r="C22" s="22" t="s">
-        <v>793</v>
+        <v>796</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13683,7 +13727,7 @@
         <v>22</v>
       </c>
       <c r="C23" s="22" t="s">
-        <v>794</v>
+        <v>797</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13694,7 +13738,7 @@
         <v>23</v>
       </c>
       <c r="C24" s="22" t="s">
-        <v>795</v>
+        <v>798</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13705,7 +13749,7 @@
         <v>24</v>
       </c>
       <c r="C25" s="22" t="s">
-        <v>796</v>
+        <v>799</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13716,7 +13760,7 @@
         <v>25</v>
       </c>
       <c r="C26" s="22" t="s">
-        <v>797</v>
+        <v>800</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13727,7 +13771,7 @@
         <v>26</v>
       </c>
       <c r="C27" s="22" t="s">
-        <v>798</v>
+        <v>801</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13738,7 +13782,7 @@
         <v>27</v>
       </c>
       <c r="C28" s="22" t="s">
-        <v>799</v>
+        <v>802</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13749,7 +13793,7 @@
         <v>28</v>
       </c>
       <c r="C29" s="22" t="s">
-        <v>800</v>
+        <v>803</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13760,7 +13804,7 @@
         <v>29</v>
       </c>
       <c r="C30" s="22" t="s">
-        <v>801</v>
+        <v>804</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13771,7 +13815,7 @@
         <v>30</v>
       </c>
       <c r="C31" s="22" t="s">
-        <v>802</v>
+        <v>805</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13782,7 +13826,7 @@
         <v>31</v>
       </c>
       <c r="C32" s="22" t="s">
-        <v>803</v>
+        <v>806</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13793,7 +13837,7 @@
         <v>32</v>
       </c>
       <c r="C33" s="22" t="s">
-        <v>804</v>
+        <v>807</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13804,7 +13848,7 @@
         <v>33</v>
       </c>
       <c r="C34" s="22" t="s">
-        <v>805</v>
+        <v>808</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13815,7 +13859,7 @@
         <v>34</v>
       </c>
       <c r="C35" s="22" t="s">
-        <v>806</v>
+        <v>809</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13826,7 +13870,7 @@
         <v>40</v>
       </c>
       <c r="C36" s="22" t="s">
-        <v>807</v>
+        <v>810</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13837,7 +13881,7 @@
         <v>41</v>
       </c>
       <c r="C37" s="22" t="s">
-        <v>808</v>
+        <v>811</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13848,7 +13892,7 @@
         <v>42</v>
       </c>
       <c r="C38" s="22" t="s">
-        <v>809</v>
+        <v>812</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13859,7 +13903,7 @@
         <v>43</v>
       </c>
       <c r="C39" s="22" t="s">
-        <v>810</v>
+        <v>813</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13870,7 +13914,7 @@
         <v>44</v>
       </c>
       <c r="C40" s="22" t="s">
-        <v>811</v>
+        <v>814</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13881,7 +13925,7 @@
         <v>45</v>
       </c>
       <c r="C41" s="22" t="s">
-        <v>812</v>
+        <v>815</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13892,7 +13936,7 @@
         <v>46</v>
       </c>
       <c r="C42" s="22" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13903,7 +13947,7 @@
         <v>288</v>
       </c>
       <c r="C43" s="22" t="s">
-        <v>814</v>
+        <v>817</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13914,7 +13958,7 @@
         <v>289</v>
       </c>
       <c r="C44" s="22" t="s">
-        <v>815</v>
+        <v>818</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13925,7 +13969,7 @@
         <v>290</v>
       </c>
       <c r="C45" s="22" t="s">
-        <v>816</v>
+        <v>819</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13936,7 +13980,7 @@
         <v>291</v>
       </c>
       <c r="C46" s="22" t="s">
-        <v>817</v>
+        <v>820</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13947,7 +13991,7 @@
         <v>292</v>
       </c>
       <c r="C47" s="22" t="s">
-        <v>818</v>
+        <v>821</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13958,7 +14002,7 @@
         <v>293</v>
       </c>
       <c r="C48" s="22" t="s">
-        <v>819</v>
+        <v>822</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13969,12 +14013,12 @@
         <v>512</v>
       </c>
       <c r="C49" s="22" t="s">
-        <v>820</v>
+        <v>823</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="26" t="s">
-        <v>821</v>
+        <v>824</v>
       </c>
       <c r="B51" s="26"/>
       <c r="C51" s="26"/>
@@ -13984,7 +14028,7 @@
     </row>
     <row r="52" customFormat="false" ht="92.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="27" t="s">
-        <v>822</v>
+        <v>825</v>
       </c>
       <c r="B52" s="27"/>
       <c r="C52" s="27"/>
@@ -14012,10 +14056,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C65"/>
+  <dimension ref="A1:C66"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B65" activeCellId="0" sqref="B65"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A50" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A66" activeCellId="0" sqref="A66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14028,402 +14072,410 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="22" t="s">
-        <v>823</v>
+        <v>826</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>824</v>
+        <v>827</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="22" t="s">
-        <v>825</v>
+        <v>828</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>826</v>
+        <v>829</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="22" t="s">
-        <v>827</v>
+        <v>830</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>828</v>
+        <v>831</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="22" t="s">
-        <v>829</v>
+        <v>832</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>830</v>
+        <v>833</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="22" t="s">
-        <v>831</v>
+        <v>834</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="22" t="s">
-        <v>832</v>
+        <v>835</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="22" t="s">
-        <v>833</v>
+        <v>836</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="22" t="s">
-        <v>834</v>
+        <v>837</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="22" t="s">
-        <v>835</v>
+        <v>838</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>836</v>
+        <v>839</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="22" t="s">
-        <v>837</v>
+        <v>840</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="22" t="s">
-        <v>838</v>
+        <v>841</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="22" t="s">
-        <v>839</v>
+        <v>842</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>840</v>
+        <v>843</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="22" t="s">
-        <v>841</v>
+        <v>844</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="22" t="s">
-        <v>842</v>
+        <v>845</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="22" t="s">
-        <v>843</v>
+        <v>846</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="22" t="s">
-        <v>844</v>
+        <v>847</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="22" t="s">
-        <v>845</v>
+        <v>848</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="22" t="s">
-        <v>846</v>
+        <v>849</v>
       </c>
       <c r="B18" s="22" t="s">
-        <v>847</v>
+        <v>850</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="22" t="s">
-        <v>848</v>
+        <v>851</v>
       </c>
       <c r="B19" s="22" t="s">
-        <v>849</v>
+        <v>852</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="22" t="s">
-        <v>850</v>
+        <v>853</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="22" t="s">
-        <v>851</v>
+        <v>854</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="22" t="s">
-        <v>852</v>
+        <v>855</v>
       </c>
       <c r="B22" s="22" t="s">
-        <v>853</v>
+        <v>856</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="22" t="s">
-        <v>854</v>
+        <v>857</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="22" t="s">
-        <v>855</v>
+        <v>858</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="22" t="s">
-        <v>856</v>
+        <v>859</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="22" t="s">
-        <v>857</v>
+        <v>860</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="22" t="s">
-        <v>858</v>
+        <v>861</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="22" t="s">
-        <v>859</v>
+        <v>862</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="22" t="s">
-        <v>860</v>
+        <v>863</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="22" t="s">
-        <v>861</v>
+        <v>864</v>
       </c>
       <c r="B30" s="22" t="s">
-        <v>862</v>
+        <v>865</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="22" t="s">
-        <v>863</v>
+        <v>866</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="22" t="s">
-        <v>864</v>
+        <v>867</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="22" t="s">
-        <v>865</v>
+        <v>868</v>
       </c>
       <c r="B33" s="22" t="s">
-        <v>866</v>
+        <v>869</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="22" t="s">
-        <v>867</v>
+        <v>870</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="22" t="s">
-        <v>868</v>
+        <v>871</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="22" t="s">
-        <v>869</v>
+        <v>872</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="22" t="s">
-        <v>870</v>
+        <v>873</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="22" t="s">
-        <v>871</v>
+        <v>874</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C39" s="28" t="s">
-        <v>872</v>
+        <v>875</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="22" t="s">
-        <v>873</v>
+        <v>876</v>
       </c>
       <c r="B40" s="22" t="s">
-        <v>874</v>
+        <v>877</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="22" t="s">
-        <v>875</v>
+        <v>878</v>
       </c>
       <c r="B41" s="22" t="s">
-        <v>876</v>
+        <v>879</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="22" t="s">
-        <v>877</v>
+        <v>880</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="22" t="s">
-        <v>878</v>
+        <v>881</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="22" t="s">
-        <v>879</v>
+        <v>882</v>
       </c>
       <c r="B44" s="22" t="s">
-        <v>880</v>
+        <v>883</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="22" t="s">
-        <v>881</v>
+        <v>884</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="22" t="s">
-        <v>882</v>
+        <v>885</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="22" t="s">
-        <v>883</v>
+        <v>886</v>
       </c>
       <c r="B47" s="22" t="s">
-        <v>884</v>
+        <v>887</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="22" t="s">
-        <v>885</v>
+        <v>888</v>
       </c>
       <c r="B48" s="22" t="s">
-        <v>886</v>
+        <v>889</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="22" t="s">
-        <v>887</v>
+        <v>890</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="22" t="s">
-        <v>888</v>
+        <v>891</v>
       </c>
       <c r="B50" s="22" t="s">
-        <v>889</v>
+        <v>892</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="22" t="s">
-        <v>890</v>
+        <v>893</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="22" t="s">
-        <v>891</v>
+        <v>894</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="22" t="s">
-        <v>892</v>
+        <v>895</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="22" t="s">
-        <v>893</v>
+        <v>896</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="22" t="s">
-        <v>894</v>
+        <v>897</v>
       </c>
       <c r="B55" s="22" t="s">
-        <v>895</v>
+        <v>898</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="22" t="s">
-        <v>896</v>
+        <v>899</v>
       </c>
       <c r="B56" s="22" t="s">
-        <v>897</v>
+        <v>900</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="22" t="s">
-        <v>898</v>
+        <v>901</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="22" t="s">
-        <v>899</v>
+        <v>902</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="22" t="s">
-        <v>900</v>
+        <v>903</v>
       </c>
       <c r="B59" s="22" t="s">
-        <v>901</v>
+        <v>904</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="22" t="s">
-        <v>902</v>
+        <v>905</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="22" t="s">
-        <v>903</v>
+        <v>906</v>
       </c>
       <c r="B61" s="22" t="s">
-        <v>904</v>
+        <v>907</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="22" t="s">
-        <v>905</v>
+        <v>908</v>
       </c>
       <c r="B62" s="22" t="s">
-        <v>906</v>
+        <v>909</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="22" t="s">
-        <v>907</v>
+        <v>910</v>
       </c>
       <c r="B63" s="22" t="s">
-        <v>908</v>
+        <v>911</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="22" t="s">
-        <v>909</v>
+        <v>912</v>
       </c>
       <c r="B64" s="22" t="s">
-        <v>910</v>
+        <v>913</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="22" t="s">
-        <v>911</v>
+        <v>914</v>
       </c>
       <c r="B65" s="22" t="s">
-        <v>912</v>
+        <v>915</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="22" t="s">
+        <v>916</v>
+      </c>
+      <c r="B66" s="22" t="s">
+        <v>917</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
corrected dbus path for generator manualstart
This does not affect operation. The attributes were correct. The Excel
sheet was not.

https://github.com/victronenergy/venus/issues/560
</commit_message>
<xml_diff>
--- a/CCGX-Modbus-TCP-register-list.xlsx
+++ b/CCGX-Modbus-TCP-register-list.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2637" uniqueCount="918">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2639" uniqueCount="921">
   <si>
     <t xml:space="preserve">NOTE: Use unit-id 100 for the com.victronenergy.system data, for more information see FAQ.</t>
   </si>
@@ -2289,24 +2289,27 @@
     <t xml:space="preserve">Manual Start</t>
   </si>
   <si>
+    <t xml:space="preserve">/Generator0/ManualStart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0=Stop generator; 1=Start generator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Condition that started the generator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Generator0/RunningByConditionCode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0=Stopped;1=Manual;2=TestRun;3=LossOfComms;4=Soc;5=AcLoad;6=BatteryCurrent;7=BatteryVoltage;8=InverterTemperatur;9=InverterOverload;10=StopOnAc1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Runtime in seconds</t>
+  </si>
+  <si>
     <t xml:space="preserve">/Generator0/Runtime</t>
   </si>
   <si>
-    <t xml:space="preserve">0=Stop generator; 1=Start generator</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Condition that started the generator</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/Generator0/RunningByConditionCode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0=Stopped;1=Manual;2=TestRun;3=LossOfComms;4=Soc;5=AcLoad;6=BatteryCurrent;7=BatteryVoltage;8=InverterTemperatur;9=InverterOverload;10=StopOnAc1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Runtime in seconds</t>
-  </si>
-  <si>
     <t xml:space="preserve">com.victronenergy.meteo</t>
   </si>
   <si>
@@ -2776,6 +2779,12 @@
   </si>
   <si>
     <t xml:space="preserve">Added GPS Altitude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rev 26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Corrected Dbus path for generator ManualStart</t>
   </si>
 </sst>
 </file>
@@ -3129,9 +3138,9 @@
   <dimension ref="A1:N345"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="2" topLeftCell="A321" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="G339" activeCellId="0" sqref="G339"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13331,7 +13340,7 @@
         <v>750</v>
       </c>
       <c r="G341" s="1" t="s">
-        <v>755</v>
+        <v>761</v>
       </c>
       <c r="H341" s="1" t="s">
         <v>17</v>
@@ -13342,10 +13351,10 @@
     </row>
     <row r="342" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A342" s="1" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="B342" s="22" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
       <c r="C342" s="1" t="n">
         <v>3600</v>
@@ -13357,21 +13366,21 @@
         <v>10</v>
       </c>
       <c r="F342" s="3" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="G342" s="1" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
       <c r="I342" s="1" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
     </row>
     <row r="343" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A343" s="1" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="B343" s="22" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="C343" s="1" t="n">
         <v>3601</v>
@@ -13383,10 +13392,10 @@
         <v>10</v>
       </c>
       <c r="F343" s="3" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="G343" s="1" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
       <c r="I343" s="1" t="s">
         <v>627</v>
@@ -13394,10 +13403,10 @@
     </row>
     <row r="344" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A344" s="1" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="B344" s="22" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
       <c r="C344" s="1" t="n">
         <v>3602</v>
@@ -13409,10 +13418,10 @@
         <v>10</v>
       </c>
       <c r="F344" s="3" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="G344" s="1" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="I344" s="1" t="s">
         <v>278</v>
@@ -13420,10 +13429,10 @@
     </row>
     <row r="345" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A345" s="1" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="B345" s="22" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
       <c r="C345" s="1" t="n">
         <v>3603</v>
@@ -13435,10 +13444,10 @@
         <v>10</v>
       </c>
       <c r="F345" s="3" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="G345" s="1" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
       <c r="I345" s="1" t="s">
         <v>278</v>
@@ -13479,13 +13488,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="24" t="s">
-        <v>773</v>
+        <v>774</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
       <c r="C1" s="24" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13496,7 +13505,7 @@
         <v>257</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13507,7 +13516,7 @@
         <v>256</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13518,7 +13527,7 @@
         <v>258</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13529,7 +13538,7 @@
         <v>260</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13540,7 +13549,7 @@
         <v>261</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13551,7 +13560,7 @@
         <v>275</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13562,7 +13571,7 @@
         <v>0</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13573,7 +13582,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>783</v>
+        <v>784</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13584,7 +13593,7 @@
         <v>2</v>
       </c>
       <c r="C10" s="22" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13595,7 +13604,7 @@
         <v>3</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13606,7 +13615,7 @@
         <v>4</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13617,7 +13626,7 @@
         <v>5</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13628,7 +13637,7 @@
         <v>6</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13639,7 +13648,7 @@
         <v>7</v>
       </c>
       <c r="C15" s="22" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13650,7 +13659,7 @@
         <v>8</v>
       </c>
       <c r="C16" s="22" t="s">
-        <v>790</v>
+        <v>791</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13661,7 +13670,7 @@
         <v>9</v>
       </c>
       <c r="C17" s="22" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13672,7 +13681,7 @@
         <v>10</v>
       </c>
       <c r="C18" s="22" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13683,7 +13692,7 @@
         <v>11</v>
       </c>
       <c r="C19" s="22" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13694,7 +13703,7 @@
         <v>12</v>
       </c>
       <c r="C20" s="22" t="s">
-        <v>794</v>
+        <v>795</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13705,7 +13714,7 @@
         <v>20</v>
       </c>
       <c r="C21" s="22" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13716,7 +13725,7 @@
         <v>21</v>
       </c>
       <c r="C22" s="22" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13727,7 +13736,7 @@
         <v>22</v>
       </c>
       <c r="C23" s="22" t="s">
-        <v>797</v>
+        <v>798</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13738,7 +13747,7 @@
         <v>23</v>
       </c>
       <c r="C24" s="22" t="s">
-        <v>798</v>
+        <v>799</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13749,7 +13758,7 @@
         <v>24</v>
       </c>
       <c r="C25" s="22" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13760,7 +13769,7 @@
         <v>25</v>
       </c>
       <c r="C26" s="22" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13771,7 +13780,7 @@
         <v>26</v>
       </c>
       <c r="C27" s="22" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13782,7 +13791,7 @@
         <v>27</v>
       </c>
       <c r="C28" s="22" t="s">
-        <v>802</v>
+        <v>803</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13793,7 +13802,7 @@
         <v>28</v>
       </c>
       <c r="C29" s="22" t="s">
-        <v>803</v>
+        <v>804</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13804,7 +13813,7 @@
         <v>29</v>
       </c>
       <c r="C30" s="22" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13815,7 +13824,7 @@
         <v>30</v>
       </c>
       <c r="C31" s="22" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13826,7 +13835,7 @@
         <v>31</v>
       </c>
       <c r="C32" s="22" t="s">
-        <v>806</v>
+        <v>807</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13837,7 +13846,7 @@
         <v>32</v>
       </c>
       <c r="C33" s="22" t="s">
-        <v>807</v>
+        <v>808</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13848,7 +13857,7 @@
         <v>33</v>
       </c>
       <c r="C34" s="22" t="s">
-        <v>808</v>
+        <v>809</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13859,7 +13868,7 @@
         <v>34</v>
       </c>
       <c r="C35" s="22" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13870,7 +13879,7 @@
         <v>40</v>
       </c>
       <c r="C36" s="22" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13881,7 +13890,7 @@
         <v>41</v>
       </c>
       <c r="C37" s="22" t="s">
-        <v>811</v>
+        <v>812</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13892,7 +13901,7 @@
         <v>42</v>
       </c>
       <c r="C38" s="22" t="s">
-        <v>812</v>
+        <v>813</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13903,7 +13912,7 @@
         <v>43</v>
       </c>
       <c r="C39" s="22" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13914,7 +13923,7 @@
         <v>44</v>
       </c>
       <c r="C40" s="22" t="s">
-        <v>814</v>
+        <v>815</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13925,7 +13934,7 @@
         <v>45</v>
       </c>
       <c r="C41" s="22" t="s">
-        <v>815</v>
+        <v>816</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13936,7 +13945,7 @@
         <v>46</v>
       </c>
       <c r="C42" s="22" t="s">
-        <v>816</v>
+        <v>817</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13947,7 +13956,7 @@
         <v>288</v>
       </c>
       <c r="C43" s="22" t="s">
-        <v>817</v>
+        <v>818</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13958,7 +13967,7 @@
         <v>289</v>
       </c>
       <c r="C44" s="22" t="s">
-        <v>818</v>
+        <v>819</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13969,7 +13978,7 @@
         <v>290</v>
       </c>
       <c r="C45" s="22" t="s">
-        <v>819</v>
+        <v>820</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13980,7 +13989,7 @@
         <v>291</v>
       </c>
       <c r="C46" s="22" t="s">
-        <v>820</v>
+        <v>821</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13991,7 +14000,7 @@
         <v>292</v>
       </c>
       <c r="C47" s="22" t="s">
-        <v>821</v>
+        <v>822</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14002,7 +14011,7 @@
         <v>293</v>
       </c>
       <c r="C48" s="22" t="s">
-        <v>822</v>
+        <v>823</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14013,12 +14022,12 @@
         <v>512</v>
       </c>
       <c r="C49" s="22" t="s">
-        <v>823</v>
+        <v>824</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="26" t="s">
-        <v>824</v>
+        <v>825</v>
       </c>
       <c r="B51" s="26"/>
       <c r="C51" s="26"/>
@@ -14028,7 +14037,7 @@
     </row>
     <row r="52" customFormat="false" ht="92.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="27" t="s">
-        <v>825</v>
+        <v>826</v>
       </c>
       <c r="B52" s="27"/>
       <c r="C52" s="27"/>
@@ -14056,10 +14065,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C66"/>
+  <dimension ref="A1:C67"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A50" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A66" activeCellId="0" sqref="A66"/>
+      <selection pane="topLeft" activeCell="B67" activeCellId="0" sqref="B67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14072,410 +14081,418 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="22" t="s">
-        <v>826</v>
+        <v>827</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>827</v>
+        <v>828</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="22" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="22" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>831</v>
+        <v>832</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="22" t="s">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="22" t="s">
-        <v>834</v>
+        <v>835</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="22" t="s">
-        <v>835</v>
+        <v>836</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="22" t="s">
-        <v>836</v>
+        <v>837</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="22" t="s">
-        <v>837</v>
+        <v>838</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="22" t="s">
-        <v>838</v>
+        <v>839</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>839</v>
+        <v>840</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="22" t="s">
-        <v>840</v>
+        <v>841</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="22" t="s">
-        <v>841</v>
+        <v>842</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="22" t="s">
-        <v>842</v>
+        <v>843</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>843</v>
+        <v>844</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="22" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="22" t="s">
-        <v>845</v>
+        <v>846</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="22" t="s">
-        <v>846</v>
+        <v>847</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="22" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="22" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="22" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="B18" s="22" t="s">
-        <v>850</v>
+        <v>851</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="22" t="s">
-        <v>851</v>
+        <v>852</v>
       </c>
       <c r="B19" s="22" t="s">
-        <v>852</v>
+        <v>853</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="22" t="s">
-        <v>853</v>
+        <v>854</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="22" t="s">
-        <v>854</v>
+        <v>855</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="22" t="s">
-        <v>855</v>
+        <v>856</v>
       </c>
       <c r="B22" s="22" t="s">
-        <v>856</v>
+        <v>857</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="22" t="s">
-        <v>857</v>
+        <v>858</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="22" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="22" t="s">
-        <v>859</v>
+        <v>860</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="22" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="22" t="s">
-        <v>861</v>
+        <v>862</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="22" t="s">
-        <v>862</v>
+        <v>863</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="22" t="s">
-        <v>863</v>
+        <v>864</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="22" t="s">
-        <v>864</v>
+        <v>865</v>
       </c>
       <c r="B30" s="22" t="s">
-        <v>865</v>
+        <v>866</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="22" t="s">
-        <v>866</v>
+        <v>867</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="22" t="s">
-        <v>867</v>
+        <v>868</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="22" t="s">
-        <v>868</v>
+        <v>869</v>
       </c>
       <c r="B33" s="22" t="s">
-        <v>869</v>
+        <v>870</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="22" t="s">
-        <v>870</v>
+        <v>871</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="22" t="s">
-        <v>871</v>
+        <v>872</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="22" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="22" t="s">
-        <v>873</v>
+        <v>874</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="22" t="s">
-        <v>874</v>
+        <v>875</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C39" s="28" t="s">
-        <v>875</v>
+        <v>876</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="22" t="s">
-        <v>876</v>
+        <v>877</v>
       </c>
       <c r="B40" s="22" t="s">
-        <v>877</v>
+        <v>878</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="22" t="s">
-        <v>878</v>
+        <v>879</v>
       </c>
       <c r="B41" s="22" t="s">
-        <v>879</v>
+        <v>880</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="22" t="s">
-        <v>880</v>
+        <v>881</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="22" t="s">
-        <v>881</v>
+        <v>882</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="22" t="s">
-        <v>882</v>
+        <v>883</v>
       </c>
       <c r="B44" s="22" t="s">
-        <v>883</v>
+        <v>884</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="22" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="22" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="22" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="B47" s="22" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="22" t="s">
-        <v>888</v>
+        <v>889</v>
       </c>
       <c r="B48" s="22" t="s">
-        <v>889</v>
+        <v>890</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="22" t="s">
-        <v>890</v>
+        <v>891</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="22" t="s">
-        <v>891</v>
+        <v>892</v>
       </c>
       <c r="B50" s="22" t="s">
-        <v>892</v>
+        <v>893</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="22" t="s">
-        <v>893</v>
+        <v>894</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="22" t="s">
-        <v>894</v>
+        <v>895</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="22" t="s">
-        <v>895</v>
+        <v>896</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="22" t="s">
-        <v>896</v>
+        <v>897</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="22" t="s">
-        <v>897</v>
+        <v>898</v>
       </c>
       <c r="B55" s="22" t="s">
-        <v>898</v>
+        <v>899</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="22" t="s">
-        <v>899</v>
+        <v>900</v>
       </c>
       <c r="B56" s="22" t="s">
-        <v>900</v>
+        <v>901</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="22" t="s">
-        <v>901</v>
+        <v>902</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="22" t="s">
-        <v>902</v>
+        <v>903</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="22" t="s">
-        <v>903</v>
+        <v>904</v>
       </c>
       <c r="B59" s="22" t="s">
-        <v>904</v>
+        <v>905</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="22" t="s">
-        <v>905</v>
+        <v>906</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="22" t="s">
-        <v>906</v>
+        <v>907</v>
       </c>
       <c r="B61" s="22" t="s">
-        <v>907</v>
+        <v>908</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="22" t="s">
-        <v>908</v>
+        <v>909</v>
       </c>
       <c r="B62" s="22" t="s">
-        <v>909</v>
+        <v>910</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="22" t="s">
-        <v>910</v>
+        <v>911</v>
       </c>
       <c r="B63" s="22" t="s">
-        <v>911</v>
+        <v>912</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="22" t="s">
-        <v>912</v>
+        <v>913</v>
       </c>
       <c r="B64" s="22" t="s">
-        <v>913</v>
+        <v>914</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="22" t="s">
-        <v>914</v>
+        <v>915</v>
       </c>
       <c r="B65" s="22" t="s">
-        <v>915</v>
+        <v>916</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="22" t="s">
-        <v>916</v>
+        <v>917</v>
       </c>
       <c r="B66" s="22" t="s">
-        <v>917</v>
+        <v>918</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="22" t="s">
+        <v>919</v>
+      </c>
+      <c r="B67" s="22" t="s">
+        <v>920</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Map unitids for Cerbo GX
227 -> 276 (VE.Bus)
226 -> 279 (VE.Direct 1)
224 -> 278 (VE.Direct 2)
223 -> 277 (VE.Direct 3)
</commit_message>
<xml_diff>
--- a/CCGX-Modbus-TCP-register-list.xlsx
+++ b/CCGX-Modbus-TCP-register-list.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2639" uniqueCount="921">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2645" uniqueCount="927">
   <si>
     <t xml:space="preserve">NOTE: Use unit-id 100 for the com.victronenergy.system data, for more information see FAQ.</t>
   </si>
@@ -2373,6 +2373,18 @@
     <t xml:space="preserve">EasySolar-II/Multiplus-II GX VE.Bus port (ttyS3)</t>
   </si>
   <si>
+    <t xml:space="preserve">Cerbo GX VE.Bus port (ttyS4)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cerbo GX VE.Direct port 1 (ttyS7)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cerbo GX VE.Direct port 2 (ttyS6)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cerbo GX VE.Direct port 3 (ttyS5)</t>
+  </si>
+  <si>
     <t xml:space="preserve">VE.Can device instance 0 and all registers listed as com.victronenergy.system</t>
   </si>
   <si>
@@ -2785,6 +2797,12 @@
   </si>
   <si>
     <t xml:space="preserve">Corrected Dbus path for generator ManualStart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rev 27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add mappings for Cerbo GX ports</t>
   </si>
 </sst>
 </file>
@@ -13472,17 +13490,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F52"/>
+  <dimension ref="A1:F56"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A33" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C49" activeCellId="0" sqref="C49"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A39" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="22" width="7.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="22" width="16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="22" width="23.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="22" width="64.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="22" width="8.57"/>
   </cols>
   <sheetData>
@@ -13563,56 +13581,56 @@
         <v>782</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="22" t="n">
-        <v>100</v>
-      </c>
-      <c r="B8" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="C8" s="22" t="s">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="25" t="n">
+        <v>227</v>
+      </c>
+      <c r="B8" s="25" t="n">
+        <v>276</v>
+      </c>
+      <c r="C8" s="25" t="s">
         <v>783</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="22" t="n">
-        <v>1</v>
-      </c>
-      <c r="B9" s="22" t="n">
-        <v>1</v>
-      </c>
-      <c r="C9" s="22" t="s">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="25" t="n">
+        <v>226</v>
+      </c>
+      <c r="B9" s="25" t="n">
+        <v>279</v>
+      </c>
+      <c r="C9" s="25" t="s">
         <v>784</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="22" t="n">
-        <v>2</v>
-      </c>
-      <c r="B10" s="22" t="n">
-        <v>2</v>
-      </c>
-      <c r="C10" s="22" t="s">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="25" t="n">
+        <v>224</v>
+      </c>
+      <c r="B10" s="25" t="n">
+        <v>278</v>
+      </c>
+      <c r="C10" s="25" t="s">
         <v>785</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="22" t="n">
-        <v>3</v>
-      </c>
-      <c r="B11" s="22" t="n">
-        <v>3</v>
-      </c>
-      <c r="C11" s="22" t="s">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="25" t="n">
+        <v>223</v>
+      </c>
+      <c r="B11" s="25" t="n">
+        <v>277</v>
+      </c>
+      <c r="C11" s="25" t="s">
         <v>786</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="22" t="n">
-        <v>4</v>
+        <v>100</v>
       </c>
       <c r="B12" s="22" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C12" s="22" t="s">
         <v>787</v>
@@ -13620,10 +13638,10 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="22" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B13" s="22" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C13" s="22" t="s">
         <v>788</v>
@@ -13631,10 +13649,10 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="22" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B14" s="22" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C14" s="22" t="s">
         <v>789</v>
@@ -13642,10 +13660,10 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="22" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B15" s="22" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C15" s="22" t="s">
         <v>790</v>
@@ -13653,10 +13671,10 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="22" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B16" s="22" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C16" s="22" t="s">
         <v>791</v>
@@ -13664,10 +13682,10 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="22" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B17" s="22" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C17" s="22" t="s">
         <v>792</v>
@@ -13675,10 +13693,10 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="22" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B18" s="22" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C18" s="22" t="s">
         <v>793</v>
@@ -13686,10 +13704,10 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="22" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B19" s="22" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C19" s="22" t="s">
         <v>794</v>
@@ -13697,10 +13715,10 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="22" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B20" s="22" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C20" s="22" t="s">
         <v>795</v>
@@ -13708,10 +13726,10 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="22" t="n">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="B21" s="22" t="n">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="C21" s="22" t="s">
         <v>796</v>
@@ -13719,10 +13737,10 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="22" t="n">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="B22" s="22" t="n">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="C22" s="22" t="s">
         <v>797</v>
@@ -13730,10 +13748,10 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="22" t="n">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="B23" s="22" t="n">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="C23" s="22" t="s">
         <v>798</v>
@@ -13741,10 +13759,10 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="22" t="n">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B24" s="22" t="n">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C24" s="22" t="s">
         <v>799</v>
@@ -13752,10 +13770,10 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="22" t="n">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B25" s="22" t="n">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C25" s="22" t="s">
         <v>800</v>
@@ -13763,10 +13781,10 @@
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="22" t="n">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B26" s="22" t="n">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C26" s="22" t="s">
         <v>801</v>
@@ -13774,10 +13792,10 @@
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="22" t="n">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B27" s="22" t="n">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C27" s="22" t="s">
         <v>802</v>
@@ -13785,10 +13803,10 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="22" t="n">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B28" s="22" t="n">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C28" s="22" t="s">
         <v>803</v>
@@ -13796,10 +13814,10 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="22" t="n">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B29" s="22" t="n">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C29" s="22" t="s">
         <v>804</v>
@@ -13807,10 +13825,10 @@
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="22" t="n">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B30" s="22" t="n">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C30" s="22" t="s">
         <v>805</v>
@@ -13818,10 +13836,10 @@
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="22" t="n">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B31" s="22" t="n">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C31" s="22" t="s">
         <v>806</v>
@@ -13829,10 +13847,10 @@
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="22" t="n">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B32" s="22" t="n">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C32" s="22" t="s">
         <v>807</v>
@@ -13840,10 +13858,10 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="22" t="n">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B33" s="22" t="n">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C33" s="22" t="s">
         <v>808</v>
@@ -13851,10 +13869,10 @@
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="22" t="n">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B34" s="22" t="n">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C34" s="22" t="s">
         <v>809</v>
@@ -13862,10 +13880,10 @@
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="22" t="n">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B35" s="22" t="n">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C35" s="22" t="s">
         <v>810</v>
@@ -13873,10 +13891,10 @@
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="22" t="n">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="B36" s="22" t="n">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="C36" s="22" t="s">
         <v>811</v>
@@ -13884,10 +13902,10 @@
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="22" t="n">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="B37" s="22" t="n">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="C37" s="22" t="s">
         <v>812</v>
@@ -13895,10 +13913,10 @@
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="22" t="n">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B38" s="22" t="n">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="C38" s="22" t="s">
         <v>813</v>
@@ -13906,10 +13924,10 @@
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="22" t="n">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="B39" s="22" t="n">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="C39" s="22" t="s">
         <v>814</v>
@@ -13917,10 +13935,10 @@
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="22" t="n">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B40" s="22" t="n">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C40" s="22" t="s">
         <v>815</v>
@@ -13928,10 +13946,10 @@
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="22" t="n">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B41" s="22" t="n">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C41" s="22" t="s">
         <v>816</v>
@@ -13939,10 +13957,10 @@
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="22" t="n">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B42" s="22" t="n">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C42" s="22" t="s">
         <v>817</v>
@@ -13950,10 +13968,10 @@
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="22" t="n">
-        <v>239</v>
+        <v>43</v>
       </c>
       <c r="B43" s="22" t="n">
-        <v>288</v>
+        <v>43</v>
       </c>
       <c r="C43" s="22" t="s">
         <v>818</v>
@@ -13961,10 +13979,10 @@
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="22" t="n">
-        <v>238</v>
+        <v>44</v>
       </c>
       <c r="B44" s="22" t="n">
-        <v>289</v>
+        <v>44</v>
       </c>
       <c r="C44" s="22" t="s">
         <v>819</v>
@@ -13972,10 +13990,10 @@
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="22" t="n">
-        <v>237</v>
+        <v>45</v>
       </c>
       <c r="B45" s="22" t="n">
-        <v>290</v>
+        <v>45</v>
       </c>
       <c r="C45" s="22" t="s">
         <v>820</v>
@@ -13983,10 +14001,10 @@
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="22" t="n">
-        <v>236</v>
+        <v>46</v>
       </c>
       <c r="B46" s="22" t="n">
-        <v>291</v>
+        <v>46</v>
       </c>
       <c r="C46" s="22" t="s">
         <v>821</v>
@@ -13994,10 +14012,10 @@
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="22" t="n">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="B47" s="22" t="n">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="C47" s="22" t="s">
         <v>822</v>
@@ -14005,10 +14023,10 @@
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="22" t="n">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="B48" s="22" t="n">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="C48" s="22" t="s">
         <v>823</v>
@@ -14016,39 +14034,83 @@
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="22" t="n">
-        <v>225</v>
+        <v>237</v>
       </c>
       <c r="B49" s="22" t="n">
-        <v>512</v>
+        <v>290</v>
       </c>
       <c r="C49" s="22" t="s">
         <v>824</v>
       </c>
     </row>
+    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="22" t="n">
+        <v>236</v>
+      </c>
+      <c r="B50" s="22" t="n">
+        <v>291</v>
+      </c>
+      <c r="C50" s="22" t="s">
+        <v>825</v>
+      </c>
+    </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="26" t="s">
-        <v>825</v>
-      </c>
-      <c r="B51" s="26"/>
-      <c r="C51" s="26"/>
-      <c r="D51" s="26"/>
-      <c r="E51" s="26"/>
-      <c r="F51" s="26"/>
-    </row>
-    <row r="52" customFormat="false" ht="92.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A52" s="27" t="s">
+      <c r="A51" s="22" t="n">
+        <v>235</v>
+      </c>
+      <c r="B51" s="22" t="n">
+        <v>292</v>
+      </c>
+      <c r="C51" s="22" t="s">
         <v>826</v>
       </c>
-      <c r="B52" s="27"/>
-      <c r="C52" s="27"/>
-      <c r="D52" s="27"/>
-      <c r="E52" s="27"/>
-      <c r="F52" s="27"/>
+    </row>
+    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="22" t="n">
+        <v>233</v>
+      </c>
+      <c r="B52" s="22" t="n">
+        <v>293</v>
+      </c>
+      <c r="C52" s="22" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="22" t="n">
+        <v>225</v>
+      </c>
+      <c r="B53" s="22" t="n">
+        <v>512</v>
+      </c>
+      <c r="C53" s="22" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="26" t="s">
+        <v>829</v>
+      </c>
+      <c r="B55" s="26"/>
+      <c r="C55" s="26"/>
+      <c r="D55" s="26"/>
+      <c r="E55" s="26"/>
+      <c r="F55" s="26"/>
+    </row>
+    <row r="56" customFormat="false" ht="92.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A56" s="27" t="s">
+        <v>830</v>
+      </c>
+      <c r="B56" s="27"/>
+      <c r="C56" s="27"/>
+      <c r="D56" s="27"/>
+      <c r="E56" s="27"/>
+      <c r="F56" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A51:F51"/>
-    <mergeCell ref="A52:F52"/>
+    <mergeCell ref="A55:F55"/>
+    <mergeCell ref="A56:F56"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -14065,10 +14127,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C67"/>
+  <dimension ref="A1:C68"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A50" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B67" activeCellId="0" sqref="B67"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A62" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B69" activeCellId="0" sqref="B69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14081,418 +14143,426 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="22" t="s">
-        <v>827</v>
+        <v>831</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>828</v>
+        <v>832</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="22" t="s">
-        <v>829</v>
+        <v>833</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>830</v>
+        <v>834</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="22" t="s">
-        <v>831</v>
+        <v>835</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>832</v>
+        <v>836</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="22" t="s">
-        <v>833</v>
+        <v>837</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>834</v>
+        <v>838</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="22" t="s">
-        <v>835</v>
+        <v>839</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="22" t="s">
-        <v>836</v>
+        <v>840</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="22" t="s">
-        <v>837</v>
+        <v>841</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="22" t="s">
-        <v>838</v>
+        <v>842</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="22" t="s">
-        <v>839</v>
+        <v>843</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>840</v>
+        <v>844</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="22" t="s">
-        <v>841</v>
+        <v>845</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="22" t="s">
-        <v>842</v>
+        <v>846</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="22" t="s">
-        <v>843</v>
+        <v>847</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>844</v>
+        <v>848</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="22" t="s">
-        <v>845</v>
+        <v>849</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="22" t="s">
-        <v>846</v>
+        <v>850</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="22" t="s">
-        <v>847</v>
+        <v>851</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="22" t="s">
-        <v>848</v>
+        <v>852</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="22" t="s">
-        <v>849</v>
+        <v>853</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="22" t="s">
-        <v>850</v>
+        <v>854</v>
       </c>
       <c r="B18" s="22" t="s">
-        <v>851</v>
+        <v>855</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="22" t="s">
-        <v>852</v>
+        <v>856</v>
       </c>
       <c r="B19" s="22" t="s">
-        <v>853</v>
+        <v>857</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="22" t="s">
-        <v>854</v>
+        <v>858</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="22" t="s">
-        <v>855</v>
+        <v>859</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="22" t="s">
-        <v>856</v>
+        <v>860</v>
       </c>
       <c r="B22" s="22" t="s">
-        <v>857</v>
+        <v>861</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="22" t="s">
-        <v>858</v>
+        <v>862</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="22" t="s">
-        <v>859</v>
+        <v>863</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="22" t="s">
-        <v>860</v>
+        <v>864</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="22" t="s">
-        <v>861</v>
+        <v>865</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="22" t="s">
-        <v>862</v>
+        <v>866</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="22" t="s">
-        <v>863</v>
+        <v>867</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="22" t="s">
-        <v>864</v>
+        <v>868</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="22" t="s">
-        <v>865</v>
+        <v>869</v>
       </c>
       <c r="B30" s="22" t="s">
-        <v>866</v>
+        <v>870</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="22" t="s">
-        <v>867</v>
+        <v>871</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="22" t="s">
-        <v>868</v>
+        <v>872</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="22" t="s">
-        <v>869</v>
+        <v>873</v>
       </c>
       <c r="B33" s="22" t="s">
-        <v>870</v>
+        <v>874</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="22" t="s">
-        <v>871</v>
+        <v>875</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="22" t="s">
-        <v>872</v>
+        <v>876</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="22" t="s">
-        <v>873</v>
+        <v>877</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="22" t="s">
-        <v>874</v>
+        <v>878</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="22" t="s">
-        <v>875</v>
+        <v>879</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C39" s="28" t="s">
-        <v>876</v>
+        <v>880</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="22" t="s">
-        <v>877</v>
+        <v>881</v>
       </c>
       <c r="B40" s="22" t="s">
-        <v>878</v>
+        <v>882</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="22" t="s">
-        <v>879</v>
+        <v>883</v>
       </c>
       <c r="B41" s="22" t="s">
-        <v>880</v>
+        <v>884</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="22" t="s">
-        <v>881</v>
+        <v>885</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="22" t="s">
-        <v>882</v>
+        <v>886</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="22" t="s">
-        <v>883</v>
+        <v>887</v>
       </c>
       <c r="B44" s="22" t="s">
-        <v>884</v>
+        <v>888</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="22" t="s">
-        <v>885</v>
+        <v>889</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="22" t="s">
-        <v>886</v>
+        <v>890</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="22" t="s">
-        <v>887</v>
+        <v>891</v>
       </c>
       <c r="B47" s="22" t="s">
-        <v>888</v>
+        <v>892</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="22" t="s">
-        <v>889</v>
+        <v>893</v>
       </c>
       <c r="B48" s="22" t="s">
-        <v>890</v>
+        <v>894</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="22" t="s">
-        <v>891</v>
+        <v>895</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="22" t="s">
-        <v>892</v>
+        <v>896</v>
       </c>
       <c r="B50" s="22" t="s">
-        <v>893</v>
+        <v>897</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="22" t="s">
-        <v>894</v>
+        <v>898</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="22" t="s">
-        <v>895</v>
+        <v>899</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="22" t="s">
-        <v>896</v>
+        <v>900</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="22" t="s">
-        <v>897</v>
+        <v>901</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="22" t="s">
-        <v>898</v>
+        <v>902</v>
       </c>
       <c r="B55" s="22" t="s">
-        <v>899</v>
+        <v>903</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="22" t="s">
-        <v>900</v>
+        <v>904</v>
       </c>
       <c r="B56" s="22" t="s">
-        <v>901</v>
+        <v>905</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="22" t="s">
-        <v>902</v>
+        <v>906</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="22" t="s">
-        <v>903</v>
+        <v>907</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="22" t="s">
-        <v>904</v>
+        <v>908</v>
       </c>
       <c r="B59" s="22" t="s">
-        <v>905</v>
+        <v>909</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="22" t="s">
-        <v>906</v>
+        <v>910</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="22" t="s">
-        <v>907</v>
+        <v>911</v>
       </c>
       <c r="B61" s="22" t="s">
-        <v>908</v>
+        <v>912</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="22" t="s">
-        <v>909</v>
+        <v>913</v>
       </c>
       <c r="B62" s="22" t="s">
-        <v>910</v>
+        <v>914</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="22" t="s">
-        <v>911</v>
+        <v>915</v>
       </c>
       <c r="B63" s="22" t="s">
-        <v>912</v>
+        <v>916</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="22" t="s">
-        <v>913</v>
+        <v>917</v>
       </c>
       <c r="B64" s="22" t="s">
-        <v>914</v>
+        <v>918</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="22" t="s">
-        <v>915</v>
+        <v>919</v>
       </c>
       <c r="B65" s="22" t="s">
-        <v>916</v>
+        <v>920</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="22" t="s">
-        <v>917</v>
+        <v>921</v>
       </c>
       <c r="B66" s="22" t="s">
-        <v>918</v>
+        <v>922</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="22" t="s">
-        <v>919</v>
+        <v>923</v>
       </c>
       <c r="B67" s="22" t="s">
-        <v>920</v>
+        <v>924</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="22" t="s">
+        <v>925</v>
+      </c>
+      <c r="B68" s="22" t="s">
+        <v>926</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add mappings for VE.Direct ports on nanopi-based boards
This adds unitid mappings for the Multiplus-II GX and EasySolar-II GX.

273 -> 230 (ttyS1)
274 -> 229 (ttyS2)

https://github.com/victronenergy/venus/issues/616
</commit_message>
<xml_diff>
--- a/CCGX-Modbus-TCP-register-list.xlsx
+++ b/CCGX-Modbus-TCP-register-list.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2645" uniqueCount="927">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2649" uniqueCount="931">
   <si>
     <t xml:space="preserve">NOTE: Use unit-id 100 for the com.victronenergy.system data, for more information see FAQ.</t>
   </si>
@@ -2370,6 +2370,12 @@
     <t xml:space="preserve">Venus GX VE.Bus port (ttyO5)</t>
   </si>
   <si>
+    <t xml:space="preserve">EasySolar-II/Multiplus-II GX VE.Direct port (ttyS1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EasySolar-II/Multiplus-II GX VE.Direct port (ttyS2)</t>
+  </si>
+  <si>
     <t xml:space="preserve">EasySolar-II/Multiplus-II GX VE.Bus port (ttyS3)</t>
   </si>
   <si>
@@ -2803,6 +2809,12 @@
   </si>
   <si>
     <t xml:space="preserve">Add mappings for Cerbo GX ports</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rev 28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Added mapping for EasySolar-II/Multiplus-II GX VE.Direct ports</t>
   </si>
 </sst>
 </file>
@@ -13490,10 +13502,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F56"/>
+  <dimension ref="A1:F58"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A39" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13572,10 +13584,10 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="25" t="n">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="B7" s="25" t="n">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C7" s="25" t="s">
         <v>782</v>
@@ -13583,10 +13595,10 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="25" t="n">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="B8" s="25" t="n">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C8" s="25" t="s">
         <v>783</v>
@@ -13594,10 +13606,10 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="25" t="n">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="B9" s="25" t="n">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="C9" s="25" t="s">
         <v>784</v>
@@ -13605,10 +13617,10 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="25" t="n">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="B10" s="25" t="n">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C10" s="25" t="s">
         <v>785</v>
@@ -13616,43 +13628,43 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="25" t="n">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="B11" s="25" t="n">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="C11" s="25" t="s">
         <v>786</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="22" t="n">
-        <v>100</v>
-      </c>
-      <c r="B12" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="C12" s="22" t="s">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="25" t="n">
+        <v>224</v>
+      </c>
+      <c r="B12" s="25" t="n">
+        <v>278</v>
+      </c>
+      <c r="C12" s="25" t="s">
         <v>787</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="22" t="n">
-        <v>1</v>
-      </c>
-      <c r="B13" s="22" t="n">
-        <v>1</v>
-      </c>
-      <c r="C13" s="22" t="s">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="25" t="n">
+        <v>223</v>
+      </c>
+      <c r="B13" s="25" t="n">
+        <v>277</v>
+      </c>
+      <c r="C13" s="25" t="s">
         <v>788</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="22" t="n">
-        <v>2</v>
+        <v>100</v>
       </c>
       <c r="B14" s="22" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C14" s="22" t="s">
         <v>789</v>
@@ -13660,10 +13672,10 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="22" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B15" s="22" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C15" s="22" t="s">
         <v>790</v>
@@ -13671,10 +13683,10 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="22" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B16" s="22" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C16" s="22" t="s">
         <v>791</v>
@@ -13682,10 +13694,10 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="22" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B17" s="22" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C17" s="22" t="s">
         <v>792</v>
@@ -13693,10 +13705,10 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="22" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B18" s="22" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C18" s="22" t="s">
         <v>793</v>
@@ -13704,10 +13716,10 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="22" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B19" s="22" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C19" s="22" t="s">
         <v>794</v>
@@ -13715,10 +13727,10 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="22" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B20" s="22" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C20" s="22" t="s">
         <v>795</v>
@@ -13726,10 +13738,10 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="22" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B21" s="22" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C21" s="22" t="s">
         <v>796</v>
@@ -13737,10 +13749,10 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="22" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B22" s="22" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C22" s="22" t="s">
         <v>797</v>
@@ -13748,10 +13760,10 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="22" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B23" s="22" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C23" s="22" t="s">
         <v>798</v>
@@ -13759,10 +13771,10 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="22" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B24" s="22" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C24" s="22" t="s">
         <v>799</v>
@@ -13770,10 +13782,10 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="22" t="n">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B25" s="22" t="n">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="C25" s="22" t="s">
         <v>800</v>
@@ -13781,10 +13793,10 @@
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="22" t="n">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B26" s="22" t="n">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C26" s="22" t="s">
         <v>801</v>
@@ -13792,10 +13804,10 @@
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="22" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B27" s="22" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C27" s="22" t="s">
         <v>802</v>
@@ -13803,10 +13815,10 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="22" t="n">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B28" s="22" t="n">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C28" s="22" t="s">
         <v>803</v>
@@ -13814,10 +13826,10 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="22" t="n">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B29" s="22" t="n">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C29" s="22" t="s">
         <v>804</v>
@@ -13825,10 +13837,10 @@
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="22" t="n">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B30" s="22" t="n">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C30" s="22" t="s">
         <v>805</v>
@@ -13836,10 +13848,10 @@
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="22" t="n">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B31" s="22" t="n">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C31" s="22" t="s">
         <v>806</v>
@@ -13847,10 +13859,10 @@
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="22" t="n">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B32" s="22" t="n">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C32" s="22" t="s">
         <v>807</v>
@@ -13858,10 +13870,10 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="22" t="n">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B33" s="22" t="n">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C33" s="22" t="s">
         <v>808</v>
@@ -13869,10 +13881,10 @@
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="22" t="n">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B34" s="22" t="n">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C34" s="22" t="s">
         <v>809</v>
@@ -13880,10 +13892,10 @@
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="22" t="n">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B35" s="22" t="n">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C35" s="22" t="s">
         <v>810</v>
@@ -13891,10 +13903,10 @@
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="22" t="n">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B36" s="22" t="n">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C36" s="22" t="s">
         <v>811</v>
@@ -13902,10 +13914,10 @@
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="22" t="n">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B37" s="22" t="n">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C37" s="22" t="s">
         <v>812</v>
@@ -13913,10 +13925,10 @@
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="22" t="n">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B38" s="22" t="n">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C38" s="22" t="s">
         <v>813</v>
@@ -13924,10 +13936,10 @@
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="22" t="n">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B39" s="22" t="n">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C39" s="22" t="s">
         <v>814</v>
@@ -13935,10 +13947,10 @@
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="22" t="n">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B40" s="22" t="n">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="C40" s="22" t="s">
         <v>815</v>
@@ -13946,10 +13958,10 @@
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="22" t="n">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B41" s="22" t="n">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C41" s="22" t="s">
         <v>816</v>
@@ -13957,10 +13969,10 @@
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="22" t="n">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B42" s="22" t="n">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C42" s="22" t="s">
         <v>817</v>
@@ -13968,10 +13980,10 @@
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="22" t="n">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B43" s="22" t="n">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C43" s="22" t="s">
         <v>818</v>
@@ -13979,10 +13991,10 @@
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="22" t="n">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B44" s="22" t="n">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C44" s="22" t="s">
         <v>819</v>
@@ -13990,10 +14002,10 @@
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="22" t="n">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B45" s="22" t="n">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C45" s="22" t="s">
         <v>820</v>
@@ -14001,10 +14013,10 @@
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="22" t="n">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B46" s="22" t="n">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C46" s="22" t="s">
         <v>821</v>
@@ -14012,10 +14024,10 @@
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="22" t="n">
-        <v>239</v>
+        <v>45</v>
       </c>
       <c r="B47" s="22" t="n">
-        <v>288</v>
+        <v>45</v>
       </c>
       <c r="C47" s="22" t="s">
         <v>822</v>
@@ -14023,10 +14035,10 @@
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="22" t="n">
-        <v>238</v>
+        <v>46</v>
       </c>
       <c r="B48" s="22" t="n">
-        <v>289</v>
+        <v>46</v>
       </c>
       <c r="C48" s="22" t="s">
         <v>823</v>
@@ -14034,10 +14046,10 @@
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="22" t="n">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="B49" s="22" t="n">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C49" s="22" t="s">
         <v>824</v>
@@ -14045,10 +14057,10 @@
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="22" t="n">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="B50" s="22" t="n">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C50" s="22" t="s">
         <v>825</v>
@@ -14056,10 +14068,10 @@
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="22" t="n">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="B51" s="22" t="n">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C51" s="22" t="s">
         <v>826</v>
@@ -14067,10 +14079,10 @@
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="22" t="n">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="B52" s="22" t="n">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C52" s="22" t="s">
         <v>827</v>
@@ -14078,39 +14090,61 @@
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="22" t="n">
-        <v>225</v>
+        <v>235</v>
       </c>
       <c r="B53" s="22" t="n">
-        <v>512</v>
+        <v>292</v>
       </c>
       <c r="C53" s="22" t="s">
         <v>828</v>
       </c>
     </row>
+    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="22" t="n">
+        <v>233</v>
+      </c>
+      <c r="B54" s="22" t="n">
+        <v>293</v>
+      </c>
+      <c r="C54" s="22" t="s">
+        <v>829</v>
+      </c>
+    </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="26" t="s">
-        <v>829</v>
-      </c>
-      <c r="B55" s="26"/>
-      <c r="C55" s="26"/>
-      <c r="D55" s="26"/>
-      <c r="E55" s="26"/>
-      <c r="F55" s="26"/>
-    </row>
-    <row r="56" customFormat="false" ht="92.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A56" s="27" t="s">
+      <c r="A55" s="22" t="n">
+        <v>225</v>
+      </c>
+      <c r="B55" s="22" t="n">
+        <v>512</v>
+      </c>
+      <c r="C55" s="22" t="s">
         <v>830</v>
       </c>
-      <c r="B56" s="27"/>
-      <c r="C56" s="27"/>
-      <c r="D56" s="27"/>
-      <c r="E56" s="27"/>
-      <c r="F56" s="27"/>
+    </row>
+    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="26" t="s">
+        <v>831</v>
+      </c>
+      <c r="B57" s="26"/>
+      <c r="C57" s="26"/>
+      <c r="D57" s="26"/>
+      <c r="E57" s="26"/>
+      <c r="F57" s="26"/>
+    </row>
+    <row r="58" customFormat="false" ht="92.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A58" s="27" t="s">
+        <v>832</v>
+      </c>
+      <c r="B58" s="27"/>
+      <c r="C58" s="27"/>
+      <c r="D58" s="27"/>
+      <c r="E58" s="27"/>
+      <c r="F58" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A55:F55"/>
-    <mergeCell ref="A56:F56"/>
+    <mergeCell ref="A57:F57"/>
+    <mergeCell ref="A58:F58"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -14127,10 +14161,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C68"/>
+  <dimension ref="A1:C69"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A62" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B69" activeCellId="0" sqref="B69"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14143,426 +14177,434 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="22" t="s">
-        <v>831</v>
+        <v>833</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>832</v>
+        <v>834</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="22" t="s">
-        <v>833</v>
+        <v>835</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>834</v>
+        <v>836</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="22" t="s">
-        <v>835</v>
+        <v>837</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>836</v>
+        <v>838</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="22" t="s">
-        <v>837</v>
+        <v>839</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>838</v>
+        <v>840</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="22" t="s">
-        <v>839</v>
+        <v>841</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="22" t="s">
-        <v>840</v>
+        <v>842</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="22" t="s">
-        <v>841</v>
+        <v>843</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="22" t="s">
-        <v>842</v>
+        <v>844</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="22" t="s">
-        <v>843</v>
+        <v>845</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>844</v>
+        <v>846</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="22" t="s">
-        <v>845</v>
+        <v>847</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="22" t="s">
-        <v>846</v>
+        <v>848</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="22" t="s">
-        <v>847</v>
+        <v>849</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>848</v>
+        <v>850</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="22" t="s">
-        <v>849</v>
+        <v>851</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="22" t="s">
-        <v>850</v>
+        <v>852</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="22" t="s">
-        <v>851</v>
+        <v>853</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="22" t="s">
-        <v>852</v>
+        <v>854</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="22" t="s">
-        <v>853</v>
+        <v>855</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="22" t="s">
-        <v>854</v>
+        <v>856</v>
       </c>
       <c r="B18" s="22" t="s">
-        <v>855</v>
+        <v>857</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="22" t="s">
-        <v>856</v>
+        <v>858</v>
       </c>
       <c r="B19" s="22" t="s">
-        <v>857</v>
+        <v>859</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="22" t="s">
-        <v>858</v>
+        <v>860</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="22" t="s">
-        <v>859</v>
+        <v>861</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="22" t="s">
-        <v>860</v>
+        <v>862</v>
       </c>
       <c r="B22" s="22" t="s">
-        <v>861</v>
+        <v>863</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="22" t="s">
-        <v>862</v>
+        <v>864</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="22" t="s">
-        <v>863</v>
+        <v>865</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="22" t="s">
-        <v>864</v>
+        <v>866</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="22" t="s">
-        <v>865</v>
+        <v>867</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="22" t="s">
-        <v>866</v>
+        <v>868</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="22" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="22" t="s">
-        <v>868</v>
+        <v>870</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="22" t="s">
-        <v>869</v>
+        <v>871</v>
       </c>
       <c r="B30" s="22" t="s">
-        <v>870</v>
+        <v>872</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="22" t="s">
-        <v>871</v>
+        <v>873</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="22" t="s">
-        <v>872</v>
+        <v>874</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="22" t="s">
-        <v>873</v>
+        <v>875</v>
       </c>
       <c r="B33" s="22" t="s">
-        <v>874</v>
+        <v>876</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="22" t="s">
-        <v>875</v>
+        <v>877</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="22" t="s">
-        <v>876</v>
+        <v>878</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="22" t="s">
-        <v>877</v>
+        <v>879</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="22" t="s">
-        <v>878</v>
+        <v>880</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="22" t="s">
-        <v>879</v>
+        <v>881</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C39" s="28" t="s">
-        <v>880</v>
+        <v>882</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="22" t="s">
-        <v>881</v>
+        <v>883</v>
       </c>
       <c r="B40" s="22" t="s">
-        <v>882</v>
+        <v>884</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="22" t="s">
-        <v>883</v>
+        <v>885</v>
       </c>
       <c r="B41" s="22" t="s">
-        <v>884</v>
+        <v>886</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="22" t="s">
-        <v>885</v>
+        <v>887</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="22" t="s">
-        <v>886</v>
+        <v>888</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="22" t="s">
-        <v>887</v>
+        <v>889</v>
       </c>
       <c r="B44" s="22" t="s">
-        <v>888</v>
+        <v>890</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="22" t="s">
-        <v>889</v>
+        <v>891</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="22" t="s">
-        <v>890</v>
+        <v>892</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="22" t="s">
-        <v>891</v>
+        <v>893</v>
       </c>
       <c r="B47" s="22" t="s">
-        <v>892</v>
+        <v>894</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="22" t="s">
-        <v>893</v>
+        <v>895</v>
       </c>
       <c r="B48" s="22" t="s">
-        <v>894</v>
+        <v>896</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="22" t="s">
-        <v>895</v>
+        <v>897</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="22" t="s">
-        <v>896</v>
+        <v>898</v>
       </c>
       <c r="B50" s="22" t="s">
-        <v>897</v>
+        <v>899</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="22" t="s">
-        <v>898</v>
+        <v>900</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="22" t="s">
-        <v>899</v>
+        <v>901</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="22" t="s">
-        <v>900</v>
+        <v>902</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="22" t="s">
-        <v>901</v>
+        <v>903</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="22" t="s">
-        <v>902</v>
+        <v>904</v>
       </c>
       <c r="B55" s="22" t="s">
-        <v>903</v>
+        <v>905</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="22" t="s">
-        <v>904</v>
+        <v>906</v>
       </c>
       <c r="B56" s="22" t="s">
-        <v>905</v>
+        <v>907</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="22" t="s">
-        <v>906</v>
+        <v>908</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="22" t="s">
-        <v>907</v>
+        <v>909</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="22" t="s">
-        <v>908</v>
+        <v>910</v>
       </c>
       <c r="B59" s="22" t="s">
-        <v>909</v>
+        <v>911</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="22" t="s">
-        <v>910</v>
+        <v>912</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="22" t="s">
-        <v>911</v>
+        <v>913</v>
       </c>
       <c r="B61" s="22" t="s">
-        <v>912</v>
+        <v>914</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="22" t="s">
-        <v>913</v>
+        <v>915</v>
       </c>
       <c r="B62" s="22" t="s">
-        <v>914</v>
+        <v>916</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="22" t="s">
-        <v>915</v>
+        <v>917</v>
       </c>
       <c r="B63" s="22" t="s">
-        <v>916</v>
+        <v>918</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="22" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
       <c r="B64" s="22" t="s">
-        <v>918</v>
+        <v>920</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="22" t="s">
-        <v>919</v>
+        <v>921</v>
       </c>
       <c r="B65" s="22" t="s">
-        <v>920</v>
+        <v>922</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="22" t="s">
-        <v>921</v>
+        <v>923</v>
       </c>
       <c r="B66" s="22" t="s">
-        <v>922</v>
+        <v>924</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="22" t="s">
-        <v>923</v>
+        <v>925</v>
       </c>
       <c r="B67" s="22" t="s">
-        <v>924</v>
+        <v>926</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="22" t="s">
-        <v>925</v>
+        <v>927</v>
       </c>
       <c r="B68" s="22" t="s">
-        <v>926</v>
+        <v>928</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="22" t="s">
+        <v>929</v>
+      </c>
+      <c r="B69" s="22" t="s">
+        <v>930</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
document Octo-GX mappings, add missing mappings
Added mappings for ttyUSB6-8, which are missing and used by
the Octo-GX.
</commit_message>
<xml_diff>
--- a/CCGX-Modbus-TCP-register-list.xlsx
+++ b/CCGX-Modbus-TCP-register-list.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Field list" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2649" uniqueCount="931">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2654" uniqueCount="936">
   <si>
     <t xml:space="preserve">NOTE: Use unit-id 100 for the com.victronenergy.system data, for more information see FAQ.</t>
   </si>
@@ -2361,10 +2361,10 @@
     <t xml:space="preserve">CCGX VE.Direct 1 port (ttyO0)</t>
   </si>
   <si>
-    <t xml:space="preserve">CCGX VE.Direct 2 port, Venus GX VE.Direct 1 port (ttyO2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Venus GX VE.Direct 2 port (ttyO4)</t>
+    <t xml:space="preserve">CCGX VE.Direct port 2, Venus GX VE.Direct port 1, Octo GX port 1 (ttyO2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Venus GX VE.Direct port 2, Octo GX port 2 (ttyO4)</t>
   </si>
   <si>
     <t xml:space="preserve">Venus GX VE.Bus port (ttyO5)</t>
@@ -2499,19 +2499,28 @@
     <t xml:space="preserve">VE.Direct via USB (ttyUSB0)</t>
   </si>
   <si>
-    <t xml:space="preserve">VE.Direct via USB (ttyUSB1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VE.Direct via USB (ttyUSB2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VE.Direct via USB (ttyUSB3)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VE.Direct via USB (ttyUSB4)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VE.Direct via USB (ttyUSB5)</t>
+    <t xml:space="preserve">VE.Direct via USB, Octo GX VE.Direct 3 (ttyUSB1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VE.Direct via USB, Octo GX VE.Direct 4 (ttyUSB2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VE.Direct via USB, Octo GX VE.Direct 5 (ttyUSB3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VE.Direct via USB, Octo GX VE.Direct 6 (ttyUSB4)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VE.Direct via USB, Octo GX VE.Direct 7 (ttyUSB5)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VE.Direct via USB, Octo GX VE.Direct 8 (ttyUSB6)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VE.Direct via USB, Octo GX VE.Direct 9 (ttyUSB7)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VE.Direct via USB, Octo GX VE.Direct 10 (ttyUSB8)</t>
   </si>
   <si>
     <t xml:space="preserve">CAN-bus BMS</t>
@@ -2815,6 +2824,12 @@
   </si>
   <si>
     <t xml:space="preserve">Added mapping for EasySolar-II/Multiplus-II GX VE.Direct ports</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Added mappings for up to 9 USB-connected VE.Direct devices</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Added Octo-GX mappings</t>
   </si>
 </sst>
 </file>
@@ -3167,10 +3182,10 @@
   </sheetPr>
   <dimension ref="A1:N345"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="2" topLeftCell="A321" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G339" activeCellId="0" sqref="G339"/>
+      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13502,10 +13517,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F58"/>
+  <dimension ref="A1:F1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14055,7 +14070,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="22" t="n">
         <v>238</v>
       </c>
@@ -14066,7 +14081,7 @@
         <v>825</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="22" t="n">
         <v>237</v>
       </c>
@@ -14077,7 +14092,7 @@
         <v>826</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="22" t="n">
         <v>236</v>
       </c>
@@ -14088,7 +14103,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="22" t="n">
         <v>235</v>
       </c>
@@ -14099,7 +14114,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="22" t="n">
         <v>233</v>
       </c>
@@ -14110,41 +14125,76 @@
         <v>829</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="22" t="n">
-        <v>225</v>
+        <v>232</v>
       </c>
       <c r="B55" s="22" t="n">
-        <v>512</v>
+        <v>294</v>
       </c>
       <c r="C55" s="22" t="s">
         <v>830</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="26" t="s">
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="22" t="n">
+        <v>231</v>
+      </c>
+      <c r="B56" s="22" t="n">
+        <v>295</v>
+      </c>
+      <c r="C56" s="22" t="s">
         <v>831</v>
       </c>
-      <c r="B57" s="26"/>
-      <c r="C57" s="26"/>
-      <c r="D57" s="26"/>
-      <c r="E57" s="26"/>
-      <c r="F57" s="26"/>
-    </row>
-    <row r="58" customFormat="false" ht="92.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A58" s="27" t="s">
+    </row>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="22" t="n">
+        <v>234</v>
+      </c>
+      <c r="B57" s="22" t="n">
+        <v>296</v>
+      </c>
+      <c r="C57" s="22" t="s">
         <v>832</v>
       </c>
-      <c r="B58" s="27"/>
-      <c r="C58" s="27"/>
-      <c r="D58" s="27"/>
-      <c r="E58" s="27"/>
-      <c r="F58" s="27"/>
-    </row>
+    </row>
+    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="22" t="n">
+        <v>225</v>
+      </c>
+      <c r="B58" s="22" t="n">
+        <v>512</v>
+      </c>
+      <c r="C58" s="22" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="26" t="s">
+        <v>834</v>
+      </c>
+      <c r="B60" s="26"/>
+      <c r="C60" s="26"/>
+      <c r="D60" s="26"/>
+      <c r="E60" s="26"/>
+      <c r="F60" s="26"/>
+    </row>
+    <row r="61" customFormat="false" ht="92.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A61" s="27" t="s">
+        <v>835</v>
+      </c>
+      <c r="B61" s="27"/>
+      <c r="C61" s="27"/>
+      <c r="D61" s="27"/>
+      <c r="E61" s="27"/>
+      <c r="F61" s="27"/>
+    </row>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A57:F57"/>
-    <mergeCell ref="A58:F58"/>
+    <mergeCell ref="A60:F60"/>
+    <mergeCell ref="A61:F61"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -14161,9 +14211,9 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C69"/>
+  <dimension ref="A1:C71"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A45" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -14177,434 +14227,444 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="22" t="s">
-        <v>833</v>
+        <v>836</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>834</v>
+        <v>837</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="22" t="s">
-        <v>835</v>
+        <v>838</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>836</v>
+        <v>839</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="22" t="s">
-        <v>837</v>
+        <v>840</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>838</v>
+        <v>841</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="22" t="s">
-        <v>839</v>
+        <v>842</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>840</v>
+        <v>843</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="22" t="s">
-        <v>841</v>
+        <v>844</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="22" t="s">
-        <v>842</v>
+        <v>845</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="22" t="s">
-        <v>843</v>
+        <v>846</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="22" t="s">
-        <v>844</v>
+        <v>847</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="22" t="s">
-        <v>845</v>
+        <v>848</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>846</v>
+        <v>849</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="22" t="s">
-        <v>847</v>
+        <v>850</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="22" t="s">
-        <v>848</v>
+        <v>851</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="22" t="s">
-        <v>849</v>
+        <v>852</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>850</v>
+        <v>853</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="22" t="s">
-        <v>851</v>
+        <v>854</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="22" t="s">
-        <v>852</v>
+        <v>855</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="22" t="s">
-        <v>853</v>
+        <v>856</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="22" t="s">
-        <v>854</v>
+        <v>857</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="22" t="s">
-        <v>855</v>
+        <v>858</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="22" t="s">
-        <v>856</v>
+        <v>859</v>
       </c>
       <c r="B18" s="22" t="s">
-        <v>857</v>
+        <v>860</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="22" t="s">
-        <v>858</v>
+        <v>861</v>
       </c>
       <c r="B19" s="22" t="s">
-        <v>859</v>
+        <v>862</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="22" t="s">
-        <v>860</v>
+        <v>863</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="22" t="s">
-        <v>861</v>
+        <v>864</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="22" t="s">
-        <v>862</v>
+        <v>865</v>
       </c>
       <c r="B22" s="22" t="s">
-        <v>863</v>
+        <v>866</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="22" t="s">
-        <v>864</v>
+        <v>867</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="22" t="s">
-        <v>865</v>
+        <v>868</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="22" t="s">
-        <v>866</v>
+        <v>869</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="22" t="s">
-        <v>867</v>
+        <v>870</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="22" t="s">
-        <v>868</v>
+        <v>871</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="22" t="s">
-        <v>869</v>
+        <v>872</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="22" t="s">
-        <v>870</v>
+        <v>873</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="22" t="s">
-        <v>871</v>
+        <v>874</v>
       </c>
       <c r="B30" s="22" t="s">
-        <v>872</v>
+        <v>875</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="22" t="s">
-        <v>873</v>
+        <v>876</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="22" t="s">
-        <v>874</v>
+        <v>877</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="22" t="s">
-        <v>875</v>
+        <v>878</v>
       </c>
       <c r="B33" s="22" t="s">
-        <v>876</v>
+        <v>879</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="22" t="s">
-        <v>877</v>
+        <v>880</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="22" t="s">
-        <v>878</v>
+        <v>881</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="22" t="s">
-        <v>879</v>
+        <v>882</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="22" t="s">
-        <v>880</v>
+        <v>883</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="22" t="s">
-        <v>881</v>
+        <v>884</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C39" s="28" t="s">
-        <v>882</v>
+        <v>885</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="22" t="s">
-        <v>883</v>
+        <v>886</v>
       </c>
       <c r="B40" s="22" t="s">
-        <v>884</v>
+        <v>887</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="22" t="s">
-        <v>885</v>
+        <v>888</v>
       </c>
       <c r="B41" s="22" t="s">
-        <v>886</v>
+        <v>889</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="22" t="s">
-        <v>887</v>
+        <v>890</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="22" t="s">
-        <v>888</v>
+        <v>891</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="22" t="s">
-        <v>889</v>
+        <v>892</v>
       </c>
       <c r="B44" s="22" t="s">
-        <v>890</v>
+        <v>893</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="22" t="s">
-        <v>891</v>
+        <v>894</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="22" t="s">
-        <v>892</v>
+        <v>895</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="22" t="s">
-        <v>893</v>
+        <v>896</v>
       </c>
       <c r="B47" s="22" t="s">
-        <v>894</v>
+        <v>897</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="22" t="s">
-        <v>895</v>
+        <v>898</v>
       </c>
       <c r="B48" s="22" t="s">
-        <v>896</v>
+        <v>899</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="22" t="s">
-        <v>897</v>
+        <v>900</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="22" t="s">
-        <v>898</v>
+        <v>901</v>
       </c>
       <c r="B50" s="22" t="s">
-        <v>899</v>
+        <v>902</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="22" t="s">
-        <v>900</v>
+        <v>903</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="22" t="s">
-        <v>901</v>
+        <v>904</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="22" t="s">
-        <v>902</v>
+        <v>905</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="22" t="s">
-        <v>903</v>
+        <v>906</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="22" t="s">
-        <v>904</v>
+        <v>907</v>
       </c>
       <c r="B55" s="22" t="s">
-        <v>905</v>
+        <v>908</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="22" t="s">
-        <v>906</v>
+        <v>909</v>
       </c>
       <c r="B56" s="22" t="s">
-        <v>907</v>
+        <v>910</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="22" t="s">
-        <v>908</v>
+        <v>911</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="22" t="s">
-        <v>909</v>
+        <v>912</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="22" t="s">
-        <v>910</v>
+        <v>913</v>
       </c>
       <c r="B59" s="22" t="s">
-        <v>911</v>
+        <v>914</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="22" t="s">
-        <v>912</v>
+        <v>915</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="22" t="s">
-        <v>913</v>
+        <v>916</v>
       </c>
       <c r="B61" s="22" t="s">
-        <v>914</v>
+        <v>917</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="22" t="s">
-        <v>915</v>
+        <v>918</v>
       </c>
       <c r="B62" s="22" t="s">
-        <v>916</v>
+        <v>919</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="22" t="s">
-        <v>917</v>
+        <v>920</v>
       </c>
       <c r="B63" s="22" t="s">
-        <v>918</v>
+        <v>921</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="22" t="s">
-        <v>919</v>
+        <v>922</v>
       </c>
       <c r="B64" s="22" t="s">
-        <v>920</v>
+        <v>923</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="22" t="s">
-        <v>921</v>
+        <v>924</v>
       </c>
       <c r="B65" s="22" t="s">
-        <v>922</v>
+        <v>925</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="22" t="s">
-        <v>923</v>
+        <v>926</v>
       </c>
       <c r="B66" s="22" t="s">
-        <v>924</v>
+        <v>927</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="22" t="s">
-        <v>925</v>
+        <v>928</v>
       </c>
       <c r="B67" s="22" t="s">
-        <v>926</v>
+        <v>929</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="22" t="s">
-        <v>927</v>
+        <v>930</v>
       </c>
       <c r="B68" s="22" t="s">
-        <v>928</v>
+        <v>931</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="22" t="s">
-        <v>929</v>
+        <v>932</v>
       </c>
       <c r="B69" s="22" t="s">
-        <v>930</v>
+        <v>933</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B70" s="22" t="s">
+        <v>934</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B71" s="22" t="s">
+        <v>935</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
GridLost alarm moved to .vebus service
</commit_message>
<xml_diff>
--- a/CCGX-Modbus-TCP-register-list.xlsx
+++ b/CCGX-Modbus-TCP-register-list.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Field list" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2654" uniqueCount="936">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2656" uniqueCount="938">
   <si>
     <t xml:space="preserve">NOTE: Use unit-id 100 for the com.victronenergy.system data, for more information see FAQ.</t>
   </si>
@@ -396,489 +396,489 @@
     <t xml:space="preserve">System value etc. AND: Positive: power flowing from the Multi to the dc system. Negative: the other way around.</t>
   </si>
   <si>
+    <t xml:space="preserve">com.victronenergy.vebus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Input voltage phase 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Ac/ActiveIn/L1/V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V AC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Input voltage phase 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Ac/ActiveIn/L2/V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Input voltage phase 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Ac/ActiveIn/L3/V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Input current phase 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Ac/ActiveIn/L1/I</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A AC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Positive: current flowing from mains to Multi. Negative: current flowing from Multi to mains.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Input current phase 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Ac/ActiveIn/L2/I</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Input current phase 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Ac/ActiveIn/L3/I</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Input frequency 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-326.68 to 326.68</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Ac/ActiveIn/L1/F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Input frequency 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Ac/ActiveIn/L2/F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Input frequency 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Ac/ActiveIn/L3/F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Input power 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-326680 to 326680</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Ac/ActiveIn/L1/P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VA or Watts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sign meaning equal to Input current</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Input power 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Ac/ActiveIn/L2/P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Input power 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Ac/ActiveIn/L3/P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sign meaning eaqual to Input current</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Output voltage phase 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Ac/Out/L1/V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Output voltage phase 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Ac/Out/L2/V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Output voltage phase 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Ac/Out/L3/V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Output current phase 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Ac/Out/L1/I</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Postive: current flowing from Multi to the load. Negative: current flowing from load to the Multi.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Output current phase 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Ac/Out/L2/I</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Output current phase 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Ac/Out/L3/I</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Output frequency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Ac/Out/L1/F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Active input current limit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Ac/ActiveIn/CurrentLimit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">See Venus-OS manual for limitations, for example when VE.Bus BMS or DMC is installed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Output power 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Ac/Out/L1/P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sign meaning equal to Output current</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Output power 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Ac/Out/L2/P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Output power 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Ac/Out/L3/P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Battery voltage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 to 653.36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Dc/0/Voltage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Battery current</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Dc/0/Current</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Positive: current flowing from the Multi to the dc system. Negative: the other way around.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phase count</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Ac/NumberOfPhases</t>
+  </si>
+  <si>
+    <t xml:space="preserve">count</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Active input</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Ac/ActiveIn/ActiveInput</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0=AC Input 1;1=AC Input 2;240=Disconnected</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VE.Bus state of charge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Soc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VE.Bus state</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/State</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0=Off;1=Low Power;2=Fault;3=Bulk;4=Absorption;5=Float;6=Storage;7=Equalize;8=Passthru;9=Inverting;10=Power assist;11=Power supply;252=Bulk protection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VE.Bus Error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/VebusError</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0=No error;1=VE.Bus Error 1: Device is switched off because one of the other phases in the system has switched off;2=VE.Bus Error 2: New and old types MK2 are mixed in the system;3=VE.Bus Error 3: Not all- or more than- the expected devices were found in the system;4=VE.Bus Error 4: No other device whatsoever detected;5=VE.Bus Error 5: Overvoltage on AC-out;6=VE.Bus Error 6: Error in DDC Program;7=VE.Bus BMS connected- which requires an Assistant- but no assistant found;10=VE.Bus Error 10: System time synchronisation problem occurred;14=VE.Bus Error 14: Device cannot transmit data;16=VE.Bus Error 16: Dongle missing;17=VE.Bus Error 17: One of the devices assumed master status because the original master failed;18=VE.Bus Error 18: AC Overvoltage on the output of a slave has occurred while already switched off;22=VE.Bus Error 22: This device cannot function as slave;24=VE.Bus Error 24: Switch-over system protection initiated;25=VE.Bus Error 25: Firmware incompatibility. The firmware of one of the connected device is not sufficiently up to date to operate in conjunction with this device;26=VE.Bus Error 26: Internal error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Switch Position</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Mode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1=Charger Only;2=Inverter Only;3=On;4=Off</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temperature alarm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Alarms/HighTemperature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0=Ok;1=Warning;2=Alarm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Low battery alarm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Alarms/LowBattery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Overload alarm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Alarms/Overload</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ESS power setpoint phase 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Hub4/L1/AcPowerSetpoint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ESS Mode 3 - Instructs the multi to charge/discharge with giving power. Negative = discharge. Used by the control loop in grid-parallel systems.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ESS disable charge flag phase</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Hub4/DisableCharge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0=Charge allowed;1=Charge disabled</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ESS Mode 3 - Enables/Disables charge (0=enabled, 1=disabled). Note that power setpoint will yield to this setting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ESS disable feedback flag phase</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Hub4/DisableFeedIn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0=Feed in allowed;1=Feed in disabled</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ESS Mode 3 - Enables/Disables feedback (0=enabled, 1=disabled). Note that power setpoint will yield to this setting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ESS power setpoint phase 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Hub4/L2/AcPowerSetpoint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ESS power setpoint phase 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Hub4/L3/AcPowerSetpoint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temperatur sensor alarm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Alarms/TemperatureSensor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Voltage sensor alarm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Alarms/VoltageSensor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temperature alarm L1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Alarms/L1/HighTemperature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Low battery alarm L1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Alarms/L1/LowBattery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Overload alarm L1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Alarms/L1/Overload</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ripple alarm L1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Alarms/L1/Ripple</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temperature alarm L2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Alarms/L2/HighTemperature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Low battery alarm L2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Alarms/L2/LowBattery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Overload alarm L2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Alarms/L2/Overload</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ripple alarm L2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Alarms/L2/Ripple</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temperature alarm L3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Alarms/L3/HighTemperature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Low battery alarm L3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Alarms/L3/LowBattery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Overload alarm L3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Alarms/L3/Overload</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ripple alarm L3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Alarms/L3/Ripple</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Disable PV inverter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/PvInverter/Disable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0=PV enabled;1=PV disabled</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Disable PV inverter on AC out (using frequency shifting). Only works when vebus device is in inverter mode. Needs ESS or PV inverter assistant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VE.Bus BMS allows battery to be charged</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Bms/AllowToCharge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0=No;1=Yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VE.Bus BMS allows the battery to be charged</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VE.Bus BMS allows battery to be discharged</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Bms/AllowToDischarge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VE.Bus BMS allows the battery to be discharged</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VE.Bus BMS is expected</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Bms/BmsExpected</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Presence of VE.Bus BMS is expected based on vebus settings (presence of ESS or BMS assistant)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VE.Bus BMS error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Bms/Error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Battery temperature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Dc/0/Temperature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Degrees celsius</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VE.Bus Reset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/SystemReset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0=No action; 1=VE.Bus reset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phase rotation warning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Alarms/PhaseRotation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0=Ok;1=Warning</t>
+  </si>
+  <si>
     <t xml:space="preserve">Grid lost alarm</t>
   </si>
   <si>
-    <t xml:space="preserve">/Ac/Alarms/GridLost</t>
+    <t xml:space="preserve">/Alarms/GridLost</t>
   </si>
   <si>
     <t xml:space="preserve">0=Ok;2=Alarm</t>
   </si>
   <si>
-    <t xml:space="preserve">com.victronenergy.vebus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Input voltage phase 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/Ac/ActiveIn/L1/V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">V AC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Input voltage phase 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/Ac/ActiveIn/L2/V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Input voltage phase 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/Ac/ActiveIn/L3/V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Input current phase 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/Ac/ActiveIn/L1/I</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A AC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Positive: current flowing from mains to Multi. Negative: current flowing from Multi to mains.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Input current phase 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/Ac/ActiveIn/L2/I</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Input current phase 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/Ac/ActiveIn/L3/I</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Input frequency 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-326.68 to 326.68</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/Ac/ActiveIn/L1/F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Input frequency 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/Ac/ActiveIn/L2/F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Input frequency 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/Ac/ActiveIn/L3/F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Input power 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-326680 to 326680</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/Ac/ActiveIn/L1/P</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VA or Watts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sign meaning equal to Input current</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Input power 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/Ac/ActiveIn/L2/P</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Input power 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/Ac/ActiveIn/L3/P</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sign meaning eaqual to Input current</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Output voltage phase 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/Ac/Out/L1/V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Output voltage phase 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/Ac/Out/L2/V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Output voltage phase 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/Ac/Out/L3/V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Output current phase 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/Ac/Out/L1/I</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Postive: current flowing from Multi to the load. Negative: current flowing from load to the Multi.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Output current phase 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/Ac/Out/L2/I</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Output current phase 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/Ac/Out/L3/I</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Output frequency</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/Ac/Out/L1/F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Active input current limit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/Ac/ActiveIn/CurrentLimit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">See Venus-OS manual for limitations, for example when VE.Bus BMS or DMC is installed.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Output power 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/Ac/Out/L1/P</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sign meaning equal to Output current</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Output power 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/Ac/Out/L2/P</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Output power 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/Ac/Out/L3/P</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Battery voltage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0 to 653.36</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/Dc/0/Voltage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Battery current</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/Dc/0/Current</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Positive: current flowing from the Multi to the dc system. Negative: the other way around.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phase count</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/Ac/NumberOfPhases</t>
-  </si>
-  <si>
-    <t xml:space="preserve">count</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Active input</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/Ac/ActiveIn/ActiveInput</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0=AC Input 1;1=AC Input 2;240=Disconnected</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VE.Bus state of charge</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/Soc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VE.Bus state</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/State</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0=Off;1=Low Power;2=Fault;3=Bulk;4=Absorption;5=Float;6=Storage;7=Equalize;8=Passthru;9=Inverting;10=Power assist;11=Power supply;252=Bulk protection</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VE.Bus Error</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/VebusError</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0=No error;1=VE.Bus Error 1: Device is switched off because one of the other phases in the system has switched off;2=VE.Bus Error 2: New and old types MK2 are mixed in the system;3=VE.Bus Error 3: Not all- or more than- the expected devices were found in the system;4=VE.Bus Error 4: No other device whatsoever detected;5=VE.Bus Error 5: Overvoltage on AC-out;6=VE.Bus Error 6: Error in DDC Program;7=VE.Bus BMS connected- which requires an Assistant- but no assistant found;10=VE.Bus Error 10: System time synchronisation problem occurred;14=VE.Bus Error 14: Device cannot transmit data;16=VE.Bus Error 16: Dongle missing;17=VE.Bus Error 17: One of the devices assumed master status because the original master failed;18=VE.Bus Error 18: AC Overvoltage on the output of a slave has occurred while already switched off;22=VE.Bus Error 22: This device cannot function as slave;24=VE.Bus Error 24: Switch-over system protection initiated;25=VE.Bus Error 25: Firmware incompatibility. The firmware of one of the connected device is not sufficiently up to date to operate in conjunction with this device;26=VE.Bus Error 26: Internal error</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Switch Position</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/Mode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1=Charger Only;2=Inverter Only;3=On;4=Off</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Temperature alarm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/Alarms/HighTemperature</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0=Ok;1=Warning;2=Alarm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Low battery alarm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/Alarms/LowBattery</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Overload alarm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/Alarms/Overload</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ESS power setpoint phase 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/Hub4/L1/AcPowerSetpoint</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ESS Mode 3 - Instructs the multi to charge/discharge with giving power. Negative = discharge. Used by the control loop in grid-parallel systems.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ESS disable charge flag phase</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/Hub4/DisableCharge</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0=Charge allowed;1=Charge disabled</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ESS Mode 3 - Enables/Disables charge (0=enabled, 1=disabled). Note that power setpoint will yield to this setting</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ESS disable feedback flag phase</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/Hub4/DisableFeedIn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0=Feed in allowed;1=Feed in disabled</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ESS Mode 3 - Enables/Disables feedback (0=enabled, 1=disabled). Note that power setpoint will yield to this setting</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ESS power setpoint phase 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/Hub4/L2/AcPowerSetpoint</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ESS power setpoint phase 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/Hub4/L3/AcPowerSetpoint</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Temperatur sensor alarm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/Alarms/TemperatureSensor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Voltage sensor alarm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/Alarms/VoltageSensor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Temperature alarm L1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/Alarms/L1/HighTemperature</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Low battery alarm L1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/Alarms/L1/LowBattery</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Overload alarm L1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/Alarms/L1/Overload</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ripple alarm L1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/Alarms/L1/Ripple</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Temperature alarm L2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/Alarms/L2/HighTemperature</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Low battery alarm L2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/Alarms/L2/LowBattery</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Overload alarm L2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/Alarms/L2/Overload</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ripple alarm L2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/Alarms/L2/Ripple</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Temperature alarm L3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/Alarms/L3/HighTemperature</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Low battery alarm L3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/Alarms/L3/LowBattery</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Overload alarm L3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/Alarms/L3/Overload</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ripple alarm L3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/Alarms/L3/Ripple</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Disable PV inverter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/PvInverter/Disable</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0=PV enabled;1=PV disabled</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Disable PV inverter on AC out (using frequency shifting). Only works when vebus device is in inverter mode. Needs ESS or PV inverter assistant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VE.Bus BMS allows battery to be charged</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/Bms/AllowToCharge</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0=No;1=Yes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VE.Bus BMS allows the battery to be charged</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VE.Bus BMS allows battery to be discharged</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/Bms/AllowToDischarge</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VE.Bus BMS allows the battery to be discharged</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VE.Bus BMS is expected</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/Bms/BmsExpected</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Presence of VE.Bus BMS is expected based on vebus settings (presence of ESS or BMS assistant)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VE.Bus BMS error</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/Bms/Error</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Battery temperature</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/Dc/0/Temperature</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Degrees celsius</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VE.Bus Reset</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/SystemReset</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0=No action; 1=VE.Bus reset</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phase rotation warning</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/Alarms/PhaseRotation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0=Ok;1=Warning</t>
-  </si>
-  <si>
     <t xml:space="preserve">com.victronenergy.battery</t>
   </si>
   <si>
@@ -2830,6 +2830,12 @@
   </si>
   <si>
     <t xml:space="preserve">Added Octo-GX mappings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rev 29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GridLost alarm moved to the vebus service</t>
   </si>
 </sst>
 </file>
@@ -3182,10 +3188,10 @@
   </sheetPr>
   <dimension ref="A1:N345"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="2" topLeftCell="A261" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A278" activeCellId="0" sqref="A278"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4369,44 +4375,44 @@
         <v>123</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>12</v>
+        <v>124</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C38" s="1" t="n">
-        <v>830</v>
+        <v>3</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E38" s="1" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>29</v>
+        <v>79</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H38" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>128</v>
       </c>
       <c r="C39" s="1" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>20</v>
@@ -4424,18 +4430,18 @@
         <v>17</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C40" s="1" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>20</v>
@@ -4447,53 +4453,56 @@
         <v>79</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H40" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C41" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>20</v>
+        <v>59</v>
       </c>
       <c r="E41" s="1" t="n">
         <v>10</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="G41" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I41" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="H41" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I41" s="1" t="s">
-        <v>130</v>
+      <c r="J41" s="1" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C42" s="1" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>59</v>
@@ -4505,27 +4514,27 @@
         <v>84</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H42" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C43" s="1" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>59</v>
@@ -4537,36 +4546,36 @@
         <v>84</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H43" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C44" s="1" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>59</v>
       </c>
       <c r="E44" s="1" t="n">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>84</v>
+        <v>141</v>
       </c>
       <c r="G44" s="1" t="s">
         <v>142</v>
@@ -4575,21 +4584,18 @@
         <v>17</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="J44" s="1" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C45" s="1" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>59</v>
@@ -4598,7 +4604,7 @@
         <v>100</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="G45" s="1" t="s">
         <v>145</v>
@@ -4607,18 +4613,18 @@
         <v>17</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C46" s="1" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>59</v>
@@ -4627,36 +4633,36 @@
         <v>100</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H46" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C47" s="1" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>59</v>
       </c>
       <c r="E47" s="1" t="n">
-        <v>100</v>
+        <v>0.1</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="G47" s="1" t="s">
         <v>150</v>
@@ -4665,18 +4671,21 @@
         <v>17</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>146</v>
+        <v>151</v>
+      </c>
+      <c r="J47" s="1" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="C48" s="1" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>59</v>
@@ -4685,30 +4694,30 @@
         <v>0.1</v>
       </c>
       <c r="F48" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I48" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="J48" s="1" t="s">
         <v>152</v>
-      </c>
-      <c r="G48" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="H48" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I48" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="J48" s="1" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C49" s="1" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>59</v>
@@ -4717,39 +4726,39 @@
         <v>0.1</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="G49" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I49" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="J49" s="1" t="s">
         <v>157</v>
-      </c>
-      <c r="H49" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I49" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="J49" s="1" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>158</v>
       </c>
       <c r="C50" s="1" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>59</v>
+        <v>20</v>
       </c>
       <c r="E50" s="1" t="n">
-        <v>0.1</v>
+        <v>10</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>152</v>
+        <v>79</v>
       </c>
       <c r="G50" s="1" t="s">
         <v>159</v>
@@ -4758,21 +4767,18 @@
         <v>17</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="J50" s="1" t="s">
-        <v>160</v>
+        <v>127</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C51" s="1" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>20</v>
@@ -4784,24 +4790,24 @@
         <v>79</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H51" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C52" s="1" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>20</v>
@@ -4813,53 +4819,56 @@
         <v>79</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H52" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C53" s="1" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>20</v>
+        <v>59</v>
       </c>
       <c r="E53" s="1" t="n">
         <v>10</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="G53" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I53" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="J53" s="1" t="s">
         <v>166</v>
-      </c>
-      <c r="H53" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I53" s="1" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>167</v>
       </c>
       <c r="C54" s="1" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>59</v>
@@ -4877,21 +4886,21 @@
         <v>17</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="J54" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C55" s="1" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>59</v>
@@ -4903,120 +4912,120 @@
         <v>84</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H55" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="J55" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C56" s="1" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>59</v>
       </c>
       <c r="E56" s="1" t="n">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>84</v>
+        <v>141</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H56" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="J56" s="1" t="s">
-        <v>169</v>
+        <v>143</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C57" s="1" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>59</v>
       </c>
       <c r="E57" s="1" t="n">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>144</v>
+        <v>84</v>
       </c>
       <c r="G57" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="H57" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I57" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="H57" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I57" s="1" t="s">
-        <v>146</v>
+      <c r="J57" s="21" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C58" s="1" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D58" s="2" t="s">
         <v>59</v>
       </c>
       <c r="E58" s="1" t="n">
-        <v>10</v>
+        <v>0.1</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>84</v>
+        <v>149</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="J58" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="J58" s="1" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>180</v>
       </c>
       <c r="C59" s="1" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>59</v>
@@ -5025,7 +5034,7 @@
         <v>0.1</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="G59" s="1" t="s">
         <v>181</v>
@@ -5034,21 +5043,21 @@
         <v>17</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="J59" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C60" s="1" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D60" s="2" t="s">
         <v>59</v>
@@ -5057,39 +5066,39 @@
         <v>0.1</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H60" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="J60" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B61" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C61" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E61" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="F61" s="3" t="s">
         <v>185</v>
-      </c>
-      <c r="C61" s="1" t="n">
-        <v>25</v>
-      </c>
-      <c r="D61" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E61" s="1" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="F61" s="3" t="s">
-        <v>152</v>
       </c>
       <c r="G61" s="1" t="s">
         <v>186</v>
@@ -5098,59 +5107,59 @@
         <v>17</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="J61" s="1" t="s">
-        <v>182</v>
+        <v>81</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>187</v>
       </c>
       <c r="C62" s="1" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>20</v>
+        <v>59</v>
       </c>
       <c r="E62" s="1" t="n">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="F62" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="G62" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="G62" s="1" t="s">
+      <c r="H62" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I62" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="J62" s="1" t="s">
         <v>189</v>
-      </c>
-      <c r="H62" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I62" s="1" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>190</v>
       </c>
       <c r="C63" s="1" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>59</v>
+        <v>20</v>
       </c>
       <c r="E63" s="1" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>84</v>
+        <v>29</v>
       </c>
       <c r="G63" s="1" t="s">
         <v>191</v>
@@ -5159,21 +5168,18 @@
         <v>17</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="J63" s="1" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>193</v>
       </c>
       <c r="C64" s="1" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>20</v>
@@ -5196,71 +5202,71 @@
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>196</v>
       </c>
       <c r="C65" s="1" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D65" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E65" s="1" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>29</v>
+        <v>79</v>
       </c>
       <c r="G65" s="1" t="s">
         <v>197</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>198</v>
+        <v>93</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B66" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C66" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E66" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F66" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G66" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="C66" s="1" t="n">
-        <v>30</v>
-      </c>
-      <c r="D66" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E66" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="F66" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="G66" s="1" t="s">
+      <c r="H66" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I66" s="1" t="s">
         <v>200</v>
-      </c>
-      <c r="H66" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I66" s="1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>201</v>
       </c>
       <c r="C67" s="1" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D67" s="2" t="s">
         <v>20</v>
@@ -5283,13 +5289,13 @@
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>204</v>
       </c>
       <c r="C68" s="1" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>20</v>
@@ -5304,21 +5310,24 @@
         <v>205</v>
       </c>
       <c r="H68" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="I68" s="1" t="s">
         <v>206</v>
       </c>
+      <c r="J68" s="21" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>207</v>
       </c>
       <c r="C69" s="1" t="n">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D69" s="2" t="s">
         <v>20</v>
@@ -5333,24 +5342,21 @@
         <v>208</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="I69" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="J69" s="21" t="s">
-        <v>179</v>
-      </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>210</v>
       </c>
       <c r="C70" s="1" t="n">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D70" s="2" t="s">
         <v>20</v>
@@ -5368,18 +5374,18 @@
         <v>17</v>
       </c>
       <c r="I70" s="1" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C71" s="1" t="n">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D71" s="2" t="s">
         <v>20</v>
@@ -5391,62 +5397,65 @@
         <v>29</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H71" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I71" s="1" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B72" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="C72" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E72" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F72" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G72" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="C72" s="1" t="n">
-        <v>36</v>
-      </c>
-      <c r="D72" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E72" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="F72" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G72" s="1" t="s">
+      <c r="H72" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I72" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J72" s="1" t="s">
         <v>216</v>
-      </c>
-      <c r="H72" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I72" s="1" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>217</v>
       </c>
       <c r="C73" s="1" t="n">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>59</v>
+        <v>20</v>
       </c>
       <c r="E73" s="1" t="n">
         <v>1</v>
       </c>
       <c r="F73" s="3" t="s">
-        <v>60</v>
+        <v>29</v>
       </c>
       <c r="G73" s="1" t="s">
         <v>218</v>
@@ -5455,21 +5464,21 @@
         <v>23</v>
       </c>
       <c r="I73" s="1" t="s">
-        <v>31</v>
+        <v>219</v>
       </c>
       <c r="J73" s="1" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C74" s="1" t="n">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>20</v>
@@ -5481,59 +5490,59 @@
         <v>29</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="H74" s="1" t="s">
         <v>23</v>
       </c>
       <c r="I74" s="1" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="J74" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C75" s="1" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>20</v>
+        <v>59</v>
       </c>
       <c r="E75" s="1" t="n">
         <v>1</v>
       </c>
       <c r="F75" s="3" t="s">
-        <v>29</v>
+        <v>60</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="H75" s="1" t="s">
         <v>23</v>
       </c>
       <c r="I75" s="1" t="s">
-        <v>226</v>
+        <v>31</v>
       </c>
       <c r="J75" s="1" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C76" s="1" t="n">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D76" s="2" t="s">
         <v>59</v>
@@ -5545,7 +5554,7 @@
         <v>60</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H76" s="1" t="s">
         <v>23</v>
@@ -5554,50 +5563,47 @@
         <v>31</v>
       </c>
       <c r="J76" s="1" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B77" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="C77" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E77" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F77" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G77" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="C77" s="1" t="n">
-        <v>41</v>
-      </c>
-      <c r="D77" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E77" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="F77" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="G77" s="1" t="s">
-        <v>231</v>
-      </c>
       <c r="H77" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="I77" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="J77" s="1" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C78" s="1" t="n">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D78" s="2" t="s">
         <v>20</v>
@@ -5609,24 +5615,24 @@
         <v>29</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H78" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I78" s="1" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C79" s="1" t="n">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D79" s="2" t="s">
         <v>20</v>
@@ -5638,24 +5644,24 @@
         <v>29</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="H79" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I79" s="1" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C80" s="1" t="n">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D80" s="2" t="s">
         <v>20</v>
@@ -5667,24 +5673,24 @@
         <v>29</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H80" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I80" s="1" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C81" s="1" t="n">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D81" s="2" t="s">
         <v>20</v>
@@ -5696,24 +5702,24 @@
         <v>29</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="H81" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I81" s="1" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C82" s="1" t="n">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D82" s="2" t="s">
         <v>20</v>
@@ -5725,24 +5731,24 @@
         <v>29</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="H82" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I82" s="1" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C83" s="1" t="n">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D83" s="2" t="s">
         <v>20</v>
@@ -5754,24 +5760,24 @@
         <v>29</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H83" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I83" s="1" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C84" s="1" t="n">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D84" s="2" t="s">
         <v>20</v>
@@ -5783,24 +5789,24 @@
         <v>29</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="H84" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I84" s="1" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C85" s="1" t="n">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D85" s="2" t="s">
         <v>20</v>
@@ -5812,24 +5818,24 @@
         <v>29</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="H85" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I85" s="1" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C86" s="1" t="n">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D86" s="2" t="s">
         <v>20</v>
@@ -5841,24 +5847,24 @@
         <v>29</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="H86" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I86" s="1" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C87" s="1" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D87" s="2" t="s">
         <v>20</v>
@@ -5870,24 +5876,24 @@
         <v>29</v>
       </c>
       <c r="G87" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="H87" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I87" s="1" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C88" s="1" t="n">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D88" s="2" t="s">
         <v>20</v>
@@ -5899,24 +5905,24 @@
         <v>29</v>
       </c>
       <c r="G88" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="H88" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I88" s="1" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C89" s="1" t="n">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D89" s="2" t="s">
         <v>20</v>
@@ -5928,24 +5934,24 @@
         <v>29</v>
       </c>
       <c r="G89" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="H89" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I89" s="1" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C90" s="1" t="n">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D90" s="2" t="s">
         <v>20</v>
@@ -5957,24 +5963,24 @@
         <v>29</v>
       </c>
       <c r="G90" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H90" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I90" s="1" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C91" s="1" t="n">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D91" s="2" t="s">
         <v>20</v>
@@ -5986,24 +5992,27 @@
         <v>29</v>
       </c>
       <c r="G91" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="H91" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I91" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="H91" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I91" s="1" t="s">
-        <v>212</v>
+      <c r="J91" s="1" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="C92" s="1" t="n">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D92" s="2" t="s">
         <v>20</v>
@@ -6015,27 +6024,27 @@
         <v>29</v>
       </c>
       <c r="G92" s="1" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="H92" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="I92" s="1" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="J92" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C93" s="1" t="n">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D93" s="2" t="s">
         <v>20</v>
@@ -6047,13 +6056,13 @@
         <v>29</v>
       </c>
       <c r="G93" s="1" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="H93" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I93" s="1" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="J93" s="1" t="s">
         <v>267</v>
@@ -6061,13 +6070,13 @@
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>268</v>
       </c>
       <c r="C94" s="1" t="n">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D94" s="2" t="s">
         <v>20</v>
@@ -6085,7 +6094,7 @@
         <v>17</v>
       </c>
       <c r="I94" s="1" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="J94" s="1" t="s">
         <v>270</v>
@@ -6093,13 +6102,13 @@
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>271</v>
       </c>
       <c r="C95" s="1" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D95" s="2" t="s">
         <v>20</v>
@@ -6117,65 +6126,62 @@
         <v>17</v>
       </c>
       <c r="I95" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="J95" s="1" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B96" s="1" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="B96" s="1" t="s">
+      <c r="C96" s="1" t="n">
+        <v>61</v>
+      </c>
+      <c r="D96" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E96" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="F96" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="G96" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="C96" s="1" t="n">
-        <v>60</v>
-      </c>
-      <c r="D96" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E96" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="F96" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G96" s="1" t="s">
+      <c r="H96" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I96" s="1" t="s">
         <v>275</v>
-      </c>
-      <c r="H96" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I96" s="1" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="B97" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B97" s="22" t="s">
         <v>276</v>
       </c>
       <c r="C97" s="1" t="n">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>59</v>
+        <v>20</v>
       </c>
       <c r="E97" s="1" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F97" s="3" t="s">
-        <v>84</v>
+        <v>29</v>
       </c>
       <c r="G97" s="1" t="s">
         <v>277</v>
       </c>
       <c r="H97" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="I97" s="1" t="s">
         <v>278</v>
@@ -6183,13 +6189,13 @@
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B98" s="22" t="s">
         <v>279</v>
       </c>
       <c r="C98" s="1" t="n">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D98" s="2" t="s">
         <v>20</v>
@@ -6204,7 +6210,7 @@
         <v>280</v>
       </c>
       <c r="H98" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="I98" s="1" t="s">
         <v>281</v>
@@ -6212,13 +6218,13 @@
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="B99" s="22" t="s">
+        <v>124</v>
+      </c>
+      <c r="B99" s="1" t="s">
         <v>282</v>
       </c>
       <c r="C99" s="1" t="n">
-        <v>63</v>
+        <v>830</v>
       </c>
       <c r="D99" s="2" t="s">
         <v>20</v>
@@ -6244,7 +6250,7 @@
         <v>285</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C100" s="1" t="n">
         <v>259</v>
@@ -6256,10 +6262,10 @@
         <v>100</v>
       </c>
       <c r="F100" s="3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G100" s="1" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="H100" s="1" t="s">
         <v>17</v>
@@ -6285,7 +6291,7 @@
         <v>100</v>
       </c>
       <c r="F101" s="3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G101" s="1" t="s">
         <v>287</v>
@@ -6317,7 +6323,7 @@
         <v>84</v>
       </c>
       <c r="G102" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="H102" s="1" t="s">
         <v>17</v>
@@ -6334,7 +6340,7 @@
         <v>285</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="C103" s="1" t="n">
         <v>262</v>
@@ -6349,13 +6355,13 @@
         <v>84</v>
       </c>
       <c r="G103" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="H103" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I103" s="1" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="J103" s="1" t="s">
         <v>289</v>
@@ -6378,7 +6384,7 @@
         <v>100</v>
       </c>
       <c r="F104" s="3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G104" s="1" t="s">
         <v>291</v>
@@ -6407,7 +6413,7 @@
         <v>100</v>
       </c>
       <c r="F105" s="3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G105" s="1" t="s">
         <v>293</v>
@@ -6471,7 +6477,7 @@
         <v>79</v>
       </c>
       <c r="G107" s="1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="H107" s="1" t="s">
         <v>17</v>
@@ -6706,7 +6712,7 @@
         <v>29</v>
       </c>
       <c r="G115" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="H115" s="1" t="s">
         <v>17</v>
@@ -7020,7 +7026,7 @@
         <v>17</v>
       </c>
       <c r="I125" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="J125" s="1" t="s">
         <v>327</v>
@@ -7052,7 +7058,7 @@
         <v>17</v>
       </c>
       <c r="I126" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="J126" s="1" t="s">
         <v>327</v>
@@ -7107,7 +7113,7 @@
         <v>100</v>
       </c>
       <c r="F128" s="3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G128" s="1" t="s">
         <v>341</v>
@@ -7139,7 +7145,7 @@
         <v>100</v>
       </c>
       <c r="F129" s="3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G129" s="1" t="s">
         <v>343</v>
@@ -7212,7 +7218,7 @@
         <v>17</v>
       </c>
       <c r="I131" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="J131" s="1" t="s">
         <v>327</v>
@@ -7244,7 +7250,7 @@
         <v>17</v>
       </c>
       <c r="I132" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="J132" s="1" t="s">
         <v>327</v>
@@ -7276,7 +7282,7 @@
         <v>17</v>
       </c>
       <c r="I133" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="J133" s="1" t="s">
         <v>327</v>
@@ -7308,7 +7314,7 @@
         <v>17</v>
       </c>
       <c r="I134" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="J134" s="1" t="s">
         <v>327</v>
@@ -7340,7 +7346,7 @@
         <v>17</v>
       </c>
       <c r="I135" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="J135" s="1" t="s">
         <v>327</v>
@@ -7363,7 +7369,7 @@
         <v>100</v>
       </c>
       <c r="F136" s="3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G136" s="1" t="s">
         <v>358</v>
@@ -7395,7 +7401,7 @@
         <v>100</v>
       </c>
       <c r="F137" s="3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G137" s="1" t="s">
         <v>360</v>
@@ -7436,7 +7442,7 @@
         <v>17</v>
       </c>
       <c r="I138" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="J138" s="1" t="s">
         <v>319</v>
@@ -7468,7 +7474,7 @@
         <v>17</v>
       </c>
       <c r="I139" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="J139" s="1" t="s">
         <v>319</v>
@@ -7491,7 +7497,7 @@
         <v>100</v>
       </c>
       <c r="F140" s="3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G140" s="1" t="s">
         <v>366</v>
@@ -7523,7 +7529,7 @@
         <v>100</v>
       </c>
       <c r="F141" s="3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G141" s="1" t="s">
         <v>368</v>
@@ -7953,7 +7959,7 @@
         <v>17</v>
       </c>
       <c r="I155" s="1" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7982,7 +7988,7 @@
         <v>17</v>
       </c>
       <c r="I156" s="1" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8193,7 +8199,7 @@
         <v>419</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C164" s="1" t="n">
         <v>771</v>
@@ -8205,10 +8211,10 @@
         <v>100</v>
       </c>
       <c r="F164" s="3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G164" s="1" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="H164" s="1" t="s">
         <v>17</v>
@@ -8222,7 +8228,7 @@
         <v>419</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C165" s="1" t="n">
         <v>772</v>
@@ -8237,7 +8243,7 @@
         <v>84</v>
       </c>
       <c r="G165" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="H165" s="1" t="s">
         <v>17</v>
@@ -8251,7 +8257,7 @@
         <v>419</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="C166" s="1" t="n">
         <v>773</v>
@@ -8266,13 +8272,13 @@
         <v>84</v>
       </c>
       <c r="G166" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="H166" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I166" s="1" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="J166" s="1" t="s">
         <v>420</v>
@@ -8298,7 +8304,7 @@
         <v>29</v>
       </c>
       <c r="G167" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="H167" s="1" t="s">
         <v>23</v>
@@ -8330,7 +8336,7 @@
         <v>29</v>
       </c>
       <c r="G168" s="1" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="H168" s="1" t="s">
         <v>17</v>
@@ -8356,7 +8362,7 @@
         <v>100</v>
       </c>
       <c r="F169" s="3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G169" s="1" t="s">
         <v>426</v>
@@ -8891,7 +8897,7 @@
         <v>17</v>
       </c>
       <c r="I186" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8920,7 +8926,7 @@
         <v>17</v>
       </c>
       <c r="I187" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8969,7 +8975,7 @@
         <v>100</v>
       </c>
       <c r="F189" s="3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G189" s="1" t="s">
         <v>473</v>
@@ -9010,7 +9016,7 @@
         <v>17</v>
       </c>
       <c r="I190" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9039,7 +9045,7 @@
         <v>17</v>
       </c>
       <c r="I191" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9088,7 +9094,7 @@
         <v>100</v>
       </c>
       <c r="F193" s="3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G193" s="1" t="s">
         <v>482</v>
@@ -9129,7 +9135,7 @@
         <v>17</v>
       </c>
       <c r="I194" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9158,7 +9164,7 @@
         <v>17</v>
       </c>
       <c r="I195" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9207,7 +9213,7 @@
         <v>100</v>
       </c>
       <c r="F197" s="3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G197" s="1" t="s">
         <v>491</v>
@@ -9358,7 +9364,7 @@
         <v>29</v>
       </c>
       <c r="G202" s="1" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="H202" s="1" t="s">
         <v>17</v>
@@ -9480,7 +9486,7 @@
         <v>17</v>
       </c>
       <c r="I206" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9509,7 +9515,7 @@
         <v>17</v>
       </c>
       <c r="I207" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9538,7 +9544,7 @@
         <v>17</v>
       </c>
       <c r="I208" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9567,7 +9573,7 @@
         <v>17</v>
       </c>
       <c r="I209" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9587,7 +9593,7 @@
         <v>100</v>
       </c>
       <c r="F210" s="3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G210" s="1" t="s">
         <v>518</v>
@@ -9616,7 +9622,7 @@
         <v>100</v>
       </c>
       <c r="F211" s="3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G211" s="1" t="s">
         <v>520</v>
@@ -9654,7 +9660,7 @@
         <v>17</v>
       </c>
       <c r="I212" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9799,7 +9805,7 @@
         <v>17</v>
       </c>
       <c r="I217" s="1" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9828,7 +9834,7 @@
         <v>17</v>
       </c>
       <c r="I218" s="1" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9877,7 +9883,7 @@
         <v>100</v>
       </c>
       <c r="F220" s="3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G220" s="1" t="s">
         <v>538</v>
@@ -9906,7 +9912,7 @@
         <v>100</v>
       </c>
       <c r="F221" s="3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G221" s="1" t="s">
         <v>540</v>
@@ -9973,7 +9979,7 @@
         <v>17</v>
       </c>
       <c r="I223" s="1" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9993,10 +9999,10 @@
         <v>100</v>
       </c>
       <c r="F224" s="3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G224" s="1" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="H224" s="1" t="s">
         <v>17</v>
@@ -10025,7 +10031,7 @@
         <v>84</v>
       </c>
       <c r="G225" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="H225" s="1" t="s">
         <v>17</v>
@@ -10092,7 +10098,7 @@
         <v>17</v>
       </c>
       <c r="I227" s="1" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10112,10 +10118,10 @@
         <v>100</v>
       </c>
       <c r="F228" s="3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G228" s="1" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="H228" s="1" t="s">
         <v>17</v>
@@ -10144,7 +10150,7 @@
         <v>84</v>
       </c>
       <c r="G229" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="H229" s="1" t="s">
         <v>17</v>
@@ -10173,13 +10179,13 @@
         <v>84</v>
       </c>
       <c r="G230" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="H230" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I230" s="1" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10199,7 +10205,7 @@
         <v>100</v>
       </c>
       <c r="F231" s="3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G231" s="1" t="s">
         <v>287</v>
@@ -10257,7 +10263,7 @@
         <v>100</v>
       </c>
       <c r="F233" s="3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G233" s="1" t="s">
         <v>562</v>
@@ -10324,7 +10330,7 @@
         <v>17</v>
       </c>
       <c r="I235" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10382,7 +10388,7 @@
         <v>23</v>
       </c>
       <c r="I237" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10405,7 +10411,7 @@
         <v>29</v>
       </c>
       <c r="G238" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="H238" s="1" t="s">
         <v>23</v>
@@ -10434,7 +10440,7 @@
         <v>29</v>
       </c>
       <c r="G239" s="1" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="H239" s="1" t="s">
         <v>17</v>
@@ -10663,7 +10669,7 @@
         <v>100</v>
       </c>
       <c r="F247" s="3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G247" s="1" t="s">
         <v>473</v>
@@ -10692,7 +10698,7 @@
         <v>100</v>
       </c>
       <c r="F248" s="3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G248" s="1" t="s">
         <v>482</v>
@@ -10721,7 +10727,7 @@
         <v>100</v>
       </c>
       <c r="F249" s="3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G249" s="1" t="s">
         <v>491</v>
@@ -10750,7 +10756,7 @@
         <v>100</v>
       </c>
       <c r="F250" s="3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G250" s="1" t="s">
         <v>582</v>
@@ -10779,7 +10785,7 @@
         <v>100</v>
       </c>
       <c r="F251" s="3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G251" s="1" t="s">
         <v>584</v>
@@ -10808,7 +10814,7 @@
         <v>100</v>
       </c>
       <c r="F252" s="3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G252" s="1" t="s">
         <v>586</v>
@@ -10872,7 +10878,7 @@
         <v>17</v>
       </c>
       <c r="I254" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="255" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10901,7 +10907,7 @@
         <v>17</v>
       </c>
       <c r="I255" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="256" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10930,7 +10936,7 @@
         <v>17</v>
       </c>
       <c r="I256" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="257" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10959,7 +10965,7 @@
         <v>17</v>
       </c>
       <c r="I257" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="258" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10988,7 +10994,7 @@
         <v>17</v>
       </c>
       <c r="I258" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="259" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11017,7 +11023,7 @@
         <v>17</v>
       </c>
       <c r="I259" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="260" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11461,7 +11467,7 @@
         <v>100</v>
       </c>
       <c r="F274" s="3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G274" s="1" t="s">
         <v>622</v>
@@ -11493,7 +11499,7 @@
         <v>100</v>
       </c>
       <c r="F275" s="3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G275" s="1" t="s">
         <v>626</v>
@@ -11872,13 +11878,13 @@
         <v>665</v>
       </c>
       <c r="G288" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="H288" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I288" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="289" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11901,13 +11907,13 @@
         <v>667</v>
       </c>
       <c r="G289" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="H289" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I289" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="290" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11915,7 +11921,7 @@
         <v>663</v>
       </c>
       <c r="B290" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C290" s="1" t="n">
         <v>3105</v>
@@ -11930,7 +11936,7 @@
         <v>668</v>
       </c>
       <c r="G290" s="1" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="H290" s="1" t="s">
         <v>17</v>
@@ -11959,7 +11965,7 @@
         <v>669</v>
       </c>
       <c r="G291" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="H291" s="1" t="s">
         <v>17</v>
@@ -12118,7 +12124,7 @@
         <v>663</v>
       </c>
       <c r="B297" s="1" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C297" s="1" t="n">
         <v>3116</v>
@@ -12133,7 +12139,7 @@
         <v>669</v>
       </c>
       <c r="G297" s="1" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="H297" s="1" t="s">
         <v>17</v>
@@ -12217,7 +12223,7 @@
         <v>669</v>
       </c>
       <c r="G300" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="H300" s="1" t="s">
         <v>23</v>
@@ -12272,7 +12278,7 @@
         <v>669</v>
       </c>
       <c r="G302" s="1" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="H302" s="1" t="s">
         <v>17</v>
@@ -12307,7 +12313,7 @@
         <v>17</v>
       </c>
       <c r="I303" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="304" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12336,7 +12342,7 @@
         <v>17</v>
       </c>
       <c r="I304" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="305" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12365,7 +12371,7 @@
         <v>17</v>
       </c>
       <c r="I305" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="306" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12394,7 +12400,7 @@
         <v>17</v>
       </c>
       <c r="I306" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="307" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12423,7 +12429,7 @@
         <v>17</v>
       </c>
       <c r="I307" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="308" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12452,7 +12458,7 @@
         <v>17</v>
       </c>
       <c r="I308" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="309" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12568,7 +12574,7 @@
         <v>17</v>
       </c>
       <c r="I312" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="313" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12597,7 +12603,7 @@
         <v>17</v>
       </c>
       <c r="I313" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="314" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12626,7 +12632,7 @@
         <v>17</v>
       </c>
       <c r="I314" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="315" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12855,7 +12861,7 @@
         <v>17</v>
       </c>
       <c r="I322" s="1" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="323" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12884,7 +12890,7 @@
         <v>17</v>
       </c>
       <c r="I323" s="1" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="324" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12913,7 +12919,7 @@
         <v>17</v>
       </c>
       <c r="I324" s="1" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="325" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13017,7 +13023,7 @@
         <v>100</v>
       </c>
       <c r="F328" s="3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G328" s="1" t="s">
         <v>730</v>
@@ -13043,7 +13049,7 @@
         <v>100</v>
       </c>
       <c r="F329" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="G329" s="1" t="s">
         <v>732</v>
@@ -13098,7 +13104,7 @@
         <v>100</v>
       </c>
       <c r="F331" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="G331" s="1" t="s">
         <v>737</v>
@@ -13107,7 +13113,7 @@
         <v>17</v>
       </c>
       <c r="I331" s="1" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="332" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13240,7 +13246,7 @@
         <v>21</v>
       </c>
       <c r="G336" s="1" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="H336" s="1" t="s">
         <v>17</v>
@@ -13469,7 +13475,7 @@
         <v>771</v>
       </c>
       <c r="I344" s="1" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="345" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13495,7 +13501,7 @@
         <v>773</v>
       </c>
       <c r="I345" s="1" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
   </sheetData>
@@ -14211,10 +14217,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C71"/>
+  <dimension ref="A1:C72"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A45" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A72" activeCellId="0" sqref="A72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14667,6 +14673,14 @@
         <v>935</v>
       </c>
     </row>
+    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="22" t="s">
+        <v>936</v>
+      </c>
+      <c r="B72" s="22" t="s">
+        <v>937</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
GridLost alarm register changed to 64.
The GridLost alarm used to be on the system service, register 830.
When it moved to the vebus service the register number was kept in
a misguided attempt to limit further breakage, but since the move means
that the slaveid changes anyway it is much neater to change the
register as well. This also allows it to be fetched as part of a larger
range.

https://github.com/victronenergy/venus/issues/629
</commit_message>
<xml_diff>
--- a/CCGX-Modbus-TCP-register-list.xlsx
+++ b/CCGX-Modbus-TCP-register-list.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Field list" sheetId="1" state="visible" r:id="rId2"/>
@@ -3188,10 +3188,10 @@
   </sheetPr>
   <dimension ref="A1:N345"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="2" topLeftCell="A261" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="2" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A278" activeCellId="0" sqref="A278"/>
+      <selection pane="bottomLeft" activeCell="C99" activeCellId="0" sqref="C99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6224,7 +6224,7 @@
         <v>282</v>
       </c>
       <c r="C99" s="1" t="n">
-        <v>830</v>
+        <v>64</v>
       </c>
       <c r="D99" s="2" t="s">
         <v>20</v>
@@ -14219,7 +14219,7 @@
   </sheetPr>
   <dimension ref="A1:C72"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A72" activeCellId="0" sqref="A72"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add more registers for generator start/stop
Add registers for state, errors for FisherPanda, and AC input alarm.

https://github.com/victronenergy/venus/issues/694
</commit_message>
<xml_diff>
--- a/CCGX-Modbus-TCP-register-list.xlsx
+++ b/CCGX-Modbus-TCP-register-list.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2727" uniqueCount="972">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2753" uniqueCount="981">
   <si>
     <t xml:space="preserve">NOTE: Use unit-id 100 for the com.victronenergy.system data, for more information see FAQ.</t>
   </si>
@@ -2392,6 +2392,33 @@
   </si>
   <si>
     <t xml:space="preserve">/Generator0/Runtime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Generator start/stop state</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Generator0/State</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0=Stopped;1=Running;10=Error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Generator remote error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Generator0/Error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0=No Error;1=Remote disabled;2=Remote fault</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Only used for FisherPanda gensets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Generator not detected at AC input alarm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Generator0/Alarms/NoGeneratorAtAcIn</t>
   </si>
   <si>
     <t xml:space="preserve">com.victronenergy.meteo</t>
@@ -3288,12 +3315,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N354"/>
+  <dimension ref="A1:N357"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="2" topLeftCell="A329" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A353" activeCellId="0" sqref="A353"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13771,105 +13798,207 @@
     </row>
     <row r="351" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A351" s="1" t="s">
+        <v>781</v>
+      </c>
+      <c r="B351" s="1" t="s">
         <v>790</v>
       </c>
-      <c r="B351" s="22" t="s">
+      <c r="C351" s="1" t="n">
+        <v>3506</v>
+      </c>
+      <c r="D351" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E351" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F351" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="G351" s="1" t="s">
         <v>791</v>
       </c>
-      <c r="C351" s="1" t="n">
-        <v>3600</v>
-      </c>
-      <c r="D351" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E351" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="F351" s="3" t="s">
+      <c r="H351" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I351" s="1" t="s">
         <v>792</v>
-      </c>
-      <c r="G351" s="1" t="s">
-        <v>793</v>
-      </c>
-      <c r="I351" s="1" t="s">
-        <v>794</v>
       </c>
     </row>
     <row r="352" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A352" s="1" t="s">
-        <v>790</v>
-      </c>
-      <c r="B352" s="22" t="s">
+        <v>781</v>
+      </c>
+      <c r="B352" s="1" t="s">
+        <v>793</v>
+      </c>
+      <c r="C352" s="1" t="n">
+        <v>3507</v>
+      </c>
+      <c r="D352" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E352" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F352" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="G352" s="1" t="s">
+        <v>794</v>
+      </c>
+      <c r="H352" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I352" s="1" t="s">
         <v>795</v>
       </c>
-      <c r="C352" s="1" t="n">
-        <v>3601</v>
-      </c>
-      <c r="D352" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E352" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="F352" s="3" t="s">
-        <v>792</v>
-      </c>
-      <c r="G352" s="1" t="s">
+      <c r="J352" s="1" t="s">
         <v>796</v>
-      </c>
-      <c r="I352" s="1" t="s">
-        <v>656</v>
       </c>
     </row>
     <row r="353" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A353" s="1" t="s">
-        <v>790</v>
-      </c>
-      <c r="B353" s="22" t="s">
+        <v>781</v>
+      </c>
+      <c r="B353" s="1" t="s">
         <v>797</v>
       </c>
       <c r="C353" s="1" t="n">
-        <v>3602</v>
+        <v>3508</v>
       </c>
       <c r="D353" s="2" t="s">
-        <v>59</v>
+        <v>20</v>
       </c>
       <c r="E353" s="1" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F353" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="G353" s="1" t="s">
         <v>798</v>
       </c>
-      <c r="G353" s="1" t="s">
-        <v>799</v>
+      <c r="H353" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="I353" s="1" t="s">
-        <v>275</v>
+        <v>312</v>
       </c>
     </row>
     <row r="354" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A354" s="1" t="s">
-        <v>790</v>
+        <v>799</v>
       </c>
       <c r="B354" s="22" t="s">
         <v>800</v>
       </c>
       <c r="C354" s="1" t="n">
-        <v>3603</v>
+        <v>3600</v>
       </c>
       <c r="D354" s="2" t="s">
-        <v>59</v>
+        <v>20</v>
       </c>
       <c r="E354" s="1" t="n">
         <v>10</v>
       </c>
       <c r="F354" s="3" t="s">
-        <v>798</v>
+        <v>801</v>
       </c>
       <c r="G354" s="1" t="s">
+        <v>802</v>
+      </c>
+      <c r="H354" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I354" s="1" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="355" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A355" s="1" t="s">
+        <v>799</v>
+      </c>
+      <c r="B355" s="22" t="s">
+        <v>804</v>
+      </c>
+      <c r="C355" s="1" t="n">
+        <v>3601</v>
+      </c>
+      <c r="D355" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E355" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="F355" s="3" t="s">
         <v>801</v>
       </c>
-      <c r="I354" s="1" t="s">
+      <c r="G355" s="1" t="s">
+        <v>805</v>
+      </c>
+      <c r="H355" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I355" s="1" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="356" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A356" s="1" t="s">
+        <v>799</v>
+      </c>
+      <c r="B356" s="22" t="s">
+        <v>806</v>
+      </c>
+      <c r="C356" s="1" t="n">
+        <v>3602</v>
+      </c>
+      <c r="D356" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E356" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="F356" s="3" t="s">
+        <v>807</v>
+      </c>
+      <c r="G356" s="1" t="s">
+        <v>808</v>
+      </c>
+      <c r="H356" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I356" s="1" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="357" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A357" s="1" t="s">
+        <v>799</v>
+      </c>
+      <c r="B357" s="22" t="s">
+        <v>809</v>
+      </c>
+      <c r="C357" s="1" t="n">
+        <v>3603</v>
+      </c>
+      <c r="D357" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E357" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="F357" s="3" t="s">
+        <v>807</v>
+      </c>
+      <c r="G357" s="1" t="s">
+        <v>810</v>
+      </c>
+      <c r="H357" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I357" s="1" t="s">
         <v>275</v>
       </c>
     </row>
@@ -13908,13 +14037,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="24" t="s">
-        <v>802</v>
+        <v>811</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>803</v>
+        <v>812</v>
       </c>
       <c r="C1" s="24" t="s">
-        <v>804</v>
+        <v>813</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13925,7 +14054,7 @@
         <v>257</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>805</v>
+        <v>814</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13936,7 +14065,7 @@
         <v>256</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>806</v>
+        <v>815</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13947,7 +14076,7 @@
         <v>258</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>807</v>
+        <v>816</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13958,7 +14087,7 @@
         <v>260</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>808</v>
+        <v>817</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13969,7 +14098,7 @@
         <v>261</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>809</v>
+        <v>818</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13980,7 +14109,7 @@
         <v>273</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>810</v>
+        <v>819</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13991,7 +14120,7 @@
         <v>274</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>811</v>
+        <v>820</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14002,7 +14131,7 @@
         <v>275</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>812</v>
+        <v>821</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14013,7 +14142,7 @@
         <v>276</v>
       </c>
       <c r="C10" s="25" t="s">
-        <v>813</v>
+        <v>822</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14024,7 +14153,7 @@
         <v>279</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>814</v>
+        <v>823</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14035,7 +14164,7 @@
         <v>278</v>
       </c>
       <c r="C12" s="25" t="s">
-        <v>815</v>
+        <v>824</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14046,7 +14175,7 @@
         <v>277</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>816</v>
+        <v>825</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14057,7 +14186,7 @@
         <v>0</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>817</v>
+        <v>826</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14068,7 +14197,7 @@
         <v>1</v>
       </c>
       <c r="C15" s="22" t="s">
-        <v>818</v>
+        <v>827</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14079,7 +14208,7 @@
         <v>2</v>
       </c>
       <c r="C16" s="22" t="s">
-        <v>819</v>
+        <v>828</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14090,7 +14219,7 @@
         <v>3</v>
       </c>
       <c r="C17" s="22" t="s">
-        <v>820</v>
+        <v>829</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14101,7 +14230,7 @@
         <v>4</v>
       </c>
       <c r="C18" s="22" t="s">
-        <v>821</v>
+        <v>830</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14112,7 +14241,7 @@
         <v>5</v>
       </c>
       <c r="C19" s="22" t="s">
-        <v>822</v>
+        <v>831</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14123,7 +14252,7 @@
         <v>6</v>
       </c>
       <c r="C20" s="22" t="s">
-        <v>823</v>
+        <v>832</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14134,7 +14263,7 @@
         <v>7</v>
       </c>
       <c r="C21" s="22" t="s">
-        <v>824</v>
+        <v>833</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14145,7 +14274,7 @@
         <v>8</v>
       </c>
       <c r="C22" s="22" t="s">
-        <v>825</v>
+        <v>834</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14156,7 +14285,7 @@
         <v>9</v>
       </c>
       <c r="C23" s="22" t="s">
-        <v>826</v>
+        <v>835</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14167,7 +14296,7 @@
         <v>10</v>
       </c>
       <c r="C24" s="22" t="s">
-        <v>827</v>
+        <v>836</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14178,7 +14307,7 @@
         <v>11</v>
       </c>
       <c r="C25" s="22" t="s">
-        <v>828</v>
+        <v>837</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14189,7 +14318,7 @@
         <v>12</v>
       </c>
       <c r="C26" s="22" t="s">
-        <v>829</v>
+        <v>838</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14200,7 +14329,7 @@
         <v>20</v>
       </c>
       <c r="C27" s="22" t="s">
-        <v>830</v>
+        <v>839</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14211,7 +14340,7 @@
         <v>21</v>
       </c>
       <c r="C28" s="22" t="s">
-        <v>831</v>
+        <v>840</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14222,7 +14351,7 @@
         <v>22</v>
       </c>
       <c r="C29" s="22" t="s">
-        <v>832</v>
+        <v>841</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14233,7 +14362,7 @@
         <v>23</v>
       </c>
       <c r="C30" s="22" t="s">
-        <v>833</v>
+        <v>842</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14244,7 +14373,7 @@
         <v>24</v>
       </c>
       <c r="C31" s="22" t="s">
-        <v>834</v>
+        <v>843</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14255,7 +14384,7 @@
         <v>25</v>
       </c>
       <c r="C32" s="22" t="s">
-        <v>835</v>
+        <v>844</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14266,7 +14395,7 @@
         <v>26</v>
       </c>
       <c r="C33" s="22" t="s">
-        <v>836</v>
+        <v>845</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14277,7 +14406,7 @@
         <v>27</v>
       </c>
       <c r="C34" s="22" t="s">
-        <v>837</v>
+        <v>846</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14288,7 +14417,7 @@
         <v>28</v>
       </c>
       <c r="C35" s="22" t="s">
-        <v>838</v>
+        <v>847</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14299,7 +14428,7 @@
         <v>29</v>
       </c>
       <c r="C36" s="22" t="s">
-        <v>839</v>
+        <v>848</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14310,7 +14439,7 @@
         <v>30</v>
       </c>
       <c r="C37" s="22" t="s">
-        <v>840</v>
+        <v>849</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14321,7 +14450,7 @@
         <v>31</v>
       </c>
       <c r="C38" s="22" t="s">
-        <v>841</v>
+        <v>850</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14332,7 +14461,7 @@
         <v>32</v>
       </c>
       <c r="C39" s="22" t="s">
-        <v>842</v>
+        <v>851</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14343,7 +14472,7 @@
         <v>33</v>
       </c>
       <c r="C40" s="22" t="s">
-        <v>843</v>
+        <v>852</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14354,7 +14483,7 @@
         <v>34</v>
       </c>
       <c r="C41" s="22" t="s">
-        <v>844</v>
+        <v>853</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14365,7 +14494,7 @@
         <v>40</v>
       </c>
       <c r="C42" s="22" t="s">
-        <v>845</v>
+        <v>854</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14376,7 +14505,7 @@
         <v>41</v>
       </c>
       <c r="C43" s="22" t="s">
-        <v>846</v>
+        <v>855</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14387,7 +14516,7 @@
         <v>42</v>
       </c>
       <c r="C44" s="22" t="s">
-        <v>847</v>
+        <v>856</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14398,7 +14527,7 @@
         <v>43</v>
       </c>
       <c r="C45" s="22" t="s">
-        <v>848</v>
+        <v>857</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14409,7 +14538,7 @@
         <v>44</v>
       </c>
       <c r="C46" s="22" t="s">
-        <v>849</v>
+        <v>858</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14420,7 +14549,7 @@
         <v>45</v>
       </c>
       <c r="C47" s="22" t="s">
-        <v>850</v>
+        <v>859</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14431,7 +14560,7 @@
         <v>46</v>
       </c>
       <c r="C48" s="22" t="s">
-        <v>851</v>
+        <v>860</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14442,7 +14571,7 @@
         <v>288</v>
       </c>
       <c r="C49" s="22" t="s">
-        <v>852</v>
+        <v>861</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14453,7 +14582,7 @@
         <v>289</v>
       </c>
       <c r="C50" s="22" t="s">
-        <v>853</v>
+        <v>862</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14464,7 +14593,7 @@
         <v>290</v>
       </c>
       <c r="C51" s="22" t="s">
-        <v>854</v>
+        <v>863</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14475,7 +14604,7 @@
         <v>291</v>
       </c>
       <c r="C52" s="22" t="s">
-        <v>855</v>
+        <v>864</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14486,7 +14615,7 @@
         <v>292</v>
       </c>
       <c r="C53" s="22" t="s">
-        <v>856</v>
+        <v>865</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14497,7 +14626,7 @@
         <v>293</v>
       </c>
       <c r="C54" s="22" t="s">
-        <v>857</v>
+        <v>866</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14508,7 +14637,7 @@
         <v>294</v>
       </c>
       <c r="C55" s="22" t="s">
-        <v>858</v>
+        <v>867</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14519,7 +14648,7 @@
         <v>295</v>
       </c>
       <c r="C56" s="22" t="s">
-        <v>859</v>
+        <v>868</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14530,7 +14659,7 @@
         <v>296</v>
       </c>
       <c r="C57" s="22" t="s">
-        <v>860</v>
+        <v>869</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14541,12 +14670,12 @@
         <v>512</v>
       </c>
       <c r="C58" s="22" t="s">
-        <v>861</v>
+        <v>870</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="26" t="s">
-        <v>862</v>
+        <v>871</v>
       </c>
       <c r="B60" s="26"/>
       <c r="C60" s="26"/>
@@ -14556,7 +14685,7 @@
     </row>
     <row r="61" customFormat="false" ht="92.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="27" t="s">
-        <v>863</v>
+        <v>872</v>
       </c>
       <c r="B61" s="27"/>
       <c r="C61" s="27"/>
@@ -14602,480 +14731,480 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="22" t="s">
-        <v>864</v>
+        <v>873</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>865</v>
+        <v>874</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="22" t="s">
-        <v>866</v>
+        <v>875</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>867</v>
+        <v>876</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="22" t="s">
-        <v>868</v>
+        <v>877</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>869</v>
+        <v>878</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="22" t="s">
-        <v>870</v>
+        <v>879</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>871</v>
+        <v>880</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="22" t="s">
-        <v>872</v>
+        <v>881</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="22" t="s">
-        <v>873</v>
+        <v>882</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="22" t="s">
-        <v>874</v>
+        <v>883</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="22" t="s">
-        <v>875</v>
+        <v>884</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="22" t="s">
-        <v>876</v>
+        <v>885</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>877</v>
+        <v>886</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="22" t="s">
-        <v>878</v>
+        <v>887</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="22" t="s">
-        <v>879</v>
+        <v>888</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="22" t="s">
-        <v>880</v>
+        <v>889</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>881</v>
+        <v>890</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="22" t="s">
-        <v>882</v>
+        <v>891</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="22" t="s">
-        <v>883</v>
+        <v>892</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="22" t="s">
-        <v>884</v>
+        <v>893</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="22" t="s">
-        <v>885</v>
+        <v>894</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="22" t="s">
-        <v>886</v>
+        <v>895</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="22" t="s">
-        <v>887</v>
+        <v>896</v>
       </c>
       <c r="B18" s="22" t="s">
-        <v>888</v>
+        <v>897</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="22" t="s">
-        <v>889</v>
+        <v>898</v>
       </c>
       <c r="B19" s="22" t="s">
-        <v>890</v>
+        <v>899</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="22" t="s">
-        <v>891</v>
+        <v>900</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="22" t="s">
-        <v>892</v>
+        <v>901</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="22" t="s">
-        <v>893</v>
+        <v>902</v>
       </c>
       <c r="B22" s="22" t="s">
-        <v>894</v>
+        <v>903</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="22" t="s">
-        <v>895</v>
+        <v>904</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="22" t="s">
-        <v>896</v>
+        <v>905</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="22" t="s">
-        <v>897</v>
+        <v>906</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="22" t="s">
-        <v>898</v>
+        <v>907</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="22" t="s">
-        <v>899</v>
+        <v>908</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="22" t="s">
-        <v>900</v>
+        <v>909</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="22" t="s">
-        <v>901</v>
+        <v>910</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="22" t="s">
-        <v>902</v>
+        <v>911</v>
       </c>
       <c r="B30" s="22" t="s">
-        <v>903</v>
+        <v>912</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="22" t="s">
-        <v>904</v>
+        <v>913</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="22" t="s">
-        <v>905</v>
+        <v>914</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="22" t="s">
-        <v>906</v>
+        <v>915</v>
       </c>
       <c r="B33" s="22" t="s">
-        <v>907</v>
+        <v>916</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="22" t="s">
-        <v>908</v>
+        <v>917</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="22" t="s">
-        <v>909</v>
+        <v>918</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="22" t="s">
-        <v>910</v>
+        <v>919</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="22" t="s">
-        <v>911</v>
+        <v>920</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="22" t="s">
-        <v>912</v>
+        <v>921</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C39" s="28" t="s">
-        <v>913</v>
+        <v>922</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="22" t="s">
-        <v>914</v>
+        <v>923</v>
       </c>
       <c r="B40" s="22" t="s">
-        <v>915</v>
+        <v>924</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="22" t="s">
-        <v>916</v>
+        <v>925</v>
       </c>
       <c r="B41" s="22" t="s">
-        <v>917</v>
+        <v>926</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="22" t="s">
-        <v>918</v>
+        <v>927</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="22" t="s">
-        <v>919</v>
+        <v>928</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="22" t="s">
-        <v>920</v>
+        <v>929</v>
       </c>
       <c r="B44" s="22" t="s">
-        <v>921</v>
+        <v>930</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="22" t="s">
-        <v>922</v>
+        <v>931</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="22" t="s">
-        <v>923</v>
+        <v>932</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="22" t="s">
-        <v>924</v>
+        <v>933</v>
       </c>
       <c r="B47" s="22" t="s">
-        <v>925</v>
+        <v>934</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="22" t="s">
-        <v>926</v>
+        <v>935</v>
       </c>
       <c r="B48" s="22" t="s">
-        <v>927</v>
+        <v>936</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="22" t="s">
-        <v>928</v>
+        <v>937</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="22" t="s">
-        <v>929</v>
+        <v>938</v>
       </c>
       <c r="B50" s="22" t="s">
-        <v>930</v>
+        <v>939</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="22" t="s">
-        <v>931</v>
+        <v>940</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="22" t="s">
-        <v>932</v>
+        <v>941</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="22" t="s">
-        <v>933</v>
+        <v>942</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="22" t="s">
-        <v>934</v>
+        <v>943</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="22" t="s">
-        <v>935</v>
+        <v>944</v>
       </c>
       <c r="B55" s="22" t="s">
-        <v>936</v>
+        <v>945</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="22" t="s">
-        <v>937</v>
+        <v>946</v>
       </c>
       <c r="B56" s="22" t="s">
-        <v>938</v>
+        <v>947</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="22" t="s">
-        <v>939</v>
+        <v>948</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="22" t="s">
-        <v>940</v>
+        <v>949</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="22" t="s">
-        <v>941</v>
+        <v>950</v>
       </c>
       <c r="B59" s="22" t="s">
-        <v>942</v>
+        <v>951</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="22" t="s">
-        <v>943</v>
+        <v>952</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="22" t="s">
-        <v>944</v>
+        <v>953</v>
       </c>
       <c r="B61" s="22" t="s">
-        <v>945</v>
+        <v>954</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="22" t="s">
-        <v>946</v>
+        <v>955</v>
       </c>
       <c r="B62" s="22" t="s">
-        <v>947</v>
+        <v>956</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="22" t="s">
-        <v>948</v>
+        <v>957</v>
       </c>
       <c r="B63" s="22" t="s">
-        <v>949</v>
+        <v>958</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="22" t="s">
-        <v>950</v>
+        <v>959</v>
       </c>
       <c r="B64" s="22" t="s">
-        <v>951</v>
+        <v>960</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="22" t="s">
-        <v>952</v>
+        <v>961</v>
       </c>
       <c r="B65" s="22" t="s">
-        <v>953</v>
+        <v>962</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="22" t="s">
-        <v>954</v>
+        <v>963</v>
       </c>
       <c r="B66" s="22" t="s">
-        <v>955</v>
+        <v>964</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="22" t="s">
-        <v>956</v>
+        <v>965</v>
       </c>
       <c r="B67" s="22" t="s">
-        <v>957</v>
+        <v>966</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="22" t="s">
-        <v>958</v>
+        <v>967</v>
       </c>
       <c r="B68" s="22" t="s">
-        <v>959</v>
+        <v>968</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="22" t="s">
-        <v>960</v>
+        <v>969</v>
       </c>
       <c r="B69" s="22" t="s">
-        <v>961</v>
+        <v>970</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B70" s="22" t="s">
-        <v>962</v>
+        <v>971</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B71" s="22" t="s">
-        <v>963</v>
+        <v>972</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="22" t="s">
-        <v>964</v>
+        <v>973</v>
       </c>
       <c r="B72" s="22" t="s">
-        <v>965</v>
+        <v>974</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B73" s="22" t="s">
-        <v>966</v>
+        <v>975</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="22" t="s">
-        <v>967</v>
+        <v>976</v>
       </c>
       <c r="B74" s="22" t="s">
-        <v>968</v>
+        <v>977</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B75" s="22" t="s">
-        <v>969</v>
+        <v>978</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B76" s="22" t="s">
-        <v>970</v>
+        <v>979</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B77" s="22" t="s">
-        <v>971</v>
+        <v>980</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update the changelog in the xls doc
</commit_message>
<xml_diff>
--- a/CCGX-Modbus-TCP-register-list.xlsx
+++ b/CCGX-Modbus-TCP-register-list.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Field list" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2753" uniqueCount="981">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2755" uniqueCount="983">
   <si>
     <t xml:space="preserve">NOTE: Use unit-id 100 for the com.victronenergy.system data, for more information see FAQ.</t>
   </si>
@@ -2965,6 +2965,12 @@
   </si>
   <si>
     <t xml:space="preserve">Added 32-bit register for generator runtime.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rev 31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Added additional registers for generator start/stop</t>
   </si>
 </sst>
 </file>
@@ -3317,10 +3323,10 @@
   </sheetPr>
   <dimension ref="A1:N357"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="2" topLeftCell="A329" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A353" activeCellId="0" sqref="A353"/>
+      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14715,10 +14721,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C77"/>
+  <dimension ref="A1:C78"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A58" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B79" activeCellId="0" sqref="B79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15207,6 +15213,14 @@
         <v>980</v>
       </c>
     </row>
+    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="22" t="s">
+        <v>981</v>
+      </c>
+      <c r="B78" s="22" t="s">
+        <v>982</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
rename acmeter service to acload
</commit_message>
<xml_diff>
--- a/CCGX-Modbus-TCP-register-list.xlsx
+++ b/CCGX-Modbus-TCP-register-list.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Field list" sheetId="1" state="visible" r:id="rId2"/>
@@ -2817,7 +2817,7 @@
     <t xml:space="preserve">/StartStop</t>
   </si>
   <si>
-    <t xml:space="preserve">com.victronenergy.acmeter</t>
+    <t xml:space="preserve">com.victronenergy.acload</t>
   </si>
   <si>
     <t xml:space="preserve">Serial number</t>
@@ -3402,7 +3402,7 @@
     <t xml:space="preserve">Rev 39</t>
   </si>
   <si>
-    <t xml:space="preserve">Add registers for acmeter service</t>
+    <t xml:space="preserve">Add registers for acload service</t>
   </si>
 </sst>
 </file>
@@ -3755,10 +3755,10 @@
   </sheetPr>
   <dimension ref="A1:N451"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A427" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A449" activeCellId="0" sqref="A449"/>
+      <selection pane="bottomLeft" activeCell="A451" activeCellId="0" sqref="A451"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -17960,7 +17960,7 @@
   </sheetPr>
   <dimension ref="A1:C91"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A64" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A64" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B92" activeCellId="0" sqref="B92"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fix scaling and writability of 2710
This is a new register added recently, which would be somewhat
useless due to the r/o nature and wrong scale. Hence we fix it
in place and don't make a new one.

https://github.com/victronenergy/venus/issues/849
</commit_message>
<xml_diff>
--- a/CCGX-Modbus-TCP-register-list.xlsx
+++ b/CCGX-Modbus-TCP-register-list.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Field list" sheetId="1" state="visible" r:id="rId2"/>
@@ -3755,10 +3755,10 @@
   </sheetPr>
   <dimension ref="A1:N451"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="2" topLeftCell="A427" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="2" topLeftCell="A298" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A451" activeCellId="0" sqref="A451"/>
+      <selection pane="bottomLeft" activeCell="C311" activeCellId="0" sqref="C311"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13215,7 +13215,7 @@
         <v>20</v>
       </c>
       <c r="E311" s="1" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F311" s="3" t="s">
         <v>232</v>
@@ -17960,7 +17960,7 @@
   </sheetPr>
   <dimension ref="A1:C91"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A64" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A64" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B92" activeCellId="0" sqref="B92"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
update definition of batterylife states
</commit_message>
<xml_diff>
--- a/CCGX-Modbus-TCP-register-list.xlsx
+++ b/CCGX-Modbus-TCP-register-list.xlsx
@@ -2262,7 +2262,7 @@
     <t xml:space="preserve">/Settings/CGwacs/BatteryLife/State</t>
   </si>
   <si>
-    <t xml:space="preserve">0=Unused, BL disabled;1=Restarting;2=Self-consumption;3=Self-consumption;4=Self-consumption;5=Discharge disabled;6=Force charge;7=Sustain;9=Keep batteries charged;10=BL Disabled;11=BL Disabled (Low SoC)</t>
+    <t xml:space="preserve">0=Unused, BL disabled;1=Restarting;2=Self-consumption;3=Self-consumption;4=Self-consumption;5=Discharge disabled;6=Force charge;7=Sustain;8=Low Soc Recharge;9=Keep batteries charged;10=BL Disabled;11=BL Disabled (Low SoC);12=BL Disabled (Low SOC recharge)</t>
   </si>
   <si>
     <t xml:space="preserve">Use value 0 (disable) and 1(enable) for writing only</t>
@@ -4028,10 +4028,10 @@
   </sheetPr>
   <dimension ref="A1:N570"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="2" topLeftCell="A383" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A408" activeCellId="0" sqref="A408"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="2" topLeftCell="A303" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="I320" activeCellId="0" sqref="I320"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
fix typo in register for PV power tracker 0
</commit_message>
<xml_diff>
--- a/CCGX-Modbus-TCP-register-list.xlsx
+++ b/CCGX-Modbus-TCP-register-list.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Field list" sheetId="1" state="visible" r:id="rId2"/>
@@ -4211,10 +4211,10 @@
   </sheetPr>
   <dimension ref="A1:N628"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="2" topLeftCell="A338" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="2" topLeftCell="A210" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A343" activeCellId="0" sqref="A343"/>
+      <selection pane="bottomLeft" activeCell="C225" activeCellId="0" sqref="C225"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11105,7 +11105,7 @@
         <v>558</v>
       </c>
       <c r="C224" s="1" t="n">
-        <v>3725</v>
+        <v>3724</v>
       </c>
       <c r="D224" s="2" t="s">
         <v>20</v>
@@ -22878,7 +22878,7 @@
     <mergeCell ref="E1:F1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="J343" r:id="rId1" location="UUID-af4a7478-4b75-68ac-cf3c-16c381335d1e" display="https://www.victronenergy.com/media/pg/Energy_Storage_System/en/controlling-depth-of-discharge.html#UUID-af4a7478-4b75-68ac-cf3c-16c381335d1e"/>
+    <hyperlink ref="J343" r:id="rId1" location="UUID-af4a7478-4b75-68ac-cf3c-16c381335d1e" display="This value is maintained by BatteryLife. The Active SOC limit is the lower of this value, and register 2901. Also see https://www.victronenergy.com/media/pg/Energy_Storage_System/en/controlling-depth-of-discharge.html#UUID-af4a7478-4b75-68ac-cf3c-16c381335d1e"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -23589,7 +23589,7 @@
   </sheetPr>
   <dimension ref="A1:C110"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A91" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A91" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A110" activeCellId="0" sqref="A110"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fix state enum 252 value
252 means External Control, not Bulk Protection. Updated csv
and xls.
</commit_message>
<xml_diff>
--- a/CCGX-Modbus-TCP-register-list.xlsx
+++ b/CCGX-Modbus-TCP-register-list.xlsx
@@ -627,7 +627,7 @@
     <t xml:space="preserve">/State</t>
   </si>
   <si>
-    <t xml:space="preserve">0=Off;1=Low Power;2=Fault;3=Bulk;4=Absorption;5=Float;6=Storage;7=Equalize;8=Passthru;9=Inverting;10=Power assist;11=Power supply;252=Bulk protection</t>
+    <t xml:space="preserve">0=Off;1=Low Power;2=Fault;3=Bulk;4=Absorption;5=Float;6=Storage;7=Equalize;8=Passthru;9=Inverting;10=Power assist;11=Power supply;252=External control</t>
   </si>
   <si>
     <t xml:space="preserve">VE.Bus Error</t>
@@ -2130,7 +2130,7 @@
     <t xml:space="preserve">0=Off;1=On;2=Error;3=Unavailable- Unknown</t>
   </si>
   <si>
-    <t xml:space="preserve">0=Off;1=Low Power Mode;2=Fault;3=Bulk;4=Absorption;5=Float;6=Storage;7=Equalize;8=Passthru;9=Inverting;10=Power assist;11=Power supply mode;252=Bulk protection</t>
+    <t xml:space="preserve">0=Off;1=Low Power Mode;2=Fault;3=Bulk;4=Absorption;5=Float;6=Storage;7=Equalize;8=Passthru;9=Inverting;10=Power assist;11=Power supply mode;252=External control</t>
   </si>
   <si>
     <t xml:space="preserve">com.victronenergy.grid</t>
@@ -4211,10 +4211,10 @@
   </sheetPr>
   <dimension ref="A1:N628"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="2" topLeftCell="A210" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C225" activeCellId="0" sqref="C225"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="2" topLeftCell="A279" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
+      <selection pane="bottomLeft" activeCell="I294" activeCellId="0" sqref="I294"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
update attributs and xls
Aligned the digital input types with dbus-digitalinputs. Adding "Generator"
</commit_message>
<xml_diff>
--- a/CCGX-Modbus-TCP-register-list.xlsx
+++ b/CCGX-Modbus-TCP-register-list.xlsx
@@ -2847,7 +2847,7 @@
     <t xml:space="preserve">/Type</t>
   </si>
   <si>
-    <t xml:space="preserve">2=Door;3=Bilge pump;4=Bilge alarm;5=Burglar alarm;6=Smoke alarm;7=Fire alarm;8=CO2 alarm</t>
+    <t xml:space="preserve">2=Door;3=Bilge pump;4=Bilge alarm;5=Burglar alarm;6=Smoke alarm;7=Fire alarm;8=CO2 alarm;9=Generator</t>
   </si>
   <si>
     <t xml:space="preserve">com.victronenergy.generator</t>
@@ -4211,20 +4211,20 @@
   </sheetPr>
   <dimension ref="A1:N628"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="2" topLeftCell="A279" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="I294" activeCellId="0" sqref="I294"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="2" topLeftCell="A414" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="I436" activeCellId="0" sqref="I436"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.01171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="30"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="30.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="37.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="8.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="8.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="10.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="26.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="26.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="8.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="75.28"/>
@@ -22881,7 +22881,7 @@
     <hyperlink ref="J343" r:id="rId1" location="UUID-af4a7478-4b75-68ac-cf3c-16c381335d1e" display="This value is maintained by BatteryLife. The Active SOC limit is the lower of this value, and register 2901. Also see https://www.victronenergy.com/media/pg/Energy_Storage_System/en/controlling-depth-of-discharge.html#UUID-af4a7478-4b75-68ac-cf3c-16c381335d1e"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555556" footer="0.511805555555556"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -22901,11 +22901,11 @@
       <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="22" width="7.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="22" width="16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="22" width="65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="22" width="65.01"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="4" style="22" width="8.57"/>
   </cols>
   <sheetData>
@@ -23573,7 +23573,7 @@
     <mergeCell ref="A61:F61"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555556" footer="0.511805555555556"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -23593,7 +23593,7 @@
       <selection pane="topLeft" activeCell="A110" activeCellId="0" sqref="A110"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="22" width="8.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="22" width="3.43"/>
@@ -24285,7 +24285,7 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555556" footer="0.511805555555556"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>

</xml_diff>

<commit_message>
Added state 17 ("Contactor check") to battery /State
</commit_message>
<xml_diff>
--- a/CCGX-Modbus-TCP-register-list.xlsx
+++ b/CCGX-Modbus-TCP-register-list.xlsx
@@ -1872,7 +1872,7 @@
     <t xml:space="preserve">State</t>
   </si>
   <si>
-    <t xml:space="preserve">0=Initializing (Wait start);1=Initializing (before boot);2=Initializing (Before boot delay);3=Initializing (Wait boot);4=Initializing;5=Initializing (Measure battery voltage);6=Initializing (Calculate battery voltage);7=Initializing (Wait bus voltage);8=Initializing (Wait for lynx shunt);9=Running;10=Error (10);11=Unused (11);12=Shutdown;13=Slave updating;14=Standby;15=Going to run;16=Pre-charging</t>
+    <t xml:space="preserve">0=Initializing (Wait start);1=Initializing (before boot);2=Initializing (Before boot delay);3=Initializing (Wait boot);4=Initializing;5=Initializing (Measure battery voltage);6=Initializing (Calculate battery voltage);7=Initializing (Wait bus voltage);8=Initializing (Wait for lynx shunt);9=Running;10=Error (10);11=Unused (11);12=Shutdown;13=Slave updating;14=Standby;15=Going to run;16=Pre-charging;17=Contactor check</t>
   </si>
   <si>
     <t xml:space="preserve">Error</t>
@@ -4217,10 +4217,10 @@
   </sheetPr>
   <dimension ref="A1:N630"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="2" topLeftCell="A247" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A277" activeCellId="0" sqref="A277"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="2" topLeftCell="A235" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="I251" activeCellId="0" sqref="I251"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.01171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
update dbus path for ve.bus Bms PreAlarm
</commit_message>
<xml_diff>
--- a/CCGX-Modbus-TCP-register-list.xlsx
+++ b/CCGX-Modbus-TCP-register-list.xlsx
@@ -1050,10 +1050,10 @@
     <t xml:space="preserve">Low cell voltage imminent</t>
   </si>
   <si>
-    <t xml:space="preserve">/Bms/PreAlarm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0=OK;1=Pre-Alarm</t>
+    <t xml:space="preserve">/Alarms/BmsPreAlarm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0=OK;1=Warning</t>
   </si>
   <si>
     <t xml:space="preserve">Charge state</t>
@@ -4307,10 +4307,10 @@
   </sheetPr>
   <dimension ref="A1:N646"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="2" topLeftCell="A194" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B212" activeCellId="0" sqref="B212"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="2" topLeftCell="A105" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="I119" activeCellId="0" sqref="I119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Fix typo in acload serial number register.
</commit_message>
<xml_diff>
--- a/CCGX-Modbus-TCP-register-list.xlsx
+++ b/CCGX-Modbus-TCP-register-list.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4830" uniqueCount="1315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4832" uniqueCount="1317">
   <si>
     <t xml:space="preserve">NOTE: Use unit-id 100 for the com.victronenergy.system data, for more information see FAQ.</t>
   </si>
@@ -3967,6 +3967,12 @@
   </si>
   <si>
     <t xml:space="preserve">Add registers for genset engine oil pressure and fuel level</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rev 45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fix typo in AC-load service serial number register</t>
   </si>
 </sst>
 </file>
@@ -4320,9 +4326,9 @@
   <dimension ref="A1:N1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="2" topLeftCell="A420" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A433" activeCellId="0" sqref="A433"/>
+      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -18680,7 +18686,7 @@
         <v>1011</v>
       </c>
       <c r="C482" s="1" t="n">
-        <v>3902</v>
+        <v>3903</v>
       </c>
       <c r="D482" s="2" t="s">
         <v>609</v>
@@ -24256,10 +24262,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C118"/>
+  <dimension ref="A1:C119"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A109" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B118" activeCellId="0" sqref="B118"/>
+      <selection pane="topLeft" activeCell="B120" activeCellId="0" sqref="B120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -24995,6 +25001,14 @@
         <v>1314</v>
       </c>
     </row>
+    <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="22" t="s">
+        <v>1315</v>
+      </c>
+      <c r="B119" s="22" t="s">
+        <v>1316</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Updated list for com.victronenergy.evcharger /Status
Update and add new status codes for register 3824.
</commit_message>
<xml_diff>
--- a/CCGX-Modbus-TCP-register-list.xlsx
+++ b/CCGX-Modbus-TCP-register-list.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Field list" sheetId="1" state="visible" r:id="rId2"/>
@@ -3390,7 +3390,7 @@
     <t xml:space="preserve">/Current</t>
   </si>
   <si>
-    <t xml:space="preserve">0=Disconnected; 1=Connected; 2=Charging; 3=Charged; 4=Waiting for sun; 5=Waiting for RFID; 6=Waiting for start; 7=Low SOC; 8=Ground fault; 9=Welded contacts; 10=CP Input shorted; 11=Residual current detected; 12=Under voltage detected; 13=Overvoltage detected; 14=Overheating detected</t>
+    <t xml:space="preserve">0=Disconnected; 1=Connected; 2=Charging; 3=Charged; 4=Waiting for sun; 5=Waiting for RFID; 6=Waiting for start; 7=Low SOC; 8=Ground test error; 9=Welded contacts test error; 10=CP input test error (shorted); 11=Residual current detected; 12=Undervoltage detected; 13=Overvoltage detected; 14=Overheating detected; 15=Reserved; 16=Reserved; 17=Reserved; 19=Reserved; 20=Charging limit; 21=Start charging; 22=Switching to 3 phase; 23=Switching to 1 phase; 24=Stop charging</t>
   </si>
   <si>
     <t xml:space="preserve">Set charge current (manual mode)</t>
@@ -4715,10 +4715,10 @@
   </sheetPr>
   <dimension ref="A1:N738"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="2" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="2" topLeftCell="A523" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A41" activeCellId="0" sqref="A41"/>
+      <selection pane="bottomLeft" activeCell="A542" activeCellId="0" sqref="A542"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20791,7 +20791,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="542" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="542" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A542" s="1" t="s">
         <v>1110</v>
       </c>
@@ -26561,8 +26561,8 @@
     <hyperlink ref="J415" r:id="rId1" location="UUID-af4a7478-4b75-68ac-cf3c-16c381335d1e" display="This value is maintained by BatteryLife. The Active SOC limit is the lower of this value, and register 2901. Also see https://www.victronenergy.com/media/pg/Energy_Storage_System/en/controlling-depth-of-discharge.html#UUID-af4a7478-4b75-68ac-cf3c-16c381335d1e"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -27054,8 +27054,8 @@
     <mergeCell ref="A47:F47"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -27070,7 +27070,7 @@
   </sheetPr>
   <dimension ref="A1:C140"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A123" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A69" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B140" activeCellId="0" sqref="B140"/>
     </sheetView>
   </sheetViews>
@@ -27931,8 +27931,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
Register 3824, adding status 18
Status 18 is "Reserved", this was missing in the list.
</commit_message>
<xml_diff>
--- a/CCGX-Modbus-TCP-register-list.xlsx
+++ b/CCGX-Modbus-TCP-register-list.xlsx
@@ -3390,7 +3390,7 @@
     <t xml:space="preserve">/Current</t>
   </si>
   <si>
-    <t xml:space="preserve">0=Disconnected; 1=Connected; 2=Charging; 3=Charged; 4=Waiting for sun; 5=Waiting for RFID; 6=Waiting for start; 7=Low SOC; 8=Ground test error; 9=Welded contacts test error; 10=CP input test error (shorted); 11=Residual current detected; 12=Undervoltage detected; 13=Overvoltage detected; 14=Overheating detected; 15=Reserved; 16=Reserved; 17=Reserved; 19=Reserved; 20=Charging limit; 21=Start charging; 22=Switching to 3 phase; 23=Switching to 1 phase; 24=Stop charging</t>
+    <t xml:space="preserve">0=Disconnected; 1=Connected; 2=Charging; 3=Charged; 4=Waiting for sun; 5=Waiting for RFID; 6=Waiting for start; 7=Low SOC; 8=Ground test error; 9=Welded contacts test error; 10=CP input test error (shorted); 11=Residual current detected; 12=Undervoltage detected; 13=Overvoltage detected; 14=Overheating detected; 15=Reserved; 16=Reserved; 17=Reserved; 18=Reserved; 19=Reserved; 20=Charging limit; 21=Start charging; 22=Switching to 3 phase; 23=Switching to 1 phase; 24=Stop charging</t>
   </si>
   <si>
     <t xml:space="preserve">Set charge current (manual mode)</t>
@@ -4715,10 +4715,10 @@
   </sheetPr>
   <dimension ref="A1:N738"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A523" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A542" activeCellId="0" sqref="A542"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="I547" activeCellId="0" sqref="I547"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Update temperature and tank status
Disconnect is now called "Open circuit" for both temperature
as tank sensors.
See issue https://github.com/victronenergy/venus-private/issues/378
</commit_message>
<xml_diff>
--- a/CCGX-Modbus-TCP-register-list.xlsx
+++ b/CCGX-Modbus-TCP-register-list.xlsx
@@ -8,9 +8,9 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Field list" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Unit ID mapping" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Document versions" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Field list" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Unit ID mapping" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="Document versions" sheetId="3" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -2844,7 +2844,7 @@
     <t xml:space="preserve">/Status</t>
   </si>
   <si>
-    <t xml:space="preserve">0=OK;1=Disconnected;2=Short circuited;3=Reverse Polarity;4=Unknown</t>
+    <t xml:space="preserve">0=OK;1=Open circuit;2=Short circuited;3=Reverse Polarity;4=Unknown</t>
   </si>
   <si>
     <t xml:space="preserve">com.victronenergy.inverter</t>
@@ -4523,15 +4523,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4540,11 +4540,11 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -4552,10 +4552,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4583,43 +4583,43 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4627,11 +4627,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4708,24 +4708,130 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:N738"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="2" topLeftCell="A523" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="I547" activeCellId="0" sqref="I547"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="2" topLeftCell="A403" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="I423" activeCellId="0" sqref="I423"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="30.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="37.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="8.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="8.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="8.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="10.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="26.6"/>
@@ -5498,7 +5604,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
         <v>12</v>
       </c>
@@ -5934,7 +6040,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
         <v>12</v>
       </c>
@@ -5957,7 +6063,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
         <v>12</v>
       </c>
@@ -5983,7 +6089,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
         <v>12</v>
       </c>
@@ -8451,7 +8557,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="1" t="s">
         <v>138</v>
       </c>
@@ -8480,7 +8586,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="1" t="s">
         <v>138</v>
       </c>
@@ -8509,7 +8615,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="1" t="s">
         <v>138</v>
       </c>
@@ -8541,7 +8647,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="1" t="s">
         <v>138</v>
       </c>
@@ -8570,7 +8676,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="1" t="s">
         <v>138</v>
       </c>
@@ -8599,7 +8705,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="1" t="s">
         <v>138</v>
       </c>
@@ -8631,7 +8737,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="1" t="s">
         <v>138</v>
       </c>
@@ -8663,7 +8769,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="1" t="s">
         <v>138</v>
       </c>
@@ -8692,7 +8798,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="1" t="s">
         <v>138</v>
       </c>
@@ -8721,7 +8827,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="1" t="s">
         <v>138</v>
       </c>
@@ -8747,7 +8853,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="1" t="s">
         <v>138</v>
       </c>
@@ -8773,7 +8879,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="1" t="s">
         <v>138</v>
       </c>
@@ -8799,7 +8905,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="1" t="s">
         <v>138</v>
       </c>
@@ -8825,7 +8931,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="1" t="s">
         <v>138</v>
       </c>
@@ -8851,7 +8957,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="1" t="s">
         <v>138</v>
       </c>
@@ -8877,7 +8983,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="1" t="s">
         <v>138</v>
       </c>
@@ -8903,7 +9009,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="1" t="s">
         <v>138</v>
       </c>
@@ -8929,7 +9035,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="1" t="s">
         <v>138</v>
       </c>
@@ -8955,7 +9061,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="1" t="s">
         <v>138</v>
       </c>
@@ -8981,7 +9087,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="1" t="s">
         <v>138</v>
       </c>
@@ -9007,7 +9113,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="1" t="s">
         <v>138</v>
       </c>
@@ -9033,7 +9139,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="1" t="s">
         <v>138</v>
       </c>
@@ -9062,7 +9168,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="1" t="s">
         <v>138</v>
       </c>
@@ -9091,7 +9197,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="1" t="s">
         <v>138</v>
       </c>
@@ -9120,7 +9226,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="1" t="s">
         <v>138</v>
       </c>
@@ -9149,7 +9255,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="1" t="s">
         <v>138</v>
       </c>
@@ -9178,7 +9284,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="1" t="s">
         <v>138</v>
       </c>
@@ -9207,7 +9313,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="1" t="s">
         <v>138</v>
       </c>
@@ -9236,7 +9342,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="151" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="1" t="s">
         <v>138</v>
       </c>
@@ -9265,7 +9371,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="152" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="1" t="s">
         <v>138</v>
       </c>
@@ -9294,7 +9400,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="153" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="1" t="s">
         <v>138</v>
       </c>
@@ -9323,7 +9429,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="154" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="1" t="s">
         <v>138</v>
       </c>
@@ -9352,7 +9458,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="155" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="1" t="s">
         <v>138</v>
       </c>
@@ -9381,7 +9487,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="156" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="1" t="s">
         <v>138</v>
       </c>
@@ -9410,7 +9516,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="157" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="1" t="s">
         <v>138</v>
       </c>
@@ -9439,7 +9545,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="158" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="1" t="s">
         <v>138</v>
       </c>
@@ -9468,7 +9574,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="159" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="1" t="s">
         <v>138</v>
       </c>
@@ -9497,7 +9603,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="160" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="1" t="s">
         <v>138</v>
       </c>
@@ -9526,7 +9632,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="161" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="1" t="s">
         <v>138</v>
       </c>
@@ -9555,7 +9661,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="162" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="1" t="s">
         <v>138</v>
       </c>
@@ -9584,7 +9690,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="163" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="1" t="s">
         <v>138</v>
       </c>
@@ -9613,7 +9719,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="164" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="1" t="s">
         <v>138</v>
       </c>
@@ -9642,7 +9748,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="165" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="1" t="s">
         <v>138</v>
       </c>
@@ -9671,7 +9777,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="166" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="1" t="s">
         <v>138</v>
       </c>
@@ -9700,7 +9806,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="167" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="1" t="s">
         <v>138</v>
       </c>
@@ -9729,7 +9835,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="168" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="1" t="s">
         <v>138</v>
       </c>
@@ -9758,7 +9864,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="169" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="1" t="s">
         <v>138</v>
       </c>
@@ -9787,7 +9893,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="170" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="1" t="s">
         <v>138</v>
       </c>
@@ -9816,7 +9922,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="171" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="1" t="s">
         <v>453</v>
       </c>
@@ -11794,7 +11900,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="236" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="236" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A236" s="1" t="s">
         <v>453</v>
       </c>
@@ -12567,7 +12673,7 @@
       <c r="M260" s="20"/>
       <c r="N260" s="20"/>
     </row>
-    <row r="261" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="261" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A261" s="1" t="s">
         <v>588</v>
       </c>
@@ -12600,7 +12706,7 @@
       <c r="M261" s="20"/>
       <c r="N261" s="20"/>
     </row>
-    <row r="262" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="262" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A262" s="1" t="s">
         <v>588</v>
       </c>
@@ -12627,7 +12733,7 @@
       <c r="M262" s="20"/>
       <c r="N262" s="20"/>
     </row>
-    <row r="263" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="263" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A263" s="1" t="s">
         <v>588</v>
       </c>
@@ -12654,7 +12760,7 @@
       <c r="M263" s="20"/>
       <c r="N263" s="20"/>
     </row>
-    <row r="264" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="264" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A264" s="1" t="s">
         <v>588</v>
       </c>
@@ -12681,7 +12787,7 @@
       <c r="M264" s="20"/>
       <c r="N264" s="20"/>
     </row>
-    <row r="265" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="265" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A265" s="1" t="s">
         <v>588</v>
       </c>
@@ -13335,7 +13441,7 @@
       <c r="M284" s="20"/>
       <c r="N284" s="20"/>
     </row>
-    <row r="285" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="285" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A285" s="1" t="s">
         <v>588</v>
       </c>
@@ -13368,7 +13474,7 @@
       <c r="M285" s="20"/>
       <c r="N285" s="20"/>
     </row>
-    <row r="286" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="286" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A286" s="1" t="s">
         <v>588</v>
       </c>
@@ -13404,7 +13510,7 @@
       <c r="M286" s="20"/>
       <c r="N286" s="20"/>
     </row>
-    <row r="287" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="287" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A287" s="1" t="s">
         <v>588</v>
       </c>
@@ -13437,7 +13543,7 @@
       <c r="M287" s="20"/>
       <c r="N287" s="20"/>
     </row>
-    <row r="288" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="288" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A288" s="1" t="s">
         <v>588</v>
       </c>
@@ -13470,7 +13576,7 @@
       <c r="M288" s="20"/>
       <c r="N288" s="20"/>
     </row>
-    <row r="289" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="289" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A289" s="1" t="s">
         <v>588</v>
       </c>
@@ -13503,7 +13609,7 @@
       <c r="M289" s="20"/>
       <c r="N289" s="20"/>
     </row>
-    <row r="290" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="290" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A290" s="1" t="s">
         <v>588</v>
       </c>
@@ -13536,7 +13642,7 @@
       <c r="M290" s="20"/>
       <c r="N290" s="20"/>
     </row>
-    <row r="291" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="291" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A291" s="1" t="s">
         <v>588</v>
       </c>
@@ -14129,7 +14235,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="311" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="311" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A311" s="1" t="s">
         <v>687</v>
       </c>
@@ -14161,7 +14267,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="312" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="312" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A312" s="1" t="s">
         <v>687</v>
       </c>
@@ -14190,7 +14296,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="313" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="313" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A313" s="1" t="s">
         <v>687</v>
       </c>
@@ -14219,7 +14325,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="314" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="314" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A314" s="1" t="s">
         <v>687</v>
       </c>
@@ -14799,7 +14905,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="334" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="334" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A334" s="1" t="s">
         <v>453</v>
       </c>
@@ -14828,7 +14934,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="335" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="335" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A335" s="1" t="s">
         <v>453</v>
       </c>
@@ -14854,7 +14960,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="336" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="336" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A336" s="1" t="s">
         <v>453</v>
       </c>
@@ -14880,7 +14986,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="337" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="337" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A337" s="1" t="s">
         <v>453</v>
       </c>
@@ -14906,7 +15012,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="338" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="338" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A338" s="1" t="s">
         <v>453</v>
       </c>
@@ -14932,7 +15038,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="339" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="339" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A339" s="1" t="s">
         <v>453</v>
       </c>
@@ -14952,7 +15058,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="340" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="340" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A340" s="1" t="s">
         <v>453</v>
       </c>
@@ -14972,7 +15078,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="341" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="341" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A341" s="1" t="s">
         <v>453</v>
       </c>
@@ -14992,7 +15098,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="342" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="342" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A342" s="1" t="s">
         <v>453</v>
       </c>
@@ -16320,7 +16426,7 @@
         <v>843</v>
       </c>
     </row>
-    <row r="388" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="388" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A388" s="1" t="s">
         <v>820</v>
       </c>
@@ -16349,7 +16455,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="389" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="389" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A389" s="1" t="s">
         <v>820</v>
       </c>
@@ -16378,7 +16484,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="390" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="390" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A390" s="1" t="s">
         <v>820</v>
       </c>
@@ -16407,7 +16513,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="391" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="391" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A391" s="1" t="s">
         <v>820</v>
       </c>
@@ -16564,7 +16670,7 @@
         <v>857</v>
       </c>
     </row>
-    <row r="396" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="396" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A396" s="1" t="s">
         <v>846</v>
       </c>
@@ -16596,7 +16702,7 @@
         <v>860</v>
       </c>
     </row>
-    <row r="397" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="397" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A397" s="1" t="s">
         <v>846</v>
       </c>
@@ -16747,7 +16853,7 @@
         <v>879</v>
       </c>
     </row>
-    <row r="402" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="402" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A402" s="1" t="s">
         <v>846</v>
       </c>
@@ -16779,7 +16885,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="403" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="403" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A403" s="1" t="s">
         <v>846</v>
       </c>
@@ -16811,7 +16917,7 @@
         <v>886</v>
       </c>
     </row>
-    <row r="404" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="404" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A404" s="1" t="s">
         <v>846</v>
       </c>
@@ -17134,7 +17240,7 @@
       </c>
       <c r="J414" s="21"/>
     </row>
-    <row r="415" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="415" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A415" s="21" t="s">
         <v>846</v>
       </c>
@@ -18663,7 +18769,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="468" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="468" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A468" s="1" t="s">
         <v>941</v>
       </c>
@@ -18692,7 +18798,7 @@
         <v>948</v>
       </c>
     </row>
-    <row r="469" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="469" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A469" s="1" t="s">
         <v>941</v>
       </c>
@@ -18721,7 +18827,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="470" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="470" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A470" s="1" t="s">
         <v>941</v>
       </c>
@@ -18750,7 +18856,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="471" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="471" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A471" s="1" t="s">
         <v>941</v>
       </c>
@@ -18779,7 +18885,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="472" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="472" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A472" s="1" t="s">
         <v>941</v>
       </c>
@@ -19472,7 +19578,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="496" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="496" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A496" s="1" t="s">
         <v>988</v>
       </c>
@@ -19504,7 +19610,7 @@
         <v>1029</v>
       </c>
     </row>
-    <row r="497" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="497" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A497" s="1" t="s">
         <v>988</v>
       </c>
@@ -20168,7 +20274,7 @@
         <v>1085</v>
       </c>
     </row>
-    <row r="520" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="520" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A520" s="1" t="s">
         <v>1068</v>
       </c>
@@ -20197,7 +20303,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="521" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="521" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A521" s="1" t="s">
         <v>1068</v>
       </c>
@@ -20226,7 +20332,7 @@
         <v>1090</v>
       </c>
     </row>
-    <row r="522" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="522" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A522" s="1" t="s">
         <v>1068</v>
       </c>
@@ -20255,7 +20361,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="523" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="523" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A523" s="1" t="s">
         <v>1068</v>
       </c>
@@ -20371,7 +20477,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="527" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="527" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A527" s="1" t="s">
         <v>1097</v>
       </c>
@@ -20400,7 +20506,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="528" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="528" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A528" s="1" t="s">
         <v>1097</v>
       </c>
@@ -20791,7 +20897,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="542" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="542" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A542" s="1" t="s">
         <v>1110</v>
       </c>
@@ -22029,7 +22135,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="585" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="585" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A585" s="22" t="s">
         <v>1136</v>
       </c>
@@ -22058,7 +22164,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="586" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="586" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A586" s="22" t="s">
         <v>1136</v>
       </c>
@@ -22087,7 +22193,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="587" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="587" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A587" s="22" t="s">
         <v>1136</v>
       </c>
@@ -22116,7 +22222,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="588" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="588" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A588" s="22" t="s">
         <v>1136</v>
       </c>
@@ -22145,7 +22251,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="589" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="589" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A589" s="22" t="s">
         <v>1136</v>
       </c>
@@ -25773,7 +25879,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="712" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="712" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A712" s="1" t="s">
         <v>1157</v>
       </c>
@@ -25802,7 +25908,7 @@
         <v>948</v>
       </c>
     </row>
-    <row r="713" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="713" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A713" s="1" t="s">
         <v>1157</v>
       </c>
@@ -25834,7 +25940,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="714" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="714" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A714" s="1" t="s">
         <v>1157</v>
       </c>
@@ -25863,7 +25969,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="715" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="715" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A715" s="1" t="s">
         <v>1157</v>
       </c>
@@ -25892,7 +25998,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="716" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="716" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A716" s="1" t="s">
         <v>1157</v>
       </c>
@@ -25921,7 +26027,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="717" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="717" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A717" s="1" t="s">
         <v>1157</v>
       </c>
@@ -25950,7 +26056,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="718" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="718" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A718" s="1" t="s">
         <v>1157</v>
       </c>
@@ -25979,7 +26085,7 @@
         <v>1206</v>
       </c>
     </row>
-    <row r="719" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="719" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A719" s="1" t="s">
         <v>1157</v>
       </c>
@@ -26008,7 +26114,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="720" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="720" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A720" s="1" t="s">
         <v>1157</v>
       </c>
@@ -26037,7 +26143,7 @@
         <v>1211</v>
       </c>
     </row>
-    <row r="721" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="721" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A721" s="1" t="s">
         <v>1157</v>
       </c>
@@ -26066,7 +26172,7 @@
         <v>1214</v>
       </c>
     </row>
-    <row r="722" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="722" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A722" s="1" t="s">
         <v>1157</v>
       </c>
@@ -26095,7 +26201,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="723" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="723" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A723" s="1" t="s">
         <v>1217</v>
       </c>
@@ -26124,7 +26230,7 @@
         <v>1219</v>
       </c>
     </row>
-    <row r="724" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="724" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A724" s="1" t="s">
         <v>846</v>
       </c>
@@ -26153,7 +26259,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="725" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="725" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A725" s="1" t="s">
         <v>846</v>
       </c>
@@ -26182,7 +26288,7 @@
         <v>1223</v>
       </c>
     </row>
-    <row r="726" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="726" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A726" s="1" t="s">
         <v>846</v>
       </c>
@@ -26211,7 +26317,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="727" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="727" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A727" s="1" t="s">
         <v>846</v>
       </c>
@@ -26240,7 +26346,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="728" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="728" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A728" s="1" t="s">
         <v>1228</v>
       </c>
@@ -26266,7 +26372,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="729" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="729" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A729" s="1" t="s">
         <v>1228</v>
       </c>
@@ -26292,7 +26398,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="730" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="730" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A730" s="1" t="s">
         <v>1228</v>
       </c>
@@ -26321,7 +26427,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="731" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="731" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A731" s="1" t="s">
         <v>1228</v>
       </c>
@@ -26350,7 +26456,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="732" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="732" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A732" s="1" t="s">
         <v>1228</v>
       </c>
@@ -26379,7 +26485,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="733" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="733" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A733" s="1" t="s">
         <v>1228</v>
       </c>
@@ -26408,7 +26514,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="734" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="734" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A734" s="1" t="s">
         <v>1228</v>
       </c>
@@ -26437,7 +26543,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="735" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="735" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A735" s="1" t="s">
         <v>1228</v>
       </c>
@@ -26466,7 +26572,7 @@
         <v>1229</v>
       </c>
     </row>
-    <row r="736" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="736" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A736" s="1" t="s">
         <v>1228</v>
       </c>
@@ -26495,7 +26601,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="737" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="737" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A737" s="1" t="s">
         <v>1228</v>
       </c>
@@ -26524,7 +26630,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="738" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="738" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A738" s="1" t="s">
         <v>1228</v>
       </c>
@@ -26571,7 +26677,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -26581,9 +26687,9 @@
       <selection pane="topLeft" activeCell="B48" activeCellId="0" sqref="B48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="22" width="7.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="22" width="7.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="22" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="22" width="65.01"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="4" style="22" width="8.57"/>
@@ -26600,7 +26706,7 @@
         <v>1232</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="22" t="n">
         <v>100</v>
       </c>
@@ -26611,7 +26717,7 @@
         <v>1233</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="22" t="n">
         <v>204</v>
       </c>
@@ -26619,7 +26725,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="22" t="n">
         <v>205</v>
       </c>
@@ -26627,7 +26733,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="22" t="n">
         <v>206</v>
       </c>
@@ -26635,7 +26741,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="22" t="n">
         <v>207</v>
       </c>
@@ -26643,7 +26749,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="22" t="n">
         <v>208</v>
       </c>
@@ -26651,7 +26757,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="22" t="n">
         <v>209</v>
       </c>
@@ -26659,7 +26765,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="22" t="n">
         <v>210</v>
       </c>
@@ -26667,7 +26773,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="22" t="n">
         <v>211</v>
       </c>
@@ -26675,7 +26781,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="22" t="n">
         <v>212</v>
       </c>
@@ -26683,7 +26789,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="22" t="n">
         <v>213</v>
       </c>
@@ -26691,7 +26797,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="22" t="n">
         <v>214</v>
       </c>
@@ -26699,7 +26805,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="22" t="n">
         <v>215</v>
       </c>
@@ -26707,7 +26813,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="22" t="n">
         <v>216</v>
       </c>
@@ -26715,7 +26821,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="22" t="n">
         <v>217</v>
       </c>
@@ -26723,7 +26829,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="22" t="n">
         <v>218</v>
       </c>
@@ -26731,7 +26837,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="22" t="n">
         <v>219</v>
       </c>
@@ -26739,7 +26845,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="22" t="n">
         <v>220</v>
       </c>
@@ -26747,7 +26853,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="22" t="n">
         <v>221</v>
       </c>
@@ -26755,7 +26861,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="22" t="n">
         <v>222</v>
       </c>
@@ -26972,7 +27078,7 @@
         <v>1252</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="25" t="n">
         <v>244</v>
       </c>
@@ -27064,7 +27170,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -27074,7 +27180,7 @@
       <selection pane="topLeft" activeCell="B140" activeCellId="0" sqref="B140"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="22" width="8.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="22" width="3.43"/>
@@ -27305,7 +27411,7 @@
         <v>1306</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="54.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C39" s="28" t="s">
         <v>1307</v>
       </c>

</xml_diff>

<commit_message>
Add missing states to generator /State
Cool-down, warm-up and stopping
</commit_message>
<xml_diff>
--- a/CCGX-Modbus-TCP-register-list.xlsx
+++ b/CCGX-Modbus-TCP-register-list.xlsx
@@ -8,9 +8,9 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Field list" sheetId="1" state="visible" r:id="rId3"/>
-    <sheet name="Unit ID mapping" sheetId="2" state="visible" r:id="rId4"/>
-    <sheet name="Document versions" sheetId="3" state="visible" r:id="rId5"/>
+    <sheet name="Field list" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Unit ID mapping" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Document versions" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -3462,7 +3462,7 @@
     <t xml:space="preserve">Generator start/stop state</t>
   </si>
   <si>
-    <t xml:space="preserve">0=Stopped;1=Running;2=Warmup;3=Cooldown;4=Stopping;10=Error</t>
+    <t xml:space="preserve">0=Stopped;1=Running;2=Warm-up;3=Cool-down;4=Stopping;10=Error</t>
   </si>
   <si>
     <t xml:space="preserve">Generator remote error</t>
@@ -4964,7 +4964,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -5054,6 +5054,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5162,130 +5166,24 @@
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
-  <a:themeElements>
-    <a:clrScheme name="LibreOffice">
-      <a:dk1>
-        <a:srgbClr val="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:srgbClr val="ffffff"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="000000"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="ffffff"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="18a303"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="0369a3"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="a33e03"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="8e03a3"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="c99c00"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="c9211e"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0000ee"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="551a8b"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme>
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:N1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="2" topLeftCell="A370" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B388" activeCellId="0" sqref="B388"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="2" topLeftCell="A509" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
+      <selection pane="bottomLeft" activeCell="I514" activeCellId="0" sqref="I514"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.01171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="30.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="37.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="8.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="8.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="8.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="10.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="26.6"/>
@@ -16832,7 +16730,7 @@
       <c r="A386" s="1" t="s">
         <v>806</v>
       </c>
-      <c r="B386" s="0" t="s">
+      <c r="B386" s="23" t="s">
         <v>849</v>
       </c>
       <c r="C386" s="1" t="n">
@@ -16841,7 +16739,7 @@
       <c r="D386" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E386" s="0" t="n">
+      <c r="E386" s="23" t="n">
         <v>1</v>
       </c>
       <c r="F386" s="3" t="s">
@@ -16861,7 +16759,7 @@
       <c r="A387" s="1" t="s">
         <v>806</v>
       </c>
-      <c r="B387" s="0" t="s">
+      <c r="B387" s="23" t="s">
         <v>852</v>
       </c>
       <c r="C387" s="1" t="n">
@@ -16870,7 +16768,7 @@
       <c r="D387" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E387" s="0" t="n">
+      <c r="E387" s="23" t="n">
         <v>1</v>
       </c>
       <c r="F387" s="3" t="s">
@@ -16890,7 +16788,7 @@
       <c r="A388" s="1" t="s">
         <v>806</v>
       </c>
-      <c r="B388" s="0" t="s">
+      <c r="B388" s="23" t="s">
         <v>854</v>
       </c>
       <c r="C388" s="1" t="n">
@@ -16899,7 +16797,7 @@
       <c r="D388" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E388" s="0" t="n">
+      <c r="E388" s="23" t="n">
         <v>1</v>
       </c>
       <c r="F388" s="3" t="s">
@@ -17263,7 +17161,7 @@
       <c r="H400" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I400" s="23"/>
+      <c r="I400" s="24"/>
     </row>
     <row r="401" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A401" s="1" t="s">
@@ -27814,19 +27712,19 @@
       <c r="B772" s="1" t="s">
         <v>1226</v>
       </c>
-      <c r="C772" s="24" t="n">
+      <c r="C772" s="25" t="n">
         <v>5200</v>
       </c>
-      <c r="D772" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="E772" s="24" t="n">
+      <c r="D772" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="E772" s="25" t="n">
         <v>1</v>
       </c>
       <c r="F772" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="G772" s="24" t="s">
+      <c r="G772" s="25" t="s">
         <v>895</v>
       </c>
       <c r="H772" s="1" t="s">
@@ -27840,19 +27738,19 @@
       <c r="B773" s="1" t="s">
         <v>970</v>
       </c>
-      <c r="C773" s="24" t="n">
+      <c r="C773" s="25" t="n">
         <v>5201</v>
       </c>
-      <c r="D773" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="E773" s="24" t="n">
+      <c r="D773" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="E773" s="25" t="n">
         <v>1</v>
       </c>
       <c r="F773" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="G773" s="24" t="s">
+      <c r="G773" s="25" t="s">
         <v>971</v>
       </c>
       <c r="H773" s="1" t="s">
@@ -27866,19 +27764,19 @@
       <c r="B774" s="1" t="s">
         <v>676</v>
       </c>
-      <c r="C774" s="24" t="n">
+      <c r="C774" s="25" t="n">
         <v>5202</v>
       </c>
-      <c r="D774" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="E774" s="24" t="n">
+      <c r="D774" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="E774" s="25" t="n">
         <v>1</v>
       </c>
       <c r="F774" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="G774" s="24" t="s">
+      <c r="G774" s="25" t="s">
         <v>564</v>
       </c>
       <c r="H774" s="1" t="s">
@@ -27892,19 +27790,19 @@
       <c r="B775" s="1" t="s">
         <v>1208</v>
       </c>
-      <c r="C775" s="24" t="n">
+      <c r="C775" s="25" t="n">
         <v>5203</v>
       </c>
-      <c r="D775" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="E775" s="24" t="n">
+      <c r="D775" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="E775" s="25" t="n">
         <v>1</v>
       </c>
       <c r="F775" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="G775" s="24" t="s">
+      <c r="G775" s="25" t="s">
         <v>975</v>
       </c>
       <c r="H775" s="1" t="s">
@@ -27918,19 +27816,19 @@
       <c r="B776" s="1" t="s">
         <v>990</v>
       </c>
-      <c r="C776" s="24" t="n">
+      <c r="C776" s="25" t="n">
         <v>5204</v>
       </c>
-      <c r="D776" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="E776" s="24" t="n">
+      <c r="D776" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="E776" s="25" t="n">
         <v>1</v>
       </c>
       <c r="F776" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="G776" s="24" t="s">
+      <c r="G776" s="25" t="s">
         <v>991</v>
       </c>
       <c r="H776" s="1" t="s">
@@ -27947,19 +27845,19 @@
       <c r="B777" s="1" t="s">
         <v>1227</v>
       </c>
-      <c r="C777" s="24" t="n">
+      <c r="C777" s="25" t="n">
         <v>5205</v>
       </c>
-      <c r="D777" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="E777" s="24" t="n">
+      <c r="D777" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="E777" s="25" t="n">
         <v>100</v>
       </c>
       <c r="F777" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="G777" s="24" t="s">
+      <c r="G777" s="25" t="s">
         <v>213</v>
       </c>
       <c r="H777" s="1" t="s">
@@ -27976,19 +27874,19 @@
       <c r="B778" s="1" t="s">
         <v>1229</v>
       </c>
-      <c r="C778" s="24" t="n">
+      <c r="C778" s="25" t="n">
         <v>5206</v>
       </c>
-      <c r="D778" s="24" t="s">
+      <c r="D778" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="E778" s="24" t="n">
+      <c r="E778" s="25" t="n">
         <v>10</v>
       </c>
       <c r="F778" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="G778" s="24" t="s">
+      <c r="G778" s="25" t="s">
         <v>215</v>
       </c>
       <c r="H778" s="1" t="s">
@@ -28002,22 +27900,22 @@
       <c r="A779" s="22" t="s">
         <v>1225</v>
       </c>
-      <c r="B779" s="24" t="s">
+      <c r="B779" s="25" t="s">
         <v>976</v>
       </c>
-      <c r="C779" s="24" t="n">
+      <c r="C779" s="25" t="n">
         <v>5207</v>
       </c>
-      <c r="D779" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="E779" s="24" t="n">
+      <c r="D779" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="E779" s="25" t="n">
         <v>1</v>
       </c>
       <c r="F779" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="G779" s="24" t="s">
+      <c r="G779" s="25" t="s">
         <v>977</v>
       </c>
       <c r="H779" s="1" t="s">
@@ -28034,19 +27932,19 @@
       <c r="B780" s="1" t="s">
         <v>1231</v>
       </c>
-      <c r="C780" s="24" t="n">
+      <c r="C780" s="25" t="n">
         <v>5208</v>
       </c>
-      <c r="D780" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="E780" s="24" t="n">
+      <c r="D780" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="E780" s="25" t="n">
         <v>1</v>
       </c>
       <c r="F780" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="G780" s="24" t="s">
+      <c r="G780" s="25" t="s">
         <v>979</v>
       </c>
       <c r="H780" s="1" t="s">
@@ -28063,19 +27961,19 @@
       <c r="B781" s="1" t="s">
         <v>997</v>
       </c>
-      <c r="C781" s="24" t="n">
+      <c r="C781" s="25" t="n">
         <v>5209</v>
       </c>
-      <c r="D781" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="E781" s="24" t="s">
+      <c r="D781" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="E781" s="25" t="s">
         <v>1232</v>
       </c>
       <c r="F781" s="3" t="s">
         <v>318</v>
       </c>
-      <c r="G781" s="24" t="s">
+      <c r="G781" s="25" t="s">
         <v>981</v>
       </c>
       <c r="H781" s="1" t="s">
@@ -28089,22 +27987,22 @@
       <c r="A782" s="22" t="s">
         <v>1225</v>
       </c>
-      <c r="B782" s="24" t="s">
+      <c r="B782" s="25" t="s">
         <v>982</v>
       </c>
-      <c r="C782" s="24" t="n">
+      <c r="C782" s="25" t="n">
         <v>5210</v>
       </c>
-      <c r="D782" s="24" t="s">
+      <c r="D782" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="E782" s="24" t="n">
+      <c r="E782" s="25" t="n">
         <v>10</v>
       </c>
       <c r="F782" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="G782" s="24" t="s">
+      <c r="G782" s="25" t="s">
         <v>983</v>
       </c>
       <c r="H782" s="1" t="s">
@@ -28118,22 +28016,22 @@
       <c r="A783" s="22" t="s">
         <v>1225</v>
       </c>
-      <c r="B783" s="24" t="s">
+      <c r="B783" s="25" t="s">
         <v>1234</v>
       </c>
-      <c r="C783" s="24" t="n">
+      <c r="C783" s="25" t="n">
         <v>5211</v>
       </c>
-      <c r="D783" s="24" t="s">
+      <c r="D783" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="E783" s="24" t="n">
+      <c r="E783" s="25" t="n">
         <v>10</v>
       </c>
       <c r="F783" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="G783" s="24" t="s">
+      <c r="G783" s="25" t="s">
         <v>985</v>
       </c>
       <c r="H783" s="1" t="s">
@@ -28147,22 +28045,22 @@
       <c r="A784" s="22" t="s">
         <v>1225</v>
       </c>
-      <c r="B784" s="24" t="s">
+      <c r="B784" s="25" t="s">
         <v>986</v>
       </c>
-      <c r="C784" s="24" t="n">
+      <c r="C784" s="25" t="n">
         <v>5212</v>
       </c>
-      <c r="D784" s="24" t="s">
+      <c r="D784" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="E784" s="24" t="n">
+      <c r="E784" s="25" t="n">
         <v>10</v>
       </c>
       <c r="F784" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="G784" s="24" t="s">
+      <c r="G784" s="25" t="s">
         <v>987</v>
       </c>
       <c r="H784" s="1" t="s">
@@ -28176,22 +28074,22 @@
       <c r="A785" s="22" t="s">
         <v>1225</v>
       </c>
-      <c r="B785" s="24" t="s">
+      <c r="B785" s="25" t="s">
         <v>400</v>
       </c>
-      <c r="C785" s="24" t="n">
+      <c r="C785" s="25" t="n">
         <v>5213</v>
       </c>
-      <c r="D785" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="E785" s="24" t="n">
+      <c r="D785" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="E785" s="25" t="n">
         <v>100</v>
       </c>
       <c r="F785" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="G785" s="24" t="s">
+      <c r="G785" s="25" t="s">
         <v>989</v>
       </c>
       <c r="H785" s="1" t="s">
@@ -28208,19 +28106,19 @@
       <c r="B786" s="1" t="s">
         <v>994</v>
       </c>
-      <c r="C786" s="24" t="n">
+      <c r="C786" s="25" t="n">
         <v>5214</v>
       </c>
-      <c r="D786" s="24" t="s">
+      <c r="D786" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="E786" s="24" t="n">
+      <c r="E786" s="25" t="n">
         <v>1</v>
       </c>
       <c r="F786" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="G786" s="24" t="s">
+      <c r="G786" s="25" t="s">
         <v>995</v>
       </c>
       <c r="H786" s="1" t="s">
@@ -28234,22 +28132,22 @@
       <c r="A787" s="22" t="s">
         <v>1225</v>
       </c>
-      <c r="B787" s="24" t="s">
+      <c r="B787" s="25" t="s">
         <v>1231</v>
       </c>
-      <c r="C787" s="24" t="n">
+      <c r="C787" s="25" t="n">
         <v>5215</v>
       </c>
-      <c r="D787" s="24" t="s">
+      <c r="D787" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="E787" s="24" t="n">
+      <c r="E787" s="25" t="n">
         <v>10</v>
       </c>
       <c r="F787" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="G787" s="24" t="s">
+      <c r="G787" s="25" t="s">
         <v>1235</v>
       </c>
       <c r="H787" s="1" t="s">
@@ -28266,19 +28164,19 @@
       <c r="B788" s="1" t="s">
         <v>997</v>
       </c>
-      <c r="C788" s="24" t="n">
+      <c r="C788" s="25" t="n">
         <v>5216</v>
       </c>
-      <c r="D788" s="24" t="s">
+      <c r="D788" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="E788" s="24" t="n">
+      <c r="E788" s="25" t="n">
         <v>1</v>
       </c>
       <c r="F788" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="G788" s="24" t="s">
+      <c r="G788" s="25" t="s">
         <v>998</v>
       </c>
       <c r="H788" s="1" t="s">
@@ -28292,19 +28190,19 @@
       <c r="A789" s="22" t="s">
         <v>1225</v>
       </c>
-      <c r="B789" s="24" t="s">
+      <c r="B789" s="25" t="s">
         <v>130</v>
       </c>
-      <c r="C789" s="24" t="n">
+      <c r="C789" s="25" t="n">
         <v>5217</v>
       </c>
-      <c r="D789" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="E789" s="24" t="n">
-        <v>1</v>
-      </c>
-      <c r="G789" s="24" t="s">
+      <c r="D789" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="E789" s="25" t="n">
+        <v>1</v>
+      </c>
+      <c r="G789" s="25" t="s">
         <v>130</v>
       </c>
       <c r="H789" s="1" t="s">
@@ -28318,16 +28216,16 @@
       <c r="B790" s="1" t="s">
         <v>999</v>
       </c>
-      <c r="C790" s="24" t="n">
+      <c r="C790" s="25" t="n">
         <v>5218</v>
       </c>
-      <c r="D790" s="24" t="s">
+      <c r="D790" s="25" t="s">
         <v>1000</v>
       </c>
-      <c r="E790" s="24" t="n">
-        <v>1</v>
-      </c>
-      <c r="G790" s="24" t="s">
+      <c r="E790" s="25" t="n">
+        <v>1</v>
+      </c>
+      <c r="G790" s="25" t="s">
         <v>1002</v>
       </c>
       <c r="H790" s="1" t="s">
@@ -28344,16 +28242,16 @@
       <c r="B791" s="1" t="s">
         <v>1004</v>
       </c>
-      <c r="C791" s="24" t="n">
+      <c r="C791" s="25" t="n">
         <v>5234</v>
       </c>
-      <c r="D791" s="24" t="s">
+      <c r="D791" s="25" t="s">
         <v>1000</v>
       </c>
-      <c r="E791" s="24" t="n">
-        <v>1</v>
-      </c>
-      <c r="G791" s="24" t="s">
+      <c r="E791" s="25" t="n">
+        <v>1</v>
+      </c>
+      <c r="G791" s="25" t="s">
         <v>1005</v>
       </c>
       <c r="H791" s="1" t="s">
@@ -28367,16 +28265,16 @@
       <c r="B792" s="1" t="s">
         <v>1006</v>
       </c>
-      <c r="C792" s="24" t="n">
+      <c r="C792" s="25" t="n">
         <v>5250</v>
       </c>
-      <c r="D792" s="24" t="s">
+      <c r="D792" s="25" t="s">
         <v>1000</v>
       </c>
-      <c r="E792" s="24" t="n">
-        <v>1</v>
-      </c>
-      <c r="G792" s="24" t="s">
+      <c r="E792" s="25" t="n">
+        <v>1</v>
+      </c>
+      <c r="G792" s="25" t="s">
         <v>1007</v>
       </c>
       <c r="H792" s="1" t="s">
@@ -28390,16 +28288,16 @@
       <c r="B793" s="1" t="s">
         <v>1008</v>
       </c>
-      <c r="C793" s="24" t="n">
+      <c r="C793" s="25" t="n">
         <v>5266</v>
       </c>
-      <c r="D793" s="24" t="s">
+      <c r="D793" s="25" t="s">
         <v>1000</v>
       </c>
-      <c r="E793" s="24" t="n">
-        <v>1</v>
-      </c>
-      <c r="G793" s="24" t="s">
+      <c r="E793" s="25" t="n">
+        <v>1</v>
+      </c>
+      <c r="G793" s="25" t="s">
         <v>1009</v>
       </c>
       <c r="H793" s="1" t="s">
@@ -28413,16 +28311,16 @@
       <c r="B794" s="1" t="s">
         <v>1010</v>
       </c>
-      <c r="C794" s="24" t="n">
+      <c r="C794" s="25" t="n">
         <v>5282</v>
       </c>
-      <c r="D794" s="24" t="s">
+      <c r="D794" s="25" t="s">
         <v>1000</v>
       </c>
-      <c r="E794" s="24" t="n">
-        <v>1</v>
-      </c>
-      <c r="G794" s="24" t="s">
+      <c r="E794" s="25" t="n">
+        <v>1</v>
+      </c>
+      <c r="G794" s="25" t="s">
         <v>1011</v>
       </c>
       <c r="H794" s="1" t="s">
@@ -28436,16 +28334,16 @@
       <c r="B795" s="1" t="s">
         <v>1012</v>
       </c>
-      <c r="C795" s="24" t="n">
+      <c r="C795" s="25" t="n">
         <v>5298</v>
       </c>
-      <c r="D795" s="24" t="s">
+      <c r="D795" s="25" t="s">
         <v>1000</v>
       </c>
-      <c r="E795" s="24" t="n">
-        <v>1</v>
-      </c>
-      <c r="G795" s="24" t="s">
+      <c r="E795" s="25" t="n">
+        <v>1</v>
+      </c>
+      <c r="G795" s="25" t="s">
         <v>1013</v>
       </c>
       <c r="H795" s="1" t="s">
@@ -28459,16 +28357,16 @@
       <c r="B796" s="1" t="s">
         <v>1014</v>
       </c>
-      <c r="C796" s="24" t="n">
+      <c r="C796" s="25" t="n">
         <v>5314</v>
       </c>
-      <c r="D796" s="24" t="s">
+      <c r="D796" s="25" t="s">
         <v>1000</v>
       </c>
-      <c r="E796" s="24" t="n">
-        <v>1</v>
-      </c>
-      <c r="G796" s="24" t="s">
+      <c r="E796" s="25" t="n">
+        <v>1</v>
+      </c>
+      <c r="G796" s="25" t="s">
         <v>1015</v>
       </c>
       <c r="H796" s="1" t="s">
@@ -28482,16 +28380,16 @@
       <c r="B797" s="1" t="s">
         <v>1016</v>
       </c>
-      <c r="C797" s="24" t="n">
+      <c r="C797" s="25" t="n">
         <v>5330</v>
       </c>
-      <c r="D797" s="24" t="s">
+      <c r="D797" s="25" t="s">
         <v>1000</v>
       </c>
-      <c r="E797" s="24" t="n">
-        <v>1</v>
-      </c>
-      <c r="G797" s="24" t="s">
+      <c r="E797" s="25" t="n">
+        <v>1</v>
+      </c>
+      <c r="G797" s="25" t="s">
         <v>1017</v>
       </c>
       <c r="H797" s="1" t="s">
@@ -28502,7 +28400,7 @@
       <c r="A798" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B798" s="24" t="s">
+      <c r="B798" s="25" t="s">
         <v>1236</v>
       </c>
       <c r="C798" s="1" t="n">
@@ -28589,7 +28487,7 @@
       <c r="A801" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B801" s="25" t="s">
+      <c r="B801" s="26" t="s">
         <v>1245</v>
       </c>
       <c r="C801" s="1" t="n">
@@ -29044,7 +28942,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -29056,20 +28954,20 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="22" width="7.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="22" width="7.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="22" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="22" width="65.01"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="4" style="22" width="8.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="27" t="s">
         <v>1281</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="27" t="s">
         <v>1282</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="27" t="s">
         <v>1283</v>
       </c>
     </row>
@@ -29237,24 +29135,24 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="27" t="n">
+      <c r="A22" s="28" t="n">
         <v>223</v>
       </c>
-      <c r="B22" s="27" t="n">
+      <c r="B22" s="28" t="n">
         <v>277</v>
       </c>
-      <c r="C22" s="27" t="s">
+      <c r="C22" s="28" t="s">
         <v>1285</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="27" t="n">
+      <c r="A23" s="28" t="n">
         <v>224</v>
       </c>
-      <c r="B23" s="27" t="n">
+      <c r="B23" s="28" t="n">
         <v>278</v>
       </c>
-      <c r="C23" s="27" t="s">
+      <c r="C23" s="28" t="s">
         <v>1286</v>
       </c>
     </row>
@@ -29270,57 +29168,57 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="27" t="n">
+      <c r="A25" s="28" t="n">
         <v>226</v>
       </c>
-      <c r="B25" s="27" t="n">
+      <c r="B25" s="28" t="n">
         <v>279</v>
       </c>
-      <c r="C25" s="27" t="s">
+      <c r="C25" s="28" t="s">
         <v>1288</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="27" t="n">
+      <c r="A26" s="28" t="n">
         <v>227</v>
       </c>
-      <c r="B26" s="27" t="n">
+      <c r="B26" s="28" t="n">
         <v>276</v>
       </c>
-      <c r="C26" s="27" t="s">
+      <c r="C26" s="28" t="s">
         <v>1289</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="27" t="n">
+      <c r="A27" s="28" t="n">
         <v>228</v>
       </c>
-      <c r="B27" s="27" t="n">
+      <c r="B27" s="28" t="n">
         <v>275</v>
       </c>
-      <c r="C27" s="27" t="s">
+      <c r="C27" s="28" t="s">
         <v>1290</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="27" t="n">
+      <c r="A28" s="28" t="n">
         <v>229</v>
       </c>
-      <c r="B28" s="27" t="n">
+      <c r="B28" s="28" t="n">
         <v>274</v>
       </c>
-      <c r="C28" s="27" t="s">
+      <c r="C28" s="28" t="s">
         <v>1291</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="27" t="n">
+      <c r="A29" s="28" t="n">
         <v>230</v>
       </c>
-      <c r="B29" s="27" t="n">
+      <c r="B29" s="28" t="n">
         <v>273</v>
       </c>
-      <c r="C29" s="27" t="s">
+      <c r="C29" s="28" t="s">
         <v>1292</v>
       </c>
     </row>
@@ -29424,35 +29322,35 @@
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="27" t="n">
+      <c r="A39" s="28" t="n">
         <v>242</v>
       </c>
-      <c r="B39" s="27" t="n">
+      <c r="B39" s="28" t="n">
         <v>261</v>
       </c>
-      <c r="C39" s="27" t="s">
+      <c r="C39" s="28" t="s">
         <v>1302</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="27" t="n">
+      <c r="A40" s="28" t="n">
         <v>243</v>
       </c>
-      <c r="B40" s="27" t="n">
+      <c r="B40" s="28" t="n">
         <v>260</v>
       </c>
-      <c r="C40" s="27" t="s">
+      <c r="C40" s="28" t="s">
         <v>1303</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="27" t="n">
+      <c r="A41" s="28" t="n">
         <v>244</v>
       </c>
-      <c r="B41" s="27" t="n">
-        <v>259</v>
-      </c>
-      <c r="C41" s="27"/>
+      <c r="B41" s="28" t="n">
+        <v>259</v>
+      </c>
+      <c r="C41" s="28"/>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="22" t="n">
@@ -29461,7 +29359,7 @@
       <c r="B42" s="22" t="n">
         <v>258</v>
       </c>
-      <c r="C42" s="27" t="s">
+      <c r="C42" s="28" t="s">
         <v>1304</v>
       </c>
     </row>
@@ -29488,24 +29386,24 @@
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="28" t="s">
+      <c r="A46" s="29" t="s">
         <v>1307</v>
       </c>
-      <c r="B46" s="28"/>
-      <c r="C46" s="28"/>
-      <c r="D46" s="28"/>
-      <c r="E46" s="28"/>
-      <c r="F46" s="28"/>
+      <c r="B46" s="29"/>
+      <c r="C46" s="29"/>
+      <c r="D46" s="29"/>
+      <c r="E46" s="29"/>
+      <c r="F46" s="29"/>
     </row>
     <row r="47" customFormat="false" ht="92.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="29" t="s">
+      <c r="A47" s="30" t="s">
         <v>1308</v>
       </c>
-      <c r="B47" s="29"/>
-      <c r="C47" s="29"/>
-      <c r="D47" s="29"/>
-      <c r="E47" s="29"/>
-      <c r="F47" s="29"/>
+      <c r="B47" s="30"/>
+      <c r="C47" s="30"/>
+      <c r="D47" s="30"/>
+      <c r="E47" s="30"/>
+      <c r="F47" s="30"/>
     </row>
     <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -29537,7 +29435,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -29779,7 +29677,7 @@
       </c>
     </row>
     <row r="39" customFormat="false" ht="54.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C39" s="30" t="s">
+      <c r="C39" s="31" t="s">
         <v>1358</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix path for peakshaving import limit
It isn't called Settings/CGwacs/AcImportLimit, but Settings/CGwacs/AcInputLimit.
</commit_message>
<xml_diff>
--- a/CCGX-Modbus-TCP-register-list.xlsx
+++ b/CCGX-Modbus-TCP-register-list.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Field list" sheetId="1" state="visible" r:id="rId2"/>
@@ -2589,7 +2589,7 @@
     <t xml:space="preserve">AC import limit when peakshaving</t>
   </si>
   <si>
-    <t xml:space="preserve">/Settings/CGwacs/AcImportLimit</t>
+    <t xml:space="preserve">/Settings/Cgwacs/AcInputLimit</t>
   </si>
   <si>
     <t xml:space="preserve">Mode for peakshaving</t>
@@ -5196,13 +5196,13 @@
   </sheetPr>
   <dimension ref="A1:N1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="2" topLeftCell="A373" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="F386" activeCellId="0" sqref="F386"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.01171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="30.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="37.43"/>
@@ -9614,7 +9614,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="1" t="s">
         <v>397</v>
       </c>
@@ -29098,8 +29098,8 @@
     <hyperlink ref="I795" r:id="rId3" location="error-codes" display="See https://github.com/victronenergy/venus/wiki/dbus#error-codes"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -29118,7 +29118,7 @@
       <selection pane="topLeft" activeCell="B48" activeCellId="0" sqref="B48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="22" width="7.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="22" width="16"/>
@@ -29591,8 +29591,8 @@
     <mergeCell ref="A47:F47"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -29607,11 +29607,11 @@
   </sheetPr>
   <dimension ref="A1:C157"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A135" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A135" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B157" activeCellId="0" sqref="B157"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="22" width="8.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="22" width="3.43"/>
@@ -30556,8 +30556,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
update enum of inverter mode
The older list of values derived from Phoenix inverters. This
is more complete to also accommodate Inverter RS and others.
</commit_message>
<xml_diff>
--- a/CCGX-Modbus-TCP-register-list.xlsx
+++ b/CCGX-Modbus-TCP-register-list.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Field list" sheetId="1" state="visible" r:id="rId2"/>
@@ -2835,7 +2835,7 @@
     <t xml:space="preserve">Inverter on/off/eco</t>
   </si>
   <si>
-    <t xml:space="preserve">2=On;4=Off;5=Eco</t>
+    <t xml:space="preserve">1=Charger only,2=Inverter only;3=On;4=Off;5=Low Power/Eco;251=Passthrough;252=Standby;253=Hibernate</t>
   </si>
   <si>
     <t xml:space="preserve">Inverter model</t>
@@ -5232,10 +5232,10 @@
   </sheetPr>
   <dimension ref="A1:N841"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="2" topLeftCell="A549" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="2" topLeftCell="A416" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A567" activeCellId="0" sqref="A567"/>
+      <selection pane="bottomLeft" activeCell="A426" activeCellId="0" sqref="A426"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -17939,7 +17939,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="426" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="426" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A426" s="1" t="s">
         <v>918</v>
       </c>
@@ -30102,7 +30102,7 @@
   </sheetPr>
   <dimension ref="A1:C159"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A137" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A137" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B159" activeCellId="0" sqref="B159"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add extra DESS strategies
0=Target SOC;1=Self-consumption;2=Pro battery;3=Pro grid
</commit_message>
<xml_diff>
--- a/CCGX-Modbus-TCP-register-list.xlsx
+++ b/CCGX-Modbus-TCP-register-list.xlsx
@@ -4104,7 +4104,7 @@
     <t xml:space="preserve">/DynamicEss/Strategy</t>
   </si>
   <si>
-    <t xml:space="preserve">0=Target SOC;1=Self-consumption</t>
+    <t xml:space="preserve">0=Target SOC;1=Self-consumption;2=Pro battery;3=Pro grid</t>
   </si>
   <si>
     <t xml:space="preserve">The set target SOC for this time slot</t>
@@ -5270,17 +5270,17 @@
   </sheetPr>
   <dimension ref="A1:N1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="2" topLeftCell="A194" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A211" activeCellId="0" sqref="A211"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="2" topLeftCell="A838" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
+      <selection pane="bottomLeft" activeCell="I859" activeCellId="0" sqref="I859"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.01171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="30.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="37.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="8.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="8.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="8.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="10.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="26.62"/>
@@ -29979,8 +29979,8 @@
     <hyperlink ref="I831" r:id="rId3" location="error-codes" display="See https://github.com/victronenergy/venus/wiki/dbus#error-codes"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -29999,9 +29999,9 @@
       <selection pane="topLeft" activeCell="B48" activeCellId="0" sqref="B48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="22" width="7.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="22" width="7.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="22" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="22" width="65.01"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="4" style="22" width="8.57"/>
@@ -30472,8 +30472,8 @@
     <mergeCell ref="A47:F47"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -30492,7 +30492,7 @@
       <selection pane="topLeft" activeCell="B159" activeCellId="0" sqref="B159"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="22" width="8.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="22" width="3.43"/>
@@ -31450,8 +31450,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>